<commit_message>
chg: Added 4 new targets (added to OPAC.miz, joint target list and "Notia as candidate for air attack")
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Army HQs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="565">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -1754,6 +1753,30 @@
   </si>
   <si>
     <t xml:space="preserve">Target in "Country as candidate for air attack" </t>
+  </si>
+  <si>
+    <t>Apatite Veichle Factory</t>
+  </si>
+  <si>
+    <t>Military vehicle factory. Produce SA-15 (2x production lines)</t>
+  </si>
+  <si>
+    <t>Apatite SAM Factory</t>
+  </si>
+  <si>
+    <t>Apatite Radar Factory</t>
+  </si>
+  <si>
+    <t>SAM factory. Produce SA-11 TEL (2x production lines)</t>
+  </si>
+  <si>
+    <t>Radar factory for SAMs (3 production lines)</t>
+  </si>
+  <si>
+    <t>Apatite West Vehicle Factory</t>
+  </si>
+  <si>
+    <t>Military vehicle factory (2x production lines)</t>
   </si>
 </sst>
 </file>
@@ -2318,15 +2341,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2347,6 +2361,15 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2385,7 +2408,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2397,7 +2420,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2417,7 +2440,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2446,7 +2469,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2484,7 +2507,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2712,9 +2735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L825"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I18" sqref="I18"/>
+      <selection pane="topRight" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -2727,31 +2750,31 @@
     <col min="8" max="8" width="6.75" customWidth="1"/>
     <col min="9" max="9" width="52.625" customWidth="1"/>
     <col min="10" max="10" width="35" style="50" customWidth="1"/>
-    <col min="11" max="11" width="18.75" style="70" customWidth="1"/>
-    <col min="12" max="12" width="40.625" style="70" customWidth="1"/>
+    <col min="11" max="11" width="18.75" style="67" customWidth="1"/>
+    <col min="12" max="12" width="40.625" style="67" customWidth="1"/>
     <col min="13" max="27" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="49.5" customHeight="1">
       <c r="A1" s="22"/>
       <c r="B1" s="23"/>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="76" t="s">
         <v>552</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="74" t="s">
         <v>553</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="20"/>
       <c r="E2" s="21"/>
       <c r="F2" s="26"/>
@@ -2790,10 +2813,10 @@
       <c r="J3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="73" t="s">
         <v>555</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="73" t="s">
         <v>556</v>
       </c>
     </row>
@@ -2819,7 +2842,7 @@
       <c r="J4" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="K4" s="71" t="s">
         <v>554</v>
       </c>
     </row>
@@ -2846,7 +2869,7 @@
       <c r="J5" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -2873,7 +2896,7 @@
       <c r="J6" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="73" t="s">
+      <c r="K6" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -2900,7 +2923,7 @@
       <c r="J7" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="73" t="s">
+      <c r="K7" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -2927,7 +2950,7 @@
       <c r="J8" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -2958,7 +2981,7 @@
       <c r="J9" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="73" t="s">
+      <c r="K9" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -2989,7 +3012,7 @@
       <c r="J10" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -3432,7 +3455,7 @@
       <c r="J28" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="K28" s="73" t="s">
+      <c r="K28" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -3459,7 +3482,7 @@
       <c r="J29" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="K29" s="73" t="s">
+      <c r="K29" s="70" t="s">
         <v>554</v>
       </c>
     </row>
@@ -3486,6 +3509,9 @@
       <c r="J30" s="50" t="s">
         <v>136</v>
       </c>
+      <c r="K30" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="31" spans="1:12" s="62" customFormat="1" ht="14.25">
       <c r="A31" s="30" t="s">
@@ -3510,8 +3536,8 @@
       <c r="J31" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="K31" s="71"/>
-      <c r="L31" s="71"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
     </row>
     <row r="32" spans="1:12" ht="14.25">
       <c r="A32" s="28" t="s">
@@ -3560,8 +3586,8 @@
       <c r="J33" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="K33" s="71"/>
-      <c r="L33" s="71"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
     </row>
     <row r="34" spans="1:12" s="49" customFormat="1" ht="14.25">
       <c r="A34" s="44" t="s">
@@ -3586,8 +3612,8 @@
       <c r="J34" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="72"/>
-      <c r="L34" s="72"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="69"/>
     </row>
     <row r="35" spans="1:12" s="62" customFormat="1" ht="14.25">
       <c r="A35" s="30" t="s">
@@ -3612,8 +3638,8 @@
       <c r="J35" s="61" t="s">
         <v>158</v>
       </c>
-      <c r="K35" s="71"/>
-      <c r="L35" s="71"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
     </row>
     <row r="36" spans="1:12" ht="14.25">
       <c r="A36" s="28" t="s">
@@ -3662,8 +3688,8 @@
       <c r="J37" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="K37" s="71"/>
-      <c r="L37" s="71"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="68"/>
     </row>
     <row r="38" spans="1:12" ht="14.25">
       <c r="A38" s="28" t="s">
@@ -3712,8 +3738,8 @@
       <c r="J39" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="K39" s="71"/>
-      <c r="L39" s="71"/>
+      <c r="K39" s="68"/>
+      <c r="L39" s="68"/>
     </row>
     <row r="40" spans="1:12" ht="14.25">
       <c r="A40" s="28" t="s">
@@ -3762,8 +3788,8 @@
       <c r="J41" s="61" t="s">
         <v>183</v>
       </c>
-      <c r="K41" s="71"/>
-      <c r="L41" s="71"/>
+      <c r="K41" s="68"/>
+      <c r="L41" s="68"/>
     </row>
     <row r="42" spans="1:12" ht="14.25">
       <c r="A42" s="28" t="s">
@@ -3812,8 +3838,8 @@
       <c r="J43" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="K43" s="71"/>
-      <c r="L43" s="71"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="68"/>
     </row>
     <row r="44" spans="1:12" ht="14.25">
       <c r="A44" s="28" t="s">
@@ -3862,8 +3888,8 @@
       <c r="J45" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="K45" s="71"/>
-      <c r="L45" s="71"/>
+      <c r="K45" s="68"/>
+      <c r="L45" s="68"/>
     </row>
     <row r="46" spans="1:12" ht="14.25">
       <c r="A46" s="28" t="s">
@@ -3914,8 +3940,8 @@
       <c r="J47" s="61" t="s">
         <v>368</v>
       </c>
-      <c r="K47" s="71"/>
-      <c r="L47" s="71"/>
+      <c r="K47" s="68"/>
+      <c r="L47" s="68"/>
     </row>
     <row r="48" spans="1:12" ht="14.25">
       <c r="A48" s="28" t="s">
@@ -3968,8 +3994,10 @@
       <c r="J49" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="K49" s="71"/>
-      <c r="L49" s="71"/>
+      <c r="K49" s="70" t="s">
+        <v>554</v>
+      </c>
+      <c r="L49" s="68"/>
     </row>
     <row r="50" spans="1:12" ht="14.25">
       <c r="A50" s="28" t="s">
@@ -4022,8 +4050,8 @@
       <c r="J51" s="61" t="s">
         <v>384</v>
       </c>
-      <c r="K51" s="71"/>
-      <c r="L51" s="71"/>
+      <c r="K51" s="68"/>
+      <c r="L51" s="68"/>
     </row>
     <row r="52" spans="1:12" ht="14.25">
       <c r="A52" s="28" t="s">
@@ -4256,7 +4284,7 @@
       <c r="J60" s="65" t="s">
         <v>410</v>
       </c>
-      <c r="K60" s="75" t="s">
+      <c r="K60" s="72" t="s">
         <v>554</v>
       </c>
     </row>
@@ -4311,7 +4339,7 @@
       <c r="J62" s="65" t="s">
         <v>417</v>
       </c>
-      <c r="K62" s="75" t="s">
+      <c r="K62" s="72" t="s">
         <v>554</v>
       </c>
     </row>
@@ -4367,7 +4395,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15.75" customHeight="1">
+    <row r="65" spans="1:12" ht="15.75" customHeight="1">
       <c r="A65" s="28" t="s">
         <v>222</v>
       </c>
@@ -4393,7 +4421,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="15.75" customHeight="1">
+    <row r="66" spans="1:12" ht="15.75" customHeight="1">
       <c r="A66" s="28" t="s">
         <v>223</v>
       </c>
@@ -4419,7 +4447,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15.75" customHeight="1">
+    <row r="67" spans="1:12" ht="15.75" customHeight="1">
       <c r="A67" s="28" t="s">
         <v>224</v>
       </c>
@@ -4443,7 +4471,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="15.75" customHeight="1">
+    <row r="68" spans="1:12" ht="15.75" customHeight="1">
       <c r="A68" s="28" t="s">
         <v>225</v>
       </c>
@@ -4467,7 +4495,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="15.75" customHeight="1">
+    <row r="69" spans="1:12" ht="15.75" customHeight="1">
       <c r="A69" s="28" t="s">
         <v>226</v>
       </c>
@@ -4493,7 +4521,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15.75" customHeight="1">
+    <row r="70" spans="1:12" ht="15.75" customHeight="1">
       <c r="A70" s="28" t="s">
         <v>227</v>
       </c>
@@ -4519,7 +4547,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15.75" customHeight="1">
+    <row r="71" spans="1:12" ht="15.75" customHeight="1">
       <c r="A71" s="28" t="s">
         <v>228</v>
       </c>
@@ -4545,7 +4573,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.75" customHeight="1">
+    <row r="72" spans="1:12" ht="15.75" customHeight="1">
       <c r="A72" s="28" t="s">
         <v>229</v>
       </c>
@@ -4571,7 +4599,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15.75" customHeight="1">
+    <row r="73" spans="1:12" ht="15.75" customHeight="1">
       <c r="A73" s="28" t="s">
         <v>230</v>
       </c>
@@ -4596,63 +4624,103 @@
       <c r="J73" s="65" t="s">
         <v>445</v>
       </c>
-      <c r="K73" s="73" t="s">
+      <c r="K73" s="70" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15.75" customHeight="1">
+    <row r="74" spans="1:12" ht="15.75" customHeight="1">
       <c r="A74" s="28" t="s">
         <v>231</v>
       </c>
       <c r="B74" s="28"/>
-      <c r="C74" s="9"/>
+      <c r="C74" s="9" t="s">
+        <v>557</v>
+      </c>
       <c r="D74" s="10"/>
       <c r="E74" s="5"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="11"/>
-      <c r="I74" s="52"/>
-    </row>
-    <row r="75" spans="1:11" ht="15.75" customHeight="1">
+      <c r="I74" s="52" t="s">
+        <v>558</v>
+      </c>
+      <c r="K74" s="70" t="s">
+        <v>554</v>
+      </c>
+      <c r="L74" s="70" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="15.75" customHeight="1">
       <c r="A75" s="28" t="s">
         <v>232</v>
       </c>
       <c r="B75" s="30"/>
-      <c r="C75" s="57"/>
+      <c r="C75" s="57" t="s">
+        <v>559</v>
+      </c>
       <c r="D75" s="58"/>
       <c r="E75" s="59"/>
       <c r="F75" s="57"/>
       <c r="G75" s="57"/>
       <c r="H75" s="60"/>
-      <c r="I75" s="53"/>
-    </row>
-    <row r="76" spans="1:11" ht="15.75" customHeight="1">
+      <c r="I75" s="53" t="s">
+        <v>561</v>
+      </c>
+      <c r="K75" s="70" t="s">
+        <v>554</v>
+      </c>
+      <c r="L75" s="70" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="15.75" customHeight="1">
       <c r="A76" s="28" t="s">
         <v>233</v>
       </c>
       <c r="B76" s="28"/>
-      <c r="C76" s="9"/>
+      <c r="C76" s="9" t="s">
+        <v>560</v>
+      </c>
       <c r="D76" s="10"/>
       <c r="E76" s="5"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="11"/>
-      <c r="I76" s="52"/>
-    </row>
-    <row r="77" spans="1:11" ht="15.75" customHeight="1">
+      <c r="I76" s="52" t="s">
+        <v>562</v>
+      </c>
+      <c r="K76" s="70" t="s">
+        <v>554</v>
+      </c>
+      <c r="L76" s="70" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15.75" customHeight="1">
       <c r="A77" s="28" t="s">
         <v>234</v>
       </c>
       <c r="B77" s="30"/>
-      <c r="C77" s="6"/>
+      <c r="C77" s="6" t="s">
+        <v>563</v>
+      </c>
       <c r="D77" s="7"/>
       <c r="E77" s="8"/>
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="34"/>
-      <c r="I77" s="53"/>
-    </row>
-    <row r="78" spans="1:11" ht="15.75" customHeight="1">
+      <c r="I77" s="52" t="s">
+        <v>564</v>
+      </c>
+      <c r="K77" s="70" t="s">
+        <v>554</v>
+      </c>
+      <c r="L77" s="70" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15.75" customHeight="1">
       <c r="A78" s="28" t="s">
         <v>235</v>
       </c>
@@ -4665,7 +4733,7 @@
       <c r="H78" s="11"/>
       <c r="I78" s="52"/>
     </row>
-    <row r="79" spans="1:11" ht="15.75" customHeight="1">
+    <row r="79" spans="1:12" ht="15.75" customHeight="1">
       <c r="A79" s="28" t="s">
         <v>236</v>
       </c>
@@ -4678,7 +4746,7 @@
       <c r="H79" s="60"/>
       <c r="I79" s="53"/>
     </row>
-    <row r="80" spans="1:11" ht="15.75" customHeight="1">
+    <row r="80" spans="1:12" ht="15.75" customHeight="1">
       <c r="A80" s="28" t="s">
         <v>237</v>
       </c>
@@ -11833,11 +11901,11 @@
       <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="20"/>
       <c r="E2" s="21"/>
       <c r="F2" s="26"/>

</xml_diff>

<commit_message>
chg: Added the 4 new targets from previous commit to the CombatFlite file
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="566">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -1777,6 +1777,9 @@
   </si>
   <si>
     <t>Military vehicle factory (2x production lines)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67° 34.1905' N, 33° 22.0444' </t>
   </si>
 </sst>
 </file>
@@ -2408,7 +2411,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2420,7 +2423,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2440,7 +2443,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2469,7 +2472,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2507,7 +2510,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2737,7 +2740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D79" sqref="D79"/>
+      <selection pane="topRight" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4643,6 +4646,9 @@
       <c r="H74" s="11"/>
       <c r="I74" s="52" t="s">
         <v>558</v>
+      </c>
+      <c r="J74" s="50" t="s">
+        <v>565</v>
       </c>
       <c r="K74" s="70" t="s">
         <v>554</v>

</xml_diff>

<commit_message>
chg: Updated target effects with several new buildings effects, added two more targets from tgt list to .miz
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="566">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -2411,7 +2411,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2423,7 +2423,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2443,7 +2443,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2472,7 +2472,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2510,7 +2510,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2738,9 +2738,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L825"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A74" sqref="A74"/>
+      <selection pane="topRight" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4261,6 +4261,9 @@
       <c r="J59" s="65" t="s">
         <v>406</v>
       </c>
+      <c r="K59" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1">
       <c r="A60" s="28" t="s">
@@ -4315,6 +4318,9 @@
       </c>
       <c r="J61" s="65" t="s">
         <v>413</v>
+      </c>
+      <c r="K61" s="70" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
chg: Several targets from target list moved to OPAC.miz
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -77,12 +77,113 @@
         </r>
       </text>
     </comment>
+    <comment ref="M3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Neck: Will be deleted, but here for SA so we know what targets have target folders for execution
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neck: Coordinate seem to be on a soccer field in DCS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neck: No structure that can be targeted at that location?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neck: Is this correct? Did not look like a power station in DCS?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neck: Is this correct? Did not look like a power relay in DCS?</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="566">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -1779,7 +1880,7 @@
     <t>Military vehicle factory (2x production lines)</t>
   </si>
   <si>
-    <t xml:space="preserve">67° 34.1905' N, 33° 22.0444' </t>
+    <t>Target folder produced?</t>
   </si>
 </sst>
 </file>
@@ -2411,7 +2512,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2423,7 +2524,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2443,7 +2544,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2472,7 +2573,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2510,7 +2611,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2736,11 +2837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L825"/>
+  <dimension ref="A1:M825"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L54" sqref="L54"/>
+      <selection pane="topRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -2752,13 +2853,14 @@
     <col min="5" max="7" width="7.125" customWidth="1"/>
     <col min="8" max="8" width="6.75" customWidth="1"/>
     <col min="9" max="9" width="52.625" customWidth="1"/>
-    <col min="10" max="10" width="35" style="50" customWidth="1"/>
-    <col min="11" max="11" width="18.75" style="67" customWidth="1"/>
-    <col min="12" max="12" width="40.625" style="67" customWidth="1"/>
-    <col min="13" max="27" width="10" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="50" customWidth="1"/>
+    <col min="11" max="11" width="18.25" style="67" customWidth="1"/>
+    <col min="12" max="12" width="37.25" style="67" customWidth="1"/>
+    <col min="13" max="13" width="20.5" customWidth="1"/>
+    <col min="14" max="27" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="49.5" customHeight="1">
+    <row r="1" spans="1:13" ht="49.5" customHeight="1">
       <c r="A1" s="22"/>
       <c r="B1" s="23"/>
       <c r="C1" s="76" t="s">
@@ -2772,7 +2874,7 @@
       <c r="I1" s="76"/>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1">
       <c r="A2" s="74" t="s">
         <v>553</v>
       </c>
@@ -2785,7 +2887,7 @@
       <c r="H2" s="32"/>
       <c r="I2" s="55"/>
     </row>
-    <row r="3" spans="1:12" ht="29.25" customHeight="1" thickBot="1">
+    <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1">
       <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
@@ -2822,8 +2924,11 @@
       <c r="L3" s="73" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="14.25">
+      <c r="M3" s="73" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="14.25">
       <c r="A4" s="28" t="s">
         <v>12</v>
       </c>
@@ -2849,7 +2954,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.25">
+    <row r="5" spans="1:13" ht="14.25">
       <c r="A5" s="30" t="s">
         <v>18</v>
       </c>
@@ -2876,7 +2981,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.25">
+    <row r="6" spans="1:13" ht="14.25">
       <c r="A6" s="28" t="s">
         <v>22</v>
       </c>
@@ -2903,7 +3008,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.25">
+    <row r="7" spans="1:13" ht="14.25">
       <c r="A7" s="30" t="s">
         <v>27</v>
       </c>
@@ -2930,7 +3035,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.25">
+    <row r="8" spans="1:13" ht="14.25">
       <c r="A8" s="28" t="s">
         <v>32</v>
       </c>
@@ -2957,7 +3062,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.25">
+    <row r="9" spans="1:13" ht="14.25">
       <c r="A9" s="30" t="s">
         <v>36</v>
       </c>
@@ -2988,7 +3093,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.25">
+    <row r="10" spans="1:13" ht="14.25">
       <c r="A10" s="28" t="s">
         <v>42</v>
       </c>
@@ -3019,7 +3124,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.25">
+    <row r="11" spans="1:13" ht="14.25">
       <c r="A11" s="30" t="s">
         <v>46</v>
       </c>
@@ -3047,7 +3152,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.25">
+    <row r="12" spans="1:13" ht="14.25">
       <c r="A12" s="28" t="s">
         <v>49</v>
       </c>
@@ -3075,7 +3180,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14.25">
+    <row r="13" spans="1:13" ht="14.25">
       <c r="A13" s="30" t="s">
         <v>52</v>
       </c>
@@ -3099,7 +3204,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="14.25">
+    <row r="14" spans="1:13" ht="14.25">
       <c r="A14" s="28" t="s">
         <v>56</v>
       </c>
@@ -3123,7 +3228,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="14.25">
+    <row r="15" spans="1:13" ht="14.25">
       <c r="A15" s="30" t="s">
         <v>61</v>
       </c>
@@ -3147,7 +3252,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="14.25">
+    <row r="16" spans="1:13" ht="14.25">
       <c r="A16" s="28" t="s">
         <v>66</v>
       </c>
@@ -3290,6 +3395,9 @@
       <c r="J21" s="50" t="s">
         <v>93</v>
       </c>
+      <c r="K21" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="14.25">
       <c r="A22" s="28" t="s">
@@ -3314,6 +3422,9 @@
       <c r="J22" s="50" t="s">
         <v>98</v>
       </c>
+      <c r="K22" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="14.25">
       <c r="A23" s="30" t="s">
@@ -3539,7 +3650,9 @@
       <c r="J31" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="K31" s="68"/>
+      <c r="K31" s="70" t="s">
+        <v>554</v>
+      </c>
       <c r="L31" s="68"/>
     </row>
     <row r="32" spans="1:12" ht="14.25">
@@ -3565,6 +3678,9 @@
       <c r="J32" s="50" t="s">
         <v>144</v>
       </c>
+      <c r="K32" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="33" spans="1:12" s="62" customFormat="1" ht="14.25">
       <c r="A33" s="30" t="s">
@@ -3943,7 +4059,9 @@
       <c r="J47" s="61" t="s">
         <v>368</v>
       </c>
-      <c r="K47" s="68"/>
+      <c r="K47" s="70" t="s">
+        <v>554</v>
+      </c>
       <c r="L47" s="68"/>
     </row>
     <row r="48" spans="1:12" ht="14.25">
@@ -3971,6 +4089,9 @@
       <c r="J48" s="50" t="s">
         <v>373</v>
       </c>
+      <c r="K48" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="49" spans="1:12" s="62" customFormat="1" ht="14.25">
       <c r="A49" s="28" t="s">
@@ -4081,6 +4202,9 @@
       <c r="J52" s="50" t="s">
         <v>387</v>
       </c>
+      <c r="K52" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="53" spans="1:12" ht="14.25">
       <c r="A53" s="28" t="s">
@@ -4106,6 +4230,9 @@
       </c>
       <c r="J53" s="50" t="s">
         <v>389</v>
+      </c>
+      <c r="K53" s="70" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1">
@@ -4209,6 +4336,9 @@
       <c r="J57" s="50" t="s">
         <v>401</v>
       </c>
+      <c r="K57" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="28" t="s">
@@ -4234,6 +4364,9 @@
       </c>
       <c r="J58" s="50" t="s">
         <v>403</v>
+      </c>
+      <c r="K58" s="70" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1">
@@ -4652,9 +4785,6 @@
       <c r="H74" s="11"/>
       <c r="I74" s="52" t="s">
         <v>558</v>
-      </c>
-      <c r="J74" s="50" t="s">
-        <v>565</v>
       </c>
       <c r="K74" s="70" t="s">
         <v>554</v>

</xml_diff>

<commit_message>
chg: Added more tgt effects, added 3 additional targets form target list into OPAC.miz (for creating tgt folders), added coordinates to last 4 targets in tgt list
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -92,6 +92,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="C14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Neck: The coordinate is not on a specific building</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C21" authorId="0">
       <text>
         <r>
@@ -183,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="570">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -1881,6 +1895,18 @@
   </si>
   <si>
     <t>Target folder produced?</t>
+  </si>
+  <si>
+    <t>N 67 34.190 E 033 22.043</t>
+  </si>
+  <si>
+    <t>N 67 34.984 E 033 23.011</t>
+  </si>
+  <si>
+    <t>N 67 34.969 E 033 23.368</t>
+  </si>
+  <si>
+    <t>N 67 32.741 E 033 44.174</t>
   </si>
 </sst>
 </file>
@@ -2052,7 +2078,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2093,6 +2119,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -2287,7 +2325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2475,6 +2513,13 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2512,7 +2557,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC3B029-0E15-780F-5F6C-F4C89D73339B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2524,7 +2569,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2544,7 +2589,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2573,7 +2618,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{936A892A-9C6A-4256-9681-2089DBB6820F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2611,7 +2656,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3529DAF3-7791-4091-B9E6-ACAC5B7DA205}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2841,7 +2886,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C26" sqref="C26"/>
+      <selection pane="topRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -3203,6 +3248,9 @@
       <c r="J13" s="50" t="s">
         <v>55</v>
       </c>
+      <c r="K13" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="14.25">
       <c r="A14" s="28" t="s">
@@ -3211,7 +3259,7 @@
       <c r="B14" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="77" t="s">
         <v>57</v>
       </c>
       <c r="D14" s="10"/>
@@ -3227,6 +3275,9 @@
       <c r="J14" s="50" t="s">
         <v>60</v>
       </c>
+      <c r="K14" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="14.25">
       <c r="A15" s="30" t="s">
@@ -3251,6 +3302,9 @@
       <c r="J15" s="50" t="s">
         <v>65</v>
       </c>
+      <c r="K15" s="70" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="14.25">
       <c r="A16" s="28" t="s">
@@ -3379,7 +3433,7 @@
       <c r="B21" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="78" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="7"/>
@@ -3607,7 +3661,7 @@
       <c r="B30" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="77" t="s">
         <v>134</v>
       </c>
       <c r="D30" s="10"/>
@@ -4041,7 +4095,7 @@
       <c r="B47" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="57" t="s">
+      <c r="C47" s="77" t="s">
         <v>369</v>
       </c>
       <c r="D47" s="58" t="s">
@@ -4071,7 +4125,7 @@
       <c r="B48" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="63" t="s">
+      <c r="C48" s="79" t="s">
         <v>374</v>
       </c>
       <c r="D48" s="10" t="s">
@@ -4786,6 +4840,9 @@
       <c r="I74" s="52" t="s">
         <v>558</v>
       </c>
+      <c r="J74" s="50" t="s">
+        <v>566</v>
+      </c>
       <c r="K74" s="70" t="s">
         <v>554</v>
       </c>
@@ -4809,6 +4866,9 @@
       <c r="I75" s="53" t="s">
         <v>561</v>
       </c>
+      <c r="J75" s="50" t="s">
+        <v>567</v>
+      </c>
       <c r="K75" s="70" t="s">
         <v>554</v>
       </c>
@@ -4832,6 +4892,9 @@
       <c r="I76" s="52" t="s">
         <v>562</v>
       </c>
+      <c r="J76" s="50" t="s">
+        <v>568</v>
+      </c>
       <c r="K76" s="70" t="s">
         <v>554</v>
       </c>
@@ -4854,6 +4917,9 @@
       <c r="H77" s="34"/>
       <c r="I77" s="52" t="s">
         <v>564</v>
+      </c>
+      <c r="J77" s="50" t="s">
+        <v>569</v>
       </c>
       <c r="K77" s="70" t="s">
         <v>554</v>

</xml_diff>

<commit_message>
updated 'Notia candidate' docx with targets and descriptions and the excel's info on the file
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\OPAT-background\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D81C8-2645-473C-9191-B41724D6484A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C60C2C1-A6D4-4B40-BCF9-C0641299DE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="757">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -3640,6 +3640,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3649,71 +3656,8 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3754,6 +3698,69 @@
     <xf numFmtId="0" fontId="29" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3771,13 +3778,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5140,9 +5140,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L825"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A95" sqref="A95:B95"/>
+      <selection pane="topRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5162,22 +5162,22 @@
   <sheetData>
     <row r="1" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18"/>
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="120" t="s">
         <v>527</v>
       </c>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
       <c r="I1"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="118" t="s">
         <v>528</v>
       </c>
-      <c r="B2" s="116"/>
+      <c r="B2" s="119"/>
       <c r="C2" s="107"/>
       <c r="D2" s="17"/>
       <c r="E2" s="22"/>
@@ -5247,6 +5247,9 @@
       <c r="J4" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K4" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
@@ -5273,6 +5276,9 @@
       <c r="J5" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K5" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
@@ -5299,6 +5305,9 @@
       <c r="J6" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K6" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
@@ -5325,6 +5334,9 @@
       <c r="J7" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K7" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
@@ -5351,6 +5363,9 @@
       <c r="J8" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K8" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
@@ -5379,6 +5394,9 @@
       <c r="J9" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K9" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
@@ -5407,6 +5425,9 @@
       <c r="J10" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K10" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
@@ -5432,6 +5453,9 @@
       <c r="I11" s="44" t="s">
         <v>47</v>
       </c>
+      <c r="K11" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
@@ -5456,6 +5480,9 @@
       </c>
       <c r="I12" s="44" t="s">
         <v>50</v>
+      </c>
+      <c r="K12" s="63" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
@@ -5481,6 +5508,9 @@
         <v>53</v>
       </c>
       <c r="J13" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="K13" s="63" t="s">
         <v>529</v>
       </c>
     </row>
@@ -6254,7 +6284,7 @@
       <c r="A47" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="B47" s="159" t="s">
+      <c r="B47" s="115" t="s">
         <v>688</v>
       </c>
       <c r="C47" s="111">
@@ -6275,13 +6305,15 @@
       <c r="J47" s="63" t="s">
         <v>529</v>
       </c>
-      <c r="K47" s="61"/>
+      <c r="K47" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="B48" s="160" t="s">
+      <c r="B48" s="116" t="s">
         <v>686</v>
       </c>
       <c r="C48" s="110">
@@ -6302,6 +6334,9 @@
       <c r="J48" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K48" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="49" spans="1:11" s="55" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -6328,7 +6363,9 @@
       <c r="J49" s="63" t="s">
         <v>529</v>
       </c>
-      <c r="K49" s="61"/>
+      <c r="K49" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="50" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="24" t="s">
@@ -6355,6 +6392,9 @@
       <c r="J50" s="64" t="s">
         <v>529</v>
       </c>
+      <c r="K50" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="51" spans="1:11" s="55" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="24" t="s">
@@ -6381,7 +6421,9 @@
       <c r="J51" s="63" t="s">
         <v>529</v>
       </c>
-      <c r="K51" s="61"/>
+      <c r="K51" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="52" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="24" t="s">
@@ -6408,6 +6450,9 @@
       <c r="J52" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K52" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="53" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="24" t="s">
@@ -6434,6 +6479,9 @@
       <c r="J53" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K53" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="24" t="s">
@@ -6460,6 +6508,9 @@
       <c r="J54" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K54" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="24" t="s">
@@ -6486,6 +6537,9 @@
       <c r="J55" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K55" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="24" t="s">
@@ -6512,6 +6566,9 @@
       <c r="J56" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K56" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="24" t="s">
@@ -6538,6 +6595,9 @@
       <c r="J57" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K57" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="24" t="s">
@@ -6564,6 +6624,9 @@
       <c r="J58" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K58" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="24" t="s">
@@ -6590,6 +6653,9 @@
       <c r="J59" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K59" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="24" t="s">
@@ -6616,6 +6682,9 @@
       <c r="J60" s="64" t="s">
         <v>529</v>
       </c>
+      <c r="K60" s="64" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="24" t="s">
@@ -6642,6 +6711,9 @@
       <c r="J61" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K61" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="24" t="s">
@@ -6668,6 +6740,9 @@
       <c r="J62" s="64" t="s">
         <v>529</v>
       </c>
+      <c r="K62" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="24" t="s">
@@ -6694,6 +6769,9 @@
       <c r="J63" s="64" t="s">
         <v>529</v>
       </c>
+      <c r="K63" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="24" t="s">
@@ -6718,6 +6796,9 @@
         <v>402</v>
       </c>
       <c r="J64" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="K64" s="63" t="s">
         <v>529</v>
       </c>
     </row>
@@ -6872,6 +6953,9 @@
       <c r="J71" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K71" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
@@ -6898,6 +6982,9 @@
       <c r="J72" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K72" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
@@ -6922,6 +7009,9 @@
         <v>420</v>
       </c>
       <c r="J73" s="63" t="s">
+        <v>529</v>
+      </c>
+      <c r="K73" s="63" t="s">
         <v>529</v>
       </c>
     </row>
@@ -7058,6 +7148,9 @@
       <c r="J78" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K78" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
@@ -7084,6 +7177,9 @@
       <c r="J79" s="63" t="s">
         <v>529</v>
       </c>
+      <c r="K79" s="63" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
@@ -7110,8 +7206,11 @@
       <c r="J80" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K80" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
         <v>231</v>
       </c>
@@ -7136,8 +7235,11 @@
       <c r="J81" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K81" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="24" t="s">
         <v>232</v>
       </c>
@@ -7162,8 +7264,11 @@
       <c r="J82" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K82" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="24" t="s">
         <v>233</v>
       </c>
@@ -7188,8 +7293,11 @@
       <c r="J83" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K83" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="24" t="s">
         <v>234</v>
       </c>
@@ -7214,8 +7322,11 @@
       <c r="J84" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K84" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="24" t="s">
         <v>235</v>
       </c>
@@ -7240,8 +7351,11 @@
       <c r="J85" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K85" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="24" t="s">
         <v>236</v>
       </c>
@@ -7266,8 +7380,11 @@
       <c r="J86" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K86" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="24" t="s">
         <v>237</v>
       </c>
@@ -7292,8 +7409,11 @@
       <c r="J87" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K87" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="24" t="s">
         <v>238</v>
       </c>
@@ -7318,8 +7438,11 @@
       <c r="J88" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K88" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="24" t="s">
         <v>239</v>
       </c>
@@ -7344,8 +7467,11 @@
       <c r="J89" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K89" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="24" t="s">
         <v>240</v>
       </c>
@@ -7370,8 +7496,11 @@
       <c r="J90" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K90" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="24" t="s">
         <v>241</v>
       </c>
@@ -7396,8 +7525,11 @@
       <c r="J91" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K91" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="24" t="s">
         <v>242</v>
       </c>
@@ -7422,12 +7554,15 @@
       <c r="J92" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K92" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="B93" s="161" t="s">
+      <c r="B93" s="117" t="s">
         <v>748</v>
       </c>
       <c r="C93" s="111">
@@ -7448,8 +7583,11 @@
       <c r="J93" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K93" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="24" t="s">
         <v>244</v>
       </c>
@@ -7474,8 +7612,11 @@
       <c r="J94" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K94" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="24" t="s">
         <v>245</v>
       </c>
@@ -7500,8 +7641,11 @@
       <c r="J95" s="63" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K95" s="63" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="24" t="s">
         <v>246</v>
       </c>
@@ -13735,50 +13879,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="122" t="s">
         <v>637</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="142"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="124"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="125" t="s">
         <v>638</v>
       </c>
-      <c r="B2" s="144"/>
+      <c r="B2" s="126"/>
       <c r="C2" s="93" t="s">
         <v>683</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="D2" s="127" t="s">
         <v>639</v>
       </c>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="148" t="s">
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="130" t="s">
         <v>640</v>
       </c>
-      <c r="I2" s="149"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="150" t="s">
+      <c r="A4" s="132" t="s">
         <v>641</v>
       </c>
-      <c r="B4" s="151"/>
-      <c r="C4" s="151"/>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
-      <c r="H4" s="151"/>
-      <c r="I4" s="152"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="134"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="94" t="s">
@@ -13840,15 +13984,15 @@
       <c r="I6" s="99" t="s">
         <v>627</v>
       </c>
-      <c r="K6" s="134" t="s">
+      <c r="K6" s="121" t="s">
         <v>654</v>
       </c>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134"/>
-      <c r="Q6" s="134"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="97">
@@ -13878,15 +14022,15 @@
       <c r="I7" s="99" t="s">
         <v>624</v>
       </c>
-      <c r="K7" s="134" t="s">
+      <c r="K7" s="121" t="s">
         <v>662</v>
       </c>
-      <c r="L7" s="134"/>
-      <c r="M7" s="134"/>
-      <c r="N7" s="134"/>
-      <c r="O7" s="134"/>
-      <c r="P7" s="134"/>
-      <c r="Q7" s="134"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
+      <c r="N7" s="121"/>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="121"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="97">
@@ -14042,15 +14186,15 @@
       <c r="D17" s="98" t="s">
         <v>630</v>
       </c>
-      <c r="E17" s="130" t="s">
+      <c r="E17" s="140" t="s">
         <v>674</v>
       </c>
-      <c r="F17" s="131"/>
-      <c r="G17" s="130" t="s">
+      <c r="F17" s="141"/>
+      <c r="G17" s="140" t="s">
         <v>675</v>
       </c>
-      <c r="H17" s="132"/>
-      <c r="I17" s="133"/>
+      <c r="H17" s="142"/>
+      <c r="I17" s="143"/>
     </row>
     <row r="18" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A18" s="103">
@@ -14065,15 +14209,15 @@
       <c r="D18" s="98" t="s">
         <v>630</v>
       </c>
-      <c r="E18" s="130" t="s">
+      <c r="E18" s="140" t="s">
         <v>674</v>
       </c>
-      <c r="F18" s="131"/>
-      <c r="G18" s="130" t="s">
+      <c r="F18" s="141"/>
+      <c r="G18" s="140" t="s">
         <v>677</v>
       </c>
-      <c r="H18" s="132"/>
-      <c r="I18" s="133"/>
+      <c r="H18" s="142"/>
+      <c r="I18" s="143"/>
     </row>
     <row r="19" spans="1:11" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A19" s="103">
@@ -14088,15 +14232,15 @@
       <c r="D19" s="98" t="s">
         <v>633</v>
       </c>
-      <c r="E19" s="130" t="s">
+      <c r="E19" s="140" t="s">
         <v>679</v>
       </c>
-      <c r="F19" s="131"/>
-      <c r="G19" s="130" t="s">
+      <c r="F19" s="141"/>
+      <c r="G19" s="140" t="s">
         <v>680</v>
       </c>
-      <c r="H19" s="132"/>
-      <c r="I19" s="133"/>
+      <c r="H19" s="142"/>
+      <c r="I19" s="143"/>
       <c r="K19" t="s">
         <v>681</v>
       </c>
@@ -14108,11 +14252,11 @@
       <c r="B20" s="88"/>
       <c r="C20" s="88"/>
       <c r="D20" s="88"/>
-      <c r="E20" s="118"/>
-      <c r="F20" s="119"/>
-      <c r="G20" s="118"/>
-      <c r="H20" s="120"/>
-      <c r="I20" s="121"/>
+      <c r="E20" s="144"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="147"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="103">
@@ -14121,11 +14265,11 @@
       <c r="B21" s="88"/>
       <c r="C21" s="88"/>
       <c r="D21" s="88"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="120"/>
-      <c r="I21" s="121"/>
+      <c r="E21" s="144"/>
+      <c r="F21" s="145"/>
+      <c r="G21" s="144"/>
+      <c r="H21" s="146"/>
+      <c r="I21" s="147"/>
       <c r="K21" t="s">
         <v>682</v>
       </c>
@@ -14137,11 +14281,11 @@
       <c r="B22" s="88"/>
       <c r="C22" s="88"/>
       <c r="D22" s="88"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="120"/>
-      <c r="I22" s="121"/>
+      <c r="E22" s="144"/>
+      <c r="F22" s="145"/>
+      <c r="G22" s="144"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="147"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="103">
@@ -14150,11 +14294,11 @@
       <c r="B23" s="88"/>
       <c r="C23" s="88"/>
       <c r="D23" s="88"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="120"/>
-      <c r="I23" s="121"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="145"/>
+      <c r="G23" s="144"/>
+      <c r="H23" s="146"/>
+      <c r="I23" s="147"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="103">
@@ -14163,11 +14307,11 @@
       <c r="B24" s="88"/>
       <c r="C24" s="88"/>
       <c r="D24" s="88"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="120"/>
-      <c r="I24" s="121"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="145"/>
+      <c r="G24" s="144"/>
+      <c r="H24" s="146"/>
+      <c r="I24" s="147"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="103">
@@ -14176,11 +14320,11 @@
       <c r="B25" s="104"/>
       <c r="C25" s="104"/>
       <c r="D25" s="104"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="122"/>
-      <c r="H25" s="124"/>
-      <c r="I25" s="125"/>
+      <c r="E25" s="148"/>
+      <c r="F25" s="149"/>
+      <c r="G25" s="148"/>
+      <c r="H25" s="150"/>
+      <c r="I25" s="151"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="105">
@@ -14189,44 +14333,44 @@
       <c r="B26" s="101"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
-      <c r="E26" s="126"/>
-      <c r="F26" s="127"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="129"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="153"/>
+      <c r="G26" s="152"/>
+      <c r="H26" s="154"/>
+      <c r="I26" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="K6:Q6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14272,11 +14416,11 @@
       <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="22"/>
@@ -14394,10 +14538,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="156" t="s">
         <v>545</v>
       </c>
-      <c r="C2" s="153"/>
+      <c r="C2" s="156"/>
       <c r="O2" t="s">
         <v>546</v>
       </c>
@@ -14637,56 +14781,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="156" t="s">
         <v>578</v>
       </c>
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
+      <c r="B3" s="156"/>
+      <c r="C3" s="156"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
         <v>579</v>
       </c>
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="158" t="s">
         <v>580</v>
       </c>
-      <c r="C4" s="155"/>
+      <c r="C4" s="158"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="73" t="s">
         <v>581</v>
       </c>
-      <c r="B5" s="154" t="s">
+      <c r="B5" s="157" t="s">
         <v>582</v>
       </c>
-      <c r="C5" s="154"/>
+      <c r="C5" s="157"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="73" t="s">
         <v>583</v>
       </c>
-      <c r="B6" s="154" t="s">
+      <c r="B6" s="157" t="s">
         <v>584</v>
       </c>
-      <c r="C6" s="154"/>
+      <c r="C6" s="157"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="157" t="s">
         <v>585</v>
       </c>
-      <c r="C7" s="154"/>
+      <c r="C7" s="157"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="73" t="s">
         <v>586</v>
       </c>
-      <c r="B8" s="154" t="s">
+      <c r="B8" s="157" t="s">
         <v>587</v>
       </c>
-      <c r="C8" s="154"/>
+      <c r="C8" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -14719,11 +14863,11 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="159" t="s">
         <v>588</v>
       </c>
-      <c r="C2" s="157"/>
-      <c r="D2" s="158"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="161"/>
       <c r="J2" t="s">
         <v>546</v>
       </c>
@@ -14901,11 +15045,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="155" t="s">
+      <c r="A5" s="158" t="s">
         <v>621</v>
       </c>
-      <c r="B5" s="155"/>
-      <c r="C5" s="155"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">

</xml_diff>

<commit_message>
chg: Updated target list with assigned targets for production for Jonde and Varzat
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="784">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -2396,6 +2396,15 @@
   </si>
   <si>
     <t>Dark green with a v means the DPIs are also visible as triggerzones (for use in tgt folder)</t>
+  </si>
+  <si>
+    <t>Target folder in production</t>
+  </si>
+  <si>
+    <t>Jonde</t>
+  </si>
+  <si>
+    <t>Varzat</t>
   </si>
 </sst>
 </file>
@@ -3256,7 +3265,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3693,6 +3702,12 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3705,6 +3720,75 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3741,75 +3825,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3834,11 +3849,8 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3878,7 +3890,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3890,7 +3902,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3910,7 +3922,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3939,7 +3951,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3988,7 +4000,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4033,7 +4045,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4078,7 +4090,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4116,7 +4128,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4164,7 +4176,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4217,7 +4229,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4270,7 +4282,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4368,7 +4380,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4421,7 +4433,7 @@
         <xdr:cNvPr id="3" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4474,7 +4486,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4568,7 +4580,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4621,7 +4633,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4716,7 +4728,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4774,7 +4786,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4827,7 +4839,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4919,7 +4931,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4972,7 +4984,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5199,11 +5211,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J825"/>
+  <dimension ref="A1:K825"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I33" sqref="I33"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5216,21 +5230,22 @@
     <col min="6" max="6" width="25.5" style="43" customWidth="1"/>
     <col min="7" max="7" width="6.75" customWidth="1"/>
     <col min="8" max="8" width="20.25" style="55" customWidth="1"/>
-    <col min="9" max="9" width="47.125" style="55" customWidth="1"/>
+    <col min="9" max="9" width="47.375" style="55" customWidth="1"/>
     <col min="10" max="10" width="20.5" customWidth="1"/>
-    <col min="11" max="24" width="10" customWidth="1"/>
+    <col min="11" max="11" width="21.125" customWidth="1"/>
+    <col min="12" max="24" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49.5" customHeight="1">
-      <c r="A1" s="174" t="s">
+    <row r="1" spans="1:11" ht="49.5" customHeight="1">
+      <c r="A1" s="176" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
       <c r="H1" s="160" t="s">
         <v>722</v>
       </c>
@@ -5240,24 +5255,26 @@
       <c r="J1" s="160" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="35.25" thickBot="1">
-      <c r="A2" s="172" t="s">
+      <c r="K1" s="61"/>
+    </row>
+    <row r="2" spans="1:11" ht="35.25" thickBot="1">
+      <c r="A2" s="174" t="s">
         <v>493</v>
       </c>
-      <c r="B2" s="173"/>
+      <c r="B2" s="175"/>
       <c r="C2" s="104"/>
       <c r="D2" s="105"/>
       <c r="E2" s="106"/>
       <c r="F2" s="106"/>
       <c r="G2" s="107"/>
-      <c r="H2" s="220" t="s">
+      <c r="H2" s="173" t="s">
         <v>780</v>
       </c>
       <c r="I2" s="60"/>
       <c r="J2" s="61"/>
-    </row>
-    <row r="3" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
+      <c r="K2" s="61"/>
+    </row>
+    <row r="3" spans="1:11" ht="29.25" customHeight="1" thickBot="1">
       <c r="A3" s="108" t="s">
         <v>2</v>
       </c>
@@ -5288,8 +5305,11 @@
       <c r="J3" s="161" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="14.25">
+      <c r="K3" s="221" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.25">
       <c r="A4" s="24" t="s">
         <v>12</v>
       </c>
@@ -5316,8 +5336,9 @@
         <v>494</v>
       </c>
       <c r="J4" s="61"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.25">
+      <c r="K4" s="61"/>
+    </row>
+    <row r="5" spans="1:11" ht="14.25">
       <c r="A5" s="126" t="s">
         <v>17</v>
       </c>
@@ -5344,8 +5365,11 @@
         <v>494</v>
       </c>
       <c r="J5" s="61"/>
-    </row>
-    <row r="6" spans="1:10" ht="14.25">
+      <c r="K5" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.25">
       <c r="A6" s="24" t="s">
         <v>21</v>
       </c>
@@ -5372,8 +5396,11 @@
         <v>494</v>
       </c>
       <c r="J6" s="61"/>
-    </row>
-    <row r="7" spans="1:10" ht="14.25">
+      <c r="K6" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.25">
       <c r="A7" s="126" t="s">
         <v>26</v>
       </c>
@@ -5400,8 +5427,11 @@
         <v>494</v>
       </c>
       <c r="J7" s="61"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.25">
+      <c r="K7" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="14.25">
       <c r="A8" s="24" t="s">
         <v>31</v>
       </c>
@@ -5428,8 +5458,9 @@
         <v>494</v>
       </c>
       <c r="J8" s="61"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.25">
+      <c r="K8" s="61"/>
+    </row>
+    <row r="9" spans="1:11" ht="14.25">
       <c r="A9" s="126" t="s">
         <v>35</v>
       </c>
@@ -5458,8 +5489,9 @@
         <v>494</v>
       </c>
       <c r="J9" s="61"/>
-    </row>
-    <row r="10" spans="1:10" ht="14.25">
+      <c r="K9" s="61"/>
+    </row>
+    <row r="10" spans="1:11" ht="14.25">
       <c r="A10" s="24" t="s">
         <v>41</v>
       </c>
@@ -5488,8 +5520,9 @@
         <v>494</v>
       </c>
       <c r="J10" s="61"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.25">
+      <c r="K10" s="61"/>
+    </row>
+    <row r="11" spans="1:11" ht="14.25">
       <c r="A11" s="126" t="s">
         <v>45</v>
       </c>
@@ -5516,8 +5549,9 @@
         <v>494</v>
       </c>
       <c r="J11" s="61"/>
-    </row>
-    <row r="12" spans="1:10" ht="14.25">
+      <c r="K11" s="61"/>
+    </row>
+    <row r="12" spans="1:11" ht="14.25">
       <c r="A12" s="24" t="s">
         <v>48</v>
       </c>
@@ -5544,8 +5578,9 @@
         <v>494</v>
       </c>
       <c r="J12" s="61"/>
-    </row>
-    <row r="13" spans="1:10" ht="14.25">
+      <c r="K12" s="61"/>
+    </row>
+    <row r="13" spans="1:11" ht="14.25">
       <c r="A13" s="126" t="s">
         <v>51</v>
       </c>
@@ -5572,8 +5607,9 @@
         <v>494</v>
       </c>
       <c r="J13" s="61"/>
-    </row>
-    <row r="14" spans="1:10" ht="14.25">
+      <c r="K13" s="61"/>
+    </row>
+    <row r="14" spans="1:11" ht="14.25">
       <c r="A14" s="24" t="s">
         <v>54</v>
       </c>
@@ -5598,8 +5634,11 @@
         <v>494</v>
       </c>
       <c r="J14" s="61"/>
-    </row>
-    <row r="15" spans="1:10" ht="14.25">
+      <c r="K14" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.25">
       <c r="A15" s="126" t="s">
         <v>56</v>
       </c>
@@ -5626,8 +5665,11 @@
         <v>494</v>
       </c>
       <c r="J15" s="61"/>
-    </row>
-    <row r="16" spans="1:10" ht="14.25">
+      <c r="K15" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.25">
       <c r="A16" s="24" t="s">
         <v>57</v>
       </c>
@@ -5654,8 +5696,11 @@
         <v>494</v>
       </c>
       <c r="J16" s="61"/>
-    </row>
-    <row r="17" spans="1:10" ht="14.25">
+      <c r="K16" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="14.25">
       <c r="A17" s="126" t="s">
         <v>58</v>
       </c>
@@ -5682,8 +5727,11 @@
         <v>494</v>
       </c>
       <c r="J17" s="61"/>
-    </row>
-    <row r="18" spans="1:10" ht="14.25">
+      <c r="K17" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.25">
       <c r="A18" s="24" t="s">
         <v>59</v>
       </c>
@@ -5705,8 +5753,9 @@
         <v>494</v>
       </c>
       <c r="J18" s="61"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.25">
+      <c r="K18" s="61"/>
+    </row>
+    <row r="19" spans="1:11" ht="14.25">
       <c r="A19" s="126" t="s">
         <v>61</v>
       </c>
@@ -5733,8 +5782,9 @@
         <v>494</v>
       </c>
       <c r="J19" s="61"/>
-    </row>
-    <row r="20" spans="1:10" ht="14.25">
+      <c r="K19" s="61"/>
+    </row>
+    <row r="20" spans="1:11" ht="14.25">
       <c r="A20" s="24" t="s">
         <v>62</v>
       </c>
@@ -5756,12 +5806,13 @@
         <v>494</v>
       </c>
       <c r="J20" s="61"/>
-    </row>
-    <row r="21" spans="1:10" ht="14.25">
+      <c r="K20" s="61"/>
+    </row>
+    <row r="21" spans="1:11" ht="14.25">
       <c r="A21" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="219" t="s">
+      <c r="B21" s="172" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="134">
@@ -5780,8 +5831,9 @@
         <v>494</v>
       </c>
       <c r="J21" s="61"/>
-    </row>
-    <row r="22" spans="1:10" ht="14.25">
+      <c r="K21" s="61"/>
+    </row>
+    <row r="22" spans="1:11" ht="14.25">
       <c r="A22" s="24" t="s">
         <v>66</v>
       </c>
@@ -5803,8 +5855,9 @@
         <v>494</v>
       </c>
       <c r="J22" s="61"/>
-    </row>
-    <row r="23" spans="1:10" ht="14.25">
+      <c r="K22" s="61"/>
+    </row>
+    <row r="23" spans="1:11" ht="14.25">
       <c r="A23" s="126" t="s">
         <v>67</v>
       </c>
@@ -5831,8 +5884,9 @@
         <v>494</v>
       </c>
       <c r="J23" s="61"/>
-    </row>
-    <row r="24" spans="1:10" ht="14.25">
+      <c r="K23" s="61"/>
+    </row>
+    <row r="24" spans="1:11" ht="14.25">
       <c r="A24" s="24" t="s">
         <v>70</v>
       </c>
@@ -5859,8 +5913,9 @@
         <v>494</v>
       </c>
       <c r="J24" s="61"/>
-    </row>
-    <row r="25" spans="1:10" ht="14.25">
+      <c r="K24" s="61"/>
+    </row>
+    <row r="25" spans="1:11" ht="14.25">
       <c r="A25" s="126" t="s">
         <v>73</v>
       </c>
@@ -5885,8 +5940,9 @@
       </c>
       <c r="I25" s="60"/>
       <c r="J25" s="61"/>
-    </row>
-    <row r="26" spans="1:10" ht="14.25">
+      <c r="K25" s="61"/>
+    </row>
+    <row r="26" spans="1:11" ht="14.25">
       <c r="A26" s="24" t="s">
         <v>77</v>
       </c>
@@ -5906,8 +5962,9 @@
       </c>
       <c r="I26" s="60"/>
       <c r="J26" s="61"/>
-    </row>
-    <row r="27" spans="1:10" ht="14.25">
+      <c r="K26" s="61"/>
+    </row>
+    <row r="27" spans="1:11" ht="14.25">
       <c r="A27" s="126" t="s">
         <v>79</v>
       </c>
@@ -5930,8 +5987,9 @@
       </c>
       <c r="I27" s="60"/>
       <c r="J27" s="61"/>
-    </row>
-    <row r="28" spans="1:10" ht="14.25">
+      <c r="K27" s="61"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.25">
       <c r="A28" s="24" t="s">
         <v>84</v>
       </c>
@@ -5954,8 +6012,9 @@
       </c>
       <c r="I28" s="60"/>
       <c r="J28" s="61"/>
-    </row>
-    <row r="29" spans="1:10" ht="14.25">
+      <c r="K28" s="61"/>
+    </row>
+    <row r="29" spans="1:11" ht="14.25">
       <c r="A29" s="126" t="s">
         <v>89</v>
       </c>
@@ -5978,8 +6037,9 @@
       </c>
       <c r="I29" s="60"/>
       <c r="J29" s="61"/>
-    </row>
-    <row r="30" spans="1:10" ht="14.25">
+      <c r="K29" s="61"/>
+    </row>
+    <row r="30" spans="1:11" ht="14.25">
       <c r="A30" s="24" t="s">
         <v>94</v>
       </c>
@@ -6002,8 +6062,9 @@
       </c>
       <c r="I30" s="60"/>
       <c r="J30" s="61"/>
-    </row>
-    <row r="31" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K30" s="61"/>
+    </row>
+    <row r="31" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A31" s="126" t="s">
         <v>98</v>
       </c>
@@ -6026,8 +6087,9 @@
       </c>
       <c r="I31" s="166"/>
       <c r="J31" s="167"/>
-    </row>
-    <row r="32" spans="1:10" ht="14.25">
+      <c r="K31" s="167"/>
+    </row>
+    <row r="32" spans="1:11" ht="14.25">
       <c r="A32" s="24" t="s">
         <v>103</v>
       </c>
@@ -6050,8 +6112,9 @@
       </c>
       <c r="I32" s="60"/>
       <c r="J32" s="61"/>
-    </row>
-    <row r="33" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K32" s="61"/>
+    </row>
+    <row r="33" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A33" s="126" t="s">
         <v>106</v>
       </c>
@@ -6074,8 +6137,9 @@
       </c>
       <c r="I33" s="166"/>
       <c r="J33" s="167"/>
-    </row>
-    <row r="34" spans="1:10" s="42" customFormat="1" ht="14.25">
+      <c r="K33" s="167"/>
+    </row>
+    <row r="34" spans="1:11" s="42" customFormat="1" ht="14.25">
       <c r="A34" s="38" t="s">
         <v>111</v>
       </c>
@@ -6096,8 +6160,9 @@
       <c r="H34" s="168"/>
       <c r="I34" s="168"/>
       <c r="J34" s="169"/>
-    </row>
-    <row r="35" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K34" s="169"/>
+    </row>
+    <row r="35" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A35" s="126" t="s">
         <v>116</v>
       </c>
@@ -6118,8 +6183,9 @@
       <c r="H35" s="166"/>
       <c r="I35" s="166"/>
       <c r="J35" s="167"/>
-    </row>
-    <row r="36" spans="1:10" ht="14.25">
+      <c r="K35" s="167"/>
+    </row>
+    <row r="36" spans="1:11" ht="14.25">
       <c r="A36" s="24" t="s">
         <v>120</v>
       </c>
@@ -6140,8 +6206,9 @@
       <c r="H36" s="60"/>
       <c r="I36" s="60"/>
       <c r="J36" s="61"/>
-    </row>
-    <row r="37" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K36" s="61"/>
+    </row>
+    <row r="37" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A37" s="126" t="s">
         <v>124</v>
       </c>
@@ -6162,8 +6229,9 @@
       <c r="H37" s="166"/>
       <c r="I37" s="166"/>
       <c r="J37" s="167"/>
-    </row>
-    <row r="38" spans="1:10" ht="14.25">
+      <c r="K37" s="167"/>
+    </row>
+    <row r="38" spans="1:11" ht="14.25">
       <c r="A38" s="24" t="s">
         <v>128</v>
       </c>
@@ -6184,8 +6252,9 @@
       <c r="H38" s="60"/>
       <c r="I38" s="60"/>
       <c r="J38" s="61"/>
-    </row>
-    <row r="39" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K38" s="61"/>
+    </row>
+    <row r="39" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A39" s="126" t="s">
         <v>132</v>
       </c>
@@ -6206,8 +6275,9 @@
       <c r="H39" s="166"/>
       <c r="I39" s="166"/>
       <c r="J39" s="167"/>
-    </row>
-    <row r="40" spans="1:10" ht="14.25">
+      <c r="K39" s="167"/>
+    </row>
+    <row r="40" spans="1:11" ht="14.25">
       <c r="A40" s="24" t="s">
         <v>136</v>
       </c>
@@ -6228,8 +6298,9 @@
       <c r="H40" s="60"/>
       <c r="I40" s="60"/>
       <c r="J40" s="61"/>
-    </row>
-    <row r="41" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K40" s="61"/>
+    </row>
+    <row r="41" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A41" s="126" t="s">
         <v>140</v>
       </c>
@@ -6250,8 +6321,9 @@
       <c r="H41" s="166"/>
       <c r="I41" s="166"/>
       <c r="J41" s="167"/>
-    </row>
-    <row r="42" spans="1:10" ht="14.25">
+      <c r="K41" s="167"/>
+    </row>
+    <row r="42" spans="1:11" ht="14.25">
       <c r="A42" s="24" t="s">
         <v>144</v>
       </c>
@@ -6272,8 +6344,9 @@
       <c r="H42" s="60"/>
       <c r="I42" s="60"/>
       <c r="J42" s="61"/>
-    </row>
-    <row r="43" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K42" s="61"/>
+    </row>
+    <row r="43" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A43" s="126" t="s">
         <v>148</v>
       </c>
@@ -6294,8 +6367,9 @@
       <c r="H43" s="166"/>
       <c r="I43" s="166"/>
       <c r="J43" s="167"/>
-    </row>
-    <row r="44" spans="1:10" ht="14.25">
+      <c r="K43" s="167"/>
+    </row>
+    <row r="44" spans="1:11" ht="14.25">
       <c r="A44" s="24" t="s">
         <v>152</v>
       </c>
@@ -6316,8 +6390,9 @@
       <c r="H44" s="60"/>
       <c r="I44" s="60"/>
       <c r="J44" s="61"/>
-    </row>
-    <row r="45" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K44" s="61"/>
+    </row>
+    <row r="45" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A45" s="126" t="s">
         <v>156</v>
       </c>
@@ -6338,8 +6413,9 @@
       <c r="H45" s="166"/>
       <c r="I45" s="166"/>
       <c r="J45" s="167"/>
-    </row>
-    <row r="46" spans="1:10" ht="14.25">
+      <c r="K45" s="167"/>
+    </row>
+    <row r="46" spans="1:11" ht="14.25">
       <c r="A46" s="24" t="s">
         <v>160</v>
       </c>
@@ -6360,8 +6436,9 @@
       <c r="H46" s="60"/>
       <c r="I46" s="60"/>
       <c r="J46" s="61"/>
-    </row>
-    <row r="47" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K46" s="61"/>
+    </row>
+    <row r="47" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A47" s="126" t="s">
         <v>164</v>
       </c>
@@ -6388,8 +6465,9 @@
         <v>494</v>
       </c>
       <c r="J47" s="167"/>
-    </row>
-    <row r="48" spans="1:10" ht="14.25">
+      <c r="K47" s="167"/>
+    </row>
+    <row r="48" spans="1:11" ht="14.25">
       <c r="A48" s="24" t="s">
         <v>165</v>
       </c>
@@ -6416,8 +6494,9 @@
         <v>494</v>
       </c>
       <c r="J48" s="61"/>
-    </row>
-    <row r="49" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K48" s="61"/>
+    </row>
+    <row r="49" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A49" s="126" t="s">
         <v>166</v>
       </c>
@@ -6444,8 +6523,9 @@
         <v>494</v>
       </c>
       <c r="J49" s="167"/>
-    </row>
-    <row r="50" spans="1:10" ht="14.25">
+      <c r="K49" s="167"/>
+    </row>
+    <row r="50" spans="1:11" ht="14.25">
       <c r="A50" s="24" t="s">
         <v>167</v>
       </c>
@@ -6472,8 +6552,9 @@
         <v>494</v>
       </c>
       <c r="J50" s="61"/>
-    </row>
-    <row r="51" spans="1:10" s="50" customFormat="1" ht="14.25">
+      <c r="K50" s="61"/>
+    </row>
+    <row r="51" spans="1:11" s="50" customFormat="1" ht="14.25">
       <c r="A51" s="126" t="s">
         <v>168</v>
       </c>
@@ -6500,8 +6581,9 @@
         <v>494</v>
       </c>
       <c r="J51" s="167"/>
-    </row>
-    <row r="52" spans="1:10" ht="14.25">
+      <c r="K51" s="167"/>
+    </row>
+    <row r="52" spans="1:11" ht="14.25">
       <c r="A52" s="24" t="s">
         <v>169</v>
       </c>
@@ -6528,8 +6610,9 @@
         <v>494</v>
       </c>
       <c r="J52" s="61"/>
-    </row>
-    <row r="53" spans="1:10" ht="14.25">
+      <c r="K52" s="61"/>
+    </row>
+    <row r="53" spans="1:11" ht="14.25">
       <c r="A53" s="126" t="s">
         <v>170</v>
       </c>
@@ -6556,8 +6639,9 @@
         <v>494</v>
       </c>
       <c r="J53" s="61"/>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K53" s="61"/>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" customHeight="1">
       <c r="A54" s="24" t="s">
         <v>171</v>
       </c>
@@ -6584,8 +6668,9 @@
         <v>494</v>
       </c>
       <c r="J54" s="61"/>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K54" s="61"/>
+    </row>
+    <row r="55" spans="1:11" ht="15.75" customHeight="1">
       <c r="A55" s="126" t="s">
         <v>172</v>
       </c>
@@ -6612,8 +6697,9 @@
         <v>494</v>
       </c>
       <c r="J55" s="61"/>
-    </row>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K55" s="61"/>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" customHeight="1">
       <c r="A56" s="24" t="s">
         <v>173</v>
       </c>
@@ -6640,8 +6726,9 @@
         <v>494</v>
       </c>
       <c r="J56" s="61"/>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K56" s="61"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" customHeight="1">
       <c r="A57" s="126" t="s">
         <v>174</v>
       </c>
@@ -6668,8 +6755,9 @@
         <v>494</v>
       </c>
       <c r="J57" s="61"/>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K57" s="61"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" customHeight="1">
       <c r="A58" s="24" t="s">
         <v>175</v>
       </c>
@@ -6696,8 +6784,9 @@
         <v>494</v>
       </c>
       <c r="J58" s="61"/>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K58" s="61"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" customHeight="1">
       <c r="A59" s="126" t="s">
         <v>176</v>
       </c>
@@ -6724,8 +6813,9 @@
         <v>494</v>
       </c>
       <c r="J59" s="61"/>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K59" s="61"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" customHeight="1">
       <c r="A60" s="24" t="s">
         <v>177</v>
       </c>
@@ -6752,8 +6842,9 @@
         <v>494</v>
       </c>
       <c r="J60" s="61"/>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K60" s="61"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" customHeight="1">
       <c r="A61" s="126" t="s">
         <v>178</v>
       </c>
@@ -6780,8 +6871,9 @@
         <v>494</v>
       </c>
       <c r="J61" s="61"/>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K61" s="61"/>
+    </row>
+    <row r="62" spans="1:11" ht="15.75" customHeight="1">
       <c r="A62" s="24" t="s">
         <v>179</v>
       </c>
@@ -6808,8 +6900,9 @@
         <v>494</v>
       </c>
       <c r="J62" s="61"/>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K62" s="61"/>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" customHeight="1">
       <c r="A63" s="126" t="s">
         <v>180</v>
       </c>
@@ -6836,8 +6929,9 @@
         <v>494</v>
       </c>
       <c r="J63" s="61"/>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K63" s="61"/>
+    </row>
+    <row r="64" spans="1:11" ht="15.75" customHeight="1">
       <c r="A64" s="24" t="s">
         <v>181</v>
       </c>
@@ -6864,8 +6958,9 @@
         <v>494</v>
       </c>
       <c r="J64" s="61"/>
-    </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K64" s="61"/>
+    </row>
+    <row r="65" spans="1:11" ht="15.75" customHeight="1">
       <c r="A65" s="126" t="s">
         <v>182</v>
       </c>
@@ -6886,8 +6981,9 @@
       <c r="H65" s="60"/>
       <c r="I65" s="60"/>
       <c r="J65" s="61"/>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K65" s="61"/>
+    </row>
+    <row r="66" spans="1:11" ht="15.75" customHeight="1">
       <c r="A66" s="114" t="s">
         <v>183</v>
       </c>
@@ -6908,8 +7004,9 @@
       <c r="H66" s="60"/>
       <c r="I66" s="60"/>
       <c r="J66" s="61"/>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K66" s="61"/>
+    </row>
+    <row r="67" spans="1:11" ht="15.75" customHeight="1">
       <c r="A67" s="126" t="s">
         <v>184</v>
       </c>
@@ -6930,8 +7027,9 @@
       <c r="H67" s="60"/>
       <c r="I67" s="60"/>
       <c r="J67" s="61"/>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K67" s="61"/>
+    </row>
+    <row r="68" spans="1:11" ht="15.75" customHeight="1">
       <c r="A68" s="24" t="s">
         <v>185</v>
       </c>
@@ -6952,8 +7050,9 @@
       <c r="H68" s="60"/>
       <c r="I68" s="60"/>
       <c r="J68" s="61"/>
-    </row>
-    <row r="69" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K68" s="61"/>
+    </row>
+    <row r="69" spans="1:11" ht="15.75" customHeight="1">
       <c r="A69" s="126" t="s">
         <v>186</v>
       </c>
@@ -6974,8 +7073,9 @@
       <c r="H69" s="60"/>
       <c r="I69" s="60"/>
       <c r="J69" s="61"/>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K69" s="61"/>
+    </row>
+    <row r="70" spans="1:11" ht="15.75" customHeight="1">
       <c r="A70" s="24" t="s">
         <v>187</v>
       </c>
@@ -6996,8 +7096,9 @@
       <c r="H70" s="60"/>
       <c r="I70" s="60"/>
       <c r="J70" s="61"/>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K70" s="61"/>
+    </row>
+    <row r="71" spans="1:11" ht="15.75" customHeight="1">
       <c r="A71" s="126" t="s">
         <v>188</v>
       </c>
@@ -7024,8 +7125,9 @@
         <v>494</v>
       </c>
       <c r="J71" s="61"/>
-    </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K71" s="61"/>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" customHeight="1">
       <c r="A72" s="24" t="s">
         <v>189</v>
       </c>
@@ -7052,8 +7154,9 @@
         <v>494</v>
       </c>
       <c r="J72" s="61"/>
-    </row>
-    <row r="73" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K72" s="61"/>
+    </row>
+    <row r="73" spans="1:11" ht="15.75" customHeight="1">
       <c r="A73" s="126" t="s">
         <v>190</v>
       </c>
@@ -7080,8 +7183,9 @@
         <v>494</v>
       </c>
       <c r="J73" s="61"/>
-    </row>
-    <row r="74" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K73" s="61"/>
+    </row>
+    <row r="74" spans="1:11" ht="15.75" customHeight="1">
       <c r="A74" s="24" t="s">
         <v>191</v>
       </c>
@@ -7106,8 +7210,9 @@
         <v>494</v>
       </c>
       <c r="J74" s="61"/>
-    </row>
-    <row r="75" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K74" s="61"/>
+    </row>
+    <row r="75" spans="1:11" ht="15.75" customHeight="1">
       <c r="A75" s="126" t="s">
         <v>192</v>
       </c>
@@ -7132,8 +7237,9 @@
         <v>494</v>
       </c>
       <c r="J75" s="61"/>
-    </row>
-    <row r="76" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K75" s="61"/>
+    </row>
+    <row r="76" spans="1:11" ht="15.75" customHeight="1">
       <c r="A76" s="24" t="s">
         <v>193</v>
       </c>
@@ -7160,8 +7266,9 @@
         <v>494</v>
       </c>
       <c r="J76" s="61"/>
-    </row>
-    <row r="77" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K76" s="61"/>
+    </row>
+    <row r="77" spans="1:11" ht="15.75" customHeight="1">
       <c r="A77" s="126" t="s">
         <v>194</v>
       </c>
@@ -7186,8 +7293,9 @@
         <v>494</v>
       </c>
       <c r="J77" s="61"/>
-    </row>
-    <row r="78" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K77" s="61"/>
+    </row>
+    <row r="78" spans="1:11" ht="15.75" customHeight="1">
       <c r="A78" s="24" t="s">
         <v>195</v>
       </c>
@@ -7214,8 +7322,9 @@
         <v>494</v>
       </c>
       <c r="J78" s="61"/>
-    </row>
-    <row r="79" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K78" s="61"/>
+    </row>
+    <row r="79" spans="1:11" ht="15.75" customHeight="1">
       <c r="A79" s="126" t="s">
         <v>196</v>
       </c>
@@ -7242,8 +7351,9 @@
         <v>494</v>
       </c>
       <c r="J79" s="61"/>
-    </row>
-    <row r="80" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K79" s="61"/>
+    </row>
+    <row r="80" spans="1:11" ht="15.75" customHeight="1">
       <c r="A80" s="24" t="s">
         <v>197</v>
       </c>
@@ -7270,8 +7380,9 @@
         <v>494</v>
       </c>
       <c r="J80" s="61"/>
-    </row>
-    <row r="81" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K80" s="61"/>
+    </row>
+    <row r="81" spans="1:11" ht="15.75" customHeight="1">
       <c r="A81" s="126" t="s">
         <v>198</v>
       </c>
@@ -7298,8 +7409,9 @@
         <v>494</v>
       </c>
       <c r="J81" s="61"/>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K81" s="61"/>
+    </row>
+    <row r="82" spans="1:11" ht="15.75" customHeight="1">
       <c r="A82" s="24" t="s">
         <v>199</v>
       </c>
@@ -7326,8 +7438,9 @@
         <v>494</v>
       </c>
       <c r="J82" s="61"/>
-    </row>
-    <row r="83" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K82" s="61"/>
+    </row>
+    <row r="83" spans="1:11" ht="15.75" customHeight="1">
       <c r="A83" s="126" t="s">
         <v>200</v>
       </c>
@@ -7354,8 +7467,9 @@
         <v>494</v>
       </c>
       <c r="J83" s="61"/>
-    </row>
-    <row r="84" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K83" s="61"/>
+    </row>
+    <row r="84" spans="1:11" ht="15.75" customHeight="1">
       <c r="A84" s="24" t="s">
         <v>201</v>
       </c>
@@ -7382,8 +7496,9 @@
         <v>494</v>
       </c>
       <c r="J84" s="61"/>
-    </row>
-    <row r="85" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K84" s="61"/>
+    </row>
+    <row r="85" spans="1:11" ht="15.75" customHeight="1">
       <c r="A85" s="126" t="s">
         <v>202</v>
       </c>
@@ -7410,8 +7525,9 @@
         <v>494</v>
       </c>
       <c r="J85" s="61"/>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K85" s="61"/>
+    </row>
+    <row r="86" spans="1:11" ht="15.75" customHeight="1">
       <c r="A86" s="24" t="s">
         <v>203</v>
       </c>
@@ -7438,8 +7554,9 @@
         <v>494</v>
       </c>
       <c r="J86" s="61"/>
-    </row>
-    <row r="87" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K86" s="61"/>
+    </row>
+    <row r="87" spans="1:11" ht="15.75" customHeight="1">
       <c r="A87" s="126" t="s">
         <v>204</v>
       </c>
@@ -7466,8 +7583,9 @@
         <v>494</v>
       </c>
       <c r="J87" s="61"/>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K87" s="61"/>
+    </row>
+    <row r="88" spans="1:11" ht="15.75" customHeight="1">
       <c r="A88" s="24" t="s">
         <v>205</v>
       </c>
@@ -7494,8 +7612,9 @@
         <v>494</v>
       </c>
       <c r="J88" s="61"/>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K88" s="61"/>
+    </row>
+    <row r="89" spans="1:11" ht="15.75" customHeight="1">
       <c r="A89" s="126" t="s">
         <v>206</v>
       </c>
@@ -7522,8 +7641,9 @@
         <v>494</v>
       </c>
       <c r="J89" s="61"/>
-    </row>
-    <row r="90" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K89" s="61"/>
+    </row>
+    <row r="90" spans="1:11" ht="15.75" customHeight="1">
       <c r="A90" s="24" t="s">
         <v>207</v>
       </c>
@@ -7550,8 +7670,9 @@
         <v>494</v>
       </c>
       <c r="J90" s="61"/>
-    </row>
-    <row r="91" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K90" s="61"/>
+    </row>
+    <row r="91" spans="1:11" ht="15.75" customHeight="1">
       <c r="A91" s="126" t="s">
         <v>208</v>
       </c>
@@ -7578,8 +7699,9 @@
         <v>494</v>
       </c>
       <c r="J91" s="61"/>
-    </row>
-    <row r="92" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K91" s="61"/>
+    </row>
+    <row r="92" spans="1:11" ht="15.75" customHeight="1">
       <c r="A92" s="24" t="s">
         <v>209</v>
       </c>
@@ -7606,8 +7728,9 @@
         <v>494</v>
       </c>
       <c r="J92" s="61"/>
-    </row>
-    <row r="93" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K92" s="61"/>
+    </row>
+    <row r="93" spans="1:11" ht="15.75" customHeight="1">
       <c r="A93" s="126" t="s">
         <v>210</v>
       </c>
@@ -7634,8 +7757,9 @@
         <v>494</v>
       </c>
       <c r="J93" s="61"/>
-    </row>
-    <row r="94" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K93" s="61"/>
+    </row>
+    <row r="94" spans="1:11" ht="15.75" customHeight="1">
       <c r="A94" s="24" t="s">
         <v>211</v>
       </c>
@@ -7662,8 +7786,9 @@
         <v>494</v>
       </c>
       <c r="J94" s="61"/>
-    </row>
-    <row r="95" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K94" s="61"/>
+    </row>
+    <row r="95" spans="1:11" ht="15.75" customHeight="1">
       <c r="A95" s="126" t="s">
         <v>212</v>
       </c>
@@ -7690,8 +7815,9 @@
         <v>494</v>
       </c>
       <c r="J95" s="61"/>
-    </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K95" s="61"/>
+    </row>
+    <row r="96" spans="1:11" ht="15.75" customHeight="1">
       <c r="A96" s="24" t="s">
         <v>213</v>
       </c>
@@ -7712,8 +7838,9 @@
         <v>494</v>
       </c>
       <c r="J96" s="61"/>
-    </row>
-    <row r="97" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K96" s="61"/>
+    </row>
+    <row r="97" spans="1:11" ht="15.75" customHeight="1">
       <c r="A97" s="126" t="s">
         <v>214</v>
       </c>
@@ -7734,8 +7861,11 @@
         <v>494</v>
       </c>
       <c r="J97" s="61"/>
-    </row>
-    <row r="98" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K97" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="15.75" customHeight="1">
       <c r="A98" s="24" t="s">
         <v>215</v>
       </c>
@@ -7758,8 +7888,9 @@
         <v>494</v>
       </c>
       <c r="J98" s="61"/>
-    </row>
-    <row r="99" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K98" s="61"/>
+    </row>
+    <row r="99" spans="1:11" ht="15.75" customHeight="1">
       <c r="A99" s="126" t="s">
         <v>216</v>
       </c>
@@ -7779,9 +7910,14 @@
       <c r="I99" s="162" t="s">
         <v>494</v>
       </c>
-      <c r="J99" s="61"/>
-    </row>
-    <row r="100" spans="1:10" ht="15.75" customHeight="1">
+      <c r="J99" s="162" t="s">
+        <v>734</v>
+      </c>
+      <c r="K99" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="15.75" customHeight="1">
       <c r="A100" s="24" t="s">
         <v>217</v>
       </c>
@@ -7804,8 +7940,11 @@
         <v>494</v>
       </c>
       <c r="J100" s="61"/>
-    </row>
-    <row r="101" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K100" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="15.75" customHeight="1">
       <c r="A101" s="126" t="s">
         <v>218</v>
       </c>
@@ -7828,8 +7967,11 @@
         <v>494</v>
       </c>
       <c r="J101" s="61"/>
-    </row>
-    <row r="102" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K101" s="61" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" customHeight="1">
       <c r="A102" s="24" t="s">
         <v>219</v>
       </c>
@@ -7852,8 +7994,11 @@
         <v>494</v>
       </c>
       <c r="J102" s="61"/>
-    </row>
-    <row r="103" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K102" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A103" s="24" t="s">
         <v>220</v>
       </c>
@@ -7866,8 +8011,9 @@
       <c r="H103" s="60"/>
       <c r="I103" s="60"/>
       <c r="J103" s="61"/>
-    </row>
-    <row r="104" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K103" s="61"/>
+    </row>
+    <row r="104" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A104" s="24" t="s">
         <v>221</v>
       </c>
@@ -7880,8 +8026,9 @@
       <c r="H104" s="60"/>
       <c r="I104" s="60"/>
       <c r="J104" s="61"/>
-    </row>
-    <row r="105" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K104" s="61"/>
+    </row>
+    <row r="105" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A105" s="24" t="s">
         <v>222</v>
       </c>
@@ -7894,8 +8041,9 @@
       <c r="H105" s="60"/>
       <c r="I105" s="60"/>
       <c r="J105" s="61"/>
-    </row>
-    <row r="106" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K105" s="61"/>
+    </row>
+    <row r="106" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A106" s="24" t="s">
         <v>223</v>
       </c>
@@ -7908,8 +8056,9 @@
       <c r="H106" s="60"/>
       <c r="I106" s="60"/>
       <c r="J106" s="61"/>
-    </row>
-    <row r="107" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K106" s="61"/>
+    </row>
+    <row r="107" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A107" s="24" t="s">
         <v>224</v>
       </c>
@@ -7922,8 +8071,9 @@
       <c r="H107" s="60"/>
       <c r="I107" s="60"/>
       <c r="J107" s="61"/>
-    </row>
-    <row r="108" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K107" s="61"/>
+    </row>
+    <row r="108" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A108" s="24" t="s">
         <v>225</v>
       </c>
@@ -7936,8 +8086,9 @@
       <c r="H108" s="60"/>
       <c r="I108" s="60"/>
       <c r="J108" s="61"/>
-    </row>
-    <row r="109" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K108" s="61"/>
+    </row>
+    <row r="109" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A109" s="24" t="s">
         <v>226</v>
       </c>
@@ -7950,8 +8101,9 @@
       <c r="H109" s="60"/>
       <c r="I109" s="60"/>
       <c r="J109" s="61"/>
-    </row>
-    <row r="110" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K109" s="61"/>
+    </row>
+    <row r="110" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A110" s="24" t="s">
         <v>227</v>
       </c>
@@ -7964,8 +8116,9 @@
       <c r="H110" s="60"/>
       <c r="I110" s="60"/>
       <c r="J110" s="61"/>
-    </row>
-    <row r="111" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K110" s="61"/>
+    </row>
+    <row r="111" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A111" s="24" t="s">
         <v>228</v>
       </c>
@@ -7978,8 +8131,9 @@
       <c r="H111" s="60"/>
       <c r="I111" s="60"/>
       <c r="J111" s="61"/>
-    </row>
-    <row r="112" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K111" s="61"/>
+    </row>
+    <row r="112" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A112" s="24" t="s">
         <v>229</v>
       </c>
@@ -7992,8 +8146,9 @@
       <c r="H112" s="60"/>
       <c r="I112" s="60"/>
       <c r="J112" s="61"/>
-    </row>
-    <row r="113" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K112" s="61"/>
+    </row>
+    <row r="113" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A113" s="24" t="s">
         <v>230</v>
       </c>
@@ -8006,8 +8161,9 @@
       <c r="H113" s="60"/>
       <c r="I113" s="60"/>
       <c r="J113" s="61"/>
-    </row>
-    <row r="114" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K113" s="61"/>
+    </row>
+    <row r="114" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A114" s="24" t="s">
         <v>231</v>
       </c>
@@ -8020,8 +8176,9 @@
       <c r="H114" s="60"/>
       <c r="I114" s="60"/>
       <c r="J114" s="61"/>
-    </row>
-    <row r="115" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K114" s="61"/>
+    </row>
+    <row r="115" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A115" s="24" t="s">
         <v>232</v>
       </c>
@@ -8034,8 +8191,9 @@
       <c r="H115" s="60"/>
       <c r="I115" s="60"/>
       <c r="J115" s="61"/>
-    </row>
-    <row r="116" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K115" s="61"/>
+    </row>
+    <row r="116" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A116" s="24" t="s">
         <v>233</v>
       </c>
@@ -8048,8 +8206,9 @@
       <c r="H116" s="60"/>
       <c r="I116" s="60"/>
       <c r="J116" s="61"/>
-    </row>
-    <row r="117" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K116" s="61"/>
+    </row>
+    <row r="117" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A117" s="24" t="s">
         <v>234</v>
       </c>
@@ -8062,8 +8221,9 @@
       <c r="H117" s="60"/>
       <c r="I117" s="60"/>
       <c r="J117" s="61"/>
-    </row>
-    <row r="118" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K117" s="61"/>
+    </row>
+    <row r="118" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A118" s="24" t="s">
         <v>235</v>
       </c>
@@ -8076,8 +8236,9 @@
       <c r="H118" s="60"/>
       <c r="I118" s="60"/>
       <c r="J118" s="61"/>
-    </row>
-    <row r="119" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K118" s="61"/>
+    </row>
+    <row r="119" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A119" s="24" t="s">
         <v>236</v>
       </c>
@@ -8090,8 +8251,9 @@
       <c r="H119" s="60"/>
       <c r="I119" s="60"/>
       <c r="J119" s="61"/>
-    </row>
-    <row r="120" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K119" s="61"/>
+    </row>
+    <row r="120" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A120" s="24" t="s">
         <v>237</v>
       </c>
@@ -8104,8 +8266,9 @@
       <c r="H120" s="60"/>
       <c r="I120" s="60"/>
       <c r="J120" s="61"/>
-    </row>
-    <row r="121" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K120" s="61"/>
+    </row>
+    <row r="121" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A121" s="24" t="s">
         <v>238</v>
       </c>
@@ -8118,8 +8281,9 @@
       <c r="H121" s="60"/>
       <c r="I121" s="60"/>
       <c r="J121" s="61"/>
-    </row>
-    <row r="122" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K121" s="61"/>
+    </row>
+    <row r="122" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A122" s="24" t="s">
         <v>239</v>
       </c>
@@ -8132,8 +8296,9 @@
       <c r="H122" s="60"/>
       <c r="I122" s="60"/>
       <c r="J122" s="61"/>
-    </row>
-    <row r="123" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K122" s="61"/>
+    </row>
+    <row r="123" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A123" s="24" t="s">
         <v>240</v>
       </c>
@@ -8146,8 +8311,9 @@
       <c r="H123" s="60"/>
       <c r="I123" s="60"/>
       <c r="J123" s="61"/>
-    </row>
-    <row r="124" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K123" s="61"/>
+    </row>
+    <row r="124" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A124" s="24" t="s">
         <v>241</v>
       </c>
@@ -8160,8 +8326,9 @@
       <c r="H124" s="60"/>
       <c r="I124" s="60"/>
       <c r="J124" s="61"/>
-    </row>
-    <row r="125" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K124" s="61"/>
+    </row>
+    <row r="125" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A125" s="24" t="s">
         <v>242</v>
       </c>
@@ -8174,8 +8341,9 @@
       <c r="H125" s="60"/>
       <c r="I125" s="60"/>
       <c r="J125" s="61"/>
-    </row>
-    <row r="126" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K125" s="61"/>
+    </row>
+    <row r="126" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A126" s="24" t="s">
         <v>243</v>
       </c>
@@ -8188,8 +8356,9 @@
       <c r="H126" s="60"/>
       <c r="I126" s="60"/>
       <c r="J126" s="61"/>
-    </row>
-    <row r="127" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K126" s="61"/>
+    </row>
+    <row r="127" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A127" s="24" t="s">
         <v>244</v>
       </c>
@@ -8202,8 +8371,9 @@
       <c r="H127" s="60"/>
       <c r="I127" s="60"/>
       <c r="J127" s="61"/>
-    </row>
-    <row r="128" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K127" s="61"/>
+    </row>
+    <row r="128" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A128" s="24" t="s">
         <v>245</v>
       </c>
@@ -8216,8 +8386,9 @@
       <c r="H128" s="60"/>
       <c r="I128" s="60"/>
       <c r="J128" s="61"/>
-    </row>
-    <row r="129" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K128" s="61"/>
+    </row>
+    <row r="129" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A129" s="24" t="s">
         <v>246</v>
       </c>
@@ -8230,8 +8401,9 @@
       <c r="H129" s="60"/>
       <c r="I129" s="60"/>
       <c r="J129" s="61"/>
-    </row>
-    <row r="130" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K129" s="61"/>
+    </row>
+    <row r="130" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A130" s="24" t="s">
         <v>247</v>
       </c>
@@ -8244,8 +8416,9 @@
       <c r="H130" s="60"/>
       <c r="I130" s="60"/>
       <c r="J130" s="61"/>
-    </row>
-    <row r="131" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K130" s="61"/>
+    </row>
+    <row r="131" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A131" s="24" t="s">
         <v>248</v>
       </c>
@@ -8258,8 +8431,9 @@
       <c r="H131" s="60"/>
       <c r="I131" s="60"/>
       <c r="J131" s="61"/>
-    </row>
-    <row r="132" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K131" s="61"/>
+    </row>
+    <row r="132" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A132" s="24" t="s">
         <v>249</v>
       </c>
@@ -8272,8 +8446,9 @@
       <c r="H132" s="60"/>
       <c r="I132" s="60"/>
       <c r="J132" s="61"/>
-    </row>
-    <row r="133" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K132" s="61"/>
+    </row>
+    <row r="133" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A133" s="24" t="s">
         <v>250</v>
       </c>
@@ -8286,8 +8461,9 @@
       <c r="H133" s="60"/>
       <c r="I133" s="60"/>
       <c r="J133" s="61"/>
-    </row>
-    <row r="134" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K133" s="61"/>
+    </row>
+    <row r="134" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A134" s="24" t="s">
         <v>251</v>
       </c>
@@ -8300,8 +8476,9 @@
       <c r="H134" s="60"/>
       <c r="I134" s="60"/>
       <c r="J134" s="61"/>
-    </row>
-    <row r="135" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K134" s="61"/>
+    </row>
+    <row r="135" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A135" s="24" t="s">
         <v>252</v>
       </c>
@@ -8314,8 +8491,9 @@
       <c r="H135" s="60"/>
       <c r="I135" s="60"/>
       <c r="J135" s="61"/>
-    </row>
-    <row r="136" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K135" s="61"/>
+    </row>
+    <row r="136" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A136" s="24" t="s">
         <v>253</v>
       </c>
@@ -8328,8 +8506,9 @@
       <c r="H136" s="60"/>
       <c r="I136" s="60"/>
       <c r="J136" s="61"/>
-    </row>
-    <row r="137" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K136" s="61"/>
+    </row>
+    <row r="137" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A137" s="24" t="s">
         <v>254</v>
       </c>
@@ -8342,8 +8521,9 @@
       <c r="H137" s="60"/>
       <c r="I137" s="60"/>
       <c r="J137" s="61"/>
-    </row>
-    <row r="138" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K137" s="61"/>
+    </row>
+    <row r="138" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A138" s="24" t="s">
         <v>255</v>
       </c>
@@ -8356,8 +8536,9 @@
       <c r="H138" s="60"/>
       <c r="I138" s="60"/>
       <c r="J138" s="61"/>
-    </row>
-    <row r="139" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K138" s="61"/>
+    </row>
+    <row r="139" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A139" s="24" t="s">
         <v>256</v>
       </c>
@@ -8370,8 +8551,9 @@
       <c r="H139" s="60"/>
       <c r="I139" s="60"/>
       <c r="J139" s="61"/>
-    </row>
-    <row r="140" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K139" s="61"/>
+    </row>
+    <row r="140" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A140" s="24" t="s">
         <v>257</v>
       </c>
@@ -8384,8 +8566,9 @@
       <c r="H140" s="60"/>
       <c r="I140" s="60"/>
       <c r="J140" s="61"/>
-    </row>
-    <row r="141" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K140" s="61"/>
+    </row>
+    <row r="141" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A141" s="24" t="s">
         <v>258</v>
       </c>
@@ -8398,8 +8581,9 @@
       <c r="H141" s="60"/>
       <c r="I141" s="60"/>
       <c r="J141" s="61"/>
-    </row>
-    <row r="142" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K141" s="61"/>
+    </row>
+    <row r="142" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A142" s="24" t="s">
         <v>259</v>
       </c>
@@ -8412,8 +8596,9 @@
       <c r="H142" s="60"/>
       <c r="I142" s="60"/>
       <c r="J142" s="61"/>
-    </row>
-    <row r="143" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K142" s="61"/>
+    </row>
+    <row r="143" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A143" s="24" t="s">
         <v>260</v>
       </c>
@@ -8426,8 +8611,9 @@
       <c r="H143" s="60"/>
       <c r="I143" s="60"/>
       <c r="J143" s="61"/>
-    </row>
-    <row r="144" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K143" s="61"/>
+    </row>
+    <row r="144" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A144" s="24" t="s">
         <v>261</v>
       </c>
@@ -8440,8 +8626,9 @@
       <c r="H144" s="60"/>
       <c r="I144" s="60"/>
       <c r="J144" s="61"/>
-    </row>
-    <row r="145" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K144" s="61"/>
+    </row>
+    <row r="145" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A145" s="24" t="s">
         <v>262</v>
       </c>
@@ -8454,8 +8641,9 @@
       <c r="H145" s="60"/>
       <c r="I145" s="60"/>
       <c r="J145" s="61"/>
-    </row>
-    <row r="146" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K145" s="61"/>
+    </row>
+    <row r="146" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A146" s="24" t="s">
         <v>263</v>
       </c>
@@ -8468,8 +8656,9 @@
       <c r="H146" s="60"/>
       <c r="I146" s="60"/>
       <c r="J146" s="61"/>
-    </row>
-    <row r="147" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K146" s="61"/>
+    </row>
+    <row r="147" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A147" s="24" t="s">
         <v>264</v>
       </c>
@@ -8482,8 +8671,9 @@
       <c r="H147" s="60"/>
       <c r="I147" s="60"/>
       <c r="J147" s="61"/>
-    </row>
-    <row r="148" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K147" s="61"/>
+    </row>
+    <row r="148" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A148" s="24" t="s">
         <v>265</v>
       </c>
@@ -8496,8 +8686,9 @@
       <c r="H148" s="60"/>
       <c r="I148" s="60"/>
       <c r="J148" s="61"/>
-    </row>
-    <row r="149" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K148" s="61"/>
+    </row>
+    <row r="149" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A149" s="24" t="s">
         <v>266</v>
       </c>
@@ -8510,8 +8701,9 @@
       <c r="H149" s="60"/>
       <c r="I149" s="60"/>
       <c r="J149" s="61"/>
-    </row>
-    <row r="150" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K149" s="61"/>
+    </row>
+    <row r="150" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A150" s="24" t="s">
         <v>267</v>
       </c>
@@ -8524,8 +8716,9 @@
       <c r="H150" s="60"/>
       <c r="I150" s="60"/>
       <c r="J150" s="61"/>
-    </row>
-    <row r="151" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K150" s="61"/>
+    </row>
+    <row r="151" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A151" s="24" t="s">
         <v>268</v>
       </c>
@@ -8538,8 +8731,9 @@
       <c r="H151" s="60"/>
       <c r="I151" s="60"/>
       <c r="J151" s="61"/>
-    </row>
-    <row r="152" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K151" s="61"/>
+    </row>
+    <row r="152" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A152" s="24" t="s">
         <v>269</v>
       </c>
@@ -8552,8 +8746,9 @@
       <c r="H152" s="60"/>
       <c r="I152" s="60"/>
       <c r="J152" s="61"/>
-    </row>
-    <row r="153" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K152" s="61"/>
+    </row>
+    <row r="153" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A153" s="24" t="s">
         <v>270</v>
       </c>
@@ -8566,8 +8761,9 @@
       <c r="H153" s="60"/>
       <c r="I153" s="60"/>
       <c r="J153" s="61"/>
-    </row>
-    <row r="154" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K153" s="61"/>
+    </row>
+    <row r="154" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A154" s="24" t="s">
         <v>271</v>
       </c>
@@ -8580,8 +8776,9 @@
       <c r="H154" s="60"/>
       <c r="I154" s="60"/>
       <c r="J154" s="61"/>
-    </row>
-    <row r="155" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K154" s="61"/>
+    </row>
+    <row r="155" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A155" s="24" t="s">
         <v>272</v>
       </c>
@@ -8594,8 +8791,9 @@
       <c r="H155" s="60"/>
       <c r="I155" s="60"/>
       <c r="J155" s="61"/>
-    </row>
-    <row r="156" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K155" s="61"/>
+    </row>
+    <row r="156" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A156" s="24" t="s">
         <v>273</v>
       </c>
@@ -8608,8 +8806,9 @@
       <c r="H156" s="60"/>
       <c r="I156" s="60"/>
       <c r="J156" s="61"/>
-    </row>
-    <row r="157" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K156" s="61"/>
+    </row>
+    <row r="157" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A157" s="24" t="s">
         <v>274</v>
       </c>
@@ -8622,8 +8821,9 @@
       <c r="H157" s="60"/>
       <c r="I157" s="60"/>
       <c r="J157" s="61"/>
-    </row>
-    <row r="158" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K157" s="61"/>
+    </row>
+    <row r="158" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A158" s="24" t="s">
         <v>275</v>
       </c>
@@ -8636,8 +8836,9 @@
       <c r="H158" s="60"/>
       <c r="I158" s="60"/>
       <c r="J158" s="61"/>
-    </row>
-    <row r="159" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K158" s="61"/>
+    </row>
+    <row r="159" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A159" s="24" t="s">
         <v>276</v>
       </c>
@@ -8650,8 +8851,9 @@
       <c r="H159" s="60"/>
       <c r="I159" s="60"/>
       <c r="J159" s="61"/>
-    </row>
-    <row r="160" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K159" s="61"/>
+    </row>
+    <row r="160" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A160" s="24" t="s">
         <v>277</v>
       </c>
@@ -8664,8 +8866,9 @@
       <c r="H160" s="60"/>
       <c r="I160" s="60"/>
       <c r="J160" s="61"/>
-    </row>
-    <row r="161" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K160" s="61"/>
+    </row>
+    <row r="161" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A161" s="24" t="s">
         <v>278</v>
       </c>
@@ -8678,8 +8881,9 @@
       <c r="H161" s="60"/>
       <c r="I161" s="60"/>
       <c r="J161" s="61"/>
-    </row>
-    <row r="162" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K161" s="61"/>
+    </row>
+    <row r="162" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A162" s="24" t="s">
         <v>279</v>
       </c>
@@ -8692,8 +8896,9 @@
       <c r="H162" s="60"/>
       <c r="I162" s="60"/>
       <c r="J162" s="61"/>
-    </row>
-    <row r="163" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K162" s="61"/>
+    </row>
+    <row r="163" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A163" s="24" t="s">
         <v>280</v>
       </c>
@@ -8706,8 +8911,9 @@
       <c r="H163" s="60"/>
       <c r="I163" s="60"/>
       <c r="J163" s="61"/>
-    </row>
-    <row r="164" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K163" s="61"/>
+    </row>
+    <row r="164" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A164" s="24" t="s">
         <v>281</v>
       </c>
@@ -8720,8 +8926,9 @@
       <c r="H164" s="60"/>
       <c r="I164" s="60"/>
       <c r="J164" s="61"/>
-    </row>
-    <row r="165" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K164" s="61"/>
+    </row>
+    <row r="165" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A165" s="24" t="s">
         <v>282</v>
       </c>
@@ -8734,8 +8941,9 @@
       <c r="H165" s="60"/>
       <c r="I165" s="60"/>
       <c r="J165" s="61"/>
-    </row>
-    <row r="166" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K165" s="61"/>
+    </row>
+    <row r="166" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A166" s="24" t="s">
         <v>283</v>
       </c>
@@ -8748,8 +8956,9 @@
       <c r="H166" s="60"/>
       <c r="I166" s="60"/>
       <c r="J166" s="61"/>
-    </row>
-    <row r="167" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K166" s="61"/>
+    </row>
+    <row r="167" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A167" s="24" t="s">
         <v>284</v>
       </c>
@@ -8762,8 +8971,9 @@
       <c r="H167" s="60"/>
       <c r="I167" s="60"/>
       <c r="J167" s="61"/>
-    </row>
-    <row r="168" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K167" s="61"/>
+    </row>
+    <row r="168" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A168" s="24" t="s">
         <v>285</v>
       </c>
@@ -8776,8 +8986,9 @@
       <c r="H168" s="60"/>
       <c r="I168" s="60"/>
       <c r="J168" s="61"/>
-    </row>
-    <row r="169" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K168" s="61"/>
+    </row>
+    <row r="169" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A169" s="24" t="s">
         <v>286</v>
       </c>
@@ -8790,8 +9001,9 @@
       <c r="H169" s="60"/>
       <c r="I169" s="60"/>
       <c r="J169" s="61"/>
-    </row>
-    <row r="170" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K169" s="61"/>
+    </row>
+    <row r="170" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A170" s="24" t="s">
         <v>287</v>
       </c>
@@ -8804,8 +9016,9 @@
       <c r="H170" s="60"/>
       <c r="I170" s="60"/>
       <c r="J170" s="61"/>
-    </row>
-    <row r="171" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K170" s="61"/>
+    </row>
+    <row r="171" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A171" s="24" t="s">
         <v>288</v>
       </c>
@@ -8818,8 +9031,9 @@
       <c r="H171" s="60"/>
       <c r="I171" s="60"/>
       <c r="J171" s="61"/>
-    </row>
-    <row r="172" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K171" s="61"/>
+    </row>
+    <row r="172" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A172" s="24" t="s">
         <v>289</v>
       </c>
@@ -8832,8 +9046,9 @@
       <c r="H172" s="60"/>
       <c r="I172" s="60"/>
       <c r="J172" s="61"/>
-    </row>
-    <row r="173" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K172" s="61"/>
+    </row>
+    <row r="173" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A173" s="24" t="s">
         <v>290</v>
       </c>
@@ -8846,8 +9061,9 @@
       <c r="H173" s="60"/>
       <c r="I173" s="60"/>
       <c r="J173" s="61"/>
-    </row>
-    <row r="174" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K173" s="61"/>
+    </row>
+    <row r="174" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A174" s="24" t="s">
         <v>291</v>
       </c>
@@ -8860,8 +9076,9 @@
       <c r="H174" s="60"/>
       <c r="I174" s="60"/>
       <c r="J174" s="61"/>
-    </row>
-    <row r="175" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K174" s="61"/>
+    </row>
+    <row r="175" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A175" s="24" t="s">
         <v>292</v>
       </c>
@@ -8874,8 +9091,9 @@
       <c r="H175" s="60"/>
       <c r="I175" s="60"/>
       <c r="J175" s="61"/>
-    </row>
-    <row r="176" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K175" s="61"/>
+    </row>
+    <row r="176" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A176" s="24" t="s">
         <v>293</v>
       </c>
@@ -8888,8 +9106,9 @@
       <c r="H176" s="60"/>
       <c r="I176" s="60"/>
       <c r="J176" s="61"/>
-    </row>
-    <row r="177" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K176" s="61"/>
+    </row>
+    <row r="177" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A177" s="24" t="s">
         <v>294</v>
       </c>
@@ -8902,8 +9121,9 @@
       <c r="H177" s="60"/>
       <c r="I177" s="60"/>
       <c r="J177" s="61"/>
-    </row>
-    <row r="178" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K177" s="61"/>
+    </row>
+    <row r="178" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A178" s="24" t="s">
         <v>295</v>
       </c>
@@ -8916,8 +9136,9 @@
       <c r="H178" s="60"/>
       <c r="I178" s="60"/>
       <c r="J178" s="61"/>
-    </row>
-    <row r="179" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K178" s="61"/>
+    </row>
+    <row r="179" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A179" s="24" t="s">
         <v>296</v>
       </c>
@@ -8930,8 +9151,9 @@
       <c r="H179" s="60"/>
       <c r="I179" s="60"/>
       <c r="J179" s="61"/>
-    </row>
-    <row r="180" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K179" s="61"/>
+    </row>
+    <row r="180" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A180" s="24" t="s">
         <v>297</v>
       </c>
@@ -8944,8 +9166,9 @@
       <c r="H180" s="60"/>
       <c r="I180" s="60"/>
       <c r="J180" s="61"/>
-    </row>
-    <row r="181" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K180" s="61"/>
+    </row>
+    <row r="181" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A181" s="24" t="s">
         <v>298</v>
       </c>
@@ -8958,8 +9181,9 @@
       <c r="H181" s="60"/>
       <c r="I181" s="60"/>
       <c r="J181" s="61"/>
-    </row>
-    <row r="182" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K181" s="61"/>
+    </row>
+    <row r="182" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A182" s="24" t="s">
         <v>299</v>
       </c>
@@ -8972,8 +9196,9 @@
       <c r="H182" s="60"/>
       <c r="I182" s="60"/>
       <c r="J182" s="61"/>
-    </row>
-    <row r="183" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K182" s="61"/>
+    </row>
+    <row r="183" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A183" s="24" t="s">
         <v>300</v>
       </c>
@@ -8986,8 +9211,9 @@
       <c r="H183" s="60"/>
       <c r="I183" s="60"/>
       <c r="J183" s="61"/>
-    </row>
-    <row r="184" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K183" s="61"/>
+    </row>
+    <row r="184" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A184" s="24" t="s">
         <v>301</v>
       </c>
@@ -9000,8 +9226,9 @@
       <c r="H184" s="60"/>
       <c r="I184" s="60"/>
       <c r="J184" s="61"/>
-    </row>
-    <row r="185" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K184" s="61"/>
+    </row>
+    <row r="185" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A185" s="24" t="s">
         <v>302</v>
       </c>
@@ -9014,8 +9241,9 @@
       <c r="H185" s="60"/>
       <c r="I185" s="60"/>
       <c r="J185" s="61"/>
-    </row>
-    <row r="186" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K185" s="61"/>
+    </row>
+    <row r="186" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A186" s="24" t="s">
         <v>303</v>
       </c>
@@ -9028,8 +9256,9 @@
       <c r="H186" s="60"/>
       <c r="I186" s="60"/>
       <c r="J186" s="61"/>
-    </row>
-    <row r="187" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K186" s="61"/>
+    </row>
+    <row r="187" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A187" s="24" t="s">
         <v>304</v>
       </c>
@@ -9042,8 +9271,9 @@
       <c r="H187" s="60"/>
       <c r="I187" s="60"/>
       <c r="J187" s="61"/>
-    </row>
-    <row r="188" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K187" s="61"/>
+    </row>
+    <row r="188" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A188" s="24" t="s">
         <v>305</v>
       </c>
@@ -9056,8 +9286,9 @@
       <c r="H188" s="60"/>
       <c r="I188" s="60"/>
       <c r="J188" s="61"/>
-    </row>
-    <row r="189" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K188" s="61"/>
+    </row>
+    <row r="189" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A189" s="24" t="s">
         <v>306</v>
       </c>
@@ -9070,8 +9301,9 @@
       <c r="H189" s="60"/>
       <c r="I189" s="60"/>
       <c r="J189" s="61"/>
-    </row>
-    <row r="190" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K189" s="61"/>
+    </row>
+    <row r="190" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A190" s="24" t="s">
         <v>307</v>
       </c>
@@ -9084,8 +9316,9 @@
       <c r="H190" s="60"/>
       <c r="I190" s="60"/>
       <c r="J190" s="61"/>
-    </row>
-    <row r="191" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K190" s="61"/>
+    </row>
+    <row r="191" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A191" s="24" t="s">
         <v>308</v>
       </c>
@@ -9098,8 +9331,9 @@
       <c r="H191" s="60"/>
       <c r="I191" s="60"/>
       <c r="J191" s="61"/>
-    </row>
-    <row r="192" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K191" s="61"/>
+    </row>
+    <row r="192" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A192" s="24" t="s">
         <v>309</v>
       </c>
@@ -9112,8 +9346,9 @@
       <c r="H192" s="60"/>
       <c r="I192" s="60"/>
       <c r="J192" s="61"/>
-    </row>
-    <row r="193" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K192" s="61"/>
+    </row>
+    <row r="193" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A193" s="24" t="s">
         <v>310</v>
       </c>
@@ -9126,8 +9361,9 @@
       <c r="H193" s="60"/>
       <c r="I193" s="60"/>
       <c r="J193" s="61"/>
-    </row>
-    <row r="194" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K193" s="61"/>
+    </row>
+    <row r="194" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A194" s="24" t="s">
         <v>311</v>
       </c>
@@ -9140,8 +9376,9 @@
       <c r="H194" s="60"/>
       <c r="I194" s="60"/>
       <c r="J194" s="61"/>
-    </row>
-    <row r="195" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K194" s="61"/>
+    </row>
+    <row r="195" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A195" s="24" t="s">
         <v>312</v>
       </c>
@@ -9154,8 +9391,9 @@
       <c r="H195" s="60"/>
       <c r="I195" s="60"/>
       <c r="J195" s="61"/>
-    </row>
-    <row r="196" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K195" s="61"/>
+    </row>
+    <row r="196" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A196" s="24" t="s">
         <v>313</v>
       </c>
@@ -9168,8 +9406,9 @@
       <c r="H196" s="60"/>
       <c r="I196" s="60"/>
       <c r="J196" s="61"/>
-    </row>
-    <row r="197" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K196" s="61"/>
+    </row>
+    <row r="197" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A197" s="24" t="s">
         <v>314</v>
       </c>
@@ -9182,8 +9421,9 @@
       <c r="H197" s="60"/>
       <c r="I197" s="60"/>
       <c r="J197" s="61"/>
-    </row>
-    <row r="198" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K197" s="61"/>
+    </row>
+    <row r="198" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A198" s="24" t="s">
         <v>315</v>
       </c>
@@ -9196,8 +9436,9 @@
       <c r="H198" s="60"/>
       <c r="I198" s="60"/>
       <c r="J198" s="61"/>
-    </row>
-    <row r="199" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K198" s="61"/>
+    </row>
+    <row r="199" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A199" s="24" t="s">
         <v>316</v>
       </c>
@@ -9210,8 +9451,9 @@
       <c r="H199" s="60"/>
       <c r="I199" s="60"/>
       <c r="J199" s="61"/>
-    </row>
-    <row r="200" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K199" s="61"/>
+    </row>
+    <row r="200" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A200" s="24" t="s">
         <v>317</v>
       </c>
@@ -9224,8 +9466,9 @@
       <c r="H200" s="60"/>
       <c r="I200" s="60"/>
       <c r="J200" s="61"/>
-    </row>
-    <row r="201" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K200" s="61"/>
+    </row>
+    <row r="201" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A201" s="24" t="s">
         <v>318</v>
       </c>
@@ -9238,8 +9481,9 @@
       <c r="H201" s="60"/>
       <c r="I201" s="60"/>
       <c r="J201" s="61"/>
-    </row>
-    <row r="202" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K201" s="61"/>
+    </row>
+    <row r="202" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A202" s="24" t="s">
         <v>319</v>
       </c>
@@ -9252,8 +9496,9 @@
       <c r="H202" s="60"/>
       <c r="I202" s="60"/>
       <c r="J202" s="61"/>
-    </row>
-    <row r="203" spans="1:10" ht="15.75" hidden="1" customHeight="1">
+      <c r="K202" s="61"/>
+    </row>
+    <row r="203" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A203" s="24" t="s">
         <v>320</v>
       </c>
@@ -9266,8 +9511,9 @@
       <c r="H203" s="60"/>
       <c r="I203" s="60"/>
       <c r="J203" s="61"/>
-    </row>
-    <row r="204" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K203" s="61"/>
+    </row>
+    <row r="204" spans="1:11" ht="15.75" customHeight="1">
       <c r="A204" s="126" t="s">
         <v>220</v>
       </c>
@@ -9290,8 +9536,11 @@
         <v>494</v>
       </c>
       <c r="J204" s="61"/>
-    </row>
-    <row r="205" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K204" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" ht="15.75" customHeight="1">
       <c r="A205" s="114" t="s">
         <v>221</v>
       </c>
@@ -9314,8 +9563,11 @@
         <v>494</v>
       </c>
       <c r="J205" s="61"/>
-    </row>
-    <row r="206" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K205" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" ht="15.75" customHeight="1">
       <c r="A206" s="126" t="s">
         <v>222</v>
       </c>
@@ -9338,8 +9590,11 @@
         <v>494</v>
       </c>
       <c r="J206" s="61"/>
-    </row>
-    <row r="207" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K206" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" ht="15.75" customHeight="1">
       <c r="A207" s="114" t="s">
         <v>223</v>
       </c>
@@ -9362,8 +9617,11 @@
         <v>494</v>
       </c>
       <c r="J207" s="61"/>
-    </row>
-    <row r="208" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K207" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" ht="15.75" customHeight="1">
       <c r="A208" s="126" t="s">
         <v>224</v>
       </c>
@@ -9386,8 +9644,11 @@
         <v>494</v>
       </c>
       <c r="J208" s="61"/>
-    </row>
-    <row r="209" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K208" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" ht="15.75" customHeight="1">
       <c r="A209" s="114" t="s">
         <v>225</v>
       </c>
@@ -9410,8 +9671,11 @@
         <v>494</v>
       </c>
       <c r="J209" s="61"/>
-    </row>
-    <row r="210" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K209" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" ht="15.75" customHeight="1">
       <c r="A210" s="126" t="s">
         <v>226</v>
       </c>
@@ -9434,8 +9698,11 @@
         <v>494</v>
       </c>
       <c r="J210" s="61"/>
-    </row>
-    <row r="211" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K210" s="61" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" ht="15.75" customHeight="1">
       <c r="A211" s="114" t="s">
         <v>227</v>
       </c>
@@ -9448,8 +9715,9 @@
       <c r="H211" s="60"/>
       <c r="I211" s="60"/>
       <c r="J211" s="61"/>
-    </row>
-    <row r="212" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K211" s="61"/>
+    </row>
+    <row r="212" spans="1:11" ht="15.75" customHeight="1">
       <c r="A212" s="126" t="s">
         <v>228</v>
       </c>
@@ -9462,8 +9730,9 @@
       <c r="H212" s="60"/>
       <c r="I212" s="60"/>
       <c r="J212" s="61"/>
-    </row>
-    <row r="213" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K212" s="61"/>
+    </row>
+    <row r="213" spans="1:11" ht="15.75" customHeight="1">
       <c r="A213" s="114" t="s">
         <v>229</v>
       </c>
@@ -9476,8 +9745,9 @@
       <c r="H213" s="60"/>
       <c r="I213" s="60"/>
       <c r="J213" s="61"/>
-    </row>
-    <row r="214" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K213" s="61"/>
+    </row>
+    <row r="214" spans="1:11" ht="15.75" customHeight="1">
       <c r="A214" s="126" t="s">
         <v>230</v>
       </c>
@@ -9490,8 +9760,9 @@
       <c r="H214" s="60"/>
       <c r="I214" s="60"/>
       <c r="J214" s="61"/>
-    </row>
-    <row r="215" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K214" s="61"/>
+    </row>
+    <row r="215" spans="1:11" ht="15.75" customHeight="1">
       <c r="A215" s="114" t="s">
         <v>231</v>
       </c>
@@ -9502,7 +9773,7 @@
       <c r="F215" s="61"/>
       <c r="G215" s="61"/>
     </row>
-    <row r="216" spans="1:10" ht="15.75" customHeight="1">
+    <row r="216" spans="1:11" ht="15.75" customHeight="1">
       <c r="A216" s="114" t="s">
         <v>232</v>
       </c>
@@ -9513,7 +9784,7 @@
       <c r="F216" s="61"/>
       <c r="G216" s="61"/>
     </row>
-    <row r="217" spans="1:10" ht="15.75" customHeight="1">
+    <row r="217" spans="1:11" ht="15.75" customHeight="1">
       <c r="A217" s="114" t="s">
         <v>233</v>
       </c>
@@ -9524,7 +9795,7 @@
       <c r="F217" s="61"/>
       <c r="G217" s="61"/>
     </row>
-    <row r="218" spans="1:10" ht="15.75" customHeight="1">
+    <row r="218" spans="1:11" ht="15.75" customHeight="1">
       <c r="A218" s="114" t="s">
         <v>234</v>
       </c>
@@ -9535,7 +9806,7 @@
       <c r="F218" s="61"/>
       <c r="G218" s="61"/>
     </row>
-    <row r="219" spans="1:10" ht="15.75" customHeight="1">
+    <row r="219" spans="1:11" ht="15.75" customHeight="1">
       <c r="A219" s="114" t="s">
         <v>235</v>
       </c>
@@ -9546,7 +9817,7 @@
       <c r="F219" s="61"/>
       <c r="G219" s="61"/>
     </row>
-    <row r="220" spans="1:10" ht="15.75" customHeight="1">
+    <row r="220" spans="1:11" ht="15.75" customHeight="1">
       <c r="A220" s="114" t="s">
         <v>236</v>
       </c>
@@ -9557,7 +9828,7 @@
       <c r="F220" s="61"/>
       <c r="G220" s="61"/>
     </row>
-    <row r="221" spans="1:10" ht="15.75" customHeight="1">
+    <row r="221" spans="1:11" ht="15.75" customHeight="1">
       <c r="A221" s="114" t="s">
         <v>237</v>
       </c>
@@ -9568,7 +9839,7 @@
       <c r="F221" s="61"/>
       <c r="G221" s="61"/>
     </row>
-    <row r="222" spans="1:10" ht="15.75" customHeight="1">
+    <row r="222" spans="1:11" ht="15.75" customHeight="1">
       <c r="A222" s="114" t="s">
         <v>238</v>
       </c>
@@ -9579,7 +9850,7 @@
       <c r="F222" s="61"/>
       <c r="G222" s="61"/>
     </row>
-    <row r="223" spans="1:10" ht="15.75" customHeight="1">
+    <row r="223" spans="1:11" ht="15.75" customHeight="1">
       <c r="A223" s="114" t="s">
         <v>239</v>
       </c>
@@ -9590,7 +9861,7 @@
       <c r="F223" s="61"/>
       <c r="G223" s="61"/>
     </row>
-    <row r="224" spans="1:10" ht="15.75" customHeight="1">
+    <row r="224" spans="1:11" ht="15.75" customHeight="1">
       <c r="A224" s="114" t="s">
         <v>240</v>
       </c>
@@ -14191,50 +14462,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="179" t="s">
         <v>601</v>
       </c>
-      <c r="B1" s="199"/>
-      <c r="C1" s="199"/>
-      <c r="D1" s="199"/>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199"/>
-      <c r="G1" s="199"/>
-      <c r="H1" s="199"/>
-      <c r="I1" s="200"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="181"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="201" t="s">
+      <c r="A2" s="182" t="s">
         <v>602</v>
       </c>
-      <c r="B2" s="202"/>
+      <c r="B2" s="183"/>
       <c r="C2" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="D2" s="203" t="s">
+      <c r="D2" s="184" t="s">
         <v>603</v>
       </c>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="205"/>
-      <c r="H2" s="206" t="s">
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="187" t="s">
         <v>604</v>
       </c>
-      <c r="I2" s="207"/>
+      <c r="I2" s="188"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="208" t="s">
+      <c r="A4" s="189" t="s">
         <v>605</v>
       </c>
-      <c r="B4" s="209"/>
-      <c r="C4" s="209"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="209"/>
-      <c r="I4" s="210"/>
+      <c r="B4" s="190"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
+      <c r="I4" s="191"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="84" t="s">
@@ -14296,15 +14567,15 @@
       <c r="I6" s="89" t="s">
         <v>591</v>
       </c>
-      <c r="K6" s="192" t="s">
+      <c r="K6" s="178" t="s">
         <v>618</v>
       </c>
-      <c r="L6" s="192"/>
-      <c r="M6" s="192"/>
-      <c r="N6" s="192"/>
-      <c r="O6" s="192"/>
-      <c r="P6" s="192"/>
-      <c r="Q6" s="192"/>
+      <c r="L6" s="178"/>
+      <c r="M6" s="178"/>
+      <c r="N6" s="178"/>
+      <c r="O6" s="178"/>
+      <c r="P6" s="178"/>
+      <c r="Q6" s="178"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="87">
@@ -14334,15 +14605,15 @@
       <c r="I7" s="89" t="s">
         <v>588</v>
       </c>
-      <c r="K7" s="192" t="s">
+      <c r="K7" s="178" t="s">
         <v>626</v>
       </c>
-      <c r="L7" s="192"/>
-      <c r="M7" s="192"/>
-      <c r="N7" s="192"/>
-      <c r="O7" s="192"/>
-      <c r="P7" s="192"/>
-      <c r="Q7" s="192"/>
+      <c r="L7" s="178"/>
+      <c r="M7" s="178"/>
+      <c r="N7" s="178"/>
+      <c r="O7" s="178"/>
+      <c r="P7" s="178"/>
+      <c r="Q7" s="178"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="87">
@@ -14450,17 +14721,17 @@
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="193" t="s">
+      <c r="A15" s="192" t="s">
         <v>634</v>
       </c>
-      <c r="B15" s="194"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="194"/>
-      <c r="E15" s="194"/>
-      <c r="F15" s="194"/>
-      <c r="G15" s="194"/>
-      <c r="H15" s="194"/>
-      <c r="I15" s="195"/>
+      <c r="B15" s="193"/>
+      <c r="C15" s="193"/>
+      <c r="D15" s="193"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="194"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="84" t="s">
@@ -14475,15 +14746,15 @@
       <c r="D16" s="85" t="s">
         <v>586</v>
       </c>
-      <c r="E16" s="196" t="s">
+      <c r="E16" s="195" t="s">
         <v>635</v>
       </c>
-      <c r="F16" s="196"/>
-      <c r="G16" s="196" t="s">
+      <c r="F16" s="195"/>
+      <c r="G16" s="195" t="s">
         <v>636</v>
       </c>
-      <c r="H16" s="196"/>
-      <c r="I16" s="197"/>
+      <c r="H16" s="195"/>
+      <c r="I16" s="196"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="93">
@@ -14498,15 +14769,15 @@
       <c r="D17" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E17" s="188" t="s">
+      <c r="E17" s="197" t="s">
         <v>638</v>
       </c>
-      <c r="F17" s="189"/>
-      <c r="G17" s="188" t="s">
+      <c r="F17" s="198"/>
+      <c r="G17" s="197" t="s">
         <v>639</v>
       </c>
-      <c r="H17" s="190"/>
-      <c r="I17" s="191"/>
+      <c r="H17" s="199"/>
+      <c r="I17" s="200"/>
     </row>
     <row r="18" spans="1:11" ht="22.5">
       <c r="A18" s="93">
@@ -14521,15 +14792,15 @@
       <c r="D18" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E18" s="188" t="s">
+      <c r="E18" s="197" t="s">
         <v>638</v>
       </c>
-      <c r="F18" s="189"/>
-      <c r="G18" s="188" t="s">
+      <c r="F18" s="198"/>
+      <c r="G18" s="197" t="s">
         <v>641</v>
       </c>
-      <c r="H18" s="190"/>
-      <c r="I18" s="191"/>
+      <c r="H18" s="199"/>
+      <c r="I18" s="200"/>
     </row>
     <row r="19" spans="1:11" ht="33.75">
       <c r="A19" s="93">
@@ -14544,15 +14815,15 @@
       <c r="D19" s="88" t="s">
         <v>597</v>
       </c>
-      <c r="E19" s="188" t="s">
+      <c r="E19" s="197" t="s">
         <v>643</v>
       </c>
-      <c r="F19" s="189"/>
-      <c r="G19" s="188" t="s">
+      <c r="F19" s="198"/>
+      <c r="G19" s="197" t="s">
         <v>644</v>
       </c>
-      <c r="H19" s="190"/>
-      <c r="I19" s="191"/>
+      <c r="H19" s="199"/>
+      <c r="I19" s="200"/>
       <c r="K19" t="s">
         <v>645</v>
       </c>
@@ -14564,11 +14835,11 @@
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
-      <c r="E20" s="176"/>
-      <c r="F20" s="177"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="178"/>
-      <c r="I20" s="179"/>
+      <c r="E20" s="201"/>
+      <c r="F20" s="202"/>
+      <c r="G20" s="201"/>
+      <c r="H20" s="203"/>
+      <c r="I20" s="204"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="93">
@@ -14577,11 +14848,11 @@
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="78"/>
-      <c r="E21" s="176"/>
-      <c r="F21" s="177"/>
-      <c r="G21" s="176"/>
-      <c r="H21" s="178"/>
-      <c r="I21" s="179"/>
+      <c r="E21" s="201"/>
+      <c r="F21" s="202"/>
+      <c r="G21" s="201"/>
+      <c r="H21" s="203"/>
+      <c r="I21" s="204"/>
       <c r="K21" t="s">
         <v>646</v>
       </c>
@@ -14593,11 +14864,11 @@
       <c r="B22" s="78"/>
       <c r="C22" s="78"/>
       <c r="D22" s="78"/>
-      <c r="E22" s="176"/>
-      <c r="F22" s="177"/>
-      <c r="G22" s="176"/>
-      <c r="H22" s="178"/>
-      <c r="I22" s="179"/>
+      <c r="E22" s="201"/>
+      <c r="F22" s="202"/>
+      <c r="G22" s="201"/>
+      <c r="H22" s="203"/>
+      <c r="I22" s="204"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="93">
@@ -14606,11 +14877,11 @@
       <c r="B23" s="78"/>
       <c r="C23" s="78"/>
       <c r="D23" s="78"/>
-      <c r="E23" s="176"/>
-      <c r="F23" s="177"/>
-      <c r="G23" s="176"/>
-      <c r="H23" s="178"/>
-      <c r="I23" s="179"/>
+      <c r="E23" s="201"/>
+      <c r="F23" s="202"/>
+      <c r="G23" s="201"/>
+      <c r="H23" s="203"/>
+      <c r="I23" s="204"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="93">
@@ -14619,11 +14890,11 @@
       <c r="B24" s="78"/>
       <c r="C24" s="78"/>
       <c r="D24" s="78"/>
-      <c r="E24" s="176"/>
-      <c r="F24" s="177"/>
-      <c r="G24" s="176"/>
-      <c r="H24" s="178"/>
-      <c r="I24" s="179"/>
+      <c r="E24" s="201"/>
+      <c r="F24" s="202"/>
+      <c r="G24" s="201"/>
+      <c r="H24" s="203"/>
+      <c r="I24" s="204"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="93">
@@ -14632,11 +14903,11 @@
       <c r="B25" s="94"/>
       <c r="C25" s="94"/>
       <c r="D25" s="94"/>
-      <c r="E25" s="180"/>
-      <c r="F25" s="181"/>
-      <c r="G25" s="180"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="183"/>
+      <c r="E25" s="205"/>
+      <c r="F25" s="206"/>
+      <c r="G25" s="205"/>
+      <c r="H25" s="207"/>
+      <c r="I25" s="208"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="95">
@@ -14645,44 +14916,44 @@
       <c r="B26" s="91"/>
       <c r="C26" s="91"/>
       <c r="D26" s="91"/>
-      <c r="E26" s="184"/>
-      <c r="F26" s="185"/>
-      <c r="G26" s="184"/>
-      <c r="H26" s="186"/>
-      <c r="I26" s="187"/>
+      <c r="E26" s="209"/>
+      <c r="F26" s="210"/>
+      <c r="G26" s="209"/>
+      <c r="H26" s="211"/>
+      <c r="I26" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="K6:Q6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14728,11 +14999,11 @@
       <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
+      <c r="B2" s="214"/>
+      <c r="C2" s="214"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="22"/>
@@ -14850,10 +15121,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75">
-      <c r="B2" s="213" t="s">
+      <c r="B2" s="215" t="s">
         <v>509</v>
       </c>
-      <c r="C2" s="213"/>
+      <c r="C2" s="215"/>
       <c r="O2" t="s">
         <v>510</v>
       </c>
@@ -15093,56 +15364,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="213" t="s">
+      <c r="A3" s="215" t="s">
         <v>542</v>
       </c>
-      <c r="B3" s="213"/>
-      <c r="C3" s="213"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="62" t="s">
         <v>543</v>
       </c>
-      <c r="B4" s="215" t="s">
+      <c r="B4" s="217" t="s">
         <v>544</v>
       </c>
-      <c r="C4" s="215"/>
+      <c r="C4" s="217"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="63" t="s">
         <v>545</v>
       </c>
-      <c r="B5" s="214" t="s">
+      <c r="B5" s="216" t="s">
         <v>546</v>
       </c>
-      <c r="C5" s="214"/>
+      <c r="C5" s="216"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="63" t="s">
         <v>547</v>
       </c>
-      <c r="B6" s="214" t="s">
+      <c r="B6" s="216" t="s">
         <v>548</v>
       </c>
-      <c r="C6" s="214"/>
+      <c r="C6" s="216"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="214" t="s">
+      <c r="B7" s="216" t="s">
         <v>549</v>
       </c>
-      <c r="C7" s="214"/>
+      <c r="C7" s="216"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="63" t="s">
         <v>550</v>
       </c>
-      <c r="B8" s="214" t="s">
+      <c r="B8" s="216" t="s">
         <v>551</v>
       </c>
-      <c r="C8" s="214"/>
+      <c r="C8" s="216"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -15175,11 +15446,11 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1"/>
     <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="C2" s="217"/>
-      <c r="D2" s="218"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="220"/>
       <c r="J2" t="s">
         <v>510</v>
       </c>
@@ -15357,11 +15628,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15">
-      <c r="A5" s="215" t="s">
+      <c r="A5" s="217" t="s">
         <v>585</v>
       </c>
-      <c r="B5" s="215"/>
-      <c r="C5" s="215"/>
+      <c r="B5" s="217"/>
+      <c r="C5" s="217"/>
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="62" t="s">

</xml_diff>

<commit_message>
chg: Added targets for target production to Lefty (In joint target list document)
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="785">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -2405,6 +2405,9 @@
   </si>
   <si>
     <t>Varzat</t>
+  </si>
+  <si>
+    <t>Lefty</t>
   </si>
 </sst>
 </file>
@@ -3265,7 +3268,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3708,6 +3711,9 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3720,9 +3726,72 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3762,69 +3831,6 @@
     <xf numFmtId="0" fontId="25" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3849,9 +3855,7 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -3890,7 +3894,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3902,7 +3906,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3922,7 +3926,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3951,7 +3955,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4000,7 +4004,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4045,7 +4049,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4090,7 +4094,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4128,7 +4132,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4176,7 +4180,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4229,7 +4233,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4282,7 +4286,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4380,7 +4384,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4433,7 +4437,7 @@
         <xdr:cNvPr id="3" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4486,7 +4490,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4580,7 +4584,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4633,7 +4637,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4728,7 +4732,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4786,7 +4790,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4839,7 +4843,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4931,7 +4935,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4984,7 +4988,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5217,7 +5221,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5237,15 +5241,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="177" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
       <c r="H1" s="160" t="s">
         <v>722</v>
       </c>
@@ -5258,10 +5262,10 @@
       <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:11" ht="35.25" thickBot="1">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="175" t="s">
         <v>493</v>
       </c>
-      <c r="B2" s="175"/>
+      <c r="B2" s="176"/>
       <c r="C2" s="104"/>
       <c r="D2" s="105"/>
       <c r="E2" s="106"/>
@@ -5305,7 +5309,7 @@
       <c r="J3" s="161" t="s">
         <v>505</v>
       </c>
-      <c r="K3" s="221" t="s">
+      <c r="K3" s="174" t="s">
         <v>781</v>
       </c>
     </row>
@@ -6813,7 +6817,9 @@
         <v>494</v>
       </c>
       <c r="J59" s="61"/>
-      <c r="K59" s="61"/>
+      <c r="K59" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1">
       <c r="A60" s="24" t="s">
@@ -6871,7 +6877,9 @@
         <v>494</v>
       </c>
       <c r="J61" s="61"/>
-      <c r="K61" s="61"/>
+      <c r="K61" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1">
       <c r="A62" s="24" t="s">
@@ -7124,7 +7132,7 @@
       <c r="I71" s="163" t="s">
         <v>494</v>
       </c>
-      <c r="J71" s="61"/>
+      <c r="J71" s="222"/>
       <c r="K71" s="61"/>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1">
@@ -7210,7 +7218,9 @@
         <v>494</v>
       </c>
       <c r="J74" s="61"/>
-      <c r="K74" s="61"/>
+      <c r="K74" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1">
       <c r="A75" s="126" t="s">
@@ -7237,7 +7247,9 @@
         <v>494</v>
       </c>
       <c r="J75" s="61"/>
-      <c r="K75" s="61"/>
+      <c r="K75" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1">
       <c r="A76" s="24" t="s">
@@ -7266,7 +7278,9 @@
         <v>494</v>
       </c>
       <c r="J76" s="61"/>
-      <c r="K76" s="61"/>
+      <c r="K76" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1">
       <c r="A77" s="126" t="s">
@@ -7728,7 +7742,9 @@
         <v>494</v>
       </c>
       <c r="J92" s="61"/>
-      <c r="K92" s="61"/>
+      <c r="K92" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1">
       <c r="A93" s="126" t="s">
@@ -7786,7 +7802,9 @@
         <v>494</v>
       </c>
       <c r="J94" s="61"/>
-      <c r="K94" s="61"/>
+      <c r="K94" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1">
       <c r="A95" s="126" t="s">
@@ -7814,8 +7832,10 @@
       <c r="I95" s="162" t="s">
         <v>494</v>
       </c>
-      <c r="J95" s="61"/>
-      <c r="K95" s="61"/>
+      <c r="J95" s="222"/>
+      <c r="K95" s="61" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1">
       <c r="A96" s="24" t="s">
@@ -14462,50 +14482,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="179" t="s">
+      <c r="A1" s="201" t="s">
         <v>601</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
-      <c r="G1" s="180"/>
-      <c r="H1" s="180"/>
-      <c r="I1" s="181"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="203"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="204" t="s">
         <v>602</v>
       </c>
-      <c r="B2" s="183"/>
+      <c r="B2" s="205"/>
       <c r="C2" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="206" t="s">
         <v>603</v>
       </c>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187" t="s">
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="209" t="s">
         <v>604</v>
       </c>
-      <c r="I2" s="188"/>
+      <c r="I2" s="210"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="189" t="s">
+      <c r="A4" s="211" t="s">
         <v>605</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="190"/>
-      <c r="I4" s="191"/>
+      <c r="B4" s="212"/>
+      <c r="C4" s="212"/>
+      <c r="D4" s="212"/>
+      <c r="E4" s="212"/>
+      <c r="F4" s="212"/>
+      <c r="G4" s="212"/>
+      <c r="H4" s="212"/>
+      <c r="I4" s="213"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="84" t="s">
@@ -14567,15 +14587,15 @@
       <c r="I6" s="89" t="s">
         <v>591</v>
       </c>
-      <c r="K6" s="178" t="s">
+      <c r="K6" s="195" t="s">
         <v>618</v>
       </c>
-      <c r="L6" s="178"/>
-      <c r="M6" s="178"/>
-      <c r="N6" s="178"/>
-      <c r="O6" s="178"/>
-      <c r="P6" s="178"/>
-      <c r="Q6" s="178"/>
+      <c r="L6" s="195"/>
+      <c r="M6" s="195"/>
+      <c r="N6" s="195"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="87">
@@ -14605,15 +14625,15 @@
       <c r="I7" s="89" t="s">
         <v>588</v>
       </c>
-      <c r="K7" s="178" t="s">
+      <c r="K7" s="195" t="s">
         <v>626</v>
       </c>
-      <c r="L7" s="178"/>
-      <c r="M7" s="178"/>
-      <c r="N7" s="178"/>
-      <c r="O7" s="178"/>
-      <c r="P7" s="178"/>
-      <c r="Q7" s="178"/>
+      <c r="L7" s="195"/>
+      <c r="M7" s="195"/>
+      <c r="N7" s="195"/>
+      <c r="O7" s="195"/>
+      <c r="P7" s="195"/>
+      <c r="Q7" s="195"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="87">
@@ -14721,17 +14741,17 @@
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="192" t="s">
+      <c r="A15" s="196" t="s">
         <v>634</v>
       </c>
-      <c r="B15" s="193"/>
-      <c r="C15" s="193"/>
-      <c r="D15" s="193"/>
-      <c r="E15" s="193"/>
-      <c r="F15" s="193"/>
-      <c r="G15" s="193"/>
-      <c r="H15" s="193"/>
-      <c r="I15" s="194"/>
+      <c r="B15" s="197"/>
+      <c r="C15" s="197"/>
+      <c r="D15" s="197"/>
+      <c r="E15" s="197"/>
+      <c r="F15" s="197"/>
+      <c r="G15" s="197"/>
+      <c r="H15" s="197"/>
+      <c r="I15" s="198"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="84" t="s">
@@ -14746,15 +14766,15 @@
       <c r="D16" s="85" t="s">
         <v>586</v>
       </c>
-      <c r="E16" s="195" t="s">
+      <c r="E16" s="199" t="s">
         <v>635</v>
       </c>
-      <c r="F16" s="195"/>
-      <c r="G16" s="195" t="s">
+      <c r="F16" s="199"/>
+      <c r="G16" s="199" t="s">
         <v>636</v>
       </c>
-      <c r="H16" s="195"/>
-      <c r="I16" s="196"/>
+      <c r="H16" s="199"/>
+      <c r="I16" s="200"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="93">
@@ -14769,15 +14789,15 @@
       <c r="D17" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E17" s="197" t="s">
+      <c r="E17" s="191" t="s">
         <v>638</v>
       </c>
-      <c r="F17" s="198"/>
-      <c r="G17" s="197" t="s">
+      <c r="F17" s="192"/>
+      <c r="G17" s="191" t="s">
         <v>639</v>
       </c>
-      <c r="H17" s="199"/>
-      <c r="I17" s="200"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="194"/>
     </row>
     <row r="18" spans="1:11" ht="22.5">
       <c r="A18" s="93">
@@ -14792,15 +14812,15 @@
       <c r="D18" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E18" s="197" t="s">
+      <c r="E18" s="191" t="s">
         <v>638</v>
       </c>
-      <c r="F18" s="198"/>
-      <c r="G18" s="197" t="s">
+      <c r="F18" s="192"/>
+      <c r="G18" s="191" t="s">
         <v>641</v>
       </c>
-      <c r="H18" s="199"/>
-      <c r="I18" s="200"/>
+      <c r="H18" s="193"/>
+      <c r="I18" s="194"/>
     </row>
     <row r="19" spans="1:11" ht="33.75">
       <c r="A19" s="93">
@@ -14815,15 +14835,15 @@
       <c r="D19" s="88" t="s">
         <v>597</v>
       </c>
-      <c r="E19" s="197" t="s">
+      <c r="E19" s="191" t="s">
         <v>643</v>
       </c>
-      <c r="F19" s="198"/>
-      <c r="G19" s="197" t="s">
+      <c r="F19" s="192"/>
+      <c r="G19" s="191" t="s">
         <v>644</v>
       </c>
-      <c r="H19" s="199"/>
-      <c r="I19" s="200"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="194"/>
       <c r="K19" t="s">
         <v>645</v>
       </c>
@@ -14835,11 +14855,11 @@
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
-      <c r="E20" s="201"/>
-      <c r="F20" s="202"/>
-      <c r="G20" s="201"/>
-      <c r="H20" s="203"/>
-      <c r="I20" s="204"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="180"/>
+      <c r="G20" s="179"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="182"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="93">
@@ -14848,11 +14868,11 @@
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="78"/>
-      <c r="E21" s="201"/>
-      <c r="F21" s="202"/>
-      <c r="G21" s="201"/>
-      <c r="H21" s="203"/>
-      <c r="I21" s="204"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="180"/>
+      <c r="G21" s="179"/>
+      <c r="H21" s="181"/>
+      <c r="I21" s="182"/>
       <c r="K21" t="s">
         <v>646</v>
       </c>
@@ -14864,11 +14884,11 @@
       <c r="B22" s="78"/>
       <c r="C22" s="78"/>
       <c r="D22" s="78"/>
-      <c r="E22" s="201"/>
-      <c r="F22" s="202"/>
-      <c r="G22" s="201"/>
-      <c r="H22" s="203"/>
-      <c r="I22" s="204"/>
+      <c r="E22" s="179"/>
+      <c r="F22" s="180"/>
+      <c r="G22" s="179"/>
+      <c r="H22" s="181"/>
+      <c r="I22" s="182"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="93">
@@ -14877,11 +14897,11 @@
       <c r="B23" s="78"/>
       <c r="C23" s="78"/>
       <c r="D23" s="78"/>
-      <c r="E23" s="201"/>
-      <c r="F23" s="202"/>
-      <c r="G23" s="201"/>
-      <c r="H23" s="203"/>
-      <c r="I23" s="204"/>
+      <c r="E23" s="179"/>
+      <c r="F23" s="180"/>
+      <c r="G23" s="179"/>
+      <c r="H23" s="181"/>
+      <c r="I23" s="182"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="93">
@@ -14890,11 +14910,11 @@
       <c r="B24" s="78"/>
       <c r="C24" s="78"/>
       <c r="D24" s="78"/>
-      <c r="E24" s="201"/>
-      <c r="F24" s="202"/>
-      <c r="G24" s="201"/>
-      <c r="H24" s="203"/>
-      <c r="I24" s="204"/>
+      <c r="E24" s="179"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="179"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="182"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="93">
@@ -14903,11 +14923,11 @@
       <c r="B25" s="94"/>
       <c r="C25" s="94"/>
       <c r="D25" s="94"/>
-      <c r="E25" s="205"/>
-      <c r="F25" s="206"/>
-      <c r="G25" s="205"/>
-      <c r="H25" s="207"/>
-      <c r="I25" s="208"/>
+      <c r="E25" s="183"/>
+      <c r="F25" s="184"/>
+      <c r="G25" s="183"/>
+      <c r="H25" s="185"/>
+      <c r="I25" s="186"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="95">
@@ -14916,44 +14936,44 @@
       <c r="B26" s="91"/>
       <c r="C26" s="91"/>
       <c r="D26" s="91"/>
-      <c r="E26" s="209"/>
-      <c r="F26" s="210"/>
-      <c r="G26" s="209"/>
-      <c r="H26" s="211"/>
-      <c r="I26" s="212"/>
+      <c r="E26" s="187"/>
+      <c r="F26" s="188"/>
+      <c r="G26" s="187"/>
+      <c r="H26" s="189"/>
+      <c r="I26" s="190"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14999,11 +15019,11 @@
       <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="214" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
+      <c r="B2" s="215"/>
+      <c r="C2" s="215"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="22"/>
@@ -15121,10 +15141,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75">
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="216" t="s">
         <v>509</v>
       </c>
-      <c r="C2" s="215"/>
+      <c r="C2" s="216"/>
       <c r="O2" t="s">
         <v>510</v>
       </c>
@@ -15364,56 +15384,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="215" t="s">
+      <c r="A3" s="216" t="s">
         <v>542</v>
       </c>
-      <c r="B3" s="215"/>
-      <c r="C3" s="215"/>
+      <c r="B3" s="216"/>
+      <c r="C3" s="216"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="62" t="s">
         <v>543</v>
       </c>
-      <c r="B4" s="217" t="s">
+      <c r="B4" s="218" t="s">
         <v>544</v>
       </c>
-      <c r="C4" s="217"/>
+      <c r="C4" s="218"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="63" t="s">
         <v>545</v>
       </c>
-      <c r="B5" s="216" t="s">
+      <c r="B5" s="217" t="s">
         <v>546</v>
       </c>
-      <c r="C5" s="216"/>
+      <c r="C5" s="217"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="63" t="s">
         <v>547</v>
       </c>
-      <c r="B6" s="216" t="s">
+      <c r="B6" s="217" t="s">
         <v>548</v>
       </c>
-      <c r="C6" s="216"/>
+      <c r="C6" s="217"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="216" t="s">
+      <c r="B7" s="217" t="s">
         <v>549</v>
       </c>
-      <c r="C7" s="216"/>
+      <c r="C7" s="217"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="63" t="s">
         <v>550</v>
       </c>
-      <c r="B8" s="216" t="s">
+      <c r="B8" s="217" t="s">
         <v>551</v>
       </c>
-      <c r="C8" s="216"/>
+      <c r="C8" s="217"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -15446,11 +15466,11 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1"/>
     <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="218" t="s">
+      <c r="B2" s="219" t="s">
         <v>552</v>
       </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="220"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="221"/>
       <c r="J2" t="s">
         <v>510</v>
       </c>
@@ -15628,11 +15648,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15">
-      <c r="A5" s="217" t="s">
+      <c r="A5" s="218" t="s">
         <v>585</v>
       </c>
-      <c r="B5" s="217"/>
-      <c r="C5" s="217"/>
+      <c r="B5" s="218"/>
+      <c r="C5" s="218"/>
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="62" t="s">

</xml_diff>

<commit_message>
chg: Updated some of the recent targets in CombatFlite and updated tgt list with coordinates
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="806">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -2317,9 +2317,6 @@
     <t>Building for the General Staff meetings</t>
   </si>
   <si>
-    <t>N68 51.315 E033 00.870</t>
-  </si>
-  <si>
     <t>Ministry of Foreign Affairs</t>
   </si>
   <si>
@@ -2341,9 +2338,6 @@
     <t>Handles security and counter-intelligence</t>
   </si>
   <si>
-    <t>N68 57.182 E033.448</t>
-  </si>
-  <si>
     <t>185ft</t>
   </si>
   <si>
@@ -2408,6 +2402,75 @@
   </si>
   <si>
     <t>Lefty</t>
+  </si>
+  <si>
+    <t>N 68 03.688 E 039 27.365</t>
+  </si>
+  <si>
+    <t>N 67 59.857 E 035 02.102</t>
+  </si>
+  <si>
+    <t>512ft</t>
+  </si>
+  <si>
+    <t>N 68 09.529 E 033 11.712</t>
+  </si>
+  <si>
+    <t>597ft</t>
+  </si>
+  <si>
+    <t>N 68 57.182 E 033 03.448</t>
+  </si>
+  <si>
+    <t>N 68 58.003 E 033 04.101</t>
+  </si>
+  <si>
+    <t>82ft</t>
+  </si>
+  <si>
+    <t>N 68 57.984 E 033 04.035</t>
+  </si>
+  <si>
+    <t>N 68 58.148 E 033 04.890</t>
+  </si>
+  <si>
+    <t>106ft</t>
+  </si>
+  <si>
+    <t>N 68 51.315 E 033 00.869</t>
+  </si>
+  <si>
+    <t>N 68 48.603 E 032 46.608</t>
+  </si>
+  <si>
+    <t>103ft</t>
+  </si>
+  <si>
+    <t>N 67 36.659 E 033 24.039</t>
+  </si>
+  <si>
+    <t>N 67 36.713 E 033 24.218</t>
+  </si>
+  <si>
+    <t>525ft</t>
+  </si>
+  <si>
+    <t>522ft</t>
+  </si>
+  <si>
+    <t>N 68 08.670 E 033 26.052</t>
+  </si>
+  <si>
+    <t>673ft</t>
+  </si>
+  <si>
+    <t>N 68 07.981 E 033 13.529</t>
+  </si>
+  <si>
+    <t>728ft</t>
+  </si>
+  <si>
+    <t>N 69 31.375 E 031 14.113</t>
   </si>
 </sst>
 </file>
@@ -3726,6 +3789,75 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3762,75 +3894,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3855,7 +3918,7 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -3894,7 +3957,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3906,7 +3969,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3926,7 +3989,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3955,7 +4018,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4004,7 +4067,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4049,7 +4112,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4094,7 +4157,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4132,7 +4195,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4180,7 +4243,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4233,7 +4296,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4286,7 +4349,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4384,7 +4447,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4437,7 +4500,7 @@
         <xdr:cNvPr id="3" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4490,7 +4553,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4584,7 +4647,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4637,7 +4700,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4732,7 +4795,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4790,7 +4853,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4843,7 +4906,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4935,7 +4998,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4988,7 +5051,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5218,10 +5281,10 @@
   <dimension ref="A1:K825"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J57" sqref="J57"/>
+      <selection pane="bottomRight" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5272,7 +5335,7 @@
       <c r="F2" s="106"/>
       <c r="G2" s="107"/>
       <c r="H2" s="173" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I2" s="60"/>
       <c r="J2" s="61"/>
@@ -5310,7 +5373,7 @@
         <v>505</v>
       </c>
       <c r="K3" s="174" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25">
@@ -5370,7 +5433,7 @@
       </c>
       <c r="J5" s="61"/>
       <c r="K5" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.25">
@@ -5401,7 +5464,7 @@
       </c>
       <c r="J6" s="61"/>
       <c r="K6" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.25">
@@ -5432,7 +5495,7 @@
       </c>
       <c r="J7" s="61"/>
       <c r="K7" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.25">
@@ -5618,15 +5681,15 @@
         <v>54</v>
       </c>
       <c r="B14" s="115" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C14" s="98"/>
       <c r="D14" s="4"/>
       <c r="E14" s="45" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>754</v>
+        <v>794</v>
       </c>
       <c r="G14" s="152" t="s">
         <v>55</v>
@@ -5639,7 +5702,7 @@
       </c>
       <c r="J14" s="61"/>
       <c r="K14" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.25">
@@ -5647,17 +5710,17 @@
         <v>56</v>
       </c>
       <c r="B15" s="133" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C15" s="134">
         <v>11</v>
       </c>
       <c r="D15" s="135"/>
       <c r="E15" s="130" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F15" s="131" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="G15" s="151" t="s">
         <v>126</v>
@@ -5670,7 +5733,7 @@
       </c>
       <c r="J15" s="61"/>
       <c r="K15" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.25">
@@ -5678,20 +5741,20 @@
         <v>57</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C16" s="98">
         <v>11</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="45" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F16" s="43" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="G16" s="152" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="H16" s="165" t="s">
         <v>734</v>
@@ -5701,7 +5764,7 @@
       </c>
       <c r="J16" s="61"/>
       <c r="K16" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="14.25">
@@ -5709,20 +5772,20 @@
         <v>58</v>
       </c>
       <c r="B17" s="133" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C17" s="134">
         <v>11</v>
       </c>
       <c r="D17" s="135"/>
       <c r="E17" s="130" t="s">
+        <v>760</v>
+      </c>
+      <c r="F17" s="131" t="s">
+        <v>788</v>
+      </c>
+      <c r="G17" s="151" t="s">
         <v>761</v>
-      </c>
-      <c r="F17" s="131" t="s">
-        <v>762</v>
-      </c>
-      <c r="G17" s="151" t="s">
-        <v>763</v>
       </c>
       <c r="H17" s="165" t="s">
         <v>734</v>
@@ -5732,7 +5795,7 @@
       </c>
       <c r="J17" s="61"/>
       <c r="K17" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.25">
@@ -5740,7 +5803,7 @@
         <v>59</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C18" s="98">
         <v>1</v>
@@ -5749,7 +5812,12 @@
       <c r="E18" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="152"/>
+      <c r="F18" s="43" t="s">
+        <v>786</v>
+      </c>
+      <c r="G18" s="152" t="s">
+        <v>787</v>
+      </c>
       <c r="H18" s="165" t="s">
         <v>734</v>
       </c>
@@ -5764,20 +5832,20 @@
         <v>61</v>
       </c>
       <c r="B19" s="133" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C19" s="134">
         <v>6</v>
       </c>
       <c r="D19" s="135"/>
       <c r="E19" s="130" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F19" s="131" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="G19" s="151" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="H19" s="165" t="s">
         <v>734</v>
@@ -5802,7 +5870,12 @@
       <c r="E20" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="152"/>
+      <c r="F20" s="43" t="s">
+        <v>784</v>
+      </c>
+      <c r="G20" s="152" t="s">
+        <v>785</v>
+      </c>
       <c r="H20" s="165" t="s">
         <v>734</v>
       </c>
@@ -5824,10 +5897,14 @@
       </c>
       <c r="D21" s="135"/>
       <c r="E21" s="130" t="s">
-        <v>778</v>
-      </c>
-      <c r="F21" s="131"/>
-      <c r="G21" s="151"/>
+        <v>776</v>
+      </c>
+      <c r="F21" s="131" t="s">
+        <v>805</v>
+      </c>
+      <c r="G21" s="151" t="s">
+        <v>785</v>
+      </c>
       <c r="H21" s="165" t="s">
         <v>734</v>
       </c>
@@ -5849,9 +5926,14 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="45" t="s">
-        <v>777</v>
-      </c>
-      <c r="G22" s="152"/>
+        <v>775</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="G22" s="152" t="s">
+        <v>804</v>
+      </c>
       <c r="H22" s="165" t="s">
         <v>734</v>
       </c>
@@ -5951,7 +6033,7 @@
         <v>77</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C26" s="98">
         <v>2</v>
@@ -5959,6 +6041,9 @@
       <c r="D26" s="4"/>
       <c r="E26" s="45" t="s">
         <v>78</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>783</v>
       </c>
       <c r="G26" s="152"/>
       <c r="H26" s="164" t="s">
@@ -6818,7 +6903,7 @@
       </c>
       <c r="J59" s="61"/>
       <c r="K59" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="15.75" customHeight="1">
@@ -6878,7 +6963,7 @@
       </c>
       <c r="J61" s="61"/>
       <c r="K61" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="15.75" customHeight="1">
@@ -7219,7 +7304,7 @@
       </c>
       <c r="J74" s="61"/>
       <c r="K74" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="15.75" customHeight="1">
@@ -7248,7 +7333,7 @@
       </c>
       <c r="J75" s="61"/>
       <c r="K75" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="15.75" customHeight="1">
@@ -7266,10 +7351,10 @@
         <v>502</v>
       </c>
       <c r="F76" s="43" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="G76" s="152" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="H76" s="171" t="s">
         <v>734</v>
@@ -7279,7 +7364,7 @@
       </c>
       <c r="J76" s="61"/>
       <c r="K76" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="15.75" customHeight="1">
@@ -7321,7 +7406,7 @@
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="45" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="F78" s="43" t="s">
         <v>674</v>
@@ -7743,7 +7828,7 @@
       </c>
       <c r="J92" s="61"/>
       <c r="K92" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1">
@@ -7803,7 +7888,7 @@
       </c>
       <c r="J94" s="61"/>
       <c r="K94" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1">
@@ -7834,7 +7919,7 @@
       </c>
       <c r="J95" s="222"/>
       <c r="K95" s="61" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1">
@@ -7851,8 +7936,8 @@
       <c r="E96" s="41"/>
       <c r="F96" s="61"/>
       <c r="G96" s="152"/>
-      <c r="H96" s="162" t="s">
-        <v>494</v>
+      <c r="H96" s="171" t="s">
+        <v>734</v>
       </c>
       <c r="I96" s="162" t="s">
         <v>494</v>
@@ -7872,8 +7957,12 @@
       </c>
       <c r="D97" s="135"/>
       <c r="E97" s="132"/>
-      <c r="F97" s="139"/>
-      <c r="G97" s="151"/>
+      <c r="F97" s="139" t="s">
+        <v>797</v>
+      </c>
+      <c r="G97" s="151" t="s">
+        <v>800</v>
+      </c>
       <c r="H97" s="171" t="s">
         <v>734</v>
       </c>
@@ -7882,7 +7971,7 @@
       </c>
       <c r="J97" s="61"/>
       <c r="K97" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="15.75" customHeight="1">
@@ -7897,10 +7986,14 @@
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="41" t="s">
-        <v>776</v>
-      </c>
-      <c r="F98" s="61"/>
-      <c r="G98" s="152"/>
+        <v>774</v>
+      </c>
+      <c r="F98" s="61" t="s">
+        <v>798</v>
+      </c>
+      <c r="G98" s="152" t="s">
+        <v>799</v>
+      </c>
       <c r="H98" s="171" t="s">
         <v>734</v>
       </c>
@@ -7924,8 +8017,8 @@
       <c r="E99" s="132"/>
       <c r="F99" s="139"/>
       <c r="G99" s="130"/>
-      <c r="H99" s="162" t="s">
-        <v>494</v>
+      <c r="H99" s="171" t="s">
+        <v>734</v>
       </c>
       <c r="I99" s="162" t="s">
         <v>494</v>
@@ -7934,7 +8027,7 @@
         <v>734</v>
       </c>
       <c r="K99" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="15.75" customHeight="1">
@@ -7961,7 +8054,7 @@
       </c>
       <c r="J100" s="61"/>
       <c r="K100" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="101" spans="1:11" ht="15.75" customHeight="1">
@@ -7988,7 +8081,7 @@
       </c>
       <c r="J101" s="61"/>
       <c r="K101" s="61" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="102" spans="1:11" ht="15.75" customHeight="1">
@@ -8015,7 +8108,7 @@
       </c>
       <c r="J102" s="61"/>
       <c r="K102" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" hidden="1" customHeight="1">
@@ -9557,7 +9650,7 @@
       </c>
       <c r="J204" s="61"/>
       <c r="K204" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="205" spans="1:11" ht="15.75" customHeight="1">
@@ -9584,7 +9677,7 @@
       </c>
       <c r="J205" s="61"/>
       <c r="K205" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="206" spans="1:11" ht="15.75" customHeight="1">
@@ -9601,8 +9694,12 @@
       <c r="E206" s="133" t="s">
         <v>743</v>
       </c>
-      <c r="F206" s="133"/>
-      <c r="G206" s="157"/>
+      <c r="F206" s="133" t="s">
+        <v>801</v>
+      </c>
+      <c r="G206" s="157" t="s">
+        <v>802</v>
+      </c>
       <c r="H206" s="171" t="s">
         <v>734</v>
       </c>
@@ -9611,7 +9708,7 @@
       </c>
       <c r="J206" s="61"/>
       <c r="K206" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="207" spans="1:11" ht="15.75" customHeight="1">
@@ -9628,8 +9725,12 @@
       <c r="E207" s="145" t="s">
         <v>745</v>
       </c>
-      <c r="F207" s="145"/>
-      <c r="G207" s="158"/>
+      <c r="F207" s="145" t="s">
+        <v>795</v>
+      </c>
+      <c r="G207" s="158" t="s">
+        <v>796</v>
+      </c>
       <c r="H207" s="171" t="s">
         <v>734</v>
       </c>
@@ -9638,7 +9739,7 @@
       </c>
       <c r="J207" s="61"/>
       <c r="K207" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="208" spans="1:11" ht="15.75" customHeight="1">
@@ -9655,8 +9756,12 @@
       <c r="E208" s="147" t="s">
         <v>750</v>
       </c>
-      <c r="F208" s="147"/>
-      <c r="G208" s="159"/>
+      <c r="F208" s="147" t="s">
+        <v>789</v>
+      </c>
+      <c r="G208" s="159" t="s">
+        <v>790</v>
+      </c>
       <c r="H208" s="171" t="s">
         <v>734</v>
       </c>
@@ -9665,7 +9770,7 @@
       </c>
       <c r="J208" s="61"/>
       <c r="K208" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="209" spans="1:11" ht="15.75" customHeight="1">
@@ -9682,8 +9787,12 @@
       <c r="E209" s="145" t="s">
         <v>749</v>
       </c>
-      <c r="F209" s="145"/>
-      <c r="G209" s="158"/>
+      <c r="F209" s="145" t="s">
+        <v>791</v>
+      </c>
+      <c r="G209" s="158" t="s">
+        <v>790</v>
+      </c>
       <c r="H209" s="171" t="s">
         <v>734</v>
       </c>
@@ -9692,7 +9801,7 @@
       </c>
       <c r="J209" s="61"/>
       <c r="K209" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="210" spans="1:11" ht="15.75" customHeight="1">
@@ -9709,8 +9818,12 @@
       <c r="E210" s="147" t="s">
         <v>753</v>
       </c>
-      <c r="F210" s="147"/>
-      <c r="G210" s="159"/>
+      <c r="F210" s="147" t="s">
+        <v>792</v>
+      </c>
+      <c r="G210" s="159" t="s">
+        <v>793</v>
+      </c>
       <c r="H210" s="171" t="s">
         <v>734</v>
       </c>
@@ -9719,7 +9832,7 @@
       </c>
       <c r="J210" s="61"/>
       <c r="K210" s="61" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="211" spans="1:11" ht="15.75" customHeight="1">
@@ -14482,50 +14595,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="180" t="s">
         <v>601</v>
       </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="203"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="182"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="204" t="s">
+      <c r="A2" s="183" t="s">
         <v>602</v>
       </c>
-      <c r="B2" s="205"/>
+      <c r="B2" s="184"/>
       <c r="C2" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="D2" s="206" t="s">
+      <c r="D2" s="185" t="s">
         <v>603</v>
       </c>
-      <c r="E2" s="207"/>
-      <c r="F2" s="207"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="209" t="s">
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="188" t="s">
         <v>604</v>
       </c>
-      <c r="I2" s="210"/>
+      <c r="I2" s="189"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="211" t="s">
+      <c r="A4" s="190" t="s">
         <v>605</v>
       </c>
-      <c r="B4" s="212"/>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
-      <c r="H4" s="212"/>
-      <c r="I4" s="213"/>
+      <c r="B4" s="191"/>
+      <c r="C4" s="191"/>
+      <c r="D4" s="191"/>
+      <c r="E4" s="191"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="191"/>
+      <c r="H4" s="191"/>
+      <c r="I4" s="192"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="84" t="s">
@@ -14587,15 +14700,15 @@
       <c r="I6" s="89" t="s">
         <v>591</v>
       </c>
-      <c r="K6" s="195" t="s">
+      <c r="K6" s="179" t="s">
         <v>618</v>
       </c>
-      <c r="L6" s="195"/>
-      <c r="M6" s="195"/>
-      <c r="N6" s="195"/>
-      <c r="O6" s="195"/>
-      <c r="P6" s="195"/>
-      <c r="Q6" s="195"/>
+      <c r="L6" s="179"/>
+      <c r="M6" s="179"/>
+      <c r="N6" s="179"/>
+      <c r="O6" s="179"/>
+      <c r="P6" s="179"/>
+      <c r="Q6" s="179"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="87">
@@ -14625,15 +14738,15 @@
       <c r="I7" s="89" t="s">
         <v>588</v>
       </c>
-      <c r="K7" s="195" t="s">
+      <c r="K7" s="179" t="s">
         <v>626</v>
       </c>
-      <c r="L7" s="195"/>
-      <c r="M7" s="195"/>
-      <c r="N7" s="195"/>
-      <c r="O7" s="195"/>
-      <c r="P7" s="195"/>
-      <c r="Q7" s="195"/>
+      <c r="L7" s="179"/>
+      <c r="M7" s="179"/>
+      <c r="N7" s="179"/>
+      <c r="O7" s="179"/>
+      <c r="P7" s="179"/>
+      <c r="Q7" s="179"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="87">
@@ -14741,17 +14854,17 @@
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="196" t="s">
+      <c r="A15" s="193" t="s">
         <v>634</v>
       </c>
-      <c r="B15" s="197"/>
-      <c r="C15" s="197"/>
-      <c r="D15" s="197"/>
-      <c r="E15" s="197"/>
-      <c r="F15" s="197"/>
-      <c r="G15" s="197"/>
-      <c r="H15" s="197"/>
-      <c r="I15" s="198"/>
+      <c r="B15" s="194"/>
+      <c r="C15" s="194"/>
+      <c r="D15" s="194"/>
+      <c r="E15" s="194"/>
+      <c r="F15" s="194"/>
+      <c r="G15" s="194"/>
+      <c r="H15" s="194"/>
+      <c r="I15" s="195"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="84" t="s">
@@ -14766,15 +14879,15 @@
       <c r="D16" s="85" t="s">
         <v>586</v>
       </c>
-      <c r="E16" s="199" t="s">
+      <c r="E16" s="196" t="s">
         <v>635</v>
       </c>
-      <c r="F16" s="199"/>
-      <c r="G16" s="199" t="s">
+      <c r="F16" s="196"/>
+      <c r="G16" s="196" t="s">
         <v>636</v>
       </c>
-      <c r="H16" s="199"/>
-      <c r="I16" s="200"/>
+      <c r="H16" s="196"/>
+      <c r="I16" s="197"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="93">
@@ -14789,15 +14902,15 @@
       <c r="D17" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E17" s="191" t="s">
+      <c r="E17" s="198" t="s">
         <v>638</v>
       </c>
-      <c r="F17" s="192"/>
-      <c r="G17" s="191" t="s">
+      <c r="F17" s="199"/>
+      <c r="G17" s="198" t="s">
         <v>639</v>
       </c>
-      <c r="H17" s="193"/>
-      <c r="I17" s="194"/>
+      <c r="H17" s="200"/>
+      <c r="I17" s="201"/>
     </row>
     <row r="18" spans="1:11" ht="22.5">
       <c r="A18" s="93">
@@ -14812,15 +14925,15 @@
       <c r="D18" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E18" s="191" t="s">
+      <c r="E18" s="198" t="s">
         <v>638</v>
       </c>
-      <c r="F18" s="192"/>
-      <c r="G18" s="191" t="s">
+      <c r="F18" s="199"/>
+      <c r="G18" s="198" t="s">
         <v>641</v>
       </c>
-      <c r="H18" s="193"/>
-      <c r="I18" s="194"/>
+      <c r="H18" s="200"/>
+      <c r="I18" s="201"/>
     </row>
     <row r="19" spans="1:11" ht="33.75">
       <c r="A19" s="93">
@@ -14835,15 +14948,15 @@
       <c r="D19" s="88" t="s">
         <v>597</v>
       </c>
-      <c r="E19" s="191" t="s">
+      <c r="E19" s="198" t="s">
         <v>643</v>
       </c>
-      <c r="F19" s="192"/>
-      <c r="G19" s="191" t="s">
+      <c r="F19" s="199"/>
+      <c r="G19" s="198" t="s">
         <v>644</v>
       </c>
-      <c r="H19" s="193"/>
-      <c r="I19" s="194"/>
+      <c r="H19" s="200"/>
+      <c r="I19" s="201"/>
       <c r="K19" t="s">
         <v>645</v>
       </c>
@@ -14855,11 +14968,11 @@
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
-      <c r="E20" s="179"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="179"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="182"/>
+      <c r="E20" s="202"/>
+      <c r="F20" s="203"/>
+      <c r="G20" s="202"/>
+      <c r="H20" s="204"/>
+      <c r="I20" s="205"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="93">
@@ -14868,11 +14981,11 @@
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="78"/>
-      <c r="E21" s="179"/>
-      <c r="F21" s="180"/>
-      <c r="G21" s="179"/>
-      <c r="H21" s="181"/>
-      <c r="I21" s="182"/>
+      <c r="E21" s="202"/>
+      <c r="F21" s="203"/>
+      <c r="G21" s="202"/>
+      <c r="H21" s="204"/>
+      <c r="I21" s="205"/>
       <c r="K21" t="s">
         <v>646</v>
       </c>
@@ -14884,11 +14997,11 @@
       <c r="B22" s="78"/>
       <c r="C22" s="78"/>
       <c r="D22" s="78"/>
-      <c r="E22" s="179"/>
-      <c r="F22" s="180"/>
-      <c r="G22" s="179"/>
-      <c r="H22" s="181"/>
-      <c r="I22" s="182"/>
+      <c r="E22" s="202"/>
+      <c r="F22" s="203"/>
+      <c r="G22" s="202"/>
+      <c r="H22" s="204"/>
+      <c r="I22" s="205"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="93">
@@ -14897,11 +15010,11 @@
       <c r="B23" s="78"/>
       <c r="C23" s="78"/>
       <c r="D23" s="78"/>
-      <c r="E23" s="179"/>
-      <c r="F23" s="180"/>
-      <c r="G23" s="179"/>
-      <c r="H23" s="181"/>
-      <c r="I23" s="182"/>
+      <c r="E23" s="202"/>
+      <c r="F23" s="203"/>
+      <c r="G23" s="202"/>
+      <c r="H23" s="204"/>
+      <c r="I23" s="205"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="93">
@@ -14910,11 +15023,11 @@
       <c r="B24" s="78"/>
       <c r="C24" s="78"/>
       <c r="D24" s="78"/>
-      <c r="E24" s="179"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="179"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="182"/>
+      <c r="E24" s="202"/>
+      <c r="F24" s="203"/>
+      <c r="G24" s="202"/>
+      <c r="H24" s="204"/>
+      <c r="I24" s="205"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="93">
@@ -14923,11 +15036,11 @@
       <c r="B25" s="94"/>
       <c r="C25" s="94"/>
       <c r="D25" s="94"/>
-      <c r="E25" s="183"/>
-      <c r="F25" s="184"/>
-      <c r="G25" s="183"/>
-      <c r="H25" s="185"/>
-      <c r="I25" s="186"/>
+      <c r="E25" s="206"/>
+      <c r="F25" s="207"/>
+      <c r="G25" s="206"/>
+      <c r="H25" s="208"/>
+      <c r="I25" s="209"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="95">
@@ -14936,44 +15049,44 @@
       <c r="B26" s="91"/>
       <c r="C26" s="91"/>
       <c r="D26" s="91"/>
-      <c r="E26" s="187"/>
-      <c r="F26" s="188"/>
-      <c r="G26" s="187"/>
-      <c r="H26" s="189"/>
-      <c r="I26" s="190"/>
+      <c r="E26" s="210"/>
+      <c r="F26" s="211"/>
+      <c r="G26" s="210"/>
+      <c r="H26" s="212"/>
+      <c r="I26" s="213"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="K6:Q6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Added remaining targets to Combatflite and updated tgt list with coordinates
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="818">
   <si>
     <t xml:space="preserve">OPERATION ARCTIC THUNDER </t>
   </si>
@@ -2471,6 +2471,42 @@
   </si>
   <si>
     <t>N 69 31.375 E 031 14.113</t>
+  </si>
+  <si>
+    <t>N 69 04.518 E 033 21.135</t>
+  </si>
+  <si>
+    <t>121ft</t>
+  </si>
+  <si>
+    <t>N 69 03.507 E 033 23.756</t>
+  </si>
+  <si>
+    <t>151ft</t>
+  </si>
+  <si>
+    <t>N 69 03.636 E 033 26.450</t>
+  </si>
+  <si>
+    <t>N 69 03.428 E 033 22.989</t>
+  </si>
+  <si>
+    <t>138ft</t>
+  </si>
+  <si>
+    <t>N 68 07.059 E 033 17.674</t>
+  </si>
+  <si>
+    <t>554ft</t>
+  </si>
+  <si>
+    <t>N 67 23.210 E 032 30.369</t>
+  </si>
+  <si>
+    <t>433ft</t>
+  </si>
+  <si>
+    <t>N 67 22.758 E 032 29.667</t>
   </si>
 </sst>
 </file>
@@ -3777,6 +3813,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3789,9 +3826,72 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3831,69 +3931,6 @@
     <xf numFmtId="0" fontId="25" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3918,7 +3955,6 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -3957,7 +3993,7 @@
         <xdr:cNvPr id="4" name="Bilde 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3969,7 +4005,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3989,7 +4025,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -4018,7 +4054,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4067,7 +4103,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4112,7 +4148,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4157,7 +4193,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4195,7 +4231,7 @@
         <xdr:cNvPr id="3" name="image4.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4243,7 +4279,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4296,7 +4332,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4349,7 +4385,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4447,7 +4483,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4500,7 +4536,7 @@
         <xdr:cNvPr id="3" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4553,7 +4589,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4647,7 +4683,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4700,7 +4736,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4795,7 +4831,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4853,7 +4889,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4906,7 +4942,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4998,7 +5034,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5051,7 +5087,7 @@
         <xdr:cNvPr id="5" name="Bilde 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5281,10 +5317,10 @@
   <dimension ref="A1:K825"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I33" sqref="I33"/>
+      <selection pane="bottomRight" activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5304,15 +5340,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="178" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
+      <c r="B1" s="179"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="179"/>
+      <c r="G1" s="179"/>
       <c r="H1" s="160" t="s">
         <v>722</v>
       </c>
@@ -5325,10 +5361,10 @@
       <c r="K1" s="61"/>
     </row>
     <row r="2" spans="1:11" ht="35.25" thickBot="1">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="176" t="s">
         <v>493</v>
       </c>
-      <c r="B2" s="176"/>
+      <c r="B2" s="177"/>
       <c r="C2" s="104"/>
       <c r="D2" s="105"/>
       <c r="E2" s="106"/>
@@ -7217,7 +7253,7 @@
       <c r="I71" s="163" t="s">
         <v>494</v>
       </c>
-      <c r="J71" s="222"/>
+      <c r="J71" s="175"/>
       <c r="K71" s="61"/>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1">
@@ -7917,7 +7953,7 @@
       <c r="I95" s="162" t="s">
         <v>494</v>
       </c>
-      <c r="J95" s="222"/>
+      <c r="J95" s="175"/>
       <c r="K95" s="61" t="s">
         <v>782</v>
       </c>
@@ -7934,8 +7970,12 @@
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="41"/>
-      <c r="F96" s="61"/>
-      <c r="G96" s="152"/>
+      <c r="F96" s="61" t="s">
+        <v>808</v>
+      </c>
+      <c r="G96" s="152" t="s">
+        <v>809</v>
+      </c>
       <c r="H96" s="171" t="s">
         <v>734</v>
       </c>
@@ -8015,8 +8055,12 @@
       </c>
       <c r="D99" s="129"/>
       <c r="E99" s="132"/>
-      <c r="F99" s="139"/>
-      <c r="G99" s="130"/>
+      <c r="F99" s="139" t="s">
+        <v>806</v>
+      </c>
+      <c r="G99" s="130" t="s">
+        <v>807</v>
+      </c>
       <c r="H99" s="171" t="s">
         <v>734</v>
       </c>
@@ -8044,8 +8088,12 @@
       <c r="E100" s="41" t="s">
         <v>724</v>
       </c>
-      <c r="F100" s="61"/>
-      <c r="G100" s="152"/>
+      <c r="F100" s="61" t="s">
+        <v>813</v>
+      </c>
+      <c r="G100" s="152" t="s">
+        <v>814</v>
+      </c>
       <c r="H100" s="171" t="s">
         <v>734</v>
       </c>
@@ -8071,8 +8119,12 @@
       <c r="E101" s="132" t="s">
         <v>726</v>
       </c>
-      <c r="F101" s="139"/>
-      <c r="G101" s="151"/>
+      <c r="F101" s="139" t="s">
+        <v>817</v>
+      </c>
+      <c r="G101" s="151" t="s">
+        <v>816</v>
+      </c>
       <c r="H101" s="171" t="s">
         <v>734</v>
       </c>
@@ -8098,8 +8150,12 @@
       <c r="E102" s="41" t="s">
         <v>727</v>
       </c>
-      <c r="F102" s="61"/>
-      <c r="G102" s="152"/>
+      <c r="F102" s="61" t="s">
+        <v>815</v>
+      </c>
+      <c r="G102" s="152" t="s">
+        <v>158</v>
+      </c>
       <c r="H102" s="171" t="s">
         <v>734</v>
       </c>
@@ -9640,8 +9696,12 @@
       <c r="E204" s="140" t="s">
         <v>730</v>
       </c>
-      <c r="F204" s="139"/>
-      <c r="G204" s="155"/>
+      <c r="F204" s="139" t="s">
+        <v>811</v>
+      </c>
+      <c r="G204" s="155" t="s">
+        <v>812</v>
+      </c>
       <c r="H204" s="171" t="s">
         <v>734</v>
       </c>
@@ -9667,8 +9727,12 @@
       <c r="E205" s="7" t="s">
         <v>732</v>
       </c>
-      <c r="F205" s="7"/>
-      <c r="G205" s="156"/>
+      <c r="F205" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="G205" s="156" t="s">
+        <v>809</v>
+      </c>
       <c r="H205" s="171" t="s">
         <v>734</v>
       </c>
@@ -14595,50 +14659,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="202" t="s">
         <v>601</v>
       </c>
-      <c r="B1" s="181"/>
-      <c r="C1" s="181"/>
-      <c r="D1" s="181"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="181"/>
-      <c r="G1" s="181"/>
-      <c r="H1" s="181"/>
-      <c r="I1" s="182"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
+      <c r="I1" s="204"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="205" t="s">
         <v>602</v>
       </c>
-      <c r="B2" s="184"/>
+      <c r="B2" s="206"/>
       <c r="C2" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="D2" s="185" t="s">
+      <c r="D2" s="207" t="s">
         <v>603</v>
       </c>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="187"/>
-      <c r="H2" s="188" t="s">
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="209"/>
+      <c r="H2" s="210" t="s">
         <v>604</v>
       </c>
-      <c r="I2" s="189"/>
+      <c r="I2" s="211"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="190" t="s">
+      <c r="A4" s="212" t="s">
         <v>605</v>
       </c>
-      <c r="B4" s="191"/>
-      <c r="C4" s="191"/>
-      <c r="D4" s="191"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="191"/>
-      <c r="G4" s="191"/>
-      <c r="H4" s="191"/>
-      <c r="I4" s="192"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
+      <c r="H4" s="213"/>
+      <c r="I4" s="214"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="84" t="s">
@@ -14700,15 +14764,15 @@
       <c r="I6" s="89" t="s">
         <v>591</v>
       </c>
-      <c r="K6" s="179" t="s">
+      <c r="K6" s="196" t="s">
         <v>618</v>
       </c>
-      <c r="L6" s="179"/>
-      <c r="M6" s="179"/>
-      <c r="N6" s="179"/>
-      <c r="O6" s="179"/>
-      <c r="P6" s="179"/>
-      <c r="Q6" s="179"/>
+      <c r="L6" s="196"/>
+      <c r="M6" s="196"/>
+      <c r="N6" s="196"/>
+      <c r="O6" s="196"/>
+      <c r="P6" s="196"/>
+      <c r="Q6" s="196"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="87">
@@ -14738,15 +14802,15 @@
       <c r="I7" s="89" t="s">
         <v>588</v>
       </c>
-      <c r="K7" s="179" t="s">
+      <c r="K7" s="196" t="s">
         <v>626</v>
       </c>
-      <c r="L7" s="179"/>
-      <c r="M7" s="179"/>
-      <c r="N7" s="179"/>
-      <c r="O7" s="179"/>
-      <c r="P7" s="179"/>
-      <c r="Q7" s="179"/>
+      <c r="L7" s="196"/>
+      <c r="M7" s="196"/>
+      <c r="N7" s="196"/>
+      <c r="O7" s="196"/>
+      <c r="P7" s="196"/>
+      <c r="Q7" s="196"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="87">
@@ -14854,17 +14918,17 @@
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="193" t="s">
+      <c r="A15" s="197" t="s">
         <v>634</v>
       </c>
-      <c r="B15" s="194"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="194"/>
-      <c r="E15" s="194"/>
-      <c r="F15" s="194"/>
-      <c r="G15" s="194"/>
-      <c r="H15" s="194"/>
-      <c r="I15" s="195"/>
+      <c r="B15" s="198"/>
+      <c r="C15" s="198"/>
+      <c r="D15" s="198"/>
+      <c r="E15" s="198"/>
+      <c r="F15" s="198"/>
+      <c r="G15" s="198"/>
+      <c r="H15" s="198"/>
+      <c r="I15" s="199"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="84" t="s">
@@ -14879,15 +14943,15 @@
       <c r="D16" s="85" t="s">
         <v>586</v>
       </c>
-      <c r="E16" s="196" t="s">
+      <c r="E16" s="200" t="s">
         <v>635</v>
       </c>
-      <c r="F16" s="196"/>
-      <c r="G16" s="196" t="s">
+      <c r="F16" s="200"/>
+      <c r="G16" s="200" t="s">
         <v>636</v>
       </c>
-      <c r="H16" s="196"/>
-      <c r="I16" s="197"/>
+      <c r="H16" s="200"/>
+      <c r="I16" s="201"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="93">
@@ -14902,15 +14966,15 @@
       <c r="D17" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E17" s="198" t="s">
+      <c r="E17" s="192" t="s">
         <v>638</v>
       </c>
-      <c r="F17" s="199"/>
-      <c r="G17" s="198" t="s">
+      <c r="F17" s="193"/>
+      <c r="G17" s="192" t="s">
         <v>639</v>
       </c>
-      <c r="H17" s="200"/>
-      <c r="I17" s="201"/>
+      <c r="H17" s="194"/>
+      <c r="I17" s="195"/>
     </row>
     <row r="18" spans="1:11" ht="22.5">
       <c r="A18" s="93">
@@ -14925,15 +14989,15 @@
       <c r="D18" s="88" t="s">
         <v>594</v>
       </c>
-      <c r="E18" s="198" t="s">
+      <c r="E18" s="192" t="s">
         <v>638</v>
       </c>
-      <c r="F18" s="199"/>
-      <c r="G18" s="198" t="s">
+      <c r="F18" s="193"/>
+      <c r="G18" s="192" t="s">
         <v>641</v>
       </c>
-      <c r="H18" s="200"/>
-      <c r="I18" s="201"/>
+      <c r="H18" s="194"/>
+      <c r="I18" s="195"/>
     </row>
     <row r="19" spans="1:11" ht="33.75">
       <c r="A19" s="93">
@@ -14948,15 +15012,15 @@
       <c r="D19" s="88" t="s">
         <v>597</v>
       </c>
-      <c r="E19" s="198" t="s">
+      <c r="E19" s="192" t="s">
         <v>643</v>
       </c>
-      <c r="F19" s="199"/>
-      <c r="G19" s="198" t="s">
+      <c r="F19" s="193"/>
+      <c r="G19" s="192" t="s">
         <v>644</v>
       </c>
-      <c r="H19" s="200"/>
-      <c r="I19" s="201"/>
+      <c r="H19" s="194"/>
+      <c r="I19" s="195"/>
       <c r="K19" t="s">
         <v>645</v>
       </c>
@@ -14968,11 +15032,11 @@
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
-      <c r="E20" s="202"/>
-      <c r="F20" s="203"/>
-      <c r="G20" s="202"/>
-      <c r="H20" s="204"/>
-      <c r="I20" s="205"/>
+      <c r="E20" s="180"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="180"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="183"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="93">
@@ -14981,11 +15045,11 @@
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="78"/>
-      <c r="E21" s="202"/>
-      <c r="F21" s="203"/>
-      <c r="G21" s="202"/>
-      <c r="H21" s="204"/>
-      <c r="I21" s="205"/>
+      <c r="E21" s="180"/>
+      <c r="F21" s="181"/>
+      <c r="G21" s="180"/>
+      <c r="H21" s="182"/>
+      <c r="I21" s="183"/>
       <c r="K21" t="s">
         <v>646</v>
       </c>
@@ -14997,11 +15061,11 @@
       <c r="B22" s="78"/>
       <c r="C22" s="78"/>
       <c r="D22" s="78"/>
-      <c r="E22" s="202"/>
-      <c r="F22" s="203"/>
-      <c r="G22" s="202"/>
-      <c r="H22" s="204"/>
-      <c r="I22" s="205"/>
+      <c r="E22" s="180"/>
+      <c r="F22" s="181"/>
+      <c r="G22" s="180"/>
+      <c r="H22" s="182"/>
+      <c r="I22" s="183"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="93">
@@ -15010,11 +15074,11 @@
       <c r="B23" s="78"/>
       <c r="C23" s="78"/>
       <c r="D23" s="78"/>
-      <c r="E23" s="202"/>
-      <c r="F23" s="203"/>
-      <c r="G23" s="202"/>
-      <c r="H23" s="204"/>
-      <c r="I23" s="205"/>
+      <c r="E23" s="180"/>
+      <c r="F23" s="181"/>
+      <c r="G23" s="180"/>
+      <c r="H23" s="182"/>
+      <c r="I23" s="183"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="93">
@@ -15023,11 +15087,11 @@
       <c r="B24" s="78"/>
       <c r="C24" s="78"/>
       <c r="D24" s="78"/>
-      <c r="E24" s="202"/>
-      <c r="F24" s="203"/>
-      <c r="G24" s="202"/>
-      <c r="H24" s="204"/>
-      <c r="I24" s="205"/>
+      <c r="E24" s="180"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="182"/>
+      <c r="I24" s="183"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="93">
@@ -15036,11 +15100,11 @@
       <c r="B25" s="94"/>
       <c r="C25" s="94"/>
       <c r="D25" s="94"/>
-      <c r="E25" s="206"/>
-      <c r="F25" s="207"/>
-      <c r="G25" s="206"/>
-      <c r="H25" s="208"/>
-      <c r="I25" s="209"/>
+      <c r="E25" s="184"/>
+      <c r="F25" s="185"/>
+      <c r="G25" s="184"/>
+      <c r="H25" s="186"/>
+      <c r="I25" s="187"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1">
       <c r="A26" s="95">
@@ -15049,44 +15113,44 @@
       <c r="B26" s="91"/>
       <c r="C26" s="91"/>
       <c r="D26" s="91"/>
-      <c r="E26" s="210"/>
-      <c r="F26" s="211"/>
-      <c r="G26" s="210"/>
-      <c r="H26" s="212"/>
-      <c r="I26" s="213"/>
+      <c r="E26" s="188"/>
+      <c r="F26" s="189"/>
+      <c r="G26" s="188"/>
+      <c r="H26" s="190"/>
+      <c r="I26" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15132,11 +15196,11 @@
       <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A2" s="214" t="s">
+      <c r="A2" s="215" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="215"/>
-      <c r="C2" s="215"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
       <c r="F2" s="22"/>
@@ -15254,10 +15318,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="217" t="s">
         <v>509</v>
       </c>
-      <c r="C2" s="216"/>
+      <c r="C2" s="217"/>
       <c r="O2" t="s">
         <v>510</v>
       </c>
@@ -15497,56 +15561,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="216" t="s">
+      <c r="A3" s="217" t="s">
         <v>542</v>
       </c>
-      <c r="B3" s="216"/>
-      <c r="C3" s="216"/>
+      <c r="B3" s="217"/>
+      <c r="C3" s="217"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="62" t="s">
         <v>543</v>
       </c>
-      <c r="B4" s="218" t="s">
+      <c r="B4" s="219" t="s">
         <v>544</v>
       </c>
-      <c r="C4" s="218"/>
+      <c r="C4" s="219"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="63" t="s">
         <v>545</v>
       </c>
-      <c r="B5" s="217" t="s">
+      <c r="B5" s="218" t="s">
         <v>546</v>
       </c>
-      <c r="C5" s="217"/>
+      <c r="C5" s="218"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="63" t="s">
         <v>547</v>
       </c>
-      <c r="B6" s="217" t="s">
+      <c r="B6" s="218" t="s">
         <v>548</v>
       </c>
-      <c r="C6" s="217"/>
+      <c r="C6" s="218"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="217" t="s">
+      <c r="B7" s="218" t="s">
         <v>549</v>
       </c>
-      <c r="C7" s="217"/>
+      <c r="C7" s="218"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="63" t="s">
         <v>550</v>
       </c>
-      <c r="B8" s="217" t="s">
+      <c r="B8" s="218" t="s">
         <v>551</v>
       </c>
-      <c r="C8" s="217"/>
+      <c r="C8" s="218"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -15579,11 +15643,11 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1"/>
     <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="219" t="s">
+      <c r="B2" s="220" t="s">
         <v>552</v>
       </c>
-      <c r="C2" s="220"/>
-      <c r="D2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="222"/>
       <c r="J2" t="s">
         <v>510</v>
       </c>
@@ -15761,11 +15825,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15">
-      <c r="A5" s="218" t="s">
+      <c r="A5" s="219" t="s">
         <v>585</v>
       </c>
-      <c r="B5" s="218"/>
-      <c r="C5" s="218"/>
+      <c r="B5" s="219"/>
+      <c r="C5" s="219"/>
     </row>
     <row r="6" spans="1:10" ht="15">
       <c r="A6" s="62" t="s">

</xml_diff>

<commit_message>
chg: Further refinement and adjusted DPIs in OPAC.miz, descriptions on targets in "NOtias as candidate for air attack".
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -19,14 +19,14 @@
   <calcPr calcId="124519"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="jqvuzJn8Lf/XHWAhwIuz09YQ2YQAYUhN1DjVsFh9M+Q="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="" roundtripDataChecksum="jqvuzJn8Lf/XHWAhwIuz09YQ2YQAYUhN1DjVsFh9M+Q="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="823">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -1105,9 +1105,6 @@
     <t>Main Metallurgy Plant</t>
   </si>
   <si>
-    <t>Basic industry</t>
-  </si>
-  <si>
     <t>N 69 00.150 E 033 07.336</t>
   </si>
   <si>
@@ -1144,16 +1141,10 @@
     <t>Tuloma Powerplant</t>
   </si>
   <si>
-    <t>Coal Powerplant</t>
-  </si>
-  <si>
     <t>N 68 48.803 E 032 41.408</t>
   </si>
   <si>
     <t>SRNTGT088</t>
-  </si>
-  <si>
-    <t>ARMY Fuel Storage (2ns Corps)</t>
   </si>
   <si>
     <t>N 69 26.053 E 030 54.534</t>
@@ -2510,6 +2501,24 @@
   </si>
   <si>
     <t>Defense against WMD (weapons of mass destruction), where consequences of failure unaceptable.</t>
+  </si>
+  <si>
+    <t>ARMY Fuel Storage (2nd Corps)</t>
+  </si>
+  <si>
+    <t>Powerplant that supports Murmansk International airport</t>
+  </si>
+  <si>
+    <t>Storage for rocket propellant for SCUDs and precursor chemicals for chemical weapons</t>
+  </si>
+  <si>
+    <t>Mixing of precursor chemicals into chemical weapon warhead</t>
+  </si>
+  <si>
+    <t>Production of chemical weapon warhead</t>
+  </si>
+  <si>
+    <t>Provides metal to most of Notias vehicle factories</t>
   </si>
 </sst>
 </file>
@@ -2519,7 +2528,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999]0000;General"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2661,6 +2670,18 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -3237,7 +3258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3615,25 +3636,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3647,17 +3663,22 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3666,14 +3687,26 @@
     <xf numFmtId="0" fontId="23" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4932,10 +4965,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomRight" activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5592,7 +5625,7 @@
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
@@ -5623,7 +5656,7 @@
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
@@ -5654,7 +5687,7 @@
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
@@ -5677,10 +5710,12 @@
       <c r="G25" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="8"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
@@ -5707,7 +5742,9 @@
       <c r="H26" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="8"/>
+      <c r="I26" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
@@ -6595,7 +6632,7 @@
       <c r="H54" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I54" s="23" t="s">
+      <c r="I54" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J54" s="2"/>
@@ -6629,7 +6666,7 @@
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
@@ -7510,19 +7547,19 @@
         <v>10</v>
       </c>
       <c r="D87" s="27"/>
-      <c r="E87" s="28" t="s">
+      <c r="E87" s="178" t="s">
+        <v>822</v>
+      </c>
+      <c r="F87" s="24" t="s">
         <v>359</v>
-      </c>
-      <c r="F87" s="24" t="s">
-        <v>360</v>
       </c>
       <c r="G87" s="28">
         <v>200</v>
       </c>
-      <c r="H87" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I87" s="23" t="s">
+      <c r="H87" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I87" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J87" s="2"/>
@@ -7530,28 +7567,28 @@
     </row>
     <row r="88" spans="1:11" ht="15.75" customHeight="1">
       <c r="A88" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B88" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="B88" s="29" t="s">
+      <c r="C88" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="C88" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="D88" s="30"/>
       <c r="E88" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="G88" s="31">
         <v>330</v>
       </c>
-      <c r="H88" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I88" s="23" t="s">
+      <c r="H88" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I88" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J88" s="2"/>
@@ -7559,26 +7596,26 @@
     </row>
     <row r="89" spans="1:11" ht="15.75" customHeight="1">
       <c r="A89" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="B89" s="25" t="s">
         <v>366</v>
-      </c>
-      <c r="B89" s="25" t="s">
-        <v>367</v>
       </c>
       <c r="C89" s="26">
         <v>7</v>
       </c>
       <c r="D89" s="27"/>
       <c r="E89" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="F89" s="24" t="s">
         <v>368</v>
-      </c>
-      <c r="F89" s="24" t="s">
-        <v>369</v>
       </c>
       <c r="G89" s="28">
         <v>1</v>
       </c>
-      <c r="H89" s="22" t="s">
-        <v>22</v>
+      <c r="H89" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="I89" s="22" t="s">
         <v>22</v>
@@ -7588,28 +7625,28 @@
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1">
       <c r="A90" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B90" s="29" t="s">
         <v>370</v>
       </c>
-      <c r="B90" s="29" t="s">
-        <v>371</v>
-      </c>
       <c r="C90" s="32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="20" t="s">
-        <v>372</v>
+        <v>818</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G90" s="31">
         <v>109</v>
       </c>
-      <c r="H90" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I90" s="23" t="s">
+      <c r="H90" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I90" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J90" s="2"/>
@@ -7617,28 +7654,28 @@
     </row>
     <row r="91" spans="1:11" ht="15.75" customHeight="1">
       <c r="A91" s="24" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>375</v>
+        <v>817</v>
       </c>
       <c r="C91" s="26">
         <v>9</v>
       </c>
       <c r="D91" s="27"/>
       <c r="E91" s="25" t="s">
-        <v>375</v>
+        <v>817</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G91" s="28">
         <v>286</v>
       </c>
-      <c r="H91" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I91" s="23" t="s">
+      <c r="H91" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I91" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J91" s="2"/>
@@ -7646,20 +7683,20 @@
     </row>
     <row r="92" spans="1:11" ht="15.75" customHeight="1">
       <c r="A92" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B92" s="29" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C92" s="32">
         <v>6</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="20" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G92" s="31">
         <v>873</v>
@@ -7667,7 +7704,7 @@
       <c r="H92" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="I92" s="23" t="s">
+      <c r="I92" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J92" s="2"/>
@@ -7677,28 +7714,28 @@
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1">
       <c r="A93" s="24" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B93" s="52" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C93" s="26">
         <v>11</v>
       </c>
       <c r="D93" s="27"/>
       <c r="E93" s="28" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F93" s="24" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G93" s="28">
         <v>230</v>
       </c>
-      <c r="H93" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I93" s="23" t="s">
+      <c r="H93" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I93" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J93" s="2"/>
@@ -7706,20 +7743,20 @@
     </row>
     <row r="94" spans="1:11" ht="15.75" customHeight="1">
       <c r="A94" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B94" s="53" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C94" s="54">
         <v>9</v>
       </c>
       <c r="D94" s="55"/>
       <c r="E94" s="56" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="F94" s="57" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G94" s="58">
         <v>882</v>
@@ -7737,20 +7774,20 @@
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1">
       <c r="A95" s="24" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C95" s="26">
         <v>9</v>
       </c>
       <c r="D95" s="27"/>
       <c r="E95" s="59" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F95" s="24" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G95" s="28">
         <v>479</v>
@@ -7768,21 +7805,23 @@
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1">
       <c r="A96" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B96" s="29" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C96" s="32">
         <v>1</v>
       </c>
       <c r="D96" s="30"/>
-      <c r="E96" s="60"/>
+      <c r="E96" s="177" t="s">
+        <v>821</v>
+      </c>
       <c r="F96" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G96" s="31" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H96" s="33" t="s">
         <v>66</v>
@@ -7795,21 +7834,23 @@
     </row>
     <row r="97" spans="1:11" ht="15.75" customHeight="1">
       <c r="A97" s="24" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C97" s="26">
         <v>1</v>
       </c>
       <c r="D97" s="27"/>
-      <c r="E97" s="59"/>
+      <c r="E97" s="176" t="s">
+        <v>820</v>
+      </c>
       <c r="F97" s="24" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G97" s="28" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H97" s="33" t="s">
         <v>66</v>
@@ -7824,23 +7865,23 @@
     </row>
     <row r="98" spans="1:11" ht="15.75" customHeight="1">
       <c r="A98" s="2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B98" s="29" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C98" s="32">
         <v>7</v>
       </c>
       <c r="D98" s="30"/>
       <c r="E98" s="60" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G98" s="31" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H98" s="33" t="s">
         <v>66</v>
@@ -7850,26 +7891,28 @@
       </c>
       <c r="J98" s="2"/>
       <c r="K98" s="61" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="99" spans="1:11" ht="15.75" customHeight="1">
       <c r="A99" s="24" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C99" s="26">
         <v>7</v>
       </c>
       <c r="D99" s="27"/>
-      <c r="E99" s="59"/>
+      <c r="E99" s="175" t="s">
+        <v>819</v>
+      </c>
       <c r="F99" s="24" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G99" s="28" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="H99" s="33" t="s">
         <v>66</v>
@@ -7881,28 +7924,28 @@
         <v>66</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="15.75" customHeight="1">
       <c r="A100" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B100" s="29" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C100" s="32">
         <v>9</v>
       </c>
       <c r="D100" s="30"/>
       <c r="E100" s="60" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G100" s="31" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H100" s="33" t="s">
         <v>66</v>
@@ -7917,23 +7960,23 @@
     </row>
     <row r="101" spans="1:11" ht="15.75" customHeight="1">
       <c r="A101" s="24" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C101" s="26">
         <v>9</v>
       </c>
       <c r="D101" s="27"/>
       <c r="E101" s="59" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F101" s="24" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G101" s="28" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H101" s="33" t="s">
         <v>66</v>
@@ -7948,20 +7991,20 @@
     </row>
     <row r="102" spans="1:11" ht="15.75" customHeight="1">
       <c r="A102" s="2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B102" s="29" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C102" s="32">
         <v>9</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="60" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G102" s="31" t="s">
         <v>201</v>
@@ -7974,12 +8017,12 @@
       </c>
       <c r="J102" s="2"/>
       <c r="K102" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A103" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B103" s="50"/>
       <c r="C103" s="62"/>
@@ -7994,7 +8037,7 @@
     </row>
     <row r="104" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A104" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B104" s="29"/>
       <c r="C104" s="32"/>
@@ -8009,7 +8052,7 @@
     </row>
     <row r="105" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A105" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B105" s="50"/>
       <c r="C105" s="62"/>
@@ -8024,7 +8067,7 @@
     </row>
     <row r="106" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A106" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B106" s="29"/>
       <c r="C106" s="32"/>
@@ -8039,7 +8082,7 @@
     </row>
     <row r="107" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A107" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B107" s="50"/>
       <c r="C107" s="62"/>
@@ -8054,7 +8097,7 @@
     </row>
     <row r="108" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A108" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B108" s="29"/>
       <c r="C108" s="32"/>
@@ -8069,7 +8112,7 @@
     </row>
     <row r="109" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A109" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B109" s="50"/>
       <c r="C109" s="62"/>
@@ -8084,7 +8127,7 @@
     </row>
     <row r="110" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B110" s="29"/>
       <c r="C110" s="32"/>
@@ -8099,7 +8142,7 @@
     </row>
     <row r="111" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A111" s="2" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B111" s="50"/>
       <c r="C111" s="62"/>
@@ -8114,7 +8157,7 @@
     </row>
     <row r="112" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A112" s="2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B112" s="29"/>
       <c r="C112" s="32"/>
@@ -8129,7 +8172,7 @@
     </row>
     <row r="113" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A113" s="2" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B113" s="50"/>
       <c r="C113" s="62"/>
@@ -8144,7 +8187,7 @@
     </row>
     <row r="114" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A114" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B114" s="29"/>
       <c r="C114" s="32"/>
@@ -8159,7 +8202,7 @@
     </row>
     <row r="115" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A115" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B115" s="50"/>
       <c r="C115" s="62"/>
@@ -8174,7 +8217,7 @@
     </row>
     <row r="116" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B116" s="29"/>
       <c r="C116" s="32"/>
@@ -8189,7 +8232,7 @@
     </row>
     <row r="117" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A117" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B117" s="50"/>
       <c r="C117" s="62"/>
@@ -8204,7 +8247,7 @@
     </row>
     <row r="118" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A118" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B118" s="29"/>
       <c r="C118" s="32"/>
@@ -8219,7 +8262,7 @@
     </row>
     <row r="119" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B119" s="50"/>
       <c r="C119" s="62"/>
@@ -8234,7 +8277,7 @@
     </row>
     <row r="120" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A120" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B120" s="29"/>
       <c r="C120" s="32"/>
@@ -8249,7 +8292,7 @@
     </row>
     <row r="121" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A121" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B121" s="50"/>
       <c r="C121" s="62"/>
@@ -8264,7 +8307,7 @@
     </row>
     <row r="122" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A122" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B122" s="29"/>
       <c r="C122" s="32"/>
@@ -8279,7 +8322,7 @@
     </row>
     <row r="123" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A123" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B123" s="50"/>
       <c r="C123" s="62"/>
@@ -8294,7 +8337,7 @@
     </row>
     <row r="124" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A124" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B124" s="29"/>
       <c r="C124" s="32"/>
@@ -8309,7 +8352,7 @@
     </row>
     <row r="125" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A125" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B125" s="50"/>
       <c r="C125" s="62"/>
@@ -8324,7 +8367,7 @@
     </row>
     <row r="126" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A126" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B126" s="29"/>
       <c r="C126" s="32"/>
@@ -8339,7 +8382,7 @@
     </row>
     <row r="127" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A127" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B127" s="50"/>
       <c r="C127" s="62"/>
@@ -8354,7 +8397,7 @@
     </row>
     <row r="128" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A128" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B128" s="29"/>
       <c r="C128" s="32"/>
@@ -8369,7 +8412,7 @@
     </row>
     <row r="129" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A129" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B129" s="50"/>
       <c r="C129" s="62"/>
@@ -8384,7 +8427,7 @@
     </row>
     <row r="130" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A130" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B130" s="29"/>
       <c r="C130" s="32"/>
@@ -8399,7 +8442,7 @@
     </row>
     <row r="131" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A131" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B131" s="50"/>
       <c r="C131" s="62"/>
@@ -8414,7 +8457,7 @@
     </row>
     <row r="132" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A132" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B132" s="29"/>
       <c r="C132" s="32"/>
@@ -8429,7 +8472,7 @@
     </row>
     <row r="133" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A133" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B133" s="50"/>
       <c r="C133" s="62"/>
@@ -8444,7 +8487,7 @@
     </row>
     <row r="134" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A134" s="2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B134" s="29"/>
       <c r="C134" s="32"/>
@@ -8459,7 +8502,7 @@
     </row>
     <row r="135" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A135" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B135" s="50"/>
       <c r="C135" s="62"/>
@@ -8474,7 +8517,7 @@
     </row>
     <row r="136" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A136" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B136" s="29"/>
       <c r="C136" s="32"/>
@@ -8489,7 +8532,7 @@
     </row>
     <row r="137" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A137" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B137" s="50"/>
       <c r="C137" s="62"/>
@@ -8504,7 +8547,7 @@
     </row>
     <row r="138" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A138" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B138" s="29"/>
       <c r="C138" s="32"/>
@@ -8519,7 +8562,7 @@
     </row>
     <row r="139" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A139" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B139" s="50"/>
       <c r="C139" s="62"/>
@@ -8534,7 +8577,7 @@
     </row>
     <row r="140" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A140" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B140" s="29"/>
       <c r="C140" s="32"/>
@@ -8549,7 +8592,7 @@
     </row>
     <row r="141" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A141" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B141" s="50"/>
       <c r="C141" s="62"/>
@@ -8564,7 +8607,7 @@
     </row>
     <row r="142" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A142" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B142" s="29"/>
       <c r="C142" s="32"/>
@@ -8579,7 +8622,7 @@
     </row>
     <row r="143" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A143" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B143" s="50"/>
       <c r="C143" s="62"/>
@@ -8594,7 +8637,7 @@
     </row>
     <row r="144" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A144" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B144" s="29"/>
       <c r="C144" s="32"/>
@@ -8609,7 +8652,7 @@
     </row>
     <row r="145" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A145" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B145" s="50"/>
       <c r="C145" s="62"/>
@@ -8624,7 +8667,7 @@
     </row>
     <row r="146" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A146" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B146" s="29"/>
       <c r="C146" s="32"/>
@@ -8639,7 +8682,7 @@
     </row>
     <row r="147" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A147" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B147" s="50"/>
       <c r="C147" s="62"/>
@@ -8654,7 +8697,7 @@
     </row>
     <row r="148" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A148" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B148" s="29"/>
       <c r="C148" s="32"/>
@@ -8669,7 +8712,7 @@
     </row>
     <row r="149" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A149" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B149" s="50"/>
       <c r="C149" s="62"/>
@@ -8684,7 +8727,7 @@
     </row>
     <row r="150" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A150" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B150" s="29"/>
       <c r="C150" s="32"/>
@@ -8699,7 +8742,7 @@
     </row>
     <row r="151" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A151" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B151" s="50"/>
       <c r="C151" s="62"/>
@@ -8714,7 +8757,7 @@
     </row>
     <row r="152" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A152" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B152" s="29"/>
       <c r="C152" s="32"/>
@@ -8729,7 +8772,7 @@
     </row>
     <row r="153" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A153" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B153" s="50"/>
       <c r="C153" s="62"/>
@@ -8744,7 +8787,7 @@
     </row>
     <row r="154" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A154" s="2" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B154" s="29"/>
       <c r="C154" s="32"/>
@@ -8759,7 +8802,7 @@
     </row>
     <row r="155" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A155" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B155" s="50"/>
       <c r="C155" s="62"/>
@@ -8774,7 +8817,7 @@
     </row>
     <row r="156" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A156" s="2" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B156" s="29"/>
       <c r="C156" s="32"/>
@@ -8789,7 +8832,7 @@
     </row>
     <row r="157" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A157" s="2" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B157" s="50"/>
       <c r="C157" s="62"/>
@@ -8804,7 +8847,7 @@
     </row>
     <row r="158" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A158" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B158" s="29"/>
       <c r="C158" s="32"/>
@@ -8819,7 +8862,7 @@
     </row>
     <row r="159" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A159" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B159" s="50"/>
       <c r="C159" s="62"/>
@@ -8834,7 +8877,7 @@
     </row>
     <row r="160" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A160" s="2" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B160" s="29"/>
       <c r="C160" s="32"/>
@@ -8849,7 +8892,7 @@
     </row>
     <row r="161" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A161" s="2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B161" s="50"/>
       <c r="C161" s="62"/>
@@ -8864,7 +8907,7 @@
     </row>
     <row r="162" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A162" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B162" s="29"/>
       <c r="C162" s="32"/>
@@ -8879,7 +8922,7 @@
     </row>
     <row r="163" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A163" s="2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B163" s="50"/>
       <c r="C163" s="62"/>
@@ -8894,7 +8937,7 @@
     </row>
     <row r="164" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A164" s="2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B164" s="29"/>
       <c r="C164" s="32"/>
@@ -8909,7 +8952,7 @@
     </row>
     <row r="165" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A165" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B165" s="50"/>
       <c r="C165" s="62"/>
@@ -8924,7 +8967,7 @@
     </row>
     <row r="166" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A166" s="2" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B166" s="29"/>
       <c r="C166" s="32"/>
@@ -8939,7 +8982,7 @@
     </row>
     <row r="167" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A167" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B167" s="50"/>
       <c r="C167" s="62"/>
@@ -8954,7 +8997,7 @@
     </row>
     <row r="168" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A168" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B168" s="29"/>
       <c r="C168" s="32"/>
@@ -8969,7 +9012,7 @@
     </row>
     <row r="169" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A169" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B169" s="50"/>
       <c r="C169" s="62"/>
@@ -8984,7 +9027,7 @@
     </row>
     <row r="170" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A170" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B170" s="29"/>
       <c r="C170" s="32"/>
@@ -8999,7 +9042,7 @@
     </row>
     <row r="171" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A171" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B171" s="50"/>
       <c r="C171" s="62"/>
@@ -9014,7 +9057,7 @@
     </row>
     <row r="172" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A172" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B172" s="29"/>
       <c r="C172" s="32"/>
@@ -9029,7 +9072,7 @@
     </row>
     <row r="173" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A173" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B173" s="50"/>
       <c r="C173" s="62"/>
@@ -9044,7 +9087,7 @@
     </row>
     <row r="174" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A174" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B174" s="29"/>
       <c r="C174" s="32"/>
@@ -9059,7 +9102,7 @@
     </row>
     <row r="175" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A175" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B175" s="50"/>
       <c r="C175" s="62"/>
@@ -9074,7 +9117,7 @@
     </row>
     <row r="176" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A176" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B176" s="29"/>
       <c r="C176" s="32"/>
@@ -9089,7 +9132,7 @@
     </row>
     <row r="177" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A177" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B177" s="50"/>
       <c r="C177" s="62"/>
@@ -9104,7 +9147,7 @@
     </row>
     <row r="178" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A178" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B178" s="29"/>
       <c r="C178" s="32"/>
@@ -9119,7 +9162,7 @@
     </row>
     <row r="179" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A179" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B179" s="50"/>
       <c r="C179" s="62"/>
@@ -9134,7 +9177,7 @@
     </row>
     <row r="180" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A180" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B180" s="29"/>
       <c r="C180" s="32"/>
@@ -9149,7 +9192,7 @@
     </row>
     <row r="181" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A181" s="2" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B181" s="50"/>
       <c r="C181" s="62"/>
@@ -9164,7 +9207,7 @@
     </row>
     <row r="182" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A182" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B182" s="29"/>
       <c r="C182" s="32"/>
@@ -9179,7 +9222,7 @@
     </row>
     <row r="183" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A183" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B183" s="50"/>
       <c r="C183" s="62"/>
@@ -9194,7 +9237,7 @@
     </row>
     <row r="184" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A184" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B184" s="29"/>
       <c r="C184" s="32"/>
@@ -9209,7 +9252,7 @@
     </row>
     <row r="185" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A185" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B185" s="50"/>
       <c r="C185" s="62"/>
@@ -9224,7 +9267,7 @@
     </row>
     <row r="186" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A186" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B186" s="29"/>
       <c r="C186" s="32"/>
@@ -9239,7 +9282,7 @@
     </row>
     <row r="187" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A187" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B187" s="50"/>
       <c r="C187" s="62"/>
@@ -9254,7 +9297,7 @@
     </row>
     <row r="188" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A188" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B188" s="29"/>
       <c r="C188" s="32"/>
@@ -9269,7 +9312,7 @@
     </row>
     <row r="189" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A189" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B189" s="50"/>
       <c r="C189" s="62"/>
@@ -9284,7 +9327,7 @@
     </row>
     <row r="190" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A190" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B190" s="29"/>
       <c r="C190" s="32"/>
@@ -9299,7 +9342,7 @@
     </row>
     <row r="191" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A191" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B191" s="50"/>
       <c r="C191" s="62"/>
@@ -9314,7 +9357,7 @@
     </row>
     <row r="192" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A192" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B192" s="29"/>
       <c r="C192" s="32"/>
@@ -9329,7 +9372,7 @@
     </row>
     <row r="193" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A193" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B193" s="50"/>
       <c r="C193" s="62"/>
@@ -9344,7 +9387,7 @@
     </row>
     <row r="194" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A194" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B194" s="29"/>
       <c r="C194" s="32"/>
@@ -9359,7 +9402,7 @@
     </row>
     <row r="195" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A195" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B195" s="50"/>
       <c r="C195" s="62"/>
@@ -9374,7 +9417,7 @@
     </row>
     <row r="196" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A196" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B196" s="29"/>
       <c r="C196" s="32"/>
@@ -9389,7 +9432,7 @@
     </row>
     <row r="197" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A197" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B197" s="50"/>
       <c r="C197" s="62"/>
@@ -9404,7 +9447,7 @@
     </row>
     <row r="198" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A198" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B198" s="29"/>
       <c r="C198" s="32"/>
@@ -9419,7 +9462,7 @@
     </row>
     <row r="199" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A199" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B199" s="50"/>
       <c r="C199" s="62"/>
@@ -9434,7 +9477,7 @@
     </row>
     <row r="200" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A200" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B200" s="29"/>
       <c r="C200" s="32"/>
@@ -9449,7 +9492,7 @@
     </row>
     <row r="201" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A201" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B201" s="50"/>
       <c r="C201" s="62"/>
@@ -9464,7 +9507,7 @@
     </row>
     <row r="202" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A202" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B202" s="29"/>
       <c r="C202" s="32"/>
@@ -9479,7 +9522,7 @@
     </row>
     <row r="203" spans="1:11" ht="15.75" hidden="1" customHeight="1">
       <c r="A203" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B203" s="50"/>
       <c r="C203" s="62"/>
@@ -9494,23 +9537,23 @@
     </row>
     <row r="204" spans="1:11" ht="15.75" customHeight="1">
       <c r="A204" s="24" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B204" s="25" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C204" s="26">
         <v>9</v>
       </c>
       <c r="D204" s="24"/>
       <c r="E204" s="65" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F204" s="24" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="G204" s="66" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H204" s="33" t="s">
         <v>66</v>
@@ -9520,28 +9563,28 @@
       </c>
       <c r="J204" s="2"/>
       <c r="K204" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="205" spans="1:11" ht="15.75" customHeight="1">
       <c r="A205" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B205" s="29" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C205" s="32">
         <v>9</v>
       </c>
       <c r="D205" s="29"/>
       <c r="E205" s="29" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F205" s="29" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G205" s="67" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H205" s="33" t="s">
         <v>66</v>
@@ -9551,28 +9594,28 @@
       </c>
       <c r="J205" s="2"/>
       <c r="K205" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="206" spans="1:11" ht="15.75" customHeight="1">
       <c r="A206" s="24" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B206" s="25" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C206" s="68">
         <v>9</v>
       </c>
       <c r="D206" s="25"/>
       <c r="E206" s="25" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F206" s="25" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="G206" s="69" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="H206" s="33" t="s">
         <v>66</v>
@@ -9582,28 +9625,28 @@
       </c>
       <c r="J206" s="2"/>
       <c r="K206" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="207" spans="1:11" ht="15.75" customHeight="1">
       <c r="A207" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B207" s="70" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C207" s="71">
         <v>9</v>
       </c>
       <c r="D207" s="70"/>
       <c r="E207" s="70" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F207" s="70" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G207" s="72" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="H207" s="33" t="s">
         <v>66</v>
@@ -9613,28 +9656,28 @@
       </c>
       <c r="J207" s="2"/>
       <c r="K207" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="208" spans="1:11" ht="15.75" customHeight="1">
       <c r="A208" s="24" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B208" s="73" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C208" s="74">
         <v>11</v>
       </c>
       <c r="D208" s="73"/>
       <c r="E208" s="73" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F208" s="73" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="G208" s="75" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="H208" s="33" t="s">
         <v>66</v>
@@ -9644,28 +9687,28 @@
       </c>
       <c r="J208" s="2"/>
       <c r="K208" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="209" spans="1:11" ht="15.75" customHeight="1">
       <c r="A209" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B209" s="70" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C209" s="71">
         <v>11</v>
       </c>
       <c r="D209" s="70"/>
       <c r="E209" s="70" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F209" s="70" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="G209" s="72" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="H209" s="33" t="s">
         <v>66</v>
@@ -9675,28 +9718,28 @@
       </c>
       <c r="J209" s="2"/>
       <c r="K209" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="210" spans="1:11" ht="15.75" customHeight="1">
       <c r="A210" s="24" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B210" s="73" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C210" s="74">
         <v>2</v>
       </c>
       <c r="D210" s="73"/>
       <c r="E210" s="73" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F210" s="73" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="G210" s="75" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="H210" s="33" t="s">
         <v>66</v>
@@ -9706,22 +9749,22 @@
       </c>
       <c r="J210" s="2"/>
       <c r="K210" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="211" spans="1:11" ht="15.75" customHeight="1">
       <c r="A211" s="2" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B211" s="70" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C211" s="71">
         <v>4</v>
       </c>
       <c r="D211" s="70"/>
       <c r="E211" s="70" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="F211" s="70"/>
       <c r="G211" s="72"/>
@@ -9736,7 +9779,7 @@
     </row>
     <row r="212" spans="1:11" ht="15.75" customHeight="1">
       <c r="A212" s="24" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B212" s="73"/>
       <c r="C212" s="74"/>
@@ -9751,7 +9794,7 @@
     </row>
     <row r="213" spans="1:11" ht="15.75" customHeight="1">
       <c r="A213" s="2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B213" s="70"/>
       <c r="C213" s="71"/>
@@ -9766,7 +9809,7 @@
     </row>
     <row r="214" spans="1:11" ht="15.75" customHeight="1">
       <c r="A214" s="24" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B214" s="73"/>
       <c r="C214" s="74"/>
@@ -9781,7 +9824,7 @@
     </row>
     <row r="215" spans="1:11" ht="15.75" customHeight="1">
       <c r="A215" s="2" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" s="76"/>
@@ -9794,7 +9837,7 @@
     </row>
     <row r="216" spans="1:11" ht="15.75" customHeight="1">
       <c r="A216" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" s="76"/>
@@ -9807,7 +9850,7 @@
     </row>
     <row r="217" spans="1:11" ht="15.75" customHeight="1">
       <c r="A217" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" s="76"/>
@@ -9820,7 +9863,7 @@
     </row>
     <row r="218" spans="1:11" ht="15.75" customHeight="1">
       <c r="A218" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" s="76"/>
@@ -9833,7 +9876,7 @@
     </row>
     <row r="219" spans="1:11" ht="15.75" customHeight="1">
       <c r="A219" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" s="76"/>
@@ -9846,7 +9889,7 @@
     </row>
     <row r="220" spans="1:11" ht="15.75" customHeight="1">
       <c r="A220" s="2" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" s="76"/>
@@ -9859,7 +9902,7 @@
     </row>
     <row r="221" spans="1:11" ht="15.75" customHeight="1">
       <c r="A221" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" s="76"/>
@@ -9872,7 +9915,7 @@
     </row>
     <row r="222" spans="1:11" ht="15.75" customHeight="1">
       <c r="A222" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" s="76"/>
@@ -9885,7 +9928,7 @@
     </row>
     <row r="223" spans="1:11" ht="15.75" customHeight="1">
       <c r="A223" s="2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B223" s="2"/>
       <c r="C223" s="76"/>
@@ -9898,7 +9941,7 @@
     </row>
     <row r="224" spans="1:11" ht="15.75" customHeight="1">
       <c r="A224" s="2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B224" s="2"/>
       <c r="C224" s="76"/>
@@ -9911,7 +9954,7 @@
     </row>
     <row r="225" spans="1:9" ht="15.75" customHeight="1">
       <c r="A225" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B225" s="2"/>
       <c r="C225" s="76"/>
@@ -9924,7 +9967,7 @@
     </row>
     <row r="226" spans="1:9" ht="15.75" customHeight="1">
       <c r="A226" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B226" s="2"/>
       <c r="C226" s="76"/>
@@ -9937,7 +9980,7 @@
     </row>
     <row r="227" spans="1:9" ht="15.75" customHeight="1">
       <c r="A227" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B227" s="2"/>
       <c r="C227" s="76"/>
@@ -9950,7 +9993,7 @@
     </row>
     <row r="228" spans="1:9" ht="15.75" customHeight="1">
       <c r="A228" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B228" s="2"/>
       <c r="C228" s="76"/>
@@ -9963,7 +10006,7 @@
     </row>
     <row r="229" spans="1:9" ht="15.75" customHeight="1">
       <c r="A229" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B229" s="2"/>
       <c r="C229" s="76"/>
@@ -9976,7 +10019,7 @@
     </row>
     <row r="230" spans="1:9" ht="15.75" customHeight="1">
       <c r="A230" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B230" s="2"/>
       <c r="C230" s="76"/>
@@ -9989,7 +10032,7 @@
     </row>
     <row r="231" spans="1:9" ht="15.75" customHeight="1">
       <c r="A231" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B231" s="2"/>
       <c r="C231" s="76"/>
@@ -10002,7 +10045,7 @@
     </row>
     <row r="232" spans="1:9" ht="15.75" customHeight="1">
       <c r="A232" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B232" s="2"/>
       <c r="C232" s="76"/>
@@ -10015,7 +10058,7 @@
     </row>
     <row r="233" spans="1:9" ht="15.75" customHeight="1">
       <c r="A233" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B233" s="2"/>
       <c r="C233" s="76"/>
@@ -10028,7 +10071,7 @@
     </row>
     <row r="234" spans="1:9" ht="15.75" customHeight="1">
       <c r="A234" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B234" s="2"/>
       <c r="C234" s="76"/>
@@ -10083,10 +10126,10 @@
     </row>
     <row r="242" spans="1:9" ht="15.75" customHeight="1">
       <c r="A242" s="80" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B242" s="50" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C242" s="62">
         <v>3</v>
@@ -10096,7 +10139,7 @@
         <v>276</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="G242" s="64">
         <v>327</v>
@@ -10106,10 +10149,10 @@
     </row>
     <row r="243" spans="1:9" ht="15.75" customHeight="1">
       <c r="A243" s="80" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B243" s="29" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C243" s="32">
         <v>3</v>
@@ -10119,7 +10162,7 @@
         <v>276</v>
       </c>
       <c r="F243" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="G243" s="81">
         <v>514</v>
@@ -10129,20 +10172,20 @@
     </row>
     <row r="244" spans="1:9" ht="15.75" customHeight="1">
       <c r="A244" s="80" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B244" s="50" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C244" s="62">
         <v>9</v>
       </c>
       <c r="D244" s="63"/>
       <c r="E244" s="51" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="F244" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="G244" s="64">
         <v>124</v>
@@ -10152,20 +10195,20 @@
     </row>
     <row r="245" spans="1:9" ht="15.75" customHeight="1">
       <c r="A245" s="80" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B245" s="29" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C245" s="32">
         <v>9</v>
       </c>
       <c r="D245" s="30"/>
       <c r="E245" s="20" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F245" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="G245" s="81">
         <v>44</v>
@@ -10177,20 +10220,20 @@
     </row>
     <row r="246" spans="1:9" ht="15.75" customHeight="1">
       <c r="A246" s="80" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B246" s="50" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C246" s="62">
         <v>11</v>
       </c>
       <c r="D246" s="63"/>
       <c r="E246" s="51" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F246" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="G246" s="64"/>
       <c r="H246" s="82" t="s">
@@ -10200,7 +10243,7 @@
     </row>
     <row r="247" spans="1:9" ht="15.75" customHeight="1">
       <c r="A247" s="80" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B247" s="29"/>
       <c r="C247" s="32"/>
@@ -10213,7 +10256,7 @@
     </row>
     <row r="248" spans="1:9" ht="15.75" customHeight="1">
       <c r="A248" s="80" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B248" s="50"/>
       <c r="C248" s="62"/>
@@ -10226,7 +10269,7 @@
     </row>
     <row r="249" spans="1:9" ht="15.75" customHeight="1">
       <c r="A249" s="80" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B249" s="29"/>
       <c r="C249" s="32"/>
@@ -10239,7 +10282,7 @@
     </row>
     <row r="250" spans="1:9" ht="15.75" customHeight="1">
       <c r="A250" s="80" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B250" s="50"/>
       <c r="C250" s="62"/>
@@ -10252,7 +10295,7 @@
     </row>
     <row r="251" spans="1:9" ht="15.75" customHeight="1">
       <c r="A251" s="80" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B251" s="29"/>
       <c r="C251" s="32"/>
@@ -10265,7 +10308,7 @@
     </row>
     <row r="252" spans="1:9" ht="15.75" customHeight="1">
       <c r="A252" s="80" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B252" s="50"/>
       <c r="C252" s="62"/>
@@ -10278,7 +10321,7 @@
     </row>
     <row r="253" spans="1:9" ht="15.75" customHeight="1">
       <c r="A253" s="80" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B253" s="29"/>
       <c r="C253" s="32"/>
@@ -10291,7 +10334,7 @@
     </row>
     <row r="254" spans="1:9" ht="15.75" customHeight="1">
       <c r="A254" s="80" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B254" s="50"/>
       <c r="C254" s="62"/>
@@ -10304,7 +10347,7 @@
     </row>
     <row r="255" spans="1:9" ht="15.75" customHeight="1">
       <c r="A255" s="80" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B255" s="29"/>
       <c r="C255" s="32"/>
@@ -10317,7 +10360,7 @@
     </row>
     <row r="256" spans="1:9" ht="15.75" customHeight="1">
       <c r="A256" s="80" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B256" s="50"/>
       <c r="C256" s="62"/>
@@ -10330,7 +10373,7 @@
     </row>
     <row r="257" spans="1:9" ht="15.75" customHeight="1">
       <c r="A257" s="80" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B257" s="29"/>
       <c r="C257" s="32"/>
@@ -10343,7 +10386,7 @@
     </row>
     <row r="258" spans="1:9" ht="15.75" customHeight="1">
       <c r="A258" s="80" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B258" s="50"/>
       <c r="C258" s="62"/>
@@ -10356,7 +10399,7 @@
     </row>
     <row r="259" spans="1:9" ht="15.75" customHeight="1">
       <c r="A259" s="80" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B259" s="29"/>
       <c r="C259" s="32"/>
@@ -10369,7 +10412,7 @@
     </row>
     <row r="260" spans="1:9" ht="15.75" customHeight="1">
       <c r="A260" s="80" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B260" s="50"/>
       <c r="C260" s="62"/>
@@ -10382,7 +10425,7 @@
     </row>
     <row r="261" spans="1:9" ht="15.75" customHeight="1">
       <c r="A261" s="80" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B261" s="29"/>
       <c r="C261" s="32"/>
@@ -10395,7 +10438,7 @@
     </row>
     <row r="262" spans="1:9" ht="15.75" customHeight="1">
       <c r="A262" s="80" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B262" s="50"/>
       <c r="C262" s="62"/>
@@ -10408,7 +10451,7 @@
     </row>
     <row r="263" spans="1:9" ht="15.75" customHeight="1">
       <c r="A263" s="80" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B263" s="29"/>
       <c r="C263" s="32"/>
@@ -10421,7 +10464,7 @@
     </row>
     <row r="264" spans="1:9" ht="15.75" customHeight="1">
       <c r="A264" s="80" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B264" s="50"/>
       <c r="C264" s="62"/>
@@ -10434,7 +10477,7 @@
     </row>
     <row r="265" spans="1:9" ht="15.75" customHeight="1">
       <c r="A265" s="80" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B265" s="29"/>
       <c r="C265" s="32"/>
@@ -10447,7 +10490,7 @@
     </row>
     <row r="266" spans="1:9" ht="15.75" customHeight="1">
       <c r="A266" s="80" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B266" s="50"/>
       <c r="C266" s="62"/>
@@ -10460,7 +10503,7 @@
     </row>
     <row r="267" spans="1:9" ht="15.75" customHeight="1">
       <c r="A267" s="80" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B267" s="29"/>
       <c r="C267" s="32"/>
@@ -10473,7 +10516,7 @@
     </row>
     <row r="268" spans="1:9" ht="15.75" customHeight="1">
       <c r="A268" s="80" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="B268" s="50"/>
       <c r="C268" s="62"/>
@@ -10486,7 +10529,7 @@
     </row>
     <row r="269" spans="1:9" ht="15.75" customHeight="1">
       <c r="A269" s="80" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B269" s="29"/>
       <c r="C269" s="32"/>
@@ -10499,7 +10542,7 @@
     </row>
     <row r="270" spans="1:9" ht="15.75" customHeight="1">
       <c r="A270" s="80" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B270" s="50"/>
       <c r="C270" s="62"/>
@@ -10512,7 +10555,7 @@
     </row>
     <row r="271" spans="1:9" ht="15.75" customHeight="1">
       <c r="A271" s="80" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B271" s="29"/>
       <c r="C271" s="32"/>
@@ -10525,7 +10568,7 @@
     </row>
     <row r="272" spans="1:9" ht="15.75" customHeight="1">
       <c r="A272" s="80" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B272" s="50"/>
       <c r="C272" s="62"/>
@@ -10538,7 +10581,7 @@
     </row>
     <row r="273" spans="1:9" ht="15.75" customHeight="1">
       <c r="A273" s="80" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="B273" s="29"/>
       <c r="C273" s="32"/>
@@ -10551,7 +10594,7 @@
     </row>
     <row r="274" spans="1:9" ht="15.75" customHeight="1">
       <c r="A274" s="80" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B274" s="50"/>
       <c r="C274" s="62"/>
@@ -10564,7 +10607,7 @@
     </row>
     <row r="275" spans="1:9" ht="15.75" customHeight="1">
       <c r="A275" s="80" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B275" s="29"/>
       <c r="C275" s="32"/>
@@ -10577,7 +10620,7 @@
     </row>
     <row r="276" spans="1:9" ht="15.75" customHeight="1">
       <c r="A276" s="80" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="B276" s="50"/>
       <c r="C276" s="62"/>
@@ -10590,7 +10633,7 @@
     </row>
     <row r="277" spans="1:9" ht="15.75" customHeight="1">
       <c r="A277" s="80" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B277" s="29"/>
       <c r="C277" s="32"/>
@@ -10603,7 +10646,7 @@
     </row>
     <row r="278" spans="1:9" ht="15.75" customHeight="1">
       <c r="A278" s="80" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="B278" s="50"/>
       <c r="C278" s="62"/>
@@ -10616,7 +10659,7 @@
     </row>
     <row r="279" spans="1:9" ht="15.75" customHeight="1">
       <c r="A279" s="80" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B279" s="29"/>
       <c r="C279" s="32"/>
@@ -10629,7 +10672,7 @@
     </row>
     <row r="280" spans="1:9" ht="15.75" customHeight="1">
       <c r="A280" s="80" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B280" s="50"/>
       <c r="C280" s="62"/>
@@ -10642,7 +10685,7 @@
     </row>
     <row r="281" spans="1:9" ht="15.75" customHeight="1">
       <c r="A281" s="80" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B281" s="29"/>
       <c r="C281" s="32"/>
@@ -10655,7 +10698,7 @@
     </row>
     <row r="282" spans="1:9" ht="15.75" customHeight="1">
       <c r="A282" s="80" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B282" s="50"/>
       <c r="C282" s="62"/>
@@ -10668,7 +10711,7 @@
     </row>
     <row r="283" spans="1:9" ht="15.75" customHeight="1">
       <c r="A283" s="80" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B283" s="29"/>
       <c r="C283" s="32"/>
@@ -10681,7 +10724,7 @@
     </row>
     <row r="284" spans="1:9" ht="15.75" customHeight="1">
       <c r="A284" s="80" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B284" s="50"/>
       <c r="C284" s="62"/>
@@ -10694,7 +10737,7 @@
     </row>
     <row r="285" spans="1:9" ht="15.75" customHeight="1">
       <c r="A285" s="80" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B285" s="29"/>
       <c r="C285" s="32"/>
@@ -10707,7 +10750,7 @@
     </row>
     <row r="286" spans="1:9" ht="15.75" customHeight="1">
       <c r="A286" s="80" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B286" s="50"/>
       <c r="C286" s="62"/>
@@ -10720,7 +10763,7 @@
     </row>
     <row r="287" spans="1:9" ht="15.75" customHeight="1">
       <c r="A287" s="80" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B287" s="29"/>
       <c r="C287" s="32"/>
@@ -10733,7 +10776,7 @@
     </row>
     <row r="288" spans="1:9" ht="15.75" customHeight="1">
       <c r="A288" s="80" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B288" s="50"/>
       <c r="C288" s="62"/>
@@ -10746,7 +10789,7 @@
     </row>
     <row r="289" spans="1:9" ht="15.75" customHeight="1">
       <c r="A289" s="80" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B289" s="29"/>
       <c r="C289" s="32"/>
@@ -10759,7 +10802,7 @@
     </row>
     <row r="290" spans="1:9" ht="15.75" customHeight="1">
       <c r="A290" s="80" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B290" s="50"/>
       <c r="C290" s="62"/>
@@ -10772,7 +10815,7 @@
     </row>
     <row r="291" spans="1:9" ht="15.75" customHeight="1">
       <c r="A291" s="80" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B291" s="29"/>
       <c r="C291" s="32"/>
@@ -10785,7 +10828,7 @@
     </row>
     <row r="292" spans="1:9" ht="15.75" customHeight="1">
       <c r="A292" s="80" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B292" s="50"/>
       <c r="C292" s="62"/>
@@ -10798,7 +10841,7 @@
     </row>
     <row r="293" spans="1:9" ht="15.75" customHeight="1">
       <c r="A293" s="80" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B293" s="29"/>
       <c r="C293" s="32"/>
@@ -10811,7 +10854,7 @@
     </row>
     <row r="294" spans="1:9" ht="15.75" customHeight="1">
       <c r="A294" s="80" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B294" s="50"/>
       <c r="C294" s="62"/>
@@ -10824,7 +10867,7 @@
     </row>
     <row r="295" spans="1:9" ht="15.75" customHeight="1">
       <c r="A295" s="80" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B295" s="29"/>
       <c r="C295" s="32"/>
@@ -10837,7 +10880,7 @@
     </row>
     <row r="296" spans="1:9" ht="15.75" customHeight="1">
       <c r="A296" s="80" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="B296" s="50"/>
       <c r="C296" s="62"/>
@@ -10850,7 +10893,7 @@
     </row>
     <row r="297" spans="1:9" ht="15.75" customHeight="1">
       <c r="A297" s="80" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B297" s="29"/>
       <c r="C297" s="32"/>
@@ -10863,7 +10906,7 @@
     </row>
     <row r="298" spans="1:9" ht="15.75" customHeight="1">
       <c r="A298" s="80" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B298" s="50"/>
       <c r="C298" s="62"/>
@@ -10876,7 +10919,7 @@
     </row>
     <row r="299" spans="1:9" ht="15.75" customHeight="1">
       <c r="A299" s="80" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B299" s="29"/>
       <c r="C299" s="32"/>
@@ -10889,7 +10932,7 @@
     </row>
     <row r="300" spans="1:9" ht="15.75" customHeight="1">
       <c r="A300" s="80" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B300" s="50"/>
       <c r="C300" s="62"/>
@@ -10902,7 +10945,7 @@
     </row>
     <row r="301" spans="1:9" ht="15.75" customHeight="1">
       <c r="A301" s="80" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="B301" s="29"/>
       <c r="C301" s="32"/>
@@ -10915,7 +10958,7 @@
     </row>
     <row r="302" spans="1:9" ht="15.75" customHeight="1">
       <c r="A302" s="80" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B302" s="50"/>
       <c r="C302" s="62"/>
@@ -10928,7 +10971,7 @@
     </row>
     <row r="303" spans="1:9" ht="15.75" customHeight="1">
       <c r="A303" s="80" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="B303" s="29"/>
       <c r="C303" s="32"/>
@@ -10941,7 +10984,7 @@
     </row>
     <row r="304" spans="1:9" ht="15.75" customHeight="1">
       <c r="A304" s="80" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B304" s="50"/>
       <c r="C304" s="62"/>
@@ -10954,7 +10997,7 @@
     </row>
     <row r="305" spans="1:9" ht="15.75" customHeight="1">
       <c r="A305" s="80" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B305" s="29"/>
       <c r="C305" s="32"/>
@@ -10967,7 +11010,7 @@
     </row>
     <row r="306" spans="1:9" ht="15.75" customHeight="1">
       <c r="A306" s="80" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B306" s="50"/>
       <c r="C306" s="62"/>
@@ -10980,7 +11023,7 @@
     </row>
     <row r="307" spans="1:9" ht="15.75" customHeight="1">
       <c r="A307" s="80" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="B307" s="29"/>
       <c r="C307" s="32"/>
@@ -10993,7 +11036,7 @@
     </row>
     <row r="308" spans="1:9" ht="15.75" customHeight="1">
       <c r="A308" s="80" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B308" s="50"/>
       <c r="C308" s="62"/>
@@ -11006,7 +11049,7 @@
     </row>
     <row r="309" spans="1:9" ht="15.75" customHeight="1">
       <c r="A309" s="80" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B309" s="29"/>
       <c r="C309" s="32"/>
@@ -11019,7 +11062,7 @@
     </row>
     <row r="310" spans="1:9" ht="15.75" customHeight="1">
       <c r="A310" s="80" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B310" s="50"/>
       <c r="C310" s="62"/>
@@ -11032,7 +11075,7 @@
     </row>
     <row r="311" spans="1:9" ht="15.75" customHeight="1">
       <c r="A311" s="80" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B311" s="29"/>
       <c r="C311" s="32"/>
@@ -11045,7 +11088,7 @@
     </row>
     <row r="312" spans="1:9" ht="15.75" customHeight="1">
       <c r="A312" s="80" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B312" s="50"/>
       <c r="C312" s="62"/>
@@ -11058,7 +11101,7 @@
     </row>
     <row r="313" spans="1:9" ht="15.75" customHeight="1">
       <c r="A313" s="80" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="B313" s="29"/>
       <c r="C313" s="32"/>
@@ -11071,7 +11114,7 @@
     </row>
     <row r="314" spans="1:9" ht="15.75" customHeight="1">
       <c r="A314" s="80" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B314" s="50"/>
       <c r="C314" s="62"/>
@@ -11084,7 +11127,7 @@
     </row>
     <row r="315" spans="1:9" ht="15.75" customHeight="1">
       <c r="A315" s="80" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B315" s="29"/>
       <c r="C315" s="32"/>
@@ -11097,7 +11140,7 @@
     </row>
     <row r="316" spans="1:9" ht="15.75" customHeight="1">
       <c r="A316" s="80" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="B316" s="50"/>
       <c r="C316" s="62"/>
@@ -11110,7 +11153,7 @@
     </row>
     <row r="317" spans="1:9" ht="15.75" customHeight="1">
       <c r="A317" s="80" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B317" s="29"/>
       <c r="C317" s="32"/>
@@ -11123,7 +11166,7 @@
     </row>
     <row r="318" spans="1:9" ht="15.75" customHeight="1">
       <c r="A318" s="80" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B318" s="50"/>
       <c r="C318" s="62"/>
@@ -11136,7 +11179,7 @@
     </row>
     <row r="319" spans="1:9" ht="15.75" customHeight="1">
       <c r="A319" s="80" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B319" s="29"/>
       <c r="C319" s="32"/>
@@ -11149,7 +11192,7 @@
     </row>
     <row r="320" spans="1:9" ht="15.75" customHeight="1">
       <c r="A320" s="80" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="B320" s="50"/>
       <c r="C320" s="62"/>
@@ -11162,7 +11205,7 @@
     </row>
     <row r="321" spans="1:9" ht="15.75" customHeight="1">
       <c r="A321" s="80" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B321" s="29"/>
       <c r="C321" s="32"/>
@@ -11175,7 +11218,7 @@
     </row>
     <row r="322" spans="1:9" ht="15.75" customHeight="1">
       <c r="A322" s="80" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B322" s="50"/>
       <c r="C322" s="62"/>
@@ -11188,7 +11231,7 @@
     </row>
     <row r="323" spans="1:9" ht="15.75" customHeight="1">
       <c r="A323" s="80" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B323" s="29"/>
       <c r="C323" s="32"/>
@@ -11201,7 +11244,7 @@
     </row>
     <row r="324" spans="1:9" ht="15.75" customHeight="1">
       <c r="A324" s="80" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B324" s="50"/>
       <c r="C324" s="62"/>
@@ -11214,7 +11257,7 @@
     </row>
     <row r="325" spans="1:9" ht="15.75" customHeight="1">
       <c r="A325" s="80" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B325" s="29"/>
       <c r="C325" s="32"/>
@@ -11227,7 +11270,7 @@
     </row>
     <row r="326" spans="1:9" ht="15.75" customHeight="1">
       <c r="A326" s="80" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B326" s="50"/>
       <c r="C326" s="62"/>
@@ -11240,7 +11283,7 @@
     </row>
     <row r="327" spans="1:9" ht="15.75" customHeight="1">
       <c r="A327" s="80" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="B327" s="29"/>
       <c r="C327" s="32"/>
@@ -11253,7 +11296,7 @@
     </row>
     <row r="328" spans="1:9" ht="15.75" customHeight="1">
       <c r="A328" s="80" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B328" s="50"/>
       <c r="C328" s="62"/>
@@ -11266,7 +11309,7 @@
     </row>
     <row r="329" spans="1:9" ht="15.75" customHeight="1">
       <c r="A329" s="80" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="B329" s="29"/>
       <c r="C329" s="32"/>
@@ -11279,7 +11322,7 @@
     </row>
     <row r="330" spans="1:9" ht="15.75" customHeight="1">
       <c r="A330" s="80" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B330" s="50"/>
       <c r="C330" s="62"/>
@@ -11292,7 +11335,7 @@
     </row>
     <row r="331" spans="1:9" ht="15.75" customHeight="1">
       <c r="A331" s="80" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B331" s="29"/>
       <c r="C331" s="32"/>
@@ -11305,7 +11348,7 @@
     </row>
     <row r="332" spans="1:9" ht="15.75" customHeight="1">
       <c r="A332" s="80" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B332" s="50"/>
       <c r="C332" s="62"/>
@@ -11318,7 +11361,7 @@
     </row>
     <row r="333" spans="1:9" ht="15.75" customHeight="1">
       <c r="A333" s="80" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B333" s="29"/>
       <c r="C333" s="32"/>
@@ -11331,7 +11374,7 @@
     </row>
     <row r="334" spans="1:9" ht="15.75" customHeight="1">
       <c r="A334" s="80" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="B334" s="50"/>
       <c r="C334" s="62"/>
@@ -11344,7 +11387,7 @@
     </row>
     <row r="335" spans="1:9" ht="15.75" customHeight="1">
       <c r="A335" s="80" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="B335" s="29"/>
       <c r="C335" s="32"/>
@@ -11357,7 +11400,7 @@
     </row>
     <row r="336" spans="1:9" ht="15.75" customHeight="1">
       <c r="A336" s="80" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B336" s="50"/>
       <c r="C336" s="62"/>
@@ -11370,7 +11413,7 @@
     </row>
     <row r="337" spans="1:9" ht="15.75" customHeight="1">
       <c r="A337" s="80" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B337" s="29"/>
       <c r="C337" s="32"/>
@@ -11383,7 +11426,7 @@
     </row>
     <row r="338" spans="1:9" ht="15.75" customHeight="1">
       <c r="A338" s="80" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="B338" s="50"/>
       <c r="C338" s="62"/>
@@ -11396,7 +11439,7 @@
     </row>
     <row r="339" spans="1:9" ht="15.75" customHeight="1">
       <c r="A339" s="80" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B339" s="29"/>
       <c r="C339" s="32"/>
@@ -11409,7 +11452,7 @@
     </row>
     <row r="340" spans="1:9" ht="15.75" customHeight="1">
       <c r="A340" s="80" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B340" s="50"/>
       <c r="C340" s="62"/>
@@ -11422,7 +11465,7 @@
     </row>
     <row r="341" spans="1:9" ht="15.75" customHeight="1">
       <c r="A341" s="80" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B341" s="29"/>
       <c r="C341" s="32"/>
@@ -16193,8 +16236,8 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16219,81 +16262,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="162" t="s">
+        <v>665</v>
+      </c>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="164"/>
+    </row>
+    <row r="2" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A2" s="165" t="s">
+        <v>666</v>
+      </c>
+      <c r="B2" s="150"/>
+      <c r="C2" s="87" t="s">
+        <v>667</v>
+      </c>
+      <c r="D2" s="166" t="s">
         <v>668</v>
-      </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="149"/>
-    </row>
-    <row r="2" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A2" s="150" t="s">
-        <v>669</v>
-      </c>
-      <c r="B2" s="151"/>
-      <c r="C2" s="87" t="s">
-        <v>670</v>
-      </c>
-      <c r="D2" s="152" t="s">
-        <v>671</v>
       </c>
       <c r="E2" s="153"/>
       <c r="F2" s="153"/>
-      <c r="G2" s="151"/>
-      <c r="H2" s="154" t="s">
-        <v>672</v>
-      </c>
-      <c r="I2" s="155"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="167" t="s">
+        <v>669</v>
+      </c>
+      <c r="I2" s="154"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A4" s="156" t="s">
-        <v>673</v>
-      </c>
-      <c r="B4" s="148"/>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="149"/>
+      <c r="A4" s="168" t="s">
+        <v>670</v>
+      </c>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="164"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="88" t="s">
+        <v>671</v>
+      </c>
+      <c r="B5" s="89" t="s">
+        <v>672</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>673</v>
+      </c>
+      <c r="D5" s="89" t="s">
         <v>674</v>
       </c>
-      <c r="B5" s="89" t="s">
+      <c r="E5" s="89" t="s">
         <v>675</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="F5" s="89" t="s">
         <v>676</v>
-      </c>
-      <c r="D5" s="89" t="s">
-        <v>677</v>
-      </c>
-      <c r="E5" s="89" t="s">
-        <v>678</v>
-      </c>
-      <c r="F5" s="89" t="s">
-        <v>679</v>
       </c>
       <c r="G5" s="89" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="89" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="I5" s="90" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="K5" s="91" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.25" customHeight="1">
@@ -16301,104 +16344,104 @@
         <v>1</v>
       </c>
       <c r="B6" s="93" t="s">
+        <v>680</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>681</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>682</v>
+      </c>
+      <c r="E6" s="93" t="s">
         <v>683</v>
       </c>
-      <c r="C6" s="93" t="s">
+      <c r="F6" s="93" t="s">
         <v>684</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="G6" s="93" t="s">
         <v>685</v>
       </c>
-      <c r="E6" s="93" t="s">
+      <c r="H6" s="93" t="s">
         <v>686</v>
       </c>
-      <c r="F6" s="93" t="s">
+      <c r="I6" s="94" t="s">
         <v>687</v>
       </c>
-      <c r="G6" s="93" t="s">
+      <c r="K6" s="156" t="s">
         <v>688</v>
       </c>
-      <c r="H6" s="93" t="s">
-        <v>689</v>
-      </c>
-      <c r="I6" s="94" t="s">
-        <v>690</v>
-      </c>
-      <c r="K6" s="157" t="s">
-        <v>691</v>
-      </c>
-      <c r="L6" s="158"/>
-      <c r="M6" s="158"/>
-      <c r="N6" s="158"/>
-      <c r="O6" s="158"/>
-      <c r="P6" s="158"/>
-      <c r="Q6" s="158"/>
+      <c r="L6" s="157"/>
+      <c r="M6" s="157"/>
+      <c r="N6" s="157"/>
+      <c r="O6" s="157"/>
+      <c r="P6" s="157"/>
+      <c r="Q6" s="157"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="A7" s="92">
         <v>2</v>
       </c>
       <c r="B7" s="93" t="s">
+        <v>689</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>690</v>
+      </c>
+      <c r="D7" s="93" t="s">
+        <v>691</v>
+      </c>
+      <c r="E7" s="93" t="s">
         <v>692</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="F7" s="93" t="s">
         <v>693</v>
       </c>
-      <c r="D7" s="93" t="s">
+      <c r="G7" s="93" t="s">
         <v>694</v>
       </c>
-      <c r="E7" s="93" t="s">
+      <c r="H7" s="93" t="s">
         <v>695</v>
       </c>
-      <c r="F7" s="93" t="s">
+      <c r="I7" s="94" t="s">
         <v>696</v>
       </c>
-      <c r="G7" s="93" t="s">
+      <c r="K7" s="156" t="s">
         <v>697</v>
       </c>
-      <c r="H7" s="93" t="s">
-        <v>698</v>
-      </c>
-      <c r="I7" s="94" t="s">
-        <v>699</v>
-      </c>
-      <c r="K7" s="157" t="s">
-        <v>700</v>
-      </c>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="158"/>
-      <c r="O7" s="158"/>
-      <c r="P7" s="158"/>
-      <c r="Q7" s="158"/>
+      <c r="L7" s="157"/>
+      <c r="M7" s="157"/>
+      <c r="N7" s="157"/>
+      <c r="O7" s="157"/>
+      <c r="P7" s="157"/>
+      <c r="Q7" s="157"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="92">
         <v>3</v>
       </c>
       <c r="B8" s="93" t="s">
+        <v>698</v>
+      </c>
+      <c r="C8" s="93" t="s">
+        <v>699</v>
+      </c>
+      <c r="D8" s="93" t="s">
+        <v>700</v>
+      </c>
+      <c r="E8" s="93" t="s">
         <v>701</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="F8" s="93" t="s">
         <v>702</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="G8" s="93" t="s">
         <v>703</v>
       </c>
-      <c r="E8" s="93" t="s">
+      <c r="H8" s="93" t="s">
         <v>704</v>
       </c>
-      <c r="F8" s="93" t="s">
+      <c r="I8" s="94" t="s">
         <v>705</v>
-      </c>
-      <c r="G8" s="93" t="s">
-        <v>706</v>
-      </c>
-      <c r="H8" s="93" t="s">
-        <v>707</v>
-      </c>
-      <c r="I8" s="94" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.25" customHeight="1">
@@ -16478,111 +16521,111 @@
       <c r="I14" s="98"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A15" s="159" t="s">
-        <v>709</v>
-      </c>
-      <c r="B15" s="160"/>
-      <c r="C15" s="160"/>
-      <c r="D15" s="160"/>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="161"/>
+      <c r="A15" s="158" t="s">
+        <v>706</v>
+      </c>
+      <c r="B15" s="159"/>
+      <c r="C15" s="159"/>
+      <c r="D15" s="159"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="159"/>
+      <c r="H15" s="159"/>
+      <c r="I15" s="160"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="A16" s="88" t="s">
+        <v>671</v>
+      </c>
+      <c r="B16" s="89" t="s">
         <v>674</v>
       </c>
-      <c r="B16" s="89" t="s">
+      <c r="C16" s="89" t="s">
         <v>677</v>
       </c>
-      <c r="C16" s="89" t="s">
-        <v>680</v>
-      </c>
       <c r="D16" s="89" t="s">
-        <v>681</v>
-      </c>
-      <c r="E16" s="162" t="s">
-        <v>710</v>
-      </c>
-      <c r="F16" s="163"/>
-      <c r="G16" s="162" t="s">
-        <v>711</v>
-      </c>
-      <c r="H16" s="164"/>
-      <c r="I16" s="165"/>
+        <v>678</v>
+      </c>
+      <c r="E16" s="161" t="s">
+        <v>707</v>
+      </c>
+      <c r="F16" s="148"/>
+      <c r="G16" s="161" t="s">
+        <v>708</v>
+      </c>
+      <c r="H16" s="151"/>
+      <c r="I16" s="152"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="99">
         <v>1</v>
       </c>
       <c r="B17" s="93" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="C17" s="93" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D17" s="93" t="s">
-        <v>708</v>
-      </c>
-      <c r="E17" s="166" t="s">
-        <v>713</v>
-      </c>
-      <c r="F17" s="163"/>
-      <c r="G17" s="166" t="s">
-        <v>714</v>
-      </c>
-      <c r="H17" s="164"/>
-      <c r="I17" s="165"/>
+        <v>705</v>
+      </c>
+      <c r="E17" s="155" t="s">
+        <v>710</v>
+      </c>
+      <c r="F17" s="148"/>
+      <c r="G17" s="155" t="s">
+        <v>711</v>
+      </c>
+      <c r="H17" s="151"/>
+      <c r="I17" s="152"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1">
       <c r="A18" s="99">
         <v>2</v>
       </c>
       <c r="B18" s="93" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="C18" s="93" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D18" s="93" t="s">
-        <v>708</v>
-      </c>
-      <c r="E18" s="166" t="s">
+        <v>705</v>
+      </c>
+      <c r="E18" s="155" t="s">
+        <v>710</v>
+      </c>
+      <c r="F18" s="148"/>
+      <c r="G18" s="155" t="s">
         <v>713</v>
       </c>
-      <c r="F18" s="163"/>
-      <c r="G18" s="166" t="s">
-        <v>716</v>
-      </c>
-      <c r="H18" s="164"/>
-      <c r="I18" s="165"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="152"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1">
       <c r="A19" s="99">
         <v>3</v>
       </c>
       <c r="B19" s="93" t="s">
+        <v>714</v>
+      </c>
+      <c r="C19" s="93" t="s">
+        <v>695</v>
+      </c>
+      <c r="D19" s="93" t="s">
+        <v>715</v>
+      </c>
+      <c r="E19" s="155" t="s">
+        <v>716</v>
+      </c>
+      <c r="F19" s="148"/>
+      <c r="G19" s="155" t="s">
         <v>717</v>
       </c>
-      <c r="C19" s="93" t="s">
-        <v>698</v>
-      </c>
-      <c r="D19" s="93" t="s">
+      <c r="H19" s="151"/>
+      <c r="I19" s="152"/>
+      <c r="K19" s="91" t="s">
         <v>718</v>
-      </c>
-      <c r="E19" s="166" t="s">
-        <v>719</v>
-      </c>
-      <c r="F19" s="163"/>
-      <c r="G19" s="166" t="s">
-        <v>720</v>
-      </c>
-      <c r="H19" s="164"/>
-      <c r="I19" s="165"/>
-      <c r="K19" s="91" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1">
@@ -16592,11 +16635,11 @@
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
-      <c r="E20" s="167"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="167"/>
-      <c r="H20" s="164"/>
-      <c r="I20" s="165"/>
+      <c r="E20" s="147"/>
+      <c r="F20" s="148"/>
+      <c r="G20" s="147"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="152"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" s="99">
@@ -16605,13 +16648,13 @@
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
-      <c r="E21" s="167"/>
-      <c r="F21" s="163"/>
-      <c r="G21" s="167"/>
-      <c r="H21" s="164"/>
-      <c r="I21" s="165"/>
+      <c r="E21" s="147"/>
+      <c r="F21" s="148"/>
+      <c r="G21" s="147"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="152"/>
       <c r="K21" s="91" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.25" customHeight="1">
@@ -16621,11 +16664,11 @@
       <c r="B22" s="100"/>
       <c r="C22" s="100"/>
       <c r="D22" s="100"/>
-      <c r="E22" s="167"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="167"/>
-      <c r="H22" s="164"/>
-      <c r="I22" s="165"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="148"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="151"/>
+      <c r="I22" s="152"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1">
       <c r="A23" s="99">
@@ -16634,11 +16677,11 @@
       <c r="B23" s="100"/>
       <c r="C23" s="100"/>
       <c r="D23" s="100"/>
-      <c r="E23" s="167"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="167"/>
-      <c r="H23" s="164"/>
-      <c r="I23" s="165"/>
+      <c r="E23" s="147"/>
+      <c r="F23" s="148"/>
+      <c r="G23" s="147"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="152"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" s="99">
@@ -16647,11 +16690,11 @@
       <c r="B24" s="100"/>
       <c r="C24" s="100"/>
       <c r="D24" s="100"/>
-      <c r="E24" s="167"/>
-      <c r="F24" s="163"/>
-      <c r="G24" s="167"/>
-      <c r="H24" s="164"/>
-      <c r="I24" s="165"/>
+      <c r="E24" s="147"/>
+      <c r="F24" s="148"/>
+      <c r="G24" s="147"/>
+      <c r="H24" s="151"/>
+      <c r="I24" s="152"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" s="99">
@@ -16660,11 +16703,11 @@
       <c r="B25" s="100"/>
       <c r="C25" s="100"/>
       <c r="D25" s="100"/>
-      <c r="E25" s="167"/>
-      <c r="F25" s="163"/>
-      <c r="G25" s="167"/>
-      <c r="H25" s="164"/>
-      <c r="I25" s="165"/>
+      <c r="E25" s="147"/>
+      <c r="F25" s="148"/>
+      <c r="G25" s="147"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="152"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" s="101">
@@ -16673,11 +16716,11 @@
       <c r="B26" s="96"/>
       <c r="C26" s="96"/>
       <c r="D26" s="96"/>
-      <c r="E26" s="168"/>
-      <c r="F26" s="151"/>
-      <c r="G26" s="168"/>
+      <c r="E26" s="149"/>
+      <c r="F26" s="150"/>
+      <c r="G26" s="149"/>
       <c r="H26" s="153"/>
-      <c r="I26" s="155"/>
+      <c r="I26" s="154"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
@@ -17655,14 +17698,16 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -17675,16 +17720,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -17719,13 +17762,13 @@
       <c r="A1" s="102"/>
       <c r="B1" s="103"/>
       <c r="C1" s="103" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D1" s="103"/>
       <c r="E1" s="103"/>
       <c r="F1" s="103"/>
       <c r="G1" s="103" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="H1" s="103"/>
       <c r="I1" s="104"/>
@@ -17733,7 +17776,7 @@
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1">
       <c r="A2" s="169" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="B2" s="170"/>
       <c r="C2" s="146"/>
@@ -17750,7 +17793,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="112" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C3" s="113" t="s">
         <v>7</v>
@@ -17762,10 +17805,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="113" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="G3" s="113" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="H3" s="116" t="s">
         <v>12</v>
@@ -17784,7 +17827,7 @@
     <row r="5" spans="1:21" ht="14.25" customHeight="1">
       <c r="A5" s="98"/>
       <c r="B5" s="118" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="D5" s="98"/>
       <c r="K5" s="119"/>
@@ -17794,7 +17837,7 @@
     </row>
     <row r="6" spans="1:21" ht="14.25" customHeight="1">
       <c r="B6" s="120" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="D6" s="98"/>
       <c r="K6" s="119"/>
@@ -17802,7 +17845,7 @@
     </row>
     <row r="7" spans="1:21" ht="14.25" customHeight="1">
       <c r="B7" s="120" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="D7" s="98"/>
       <c r="K7" s="119"/>
@@ -17810,7 +17853,7 @@
     </row>
     <row r="8" spans="1:21" ht="14.25" customHeight="1">
       <c r="B8" s="120" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D8" s="98"/>
       <c r="K8" s="119"/>
@@ -17822,14 +17865,14 @@
     </row>
     <row r="10" spans="1:21" ht="14.25" customHeight="1">
       <c r="B10" s="118" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="K10" s="119"/>
       <c r="O10" s="105"/>
     </row>
     <row r="11" spans="1:21" ht="14.25" customHeight="1">
       <c r="B11" s="120" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="K11" s="119"/>
       <c r="O11" s="105"/>
@@ -20829,19 +20872,19 @@
     <row r="1" spans="2:15" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:15" ht="14.25" customHeight="1">
       <c r="B2" s="171" t="s">
-        <v>733</v>
-      </c>
-      <c r="C2" s="163"/>
+        <v>730</v>
+      </c>
+      <c r="C2" s="148"/>
       <c r="O2" s="91" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
       <c r="B3" s="121" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C3" s="122" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="15.75" customHeight="1">
@@ -20849,10 +20892,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="14.25" customHeight="1">
@@ -20860,10 +20903,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D5" s="91" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="14.25" customHeight="1">
@@ -20871,10 +20914,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="D6" s="91" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="14.25" customHeight="1">
@@ -20882,10 +20925,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="D7" s="91" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="14.25" customHeight="1">
@@ -20893,10 +20936,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="D8" s="91" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="14.25" customHeight="1">
@@ -20904,10 +20947,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="D9" s="91" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="14.25" customHeight="1">
@@ -20915,10 +20958,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="D10" s="91" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" customHeight="1">
@@ -20926,10 +20969,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="14.25" customHeight="1">
@@ -20937,10 +20980,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="D12" s="91" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="14.25" customHeight="1">
@@ -20948,10 +20991,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="D13" s="91" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="14.25" customHeight="1">
@@ -20959,10 +21002,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D14" s="91" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="14.25" customHeight="1">
@@ -20970,10 +21013,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="D15" s="91" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="14.25" customHeight="1">
@@ -20981,10 +21024,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D16" s="91" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="14.25" customHeight="1">
@@ -20992,10 +21035,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D17" s="91" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="14.25" customHeight="1">
@@ -22041,60 +22084,60 @@
     <row r="1" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
       <c r="J2" s="91" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
       <c r="A3" s="171" t="s">
-        <v>766</v>
-      </c>
-      <c r="B3" s="164"/>
-      <c r="C3" s="163"/>
+        <v>763</v>
+      </c>
+      <c r="B3" s="151"/>
+      <c r="C3" s="148"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="123" t="s">
-        <v>674</v>
-      </c>
-      <c r="B4" s="172" t="s">
-        <v>767</v>
-      </c>
-      <c r="C4" s="163"/>
+        <v>671</v>
+      </c>
+      <c r="B4" s="173" t="s">
+        <v>764</v>
+      </c>
+      <c r="C4" s="148"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="124" t="s">
-        <v>768</v>
-      </c>
-      <c r="B5" s="173" t="s">
-        <v>769</v>
-      </c>
-      <c r="C5" s="163"/>
+        <v>765</v>
+      </c>
+      <c r="B5" s="172" t="s">
+        <v>766</v>
+      </c>
+      <c r="C5" s="148"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="124" t="s">
-        <v>770</v>
-      </c>
-      <c r="B6" s="173" t="s">
-        <v>771</v>
-      </c>
-      <c r="C6" s="163"/>
+        <v>767</v>
+      </c>
+      <c r="B6" s="172" t="s">
+        <v>768</v>
+      </c>
+      <c r="C6" s="148"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="124" t="s">
-        <v>772</v>
-      </c>
-      <c r="B7" s="173" t="s">
-        <v>773</v>
-      </c>
-      <c r="C7" s="163"/>
+        <v>769</v>
+      </c>
+      <c r="B7" s="172" t="s">
+        <v>770</v>
+      </c>
+      <c r="C7" s="148"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="124" t="s">
-        <v>774</v>
-      </c>
-      <c r="B8" s="173" t="s">
-        <v>775</v>
-      </c>
-      <c r="C8" s="163"/>
+        <v>771</v>
+      </c>
+      <c r="B8" s="172" t="s">
+        <v>772</v>
+      </c>
+      <c r="C8" s="148"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
@@ -23123,111 +23166,111 @@
     </row>
     <row r="2" spans="2:10" ht="14.25" customHeight="1">
       <c r="B2" s="174" t="s">
-        <v>776</v>
-      </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="149"/>
+        <v>773</v>
+      </c>
+      <c r="C2" s="163"/>
+      <c r="D2" s="164"/>
       <c r="J2" s="91" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1">
       <c r="B3" s="126" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C3" s="122" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D3" s="127" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="14.25" customHeight="1">
       <c r="B4" s="128" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="C4" s="129" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D4" s="130" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="14.25" customHeight="1">
       <c r="B5" s="128" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C5" s="129" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D5" s="131" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="42" customHeight="1">
       <c r="B6" s="128" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="C6" s="129" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="D6" s="131" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="14.25" customHeight="1">
       <c r="B7" s="128" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C7" s="132" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="D7" s="131" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="14.25" customHeight="1">
       <c r="B8" s="128" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C8" s="129" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D8" s="131" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="84" customHeight="1">
       <c r="B9" s="128" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C9" s="129" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="D9" s="133" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="14.25" customHeight="1">
       <c r="B10" s="128" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="C10" s="132" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="D10" s="131" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="27" customHeight="1">
       <c r="B11" s="134" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="C11" s="135" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="D11" s="97" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="14.25" customHeight="1">
@@ -26224,24 +26267,24 @@
     <row r="2" spans="3:4" ht="14.25" customHeight="1"/>
     <row r="3" spans="3:4" ht="14.25" customHeight="1">
       <c r="C3" s="91" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="14.25" customHeight="1">
       <c r="C4" s="91" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="D4" s="136" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="14.25" customHeight="1"/>
     <row r="6" spans="3:4" ht="14.25" customHeight="1">
       <c r="C6" s="91" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="D6" s="136" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="14.25" customHeight="1"/>
@@ -27252,7 +27295,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -27266,75 +27311,75 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
       <c r="J1" s="91" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="172" t="s">
-        <v>809</v>
-      </c>
-      <c r="B5" s="164"/>
-      <c r="C5" s="163"/>
+      <c r="A5" s="173" t="s">
+        <v>806</v>
+      </c>
+      <c r="B5" s="151"/>
+      <c r="C5" s="148"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
       <c r="A6" s="123" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="B6" s="123" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="C6" s="123" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1">
       <c r="A7" s="137" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="B7" s="100" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
       <c r="A8" s="138" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="B8" s="139" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="C8" s="129" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="I8" s="91" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="42.75" customHeight="1">
       <c r="A9" s="140" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B9" s="132" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="C9" s="129" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
       <c r="A10" s="141" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B10" s="100" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="C10" s="129" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
chg: Added DPIs to airfields in OPAC.miz, updated target list and "Notia as candidate for air attack accordingly
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -3627,6 +3627,18 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3636,20 +3648,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3663,22 +3680,17 @@
     <xf numFmtId="0" fontId="16" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3695,18 +3707,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4968,7 +4968,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H82" sqref="H82"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4987,15 +4987,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="144"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="148"/>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5008,10 +5008,10 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="34.5">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="146"/>
+      <c r="B2" s="150"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
@@ -5079,10 +5079,10 @@
       <c r="G4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="23" t="s">
+      <c r="H4" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="2"/>
@@ -5108,10 +5108,10 @@
       <c r="G5" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="23" t="s">
+      <c r="H5" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="2"/>
@@ -5139,10 +5139,10 @@
       <c r="G6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="23" t="s">
+      <c r="H6" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="2"/>
@@ -5170,10 +5170,10 @@
       <c r="G7" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="23" t="s">
+      <c r="H7" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="2"/>
@@ -5201,10 +5201,10 @@
       <c r="G8" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="23" t="s">
+      <c r="H8" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="2"/>
@@ -7547,7 +7547,7 @@
         <v>10</v>
       </c>
       <c r="D87" s="27"/>
-      <c r="E87" s="178" t="s">
+      <c r="E87" s="145" t="s">
         <v>822</v>
       </c>
       <c r="F87" s="24" t="s">
@@ -7814,7 +7814,7 @@
         <v>1</v>
       </c>
       <c r="D96" s="30"/>
-      <c r="E96" s="177" t="s">
+      <c r="E96" s="144" t="s">
         <v>821</v>
       </c>
       <c r="F96" s="2" t="s">
@@ -7843,7 +7843,7 @@
         <v>1</v>
       </c>
       <c r="D97" s="27"/>
-      <c r="E97" s="176" t="s">
+      <c r="E97" s="143" t="s">
         <v>820</v>
       </c>
       <c r="F97" s="24" t="s">
@@ -7905,7 +7905,7 @@
         <v>7</v>
       </c>
       <c r="D99" s="27"/>
-      <c r="E99" s="175" t="s">
+      <c r="E99" s="142" t="s">
         <v>819</v>
       </c>
       <c r="F99" s="24" t="s">
@@ -16262,50 +16262,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="151" t="s">
         <v>665</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="164"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="153"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="154" t="s">
         <v>666</v>
       </c>
-      <c r="B2" s="150"/>
+      <c r="B2" s="155"/>
       <c r="C2" s="87" t="s">
         <v>667</v>
       </c>
-      <c r="D2" s="166" t="s">
+      <c r="D2" s="156" t="s">
         <v>668</v>
       </c>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="167" t="s">
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="158" t="s">
         <v>669</v>
       </c>
-      <c r="I2" s="154"/>
+      <c r="I2" s="159"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A4" s="168" t="s">
+      <c r="A4" s="160" t="s">
         <v>670</v>
       </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="164"/>
+      <c r="B4" s="152"/>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="153"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="88" t="s">
@@ -16367,15 +16367,15 @@
       <c r="I6" s="94" t="s">
         <v>687</v>
       </c>
-      <c r="K6" s="156" t="s">
+      <c r="K6" s="161" t="s">
         <v>688</v>
       </c>
-      <c r="L6" s="157"/>
-      <c r="M6" s="157"/>
-      <c r="N6" s="157"/>
-      <c r="O6" s="157"/>
-      <c r="P6" s="157"/>
-      <c r="Q6" s="157"/>
+      <c r="L6" s="162"/>
+      <c r="M6" s="162"/>
+      <c r="N6" s="162"/>
+      <c r="O6" s="162"/>
+      <c r="P6" s="162"/>
+      <c r="Q6" s="162"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="A7" s="92">
@@ -16405,15 +16405,15 @@
       <c r="I7" s="94" t="s">
         <v>696</v>
       </c>
-      <c r="K7" s="156" t="s">
+      <c r="K7" s="161" t="s">
         <v>697</v>
       </c>
-      <c r="L7" s="157"/>
-      <c r="M7" s="157"/>
-      <c r="N7" s="157"/>
-      <c r="O7" s="157"/>
-      <c r="P7" s="157"/>
-      <c r="Q7" s="157"/>
+      <c r="L7" s="162"/>
+      <c r="M7" s="162"/>
+      <c r="N7" s="162"/>
+      <c r="O7" s="162"/>
+      <c r="P7" s="162"/>
+      <c r="Q7" s="162"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="92">
@@ -16521,17 +16521,17 @@
       <c r="I14" s="98"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="163" t="s">
         <v>706</v>
       </c>
-      <c r="B15" s="159"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="159"/>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="160"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="164"/>
+      <c r="D15" s="164"/>
+      <c r="E15" s="164"/>
+      <c r="F15" s="164"/>
+      <c r="G15" s="164"/>
+      <c r="H15" s="164"/>
+      <c r="I15" s="165"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="A16" s="88" t="s">
@@ -16546,15 +16546,15 @@
       <c r="D16" s="89" t="s">
         <v>678</v>
       </c>
-      <c r="E16" s="161" t="s">
+      <c r="E16" s="166" t="s">
         <v>707</v>
       </c>
-      <c r="F16" s="148"/>
-      <c r="G16" s="161" t="s">
+      <c r="F16" s="167"/>
+      <c r="G16" s="166" t="s">
         <v>708</v>
       </c>
-      <c r="H16" s="151"/>
-      <c r="I16" s="152"/>
+      <c r="H16" s="168"/>
+      <c r="I16" s="169"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="99">
@@ -16569,15 +16569,15 @@
       <c r="D17" s="93" t="s">
         <v>705</v>
       </c>
-      <c r="E17" s="155" t="s">
+      <c r="E17" s="170" t="s">
         <v>710</v>
       </c>
-      <c r="F17" s="148"/>
-      <c r="G17" s="155" t="s">
+      <c r="F17" s="167"/>
+      <c r="G17" s="170" t="s">
         <v>711</v>
       </c>
-      <c r="H17" s="151"/>
-      <c r="I17" s="152"/>
+      <c r="H17" s="168"/>
+      <c r="I17" s="169"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1">
       <c r="A18" s="99">
@@ -16592,15 +16592,15 @@
       <c r="D18" s="93" t="s">
         <v>705</v>
       </c>
-      <c r="E18" s="155" t="s">
+      <c r="E18" s="170" t="s">
         <v>710</v>
       </c>
-      <c r="F18" s="148"/>
-      <c r="G18" s="155" t="s">
+      <c r="F18" s="167"/>
+      <c r="G18" s="170" t="s">
         <v>713</v>
       </c>
-      <c r="H18" s="151"/>
-      <c r="I18" s="152"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="169"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1">
       <c r="A19" s="99">
@@ -16615,15 +16615,15 @@
       <c r="D19" s="93" t="s">
         <v>715</v>
       </c>
-      <c r="E19" s="155" t="s">
+      <c r="E19" s="170" t="s">
         <v>716</v>
       </c>
-      <c r="F19" s="148"/>
-      <c r="G19" s="155" t="s">
+      <c r="F19" s="167"/>
+      <c r="G19" s="170" t="s">
         <v>717</v>
       </c>
-      <c r="H19" s="151"/>
-      <c r="I19" s="152"/>
+      <c r="H19" s="168"/>
+      <c r="I19" s="169"/>
       <c r="K19" s="91" t="s">
         <v>718</v>
       </c>
@@ -16635,11 +16635,11 @@
       <c r="B20" s="100"/>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
-      <c r="E20" s="147"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="147"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="152"/>
+      <c r="E20" s="171"/>
+      <c r="F20" s="167"/>
+      <c r="G20" s="171"/>
+      <c r="H20" s="168"/>
+      <c r="I20" s="169"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" s="99">
@@ -16648,11 +16648,11 @@
       <c r="B21" s="100"/>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
-      <c r="E21" s="147"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="147"/>
-      <c r="H21" s="151"/>
-      <c r="I21" s="152"/>
+      <c r="E21" s="171"/>
+      <c r="F21" s="167"/>
+      <c r="G21" s="171"/>
+      <c r="H21" s="168"/>
+      <c r="I21" s="169"/>
       <c r="K21" s="91" t="s">
         <v>719</v>
       </c>
@@ -16664,11 +16664,11 @@
       <c r="B22" s="100"/>
       <c r="C22" s="100"/>
       <c r="D22" s="100"/>
-      <c r="E22" s="147"/>
-      <c r="F22" s="148"/>
-      <c r="G22" s="147"/>
-      <c r="H22" s="151"/>
-      <c r="I22" s="152"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="167"/>
+      <c r="G22" s="171"/>
+      <c r="H22" s="168"/>
+      <c r="I22" s="169"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1">
       <c r="A23" s="99">
@@ -16677,11 +16677,11 @@
       <c r="B23" s="100"/>
       <c r="C23" s="100"/>
       <c r="D23" s="100"/>
-      <c r="E23" s="147"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="147"/>
-      <c r="H23" s="151"/>
-      <c r="I23" s="152"/>
+      <c r="E23" s="171"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="171"/>
+      <c r="H23" s="168"/>
+      <c r="I23" s="169"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" s="99">
@@ -16690,11 +16690,11 @@
       <c r="B24" s="100"/>
       <c r="C24" s="100"/>
       <c r="D24" s="100"/>
-      <c r="E24" s="147"/>
-      <c r="F24" s="148"/>
-      <c r="G24" s="147"/>
-      <c r="H24" s="151"/>
-      <c r="I24" s="152"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="167"/>
+      <c r="G24" s="171"/>
+      <c r="H24" s="168"/>
+      <c r="I24" s="169"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" s="99">
@@ -16703,11 +16703,11 @@
       <c r="B25" s="100"/>
       <c r="C25" s="100"/>
       <c r="D25" s="100"/>
-      <c r="E25" s="147"/>
-      <c r="F25" s="148"/>
-      <c r="G25" s="147"/>
-      <c r="H25" s="151"/>
-      <c r="I25" s="152"/>
+      <c r="E25" s="171"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="171"/>
+      <c r="H25" s="168"/>
+      <c r="I25" s="169"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" s="101">
@@ -16716,11 +16716,11 @@
       <c r="B26" s="96"/>
       <c r="C26" s="96"/>
       <c r="D26" s="96"/>
-      <c r="E26" s="149"/>
-      <c r="F26" s="150"/>
-      <c r="G26" s="149"/>
-      <c r="H26" s="153"/>
-      <c r="I26" s="154"/>
+      <c r="E26" s="172"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="157"/>
+      <c r="I26" s="159"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
@@ -17698,16 +17698,14 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -17720,14 +17718,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -17775,11 +17775,11 @@
       <c r="O1" s="105"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A2" s="169" t="s">
+      <c r="A2" s="173" t="s">
         <v>722</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="146"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="150"/>
       <c r="D2" s="106"/>
       <c r="E2" s="107"/>
       <c r="F2" s="108"/>
@@ -20871,10 +20871,10 @@
   <sheetData>
     <row r="1" spans="2:15" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:15" ht="14.25" customHeight="1">
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="175" t="s">
         <v>730</v>
       </c>
-      <c r="C2" s="148"/>
+      <c r="C2" s="167"/>
       <c r="O2" s="91" t="s">
         <v>731</v>
       </c>
@@ -22088,56 +22088,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="175" t="s">
         <v>763</v>
       </c>
-      <c r="B3" s="151"/>
-      <c r="C3" s="148"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="167"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="123" t="s">
         <v>671</v>
       </c>
-      <c r="B4" s="173" t="s">
+      <c r="B4" s="177" t="s">
         <v>764</v>
       </c>
-      <c r="C4" s="148"/>
+      <c r="C4" s="167"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="124" t="s">
         <v>765</v>
       </c>
-      <c r="B5" s="172" t="s">
+      <c r="B5" s="176" t="s">
         <v>766</v>
       </c>
-      <c r="C5" s="148"/>
+      <c r="C5" s="167"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="124" t="s">
         <v>767</v>
       </c>
-      <c r="B6" s="172" t="s">
+      <c r="B6" s="176" t="s">
         <v>768</v>
       </c>
-      <c r="C6" s="148"/>
+      <c r="C6" s="167"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="124" t="s">
         <v>769</v>
       </c>
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="176" t="s">
         <v>770</v>
       </c>
-      <c r="C7" s="148"/>
+      <c r="C7" s="167"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="124" t="s">
         <v>771</v>
       </c>
-      <c r="B8" s="172" t="s">
+      <c r="B8" s="176" t="s">
         <v>772</v>
       </c>
-      <c r="C8" s="148"/>
+      <c r="C8" s="167"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
@@ -23165,11 +23165,11 @@
       <c r="D1" s="125"/>
     </row>
     <row r="2" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="178" t="s">
         <v>773</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="164"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="153"/>
       <c r="J2" s="91" t="s">
         <v>731</v>
       </c>
@@ -27318,11 +27318,11 @@
     <row r="3" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="173" t="s">
+      <c r="A5" s="177" t="s">
         <v>806</v>
       </c>
-      <c r="B5" s="151"/>
-      <c r="C5" s="148"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="167"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
       <c r="A6" s="123" t="s">

</xml_diff>

<commit_message>
chg: Added 4 targets (ADCC, SCC North, SCC South and AWACS relay station). Added to OPAC.miz, target list, CF tgt list, master intel CF, "Notia as candidate for air attack".
chg: Finished INTREP VID OPAC-002 - Notia IADS
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="861">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -2585,6 +2585,54 @@
   </si>
   <si>
     <t>Neck</t>
+  </si>
+  <si>
+    <t>Air Defense Command Center (ADCC)</t>
+  </si>
+  <si>
+    <t>Command and control of Notian IADS network</t>
+  </si>
+  <si>
+    <t>Sector Command Center North (SCC North)</t>
+  </si>
+  <si>
+    <t>Sector Command Center South (SCC South)</t>
+  </si>
+  <si>
+    <t>IADS Command and control of Sector NORTH</t>
+  </si>
+  <si>
+    <t>665ft</t>
+  </si>
+  <si>
+    <t>262ft</t>
+  </si>
+  <si>
+    <t>967ft</t>
+  </si>
+  <si>
+    <t>N68 55.713 E033 10.092</t>
+  </si>
+  <si>
+    <t>N69 02.910 E033 24.593</t>
+  </si>
+  <si>
+    <t>N68 09.708 E033 26.228</t>
+  </si>
+  <si>
+    <t>AWACS Connection Node</t>
+  </si>
+  <si>
+    <t>Connection node from AWACS to ADCC as part of IADS</t>
+  </si>
+  <si>
+    <t>Not urgent</t>
+  </si>
+  <si>
+    <t>N69 21.886 E034 13.457</t>
+  </si>
+  <si>
+    <t>747ft</t>
   </si>
 </sst>
 </file>
@@ -3356,7 +3404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3761,20 +3809,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3788,22 +3841,17 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3820,6 +3868,9 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3853,7 +3904,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3887,7 +3938,7 @@
         <xdr:cNvPr id="3" name="image2.png" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3926,7 +3977,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3960,7 +4011,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3999,7 +4050,7 @@
         <xdr:cNvPr id="2" name="image10.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4033,7 +4084,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4072,7 +4123,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4229,7 +4280,7 @@
         <xdr:cNvPr id="4" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4263,7 +4314,7 @@
         <xdr:cNvPr id="5" name="image6.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4302,7 +4353,7 @@
         <xdr:cNvPr id="4" name="Shape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4459,7 +4510,7 @@
         <xdr:cNvPr id="3" name="image8.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4493,7 +4544,7 @@
         <xdr:cNvPr id="5" name="image9.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4532,7 +4583,7 @@
         <xdr:cNvPr id="5" name="Shape 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4713,7 +4764,7 @@
         <xdr:cNvPr id="3" name="image7.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4747,7 +4798,7 @@
         <xdr:cNvPr id="4" name="image14.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4786,7 +4837,7 @@
         <xdr:cNvPr id="6" name="Shape 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4907,7 +4958,7 @@
         <xdr:cNvPr id="3" name="image13.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4941,7 +4992,7 @@
         <xdr:cNvPr id="4" name="image11.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4975,7 +5026,7 @@
         <xdr:cNvPr id="5" name="image12.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5200,10 +5251,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K68" sqref="K68"/>
+      <selection pane="bottomRight" activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -7762,7 +7813,9 @@
       <c r="I82" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J82" s="8"/>
+      <c r="J82" s="8" t="s">
+        <v>843</v>
+      </c>
       <c r="K82" s="2"/>
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1">
@@ -7849,7 +7902,9 @@
       <c r="I85" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J85" s="8"/>
+      <c r="J85" s="8" t="s">
+        <v>858</v>
+      </c>
       <c r="K85" s="2"/>
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1">
@@ -7965,7 +8020,9 @@
       <c r="I89" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J89" s="8"/>
+      <c r="J89" s="8" t="s">
+        <v>843</v>
+      </c>
       <c r="K89" s="2"/>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1">
@@ -9912,7 +9969,9 @@
       <c r="I204" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J204" s="8"/>
+      <c r="J204" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="K204" s="2" t="s">
         <v>369</v>
       </c>
@@ -9943,7 +10002,9 @@
       <c r="I205" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J205" s="8"/>
+      <c r="J205" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="K205" s="2" t="s">
         <v>369</v>
       </c>
@@ -10136,14 +10197,28 @@
       <c r="A212" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B212" s="66"/>
-      <c r="C212" s="67"/>
+      <c r="B212" s="66" t="s">
+        <v>845</v>
+      </c>
+      <c r="C212" s="67">
+        <v>2</v>
+      </c>
       <c r="D212" s="66"/>
-      <c r="E212" s="66"/>
-      <c r="F212" s="66"/>
-      <c r="G212" s="68"/>
-      <c r="H212" s="8"/>
-      <c r="I212" s="8"/>
+      <c r="E212" s="66" t="s">
+        <v>846</v>
+      </c>
+      <c r="F212" s="66" t="s">
+        <v>853</v>
+      </c>
+      <c r="G212" s="68" t="s">
+        <v>852</v>
+      </c>
+      <c r="H212" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I212" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="J212" s="8"/>
       <c r="K212" s="2"/>
     </row>
@@ -10151,14 +10226,28 @@
       <c r="A213" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B213" s="63"/>
-      <c r="C213" s="64"/>
+      <c r="B213" s="63" t="s">
+        <v>847</v>
+      </c>
+      <c r="C213" s="64">
+        <v>2</v>
+      </c>
       <c r="D213" s="63"/>
-      <c r="E213" s="63"/>
-      <c r="F213" s="63"/>
-      <c r="G213" s="65"/>
-      <c r="H213" s="8"/>
-      <c r="I213" s="8"/>
+      <c r="E213" s="63" t="s">
+        <v>849</v>
+      </c>
+      <c r="F213" s="63" t="s">
+        <v>854</v>
+      </c>
+      <c r="G213" s="65" t="s">
+        <v>851</v>
+      </c>
+      <c r="H213" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I213" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="J213" s="8"/>
       <c r="K213" s="2"/>
     </row>
@@ -10166,14 +10255,28 @@
       <c r="A214" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="B214" s="66"/>
-      <c r="C214" s="67"/>
+      <c r="B214" s="66" t="s">
+        <v>848</v>
+      </c>
+      <c r="C214" s="67">
+        <v>2</v>
+      </c>
       <c r="D214" s="66"/>
-      <c r="E214" s="66"/>
-      <c r="F214" s="66"/>
-      <c r="G214" s="68"/>
-      <c r="H214" s="8"/>
-      <c r="I214" s="8"/>
+      <c r="E214" s="66" t="s">
+        <v>849</v>
+      </c>
+      <c r="F214" s="66" t="s">
+        <v>855</v>
+      </c>
+      <c r="G214" s="68" t="s">
+        <v>850</v>
+      </c>
+      <c r="H214" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I214" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="J214" s="8"/>
       <c r="K214" s="2"/>
     </row>
@@ -10181,25 +10284,39 @@
       <c r="A215" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B215" s="2"/>
-      <c r="C215" s="69"/>
-      <c r="D215" s="2"/>
-      <c r="E215" s="2"/>
-      <c r="F215" s="2"/>
-      <c r="G215" s="2"/>
-      <c r="H215" s="70"/>
-      <c r="I215" s="70"/>
+      <c r="B215" s="63" t="s">
+        <v>856</v>
+      </c>
+      <c r="C215" s="184">
+        <v>2</v>
+      </c>
+      <c r="D215" s="63"/>
+      <c r="E215" s="63" t="s">
+        <v>857</v>
+      </c>
+      <c r="F215" s="63" t="s">
+        <v>859</v>
+      </c>
+      <c r="G215" s="65" t="s">
+        <v>860</v>
+      </c>
+      <c r="H215" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I215" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="216" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A216" s="2" t="s">
+      <c r="A216" s="21" t="s">
         <v>396</v>
       </c>
-      <c r="B216" s="2"/>
-      <c r="C216" s="69"/>
-      <c r="D216" s="2"/>
-      <c r="E216" s="2"/>
-      <c r="F216" s="2"/>
-      <c r="G216" s="2"/>
+      <c r="B216" s="66"/>
+      <c r="C216" s="67"/>
+      <c r="D216" s="66"/>
+      <c r="E216" s="66"/>
+      <c r="F216" s="66"/>
+      <c r="G216" s="68"/>
       <c r="H216" s="70"/>
       <c r="I216" s="70"/>
     </row>
@@ -16617,50 +16734,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="156" t="s">
         <v>626</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="172"/>
-      <c r="E1" s="172"/>
-      <c r="F1" s="172"/>
-      <c r="G1" s="172"/>
-      <c r="H1" s="172"/>
-      <c r="I1" s="173"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="158"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="159" t="s">
         <v>627</v>
       </c>
-      <c r="B2" s="159"/>
+      <c r="B2" s="160"/>
       <c r="C2" s="80" t="s">
         <v>628</v>
       </c>
-      <c r="D2" s="175" t="s">
+      <c r="D2" s="161" t="s">
         <v>629</v>
       </c>
       <c r="E2" s="162"/>
       <c r="F2" s="162"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="176" t="s">
+      <c r="G2" s="160"/>
+      <c r="H2" s="163" t="s">
         <v>630</v>
       </c>
-      <c r="I2" s="163"/>
+      <c r="I2" s="164"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A4" s="177" t="s">
+      <c r="A4" s="165" t="s">
         <v>631</v>
       </c>
-      <c r="B4" s="172"/>
-      <c r="C4" s="172"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
-      <c r="F4" s="172"/>
-      <c r="G4" s="172"/>
-      <c r="H4" s="172"/>
-      <c r="I4" s="173"/>
+      <c r="B4" s="157"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="157"/>
+      <c r="E4" s="157"/>
+      <c r="F4" s="157"/>
+      <c r="G4" s="157"/>
+      <c r="H4" s="157"/>
+      <c r="I4" s="158"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="81" t="s">
@@ -16722,15 +16839,15 @@
       <c r="I6" s="87" t="s">
         <v>648</v>
       </c>
-      <c r="K6" s="165" t="s">
+      <c r="K6" s="166" t="s">
         <v>649</v>
       </c>
-      <c r="L6" s="166"/>
-      <c r="M6" s="166"/>
-      <c r="N6" s="166"/>
-      <c r="O6" s="166"/>
-      <c r="P6" s="166"/>
-      <c r="Q6" s="166"/>
+      <c r="L6" s="167"/>
+      <c r="M6" s="167"/>
+      <c r="N6" s="167"/>
+      <c r="O6" s="167"/>
+      <c r="P6" s="167"/>
+      <c r="Q6" s="167"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="A7" s="85">
@@ -16760,15 +16877,15 @@
       <c r="I7" s="87" t="s">
         <v>657</v>
       </c>
-      <c r="K7" s="165" t="s">
+      <c r="K7" s="166" t="s">
         <v>658</v>
       </c>
-      <c r="L7" s="166"/>
-      <c r="M7" s="166"/>
-      <c r="N7" s="166"/>
-      <c r="O7" s="166"/>
-      <c r="P7" s="166"/>
-      <c r="Q7" s="166"/>
+      <c r="L7" s="167"/>
+      <c r="M7" s="167"/>
+      <c r="N7" s="167"/>
+      <c r="O7" s="167"/>
+      <c r="P7" s="167"/>
+      <c r="Q7" s="167"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="85">
@@ -16876,17 +16993,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A15" s="167" t="s">
+      <c r="A15" s="168" t="s">
         <v>667</v>
       </c>
-      <c r="B15" s="168"/>
-      <c r="C15" s="168"/>
-      <c r="D15" s="168"/>
-      <c r="E15" s="168"/>
-      <c r="F15" s="168"/>
-      <c r="G15" s="168"/>
-      <c r="H15" s="168"/>
-      <c r="I15" s="169"/>
+      <c r="B15" s="169"/>
+      <c r="C15" s="169"/>
+      <c r="D15" s="169"/>
+      <c r="E15" s="169"/>
+      <c r="F15" s="169"/>
+      <c r="G15" s="169"/>
+      <c r="H15" s="169"/>
+      <c r="I15" s="170"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="A16" s="81" t="s">
@@ -16901,15 +17018,15 @@
       <c r="D16" s="82" t="s">
         <v>639</v>
       </c>
-      <c r="E16" s="170" t="s">
+      <c r="E16" s="171" t="s">
         <v>668</v>
       </c>
-      <c r="F16" s="157"/>
-      <c r="G16" s="170" t="s">
+      <c r="F16" s="172"/>
+      <c r="G16" s="171" t="s">
         <v>669</v>
       </c>
-      <c r="H16" s="160"/>
-      <c r="I16" s="161"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="174"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="92">
@@ -16924,15 +17041,15 @@
       <c r="D17" s="86" t="s">
         <v>666</v>
       </c>
-      <c r="E17" s="164" t="s">
+      <c r="E17" s="175" t="s">
         <v>671</v>
       </c>
-      <c r="F17" s="157"/>
-      <c r="G17" s="164" t="s">
+      <c r="F17" s="172"/>
+      <c r="G17" s="175" t="s">
         <v>672</v>
       </c>
-      <c r="H17" s="160"/>
-      <c r="I17" s="161"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="174"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1">
       <c r="A18" s="92">
@@ -16947,15 +17064,15 @@
       <c r="D18" s="86" t="s">
         <v>666</v>
       </c>
-      <c r="E18" s="164" t="s">
+      <c r="E18" s="175" t="s">
         <v>671</v>
       </c>
-      <c r="F18" s="157"/>
-      <c r="G18" s="164" t="s">
+      <c r="F18" s="172"/>
+      <c r="G18" s="175" t="s">
         <v>674</v>
       </c>
-      <c r="H18" s="160"/>
-      <c r="I18" s="161"/>
+      <c r="H18" s="173"/>
+      <c r="I18" s="174"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1">
       <c r="A19" s="92">
@@ -16970,15 +17087,15 @@
       <c r="D19" s="86" t="s">
         <v>676</v>
       </c>
-      <c r="E19" s="164" t="s">
+      <c r="E19" s="175" t="s">
         <v>677</v>
       </c>
-      <c r="F19" s="157"/>
-      <c r="G19" s="164" t="s">
+      <c r="F19" s="172"/>
+      <c r="G19" s="175" t="s">
         <v>678</v>
       </c>
-      <c r="H19" s="160"/>
-      <c r="I19" s="161"/>
+      <c r="H19" s="173"/>
+      <c r="I19" s="174"/>
       <c r="K19" s="84" t="s">
         <v>679</v>
       </c>
@@ -16990,11 +17107,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="156"/>
-      <c r="F20" s="157"/>
-      <c r="G20" s="156"/>
-      <c r="H20" s="160"/>
-      <c r="I20" s="161"/>
+      <c r="E20" s="176"/>
+      <c r="F20" s="172"/>
+      <c r="G20" s="176"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="174"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" s="92">
@@ -17003,11 +17120,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="156"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="156"/>
-      <c r="H21" s="160"/>
-      <c r="I21" s="161"/>
+      <c r="E21" s="176"/>
+      <c r="F21" s="172"/>
+      <c r="G21" s="176"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="174"/>
       <c r="K21" s="84" t="s">
         <v>680</v>
       </c>
@@ -17019,11 +17136,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="156"/>
-      <c r="F22" s="157"/>
-      <c r="G22" s="156"/>
-      <c r="H22" s="160"/>
-      <c r="I22" s="161"/>
+      <c r="E22" s="176"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="176"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="174"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1">
       <c r="A23" s="92">
@@ -17032,11 +17149,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="156"/>
-      <c r="F23" s="157"/>
-      <c r="G23" s="156"/>
-      <c r="H23" s="160"/>
-      <c r="I23" s="161"/>
+      <c r="E23" s="176"/>
+      <c r="F23" s="172"/>
+      <c r="G23" s="176"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="174"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" s="92">
@@ -17045,11 +17162,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="160"/>
-      <c r="I24" s="161"/>
+      <c r="E24" s="176"/>
+      <c r="F24" s="172"/>
+      <c r="G24" s="176"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="174"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" s="92">
@@ -17058,11 +17175,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="156"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="156"/>
-      <c r="H25" s="160"/>
-      <c r="I25" s="161"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="172"/>
+      <c r="G25" s="176"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="174"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" s="94">
@@ -17071,11 +17188,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="158"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="158"/>
+      <c r="E26" s="177"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="177"/>
       <c r="H26" s="162"/>
-      <c r="I26" s="163"/>
+      <c r="I26" s="164"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
@@ -18053,16 +18170,14 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18075,14 +18190,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21229,7 +21346,7 @@
       <c r="B2" s="180" t="s">
         <v>691</v>
       </c>
-      <c r="C2" s="157"/>
+      <c r="C2" s="172"/>
       <c r="O2" s="84" t="s">
         <v>692</v>
       </c>
@@ -22446,8 +22563,8 @@
       <c r="A3" s="180" t="s">
         <v>724</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="157"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="172"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="116" t="s">
@@ -22456,7 +22573,7 @@
       <c r="B4" s="182" t="s">
         <v>725</v>
       </c>
-      <c r="C4" s="157"/>
+      <c r="C4" s="172"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="117" t="s">
@@ -22465,7 +22582,7 @@
       <c r="B5" s="181" t="s">
         <v>727</v>
       </c>
-      <c r="C5" s="157"/>
+      <c r="C5" s="172"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="117" t="s">
@@ -22474,7 +22591,7 @@
       <c r="B6" s="181" t="s">
         <v>729</v>
       </c>
-      <c r="C6" s="157"/>
+      <c r="C6" s="172"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="117" t="s">
@@ -22483,7 +22600,7 @@
       <c r="B7" s="181" t="s">
         <v>731</v>
       </c>
-      <c r="C7" s="157"/>
+      <c r="C7" s="172"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="117" t="s">
@@ -22492,7 +22609,7 @@
       <c r="B8" s="181" t="s">
         <v>733</v>
       </c>
-      <c r="C8" s="157"/>
+      <c r="C8" s="172"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
@@ -23523,8 +23640,8 @@
       <c r="B2" s="183" t="s">
         <v>734</v>
       </c>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="158"/>
       <c r="J2" s="84" t="s">
         <v>692</v>
       </c>
@@ -27676,8 +27793,8 @@
       <c r="A5" s="182" t="s">
         <v>767</v>
       </c>
-      <c r="B5" s="160"/>
-      <c r="C5" s="157"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="172"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
chg: Updated target list with more tgts for Jonde. Updated introduction brief, added information about Xilong and the Xilong flag
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="857">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -3800,20 +3800,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3827,22 +3832,17 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3892,7 +3892,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3926,7 +3926,7 @@
         <xdr:cNvPr id="3" name="image2.png" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3965,7 +3965,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3999,7 +3999,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4038,7 +4038,7 @@
         <xdr:cNvPr id="2" name="image10.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4072,7 +4072,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4111,7 +4111,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4268,7 +4268,7 @@
         <xdr:cNvPr id="4" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4302,7 +4302,7 @@
         <xdr:cNvPr id="5" name="image6.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4341,7 +4341,7 @@
         <xdr:cNvPr id="4" name="Shape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4498,7 +4498,7 @@
         <xdr:cNvPr id="3" name="image8.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4532,7 +4532,7 @@
         <xdr:cNvPr id="5" name="image9.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4571,7 +4571,7 @@
         <xdr:cNvPr id="5" name="Shape 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4752,7 +4752,7 @@
         <xdr:cNvPr id="3" name="image7.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4786,7 +4786,7 @@
         <xdr:cNvPr id="4" name="image14.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4825,7 +4825,7 @@
         <xdr:cNvPr id="6" name="Shape 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4946,7 +4946,7 @@
         <xdr:cNvPr id="3" name="image13.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4980,7 +4980,7 @@
         <xdr:cNvPr id="4" name="image11.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5014,7 +5014,7 @@
         <xdr:cNvPr id="5" name="image12.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5239,10 +5239,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C93" sqref="C93"/>
+      <selection pane="bottomRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -5360,7 +5360,9 @@
         <v>22</v>
       </c>
       <c r="J4" s="8"/>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="14.25">
       <c r="A5" s="21" t="s">
@@ -5792,7 +5794,9 @@
         <v>22</v>
       </c>
       <c r="J18" s="8"/>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="19" spans="1:26" ht="14.25">
       <c r="A19" s="21" t="s">
@@ -6059,7 +6063,9 @@
         <v>22</v>
       </c>
       <c r="J27" s="8"/>
-      <c r="K27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
@@ -6088,7 +6094,9 @@
         <v>22</v>
       </c>
       <c r="J28" s="8"/>
-      <c r="K28" s="2"/>
+      <c r="K28" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="21" t="s">
@@ -6117,7 +6125,9 @@
         <v>22</v>
       </c>
       <c r="J29" s="8"/>
-      <c r="K29" s="2"/>
+      <c r="K29" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
@@ -6146,7 +6156,9 @@
         <v>22</v>
       </c>
       <c r="J30" s="8"/>
-      <c r="K30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="21" t="s">
@@ -6248,7 +6260,9 @@
         <v>22</v>
       </c>
       <c r="J33" s="41"/>
-      <c r="K33" s="33"/>
+      <c r="K33" s="33" t="s">
+        <v>363</v>
+      </c>
       <c r="L33" s="34"/>
       <c r="M33" s="34"/>
       <c r="N33" s="34"/>
@@ -6847,7 +6861,9 @@
         <v>22</v>
       </c>
       <c r="J49" s="41"/>
-      <c r="K49" s="33"/>
+      <c r="K49" s="33" t="s">
+        <v>363</v>
+      </c>
       <c r="L49" s="34"/>
       <c r="M49" s="34"/>
       <c r="N49" s="34"/>
@@ -6891,7 +6907,9 @@
         <v>22</v>
       </c>
       <c r="J50" s="8"/>
-      <c r="K50" s="2"/>
+      <c r="K50" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="21" t="s">
@@ -7111,7 +7129,9 @@
         <v>22</v>
       </c>
       <c r="J57" s="8"/>
-      <c r="K57" s="2"/>
+      <c r="K57" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1">
       <c r="A58" s="2" t="s">
@@ -8282,7 +8302,9 @@
         <v>22</v>
       </c>
       <c r="J96" s="8"/>
-      <c r="K96" s="2"/>
+      <c r="K96" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="97" spans="1:11" ht="15.75" customHeight="1">
       <c r="A97" s="21" t="s">
@@ -16798,50 +16820,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="157" t="s">
         <v>620</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="174"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="159"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="160" t="s">
         <v>621</v>
       </c>
-      <c r="B2" s="160"/>
+      <c r="B2" s="161"/>
       <c r="C2" s="80" t="s">
         <v>622</v>
       </c>
-      <c r="D2" s="176" t="s">
+      <c r="D2" s="162" t="s">
         <v>623</v>
       </c>
       <c r="E2" s="163"/>
       <c r="F2" s="163"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="177" t="s">
+      <c r="G2" s="161"/>
+      <c r="H2" s="164" t="s">
         <v>624</v>
       </c>
-      <c r="I2" s="164"/>
+      <c r="I2" s="165"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="166" t="s">
         <v>625</v>
       </c>
-      <c r="B4" s="173"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="174"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="159"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="81" t="s">
@@ -16903,15 +16925,15 @@
       <c r="I6" s="87" t="s">
         <v>642</v>
       </c>
-      <c r="K6" s="166" t="s">
+      <c r="K6" s="167" t="s">
         <v>643</v>
       </c>
-      <c r="L6" s="167"/>
-      <c r="M6" s="167"/>
-      <c r="N6" s="167"/>
-      <c r="O6" s="167"/>
-      <c r="P6" s="167"/>
-      <c r="Q6" s="167"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="A7" s="85">
@@ -16941,15 +16963,15 @@
       <c r="I7" s="87" t="s">
         <v>651</v>
       </c>
-      <c r="K7" s="166" t="s">
+      <c r="K7" s="167" t="s">
         <v>652</v>
       </c>
-      <c r="L7" s="167"/>
-      <c r="M7" s="167"/>
-      <c r="N7" s="167"/>
-      <c r="O7" s="167"/>
-      <c r="P7" s="167"/>
-      <c r="Q7" s="167"/>
+      <c r="L7" s="168"/>
+      <c r="M7" s="168"/>
+      <c r="N7" s="168"/>
+      <c r="O7" s="168"/>
+      <c r="P7" s="168"/>
+      <c r="Q7" s="168"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="85">
@@ -17057,17 +17079,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A15" s="168" t="s">
+      <c r="A15" s="169" t="s">
         <v>661</v>
       </c>
-      <c r="B15" s="169"/>
-      <c r="C15" s="169"/>
-      <c r="D15" s="169"/>
-      <c r="E15" s="169"/>
-      <c r="F15" s="169"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="170"/>
+      <c r="B15" s="170"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="170"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="170"/>
+      <c r="G15" s="170"/>
+      <c r="H15" s="170"/>
+      <c r="I15" s="171"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="A16" s="81" t="s">
@@ -17082,15 +17104,15 @@
       <c r="D16" s="82" t="s">
         <v>633</v>
       </c>
-      <c r="E16" s="171" t="s">
+      <c r="E16" s="172" t="s">
         <v>662</v>
       </c>
-      <c r="F16" s="158"/>
-      <c r="G16" s="171" t="s">
+      <c r="F16" s="173"/>
+      <c r="G16" s="172" t="s">
         <v>663</v>
       </c>
-      <c r="H16" s="161"/>
-      <c r="I16" s="162"/>
+      <c r="H16" s="174"/>
+      <c r="I16" s="175"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="92">
@@ -17105,15 +17127,15 @@
       <c r="D17" s="86" t="s">
         <v>660</v>
       </c>
-      <c r="E17" s="165" t="s">
+      <c r="E17" s="176" t="s">
         <v>665</v>
       </c>
-      <c r="F17" s="158"/>
-      <c r="G17" s="165" t="s">
+      <c r="F17" s="173"/>
+      <c r="G17" s="176" t="s">
         <v>666</v>
       </c>
-      <c r="H17" s="161"/>
-      <c r="I17" s="162"/>
+      <c r="H17" s="174"/>
+      <c r="I17" s="175"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1">
       <c r="A18" s="92">
@@ -17128,15 +17150,15 @@
       <c r="D18" s="86" t="s">
         <v>660</v>
       </c>
-      <c r="E18" s="165" t="s">
+      <c r="E18" s="176" t="s">
         <v>665</v>
       </c>
-      <c r="F18" s="158"/>
-      <c r="G18" s="165" t="s">
+      <c r="F18" s="173"/>
+      <c r="G18" s="176" t="s">
         <v>668</v>
       </c>
-      <c r="H18" s="161"/>
-      <c r="I18" s="162"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="175"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1">
       <c r="A19" s="92">
@@ -17151,15 +17173,15 @@
       <c r="D19" s="86" t="s">
         <v>670</v>
       </c>
-      <c r="E19" s="165" t="s">
+      <c r="E19" s="176" t="s">
         <v>671</v>
       </c>
-      <c r="F19" s="158"/>
-      <c r="G19" s="165" t="s">
+      <c r="F19" s="173"/>
+      <c r="G19" s="176" t="s">
         <v>672</v>
       </c>
-      <c r="H19" s="161"/>
-      <c r="I19" s="162"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="175"/>
       <c r="K19" s="84" t="s">
         <v>673</v>
       </c>
@@ -17171,11 +17193,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="157"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="162"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="175"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" s="92">
@@ -17184,11 +17206,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="162"/>
+      <c r="E21" s="177"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="174"/>
+      <c r="I21" s="175"/>
       <c r="K21" s="84" t="s">
         <v>674</v>
       </c>
@@ -17200,11 +17222,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="157"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="157"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="162"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="174"/>
+      <c r="I22" s="175"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1">
       <c r="A23" s="92">
@@ -17213,11 +17235,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="157"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="162"/>
+      <c r="E23" s="177"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="174"/>
+      <c r="I23" s="175"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" s="92">
@@ -17226,11 +17248,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="162"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="174"/>
+      <c r="I24" s="175"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" s="92">
@@ -17239,11 +17261,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="162"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="173"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="174"/>
+      <c r="I25" s="175"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" s="94">
@@ -17252,11 +17274,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="159"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="161"/>
+      <c r="G26" s="178"/>
       <c r="H26" s="163"/>
-      <c r="I26" s="164"/>
+      <c r="I26" s="165"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
@@ -18234,16 +18256,14 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18256,14 +18276,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21410,7 +21432,7 @@
       <c r="B2" s="181" t="s">
         <v>685</v>
       </c>
-      <c r="C2" s="158"/>
+      <c r="C2" s="173"/>
       <c r="O2" s="84" t="s">
         <v>686</v>
       </c>
@@ -22627,8 +22649,8 @@
       <c r="A3" s="181" t="s">
         <v>718</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="158"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="173"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="116" t="s">
@@ -22637,7 +22659,7 @@
       <c r="B4" s="183" t="s">
         <v>719</v>
       </c>
-      <c r="C4" s="158"/>
+      <c r="C4" s="173"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="117" t="s">
@@ -22646,7 +22668,7 @@
       <c r="B5" s="182" t="s">
         <v>721</v>
       </c>
-      <c r="C5" s="158"/>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="117" t="s">
@@ -22655,7 +22677,7 @@
       <c r="B6" s="182" t="s">
         <v>723</v>
       </c>
-      <c r="C6" s="158"/>
+      <c r="C6" s="173"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="117" t="s">
@@ -22664,7 +22686,7 @@
       <c r="B7" s="182" t="s">
         <v>725</v>
       </c>
-      <c r="C7" s="158"/>
+      <c r="C7" s="173"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="117" t="s">
@@ -22673,7 +22695,7 @@
       <c r="B8" s="182" t="s">
         <v>727</v>
       </c>
-      <c r="C8" s="158"/>
+      <c r="C8" s="173"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
@@ -23704,8 +23726,8 @@
       <c r="B2" s="184" t="s">
         <v>728</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="159"/>
       <c r="J2" s="84" t="s">
         <v>686</v>
       </c>
@@ -27857,8 +27879,8 @@
       <c r="A5" s="183" t="s">
         <v>761</v>
       </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="158"/>
+      <c r="B5" s="174"/>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
chg: Added 4 targets (Air Division HQs) to OPAC.miz, JTL, OPAC DPIs for CF, updated introductionary brief, updated DPIs for target folder, continued work on OPAC_VID_INTREP-002 Notian Air Assets
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="873">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -2621,6 +2621,54 @@
   </si>
   <si>
     <t>Kola Bay</t>
+  </si>
+  <si>
+    <t>40th Composite Maritime Aviation Division HQ</t>
+  </si>
+  <si>
+    <t>60th Air Division HQ</t>
+  </si>
+  <si>
+    <t>70th Air Division HQ</t>
+  </si>
+  <si>
+    <t>80th Air Support Division HQ</t>
+  </si>
+  <si>
+    <t>280ft</t>
+  </si>
+  <si>
+    <t>216ft</t>
+  </si>
+  <si>
+    <t>161ft</t>
+  </si>
+  <si>
+    <t>N 69 04.364 E 033 24.593</t>
+  </si>
+  <si>
+    <t>N 69 05.012 E 033 28.750</t>
+  </si>
+  <si>
+    <t>N 69 03.978 E 033 25.054</t>
+  </si>
+  <si>
+    <t>N 68 48.916 E 032 49.370</t>
+  </si>
+  <si>
+    <t>206ft</t>
+  </si>
+  <si>
+    <t>HQ for 40th Composite Maritime Aviation Division</t>
+  </si>
+  <si>
+    <t>HQ for 60th Air Division</t>
+  </si>
+  <si>
+    <t>HQ for 70th Air Divison</t>
+  </si>
+  <si>
+    <t>HQ for 80th Air Support Division</t>
   </si>
 </sst>
 </file>
@@ -3800,20 +3848,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3827,22 +3880,17 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3892,7 +3940,7 @@
         <xdr:cNvPr id="2" name="image1.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3926,7 +3974,7 @@
         <xdr:cNvPr id="3" name="image2.png" descr="JFACC symbol.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3965,7 +4013,7 @@
         <xdr:cNvPr id="2" name="image3.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3999,7 +4047,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4038,7 +4086,7 @@
         <xdr:cNvPr id="2" name="image10.png" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4072,7 +4120,7 @@
         <xdr:cNvPr id="3" name="image5.png" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4111,7 +4159,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4268,7 +4316,7 @@
         <xdr:cNvPr id="4" name="image4.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4302,7 +4350,7 @@
         <xdr:cNvPr id="5" name="image6.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4341,7 +4389,7 @@
         <xdr:cNvPr id="4" name="Shape 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4498,7 +4546,7 @@
         <xdr:cNvPr id="3" name="image8.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4532,7 +4580,7 @@
         <xdr:cNvPr id="5" name="image9.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4571,7 +4619,7 @@
         <xdr:cNvPr id="5" name="Shape 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4752,7 +4800,7 @@
         <xdr:cNvPr id="3" name="image7.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4786,7 +4834,7 @@
         <xdr:cNvPr id="4" name="image14.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4825,7 +4873,7 @@
         <xdr:cNvPr id="6" name="Shape 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4946,7 +4994,7 @@
         <xdr:cNvPr id="3" name="image13.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4980,7 +5028,7 @@
         <xdr:cNvPr id="4" name="image11.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5014,7 +5062,7 @@
         <xdr:cNvPr id="5" name="image12.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5239,10 +5287,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B207" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -10405,64 +10453,120 @@
       <c r="A216" s="21" t="s">
         <v>390</v>
       </c>
-      <c r="B216" s="66"/>
-      <c r="C216" s="67"/>
+      <c r="B216" s="66" t="s">
+        <v>857</v>
+      </c>
+      <c r="C216" s="67">
+        <v>2</v>
+      </c>
       <c r="D216" s="66"/>
-      <c r="E216" s="66"/>
-      <c r="F216" s="66"/>
-      <c r="G216" s="68"/>
-      <c r="H216" s="70"/>
-      <c r="I216" s="70"/>
+      <c r="E216" s="66" t="s">
+        <v>869</v>
+      </c>
+      <c r="F216" s="66" t="s">
+        <v>864</v>
+      </c>
+      <c r="G216" s="68" t="s">
+        <v>862</v>
+      </c>
+      <c r="H216" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I216" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="217" spans="1:11" ht="15.75" customHeight="1">
       <c r="A217" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B217" s="2"/>
-      <c r="C217" s="69"/>
+      <c r="B217" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="C217" s="69">
+        <v>2</v>
+      </c>
       <c r="D217" s="2"/>
-      <c r="E217" s="2"/>
-      <c r="F217" s="2"/>
-      <c r="G217" s="2"/>
-      <c r="H217" s="70"/>
-      <c r="I217" s="70"/>
+      <c r="E217" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="F217" s="63" t="s">
+        <v>865</v>
+      </c>
+      <c r="G217" s="65" t="s">
+        <v>863</v>
+      </c>
+      <c r="H217" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I217" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="218" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A218" s="2" t="s">
+      <c r="A218" s="21" t="s">
         <v>392</v>
       </c>
-      <c r="B218" s="2"/>
-      <c r="C218" s="69"/>
-      <c r="D218" s="2"/>
-      <c r="E218" s="2"/>
-      <c r="F218" s="2"/>
-      <c r="G218" s="2"/>
-      <c r="H218" s="70"/>
-      <c r="I218" s="70"/>
+      <c r="B218" s="66" t="s">
+        <v>859</v>
+      </c>
+      <c r="C218" s="67">
+        <v>2</v>
+      </c>
+      <c r="D218" s="66"/>
+      <c r="E218" s="66" t="s">
+        <v>871</v>
+      </c>
+      <c r="F218" s="66" t="s">
+        <v>866</v>
+      </c>
+      <c r="G218" s="68" t="s">
+        <v>861</v>
+      </c>
+      <c r="H218" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I218" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="219" spans="1:11" ht="15.75" customHeight="1">
       <c r="A219" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B219" s="2"/>
-      <c r="C219" s="69"/>
+      <c r="B219" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="C219" s="69">
+        <v>2</v>
+      </c>
       <c r="D219" s="2"/>
-      <c r="E219" s="2"/>
-      <c r="F219" s="2"/>
-      <c r="G219" s="2"/>
-      <c r="H219" s="70"/>
-      <c r="I219" s="70"/>
+      <c r="E219" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="F219" s="63" t="s">
+        <v>867</v>
+      </c>
+      <c r="G219" s="65" t="s">
+        <v>868</v>
+      </c>
+      <c r="H219" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I219" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="220" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A220" s="2" t="s">
+      <c r="A220" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="B220" s="2"/>
-      <c r="C220" s="69"/>
-      <c r="D220" s="2"/>
-      <c r="E220" s="2"/>
-      <c r="F220" s="2"/>
-      <c r="G220" s="2"/>
+      <c r="B220" s="66"/>
+      <c r="C220" s="67"/>
+      <c r="D220" s="66"/>
+      <c r="E220" s="66"/>
+      <c r="F220" s="66"/>
+      <c r="G220" s="68"/>
       <c r="H220" s="70"/>
       <c r="I220" s="70"/>
     </row>
@@ -16828,50 +16932,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="157" t="s">
         <v>620</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="174"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="159"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="160" t="s">
         <v>621</v>
       </c>
-      <c r="B2" s="160"/>
+      <c r="B2" s="161"/>
       <c r="C2" s="80" t="s">
         <v>622</v>
       </c>
-      <c r="D2" s="176" t="s">
+      <c r="D2" s="162" t="s">
         <v>623</v>
       </c>
       <c r="E2" s="163"/>
       <c r="F2" s="163"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="177" t="s">
+      <c r="G2" s="161"/>
+      <c r="H2" s="164" t="s">
         <v>624</v>
       </c>
-      <c r="I2" s="164"/>
+      <c r="I2" s="165"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="166" t="s">
         <v>625</v>
       </c>
-      <c r="B4" s="173"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="174"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="159"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="81" t="s">
@@ -16933,15 +17037,15 @@
       <c r="I6" s="87" t="s">
         <v>642</v>
       </c>
-      <c r="K6" s="166" t="s">
+      <c r="K6" s="167" t="s">
         <v>643</v>
       </c>
-      <c r="L6" s="167"/>
-      <c r="M6" s="167"/>
-      <c r="N6" s="167"/>
-      <c r="O6" s="167"/>
-      <c r="P6" s="167"/>
-      <c r="Q6" s="167"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1">
       <c r="A7" s="85">
@@ -16971,15 +17075,15 @@
       <c r="I7" s="87" t="s">
         <v>651</v>
       </c>
-      <c r="K7" s="166" t="s">
+      <c r="K7" s="167" t="s">
         <v>652</v>
       </c>
-      <c r="L7" s="167"/>
-      <c r="M7" s="167"/>
-      <c r="N7" s="167"/>
-      <c r="O7" s="167"/>
-      <c r="P7" s="167"/>
-      <c r="Q7" s="167"/>
+      <c r="L7" s="168"/>
+      <c r="M7" s="168"/>
+      <c r="N7" s="168"/>
+      <c r="O7" s="168"/>
+      <c r="P7" s="168"/>
+      <c r="Q7" s="168"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1">
       <c r="A8" s="85">
@@ -17087,17 +17191,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1">
-      <c r="A15" s="168" t="s">
+      <c r="A15" s="169" t="s">
         <v>661</v>
       </c>
-      <c r="B15" s="169"/>
-      <c r="C15" s="169"/>
-      <c r="D15" s="169"/>
-      <c r="E15" s="169"/>
-      <c r="F15" s="169"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="170"/>
+      <c r="B15" s="170"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="170"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="170"/>
+      <c r="G15" s="170"/>
+      <c r="H15" s="170"/>
+      <c r="I15" s="171"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1">
       <c r="A16" s="81" t="s">
@@ -17112,15 +17216,15 @@
       <c r="D16" s="82" t="s">
         <v>633</v>
       </c>
-      <c r="E16" s="171" t="s">
+      <c r="E16" s="172" t="s">
         <v>662</v>
       </c>
-      <c r="F16" s="158"/>
-      <c r="G16" s="171" t="s">
+      <c r="F16" s="173"/>
+      <c r="G16" s="172" t="s">
         <v>663</v>
       </c>
-      <c r="H16" s="161"/>
-      <c r="I16" s="162"/>
+      <c r="H16" s="174"/>
+      <c r="I16" s="175"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1">
       <c r="A17" s="92">
@@ -17135,15 +17239,15 @@
       <c r="D17" s="86" t="s">
         <v>660</v>
       </c>
-      <c r="E17" s="165" t="s">
+      <c r="E17" s="176" t="s">
         <v>665</v>
       </c>
-      <c r="F17" s="158"/>
-      <c r="G17" s="165" t="s">
+      <c r="F17" s="173"/>
+      <c r="G17" s="176" t="s">
         <v>666</v>
       </c>
-      <c r="H17" s="161"/>
-      <c r="I17" s="162"/>
+      <c r="H17" s="174"/>
+      <c r="I17" s="175"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1">
       <c r="A18" s="92">
@@ -17158,15 +17262,15 @@
       <c r="D18" s="86" t="s">
         <v>660</v>
       </c>
-      <c r="E18" s="165" t="s">
+      <c r="E18" s="176" t="s">
         <v>665</v>
       </c>
-      <c r="F18" s="158"/>
-      <c r="G18" s="165" t="s">
+      <c r="F18" s="173"/>
+      <c r="G18" s="176" t="s">
         <v>668</v>
       </c>
-      <c r="H18" s="161"/>
-      <c r="I18" s="162"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="175"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1">
       <c r="A19" s="92">
@@ -17181,15 +17285,15 @@
       <c r="D19" s="86" t="s">
         <v>670</v>
       </c>
-      <c r="E19" s="165" t="s">
+      <c r="E19" s="176" t="s">
         <v>671</v>
       </c>
-      <c r="F19" s="158"/>
-      <c r="G19" s="165" t="s">
+      <c r="F19" s="173"/>
+      <c r="G19" s="176" t="s">
         <v>672</v>
       </c>
-      <c r="H19" s="161"/>
-      <c r="I19" s="162"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="175"/>
       <c r="K19" s="84" t="s">
         <v>673</v>
       </c>
@@ -17201,11 +17305,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="157"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="162"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="175"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1">
       <c r="A21" s="92">
@@ -17214,11 +17318,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="162"/>
+      <c r="E21" s="177"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="174"/>
+      <c r="I21" s="175"/>
       <c r="K21" s="84" t="s">
         <v>674</v>
       </c>
@@ -17230,11 +17334,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="157"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="157"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="162"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="174"/>
+      <c r="I22" s="175"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1">
       <c r="A23" s="92">
@@ -17243,11 +17347,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="157"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="162"/>
+      <c r="E23" s="177"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="174"/>
+      <c r="I23" s="175"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1">
       <c r="A24" s="92">
@@ -17256,11 +17360,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="162"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="174"/>
+      <c r="I24" s="175"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1">
       <c r="A25" s="92">
@@ -17269,11 +17373,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="162"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="173"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="174"/>
+      <c r="I25" s="175"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1">
       <c r="A26" s="94">
@@ -17282,11 +17386,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="159"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="161"/>
+      <c r="G26" s="178"/>
       <c r="H26" s="163"/>
-      <c r="I26" s="164"/>
+      <c r="I26" s="165"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
@@ -18264,16 +18368,14 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18286,14 +18388,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21440,7 +21544,7 @@
       <c r="B2" s="181" t="s">
         <v>685</v>
       </c>
-      <c r="C2" s="158"/>
+      <c r="C2" s="173"/>
       <c r="O2" s="84" t="s">
         <v>686</v>
       </c>
@@ -22657,8 +22761,8 @@
       <c r="A3" s="181" t="s">
         <v>718</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="158"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="173"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1">
       <c r="A4" s="116" t="s">
@@ -22667,7 +22771,7 @@
       <c r="B4" s="183" t="s">
         <v>719</v>
       </c>
-      <c r="C4" s="158"/>
+      <c r="C4" s="173"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="117" t="s">
@@ -22676,7 +22780,7 @@
       <c r="B5" s="182" t="s">
         <v>721</v>
       </c>
-      <c r="C5" s="158"/>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="117" t="s">
@@ -22685,7 +22789,7 @@
       <c r="B6" s="182" t="s">
         <v>723</v>
       </c>
-      <c r="C6" s="158"/>
+      <c r="C6" s="173"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="117" t="s">
@@ -22694,7 +22798,7 @@
       <c r="B7" s="182" t="s">
         <v>725</v>
       </c>
-      <c r="C7" s="158"/>
+      <c r="C7" s="173"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="117" t="s">
@@ -22703,7 +22807,7 @@
       <c r="B8" s="182" t="s">
         <v>727</v>
       </c>
-      <c r="C8" s="158"/>
+      <c r="C8" s="173"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1"/>
@@ -23734,8 +23838,8 @@
       <c r="B2" s="184" t="s">
         <v>728</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="159"/>
       <c r="J2" s="84" t="s">
         <v>686</v>
       </c>
@@ -27887,8 +27991,8 @@
       <c r="A5" s="183" t="s">
         <v>761</v>
       </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="158"/>
+      <c r="B5" s="174"/>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
Added SRNTGT001 target folder
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olahe\Git-projects\OPAT-background\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C635E93-9D77-48F6-84B7-51632BBABD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656776C2-3F28-4EB1-8426-0368D61853EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="873">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -3854,20 +3854,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3881,22 +3886,17 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5293,10 +5293,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5727,7 +5727,9 @@
       <c r="I14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="8"/>
+      <c r="J14" s="143" t="s">
+        <v>63</v>
+      </c>
       <c r="K14" s="2" t="s">
         <v>27</v>
       </c>
@@ -16940,50 +16942,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="157" t="s">
         <v>620</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="174"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="159"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="160" t="s">
         <v>621</v>
       </c>
-      <c r="B2" s="160"/>
+      <c r="B2" s="161"/>
       <c r="C2" s="80" t="s">
         <v>622</v>
       </c>
-      <c r="D2" s="176" t="s">
+      <c r="D2" s="162" t="s">
         <v>623</v>
       </c>
       <c r="E2" s="163"/>
       <c r="F2" s="163"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="177" t="s">
+      <c r="G2" s="161"/>
+      <c r="H2" s="164" t="s">
         <v>624</v>
       </c>
-      <c r="I2" s="164"/>
+      <c r="I2" s="165"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="166" t="s">
         <v>625</v>
       </c>
-      <c r="B4" s="173"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="174"/>
+      <c r="B4" s="158"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="159"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -17045,15 +17047,15 @@
       <c r="I6" s="87" t="s">
         <v>642</v>
       </c>
-      <c r="K6" s="166" t="s">
+      <c r="K6" s="167" t="s">
         <v>643</v>
       </c>
-      <c r="L6" s="167"/>
-      <c r="M6" s="167"/>
-      <c r="N6" s="167"/>
-      <c r="O6" s="167"/>
-      <c r="P6" s="167"/>
-      <c r="Q6" s="167"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
@@ -17083,15 +17085,15 @@
       <c r="I7" s="87" t="s">
         <v>651</v>
       </c>
-      <c r="K7" s="166" t="s">
+      <c r="K7" s="167" t="s">
         <v>652</v>
       </c>
-      <c r="L7" s="167"/>
-      <c r="M7" s="167"/>
-      <c r="N7" s="167"/>
-      <c r="O7" s="167"/>
-      <c r="P7" s="167"/>
-      <c r="Q7" s="167"/>
+      <c r="L7" s="168"/>
+      <c r="M7" s="168"/>
+      <c r="N7" s="168"/>
+      <c r="O7" s="168"/>
+      <c r="P7" s="168"/>
+      <c r="Q7" s="168"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
@@ -17199,17 +17201,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="168" t="s">
+      <c r="A15" s="169" t="s">
         <v>661</v>
       </c>
-      <c r="B15" s="169"/>
-      <c r="C15" s="169"/>
-      <c r="D15" s="169"/>
-      <c r="E15" s="169"/>
-      <c r="F15" s="169"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="170"/>
+      <c r="B15" s="170"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="170"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="170"/>
+      <c r="G15" s="170"/>
+      <c r="H15" s="170"/>
+      <c r="I15" s="171"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
@@ -17224,15 +17226,15 @@
       <c r="D16" s="82" t="s">
         <v>633</v>
       </c>
-      <c r="E16" s="171" t="s">
+      <c r="E16" s="172" t="s">
         <v>662</v>
       </c>
-      <c r="F16" s="158"/>
-      <c r="G16" s="171" t="s">
+      <c r="F16" s="173"/>
+      <c r="G16" s="172" t="s">
         <v>663</v>
       </c>
-      <c r="H16" s="161"/>
-      <c r="I16" s="162"/>
+      <c r="H16" s="174"/>
+      <c r="I16" s="175"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -17247,15 +17249,15 @@
       <c r="D17" s="86" t="s">
         <v>660</v>
       </c>
-      <c r="E17" s="165" t="s">
+      <c r="E17" s="176" t="s">
         <v>665</v>
       </c>
-      <c r="F17" s="158"/>
-      <c r="G17" s="165" t="s">
+      <c r="F17" s="173"/>
+      <c r="G17" s="176" t="s">
         <v>666</v>
       </c>
-      <c r="H17" s="161"/>
-      <c r="I17" s="162"/>
+      <c r="H17" s="174"/>
+      <c r="I17" s="175"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -17270,15 +17272,15 @@
       <c r="D18" s="86" t="s">
         <v>660</v>
       </c>
-      <c r="E18" s="165" t="s">
+      <c r="E18" s="176" t="s">
         <v>665</v>
       </c>
-      <c r="F18" s="158"/>
-      <c r="G18" s="165" t="s">
+      <c r="F18" s="173"/>
+      <c r="G18" s="176" t="s">
         <v>668</v>
       </c>
-      <c r="H18" s="161"/>
-      <c r="I18" s="162"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="175"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
@@ -17293,15 +17295,15 @@
       <c r="D19" s="86" t="s">
         <v>670</v>
       </c>
-      <c r="E19" s="165" t="s">
+      <c r="E19" s="176" t="s">
         <v>671</v>
       </c>
-      <c r="F19" s="158"/>
-      <c r="G19" s="165" t="s">
+      <c r="F19" s="173"/>
+      <c r="G19" s="176" t="s">
         <v>672</v>
       </c>
-      <c r="H19" s="161"/>
-      <c r="I19" s="162"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="175"/>
       <c r="K19" s="84" t="s">
         <v>673</v>
       </c>
@@ -17313,11 +17315,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="157"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="162"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="175"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17326,11 +17328,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="162"/>
+      <c r="E21" s="177"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="174"/>
+      <c r="I21" s="175"/>
       <c r="K21" s="84" t="s">
         <v>674</v>
       </c>
@@ -17342,11 +17344,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="157"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="157"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="162"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="174"/>
+      <c r="I22" s="175"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17355,11 +17357,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="157"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="162"/>
+      <c r="E23" s="177"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="174"/>
+      <c r="I23" s="175"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17368,11 +17370,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="162"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="174"/>
+      <c r="I24" s="175"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17381,11 +17383,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="162"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="173"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="174"/>
+      <c r="I25" s="175"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17394,11 +17396,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="159"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="161"/>
+      <c r="G26" s="178"/>
       <c r="H26" s="163"/>
-      <c r="I26" s="164"/>
+      <c r="I26" s="165"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18376,16 +18378,14 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18398,14 +18398,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21552,7 +21554,7 @@
       <c r="B2" s="181" t="s">
         <v>685</v>
       </c>
-      <c r="C2" s="158"/>
+      <c r="C2" s="173"/>
       <c r="O2" s="84" t="s">
         <v>686</v>
       </c>
@@ -22769,8 +22771,8 @@
       <c r="A3" s="181" t="s">
         <v>718</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="158"/>
+      <c r="B3" s="174"/>
+      <c r="C3" s="173"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
@@ -22779,7 +22781,7 @@
       <c r="B4" s="183" t="s">
         <v>719</v>
       </c>
-      <c r="C4" s="158"/>
+      <c r="C4" s="173"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
@@ -22788,7 +22790,7 @@
       <c r="B5" s="182" t="s">
         <v>721</v>
       </c>
-      <c r="C5" s="158"/>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
@@ -22797,7 +22799,7 @@
       <c r="B6" s="182" t="s">
         <v>723</v>
       </c>
-      <c r="C6" s="158"/>
+      <c r="C6" s="173"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
@@ -22806,7 +22808,7 @@
       <c r="B7" s="182" t="s">
         <v>725</v>
       </c>
-      <c r="C7" s="158"/>
+      <c r="C7" s="173"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
@@ -22815,7 +22817,7 @@
       <c r="B8" s="182" t="s">
         <v>727</v>
       </c>
-      <c r="C8" s="158"/>
+      <c r="C8" s="173"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23846,8 +23848,8 @@
       <c r="B2" s="184" t="s">
         <v>728</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="159"/>
       <c r="J2" s="84" t="s">
         <v>686</v>
       </c>
@@ -27999,8 +28001,8 @@
       <c r="A5" s="183" t="s">
         <v>761</v>
       </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="158"/>
+      <c r="B5" s="174"/>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
Added SRNTGT012 target folder
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olahe\Git-projects\OPAT-background\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656776C2-3F28-4EB1-8426-0368D61853EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB998D72-24B0-4BD6-AA0D-D18C82ADD88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="873">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -5293,10 +5293,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5760,7 +5760,9 @@
       <c r="I15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="8"/>
+      <c r="J15" s="143" t="s">
+        <v>63</v>
+      </c>
       <c r="K15" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Added some DRK targets, 5th and 6th army relocated!
redesignated fuel docks for refinery, targets are in the xls, miz, and some in the KCAA but not yet in CF! Added and tested few buildings in TGT EFFECTS
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\OPAT-background\INTEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\_I\Dokumentumok\132\_OPAT\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6730BE-FE46-44C5-A4AD-D764794C6A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE339416-08C4-4A91-814C-9FF41324D4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAC Joint Target List" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="892">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -1561,18 +1561,12 @@
     <t>Kambiland Army 5th Corps HQ</t>
   </si>
   <si>
-    <t>N 66 04.039 E 033 05.437</t>
-  </si>
-  <si>
     <t>DRKTGT002</t>
   </si>
   <si>
     <t>Kambiland Army 6th Corps HQ</t>
   </si>
   <si>
-    <t>N 66 57.242 E 030 21.386</t>
-  </si>
-  <si>
     <t>DRKTGT003</t>
   </si>
   <si>
@@ -1582,25 +1576,13 @@
     <t>ARMY base</t>
   </si>
   <si>
-    <t>N 67 11.252 E 032 21.834</t>
-  </si>
-  <si>
     <t>DRKTGT004</t>
   </si>
   <si>
-    <t>Fuel and Gas Storage</t>
-  </si>
-  <si>
-    <t>*** feel free to redesignate to refinery, a nice looking plant - rare</t>
-  </si>
-  <si>
     <t>N 67 04.923 E 033 17.900</t>
   </si>
   <si>
     <t>DRKTGT005</t>
-  </si>
-  <si>
-    <t>Railway Maintenance Depot</t>
   </si>
   <si>
     <t>The biggest Railway Infrastructure of the Region</t>
@@ -2675,6 +2657,81 @@
   </si>
   <si>
     <t>HQ for 80th Air Support Division</t>
+  </si>
+  <si>
+    <t>Docks for DRKTGT004</t>
+  </si>
+  <si>
+    <t>Fuel  Refinery and Storage</t>
+  </si>
+  <si>
+    <t>N 67 04.657 E032 19.701</t>
+  </si>
+  <si>
+    <t>10,11,14</t>
+  </si>
+  <si>
+    <t>Main DUSS Fuel production in AO. Docks are DRKTGT006</t>
+  </si>
+  <si>
+    <t>Railway Depot</t>
+  </si>
+  <si>
+    <t>Fuel Docks</t>
+  </si>
+  <si>
+    <t>Army Fuel Depot</t>
+  </si>
+  <si>
+    <t>Fuel for ARMY</t>
+  </si>
+  <si>
+    <t>N 67 00.470 E030 18.951</t>
+  </si>
+  <si>
+    <t>Headquarters of the Supreme High Command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Main Military Council </t>
+  </si>
+  <si>
+    <t>The General Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The General Staff work and meet in thebuilding </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Council of Defense </t>
+  </si>
+  <si>
+    <t>State Committee of Defense (War cabinet)</t>
+  </si>
+  <si>
+    <t>Alakourtti Airbase</t>
+  </si>
+  <si>
+    <t>N 66 57.658 E 030 20.346</t>
+  </si>
+  <si>
+    <t>N 66 57.854 E 030 24.161</t>
+  </si>
+  <si>
+    <t>N 66 58.417 E 030 20.992</t>
+  </si>
+  <si>
+    <t>MiG-29 SQN (311) MiG-25 SQN (312)</t>
+  </si>
+  <si>
+    <t>N 67 11.375 E 032 22.066</t>
+  </si>
+  <si>
+    <t>N 66 52.395 E 3224.292</t>
+  </si>
+  <si>
+    <t>N 66 57.737 E 30 23.691</t>
+  </si>
+  <si>
+    <t>N 65 49.046 E 031 28.752</t>
   </si>
 </sst>
 </file>
@@ -2684,11 +2741,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999]0000;General"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2844,6 +2909,20 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="16">
@@ -3446,290 +3525,287 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="14" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="15" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3737,186 +3813,200 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5292,11 +5382,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B240" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A57" sqref="A57:XFD57"/>
+      <selection pane="bottomRight" activeCell="E249" sqref="E249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5568,7 +5658,7 @@
         <v>45</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>63</v>
@@ -5599,7 +5689,7 @@
         <v>49</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="H10" s="30" t="s">
         <v>63</v>
@@ -5627,10 +5717,10 @@
         <v>48</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="H11" s="30" t="s">
         <v>63</v>
@@ -5646,7 +5736,7 @@
         <v>52</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="C12" s="29">
         <v>6</v>
@@ -5661,7 +5751,7 @@
         <v>53</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>63</v>
@@ -5690,7 +5780,7 @@
         <v>57</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="H13" s="30" t="s">
         <v>63</v>
@@ -5793,9 +5883,7 @@
       <c r="I16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="143" t="s">
-        <v>63</v>
-      </c>
+      <c r="J16" s="8"/>
       <c r="K16" s="2" t="s">
         <v>27</v>
       </c>
@@ -5826,9 +5914,7 @@
       <c r="I17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="143" t="s">
-        <v>63</v>
-      </c>
+      <c r="J17" s="8"/>
       <c r="K17" s="2" t="s">
         <v>27</v>
       </c>
@@ -6123,10 +6209,10 @@
         <v>123</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="H27" s="30" t="s">
         <v>63</v>
@@ -6146,20 +6232,20 @@
         <v>124</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="C28" s="29">
         <v>5</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="18" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="H28" s="30" t="s">
         <v>63</v>
@@ -6179,20 +6265,20 @@
         <v>125</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C29" s="23">
         <v>5</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="25" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="H29" s="30" t="s">
         <v>63</v>
@@ -6212,7 +6298,7 @@
         <v>126</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="C30" s="29">
         <v>1</v>
@@ -6222,10 +6308,10 @@
         <v>127</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="H30" s="30" t="s">
         <v>63</v>
@@ -6328,10 +6414,10 @@
         <v>138</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="H33" s="30" t="s">
         <v>63</v>
@@ -6382,10 +6468,10 @@
         <v>143</v>
       </c>
       <c r="H34" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I34" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J34" s="39"/>
       <c r="K34" s="35"/>
@@ -6426,10 +6512,10 @@
         <v>147</v>
       </c>
       <c r="H35" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I35" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J35" s="41"/>
       <c r="K35" s="33"/>
@@ -6470,10 +6556,10 @@
         <v>151</v>
       </c>
       <c r="H36" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I36" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="2"/>
@@ -6499,10 +6585,10 @@
         <v>68</v>
       </c>
       <c r="H37" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I37" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J37" s="41"/>
       <c r="K37" s="33"/>
@@ -6543,10 +6629,10 @@
         <v>158</v>
       </c>
       <c r="H38" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I38" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="2"/>
@@ -6572,10 +6658,10 @@
         <v>162</v>
       </c>
       <c r="H39" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I39" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J39" s="41"/>
       <c r="K39" s="33"/>
@@ -6616,10 +6702,10 @@
         <v>166</v>
       </c>
       <c r="H40" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I40" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J40" s="8"/>
       <c r="K40" s="2"/>
@@ -6645,10 +6731,10 @@
         <v>170</v>
       </c>
       <c r="H41" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I41" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J41" s="41"/>
       <c r="K41" s="33"/>
@@ -6689,10 +6775,10 @@
         <v>174</v>
       </c>
       <c r="H42" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I42" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J42" s="8"/>
       <c r="K42" s="2"/>
@@ -6718,10 +6804,10 @@
         <v>178</v>
       </c>
       <c r="H43" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I43" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J43" s="41"/>
       <c r="K43" s="33"/>
@@ -6762,10 +6848,10 @@
         <v>182</v>
       </c>
       <c r="H44" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I44" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="2"/>
@@ -6791,10 +6877,10 @@
         <v>186</v>
       </c>
       <c r="H45" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I45" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J45" s="41"/>
       <c r="K45" s="33"/>
@@ -6835,10 +6921,10 @@
         <v>190</v>
       </c>
       <c r="H46" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I46" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="2"/>
@@ -6848,20 +6934,20 @@
         <v>191</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="C47" s="23">
         <v>5</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="138" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="F47" s="144" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="G47" s="138" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="H47" s="30" t="s">
         <v>63</v>
@@ -6899,7 +6985,7 @@
       </c>
       <c r="D48" s="27"/>
       <c r="E48" s="145" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>194</v>
@@ -6913,9 +6999,7 @@
       <c r="I48" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J48" s="143" t="s">
-        <v>63</v>
-      </c>
+      <c r="J48" s="8"/>
       <c r="K48" s="2" t="s">
         <v>363</v>
       </c>
@@ -6925,14 +7009,14 @@
         <v>195</v>
       </c>
       <c r="B49" s="146" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="C49" s="23">
         <v>9</v>
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="138" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="F49" s="21" t="s">
         <v>196</v>
@@ -6978,7 +7062,7 @@
       </c>
       <c r="D50" s="27"/>
       <c r="E50" s="145" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>199</v>
@@ -6992,9 +7076,7 @@
       <c r="I50" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J50" s="143" t="s">
-        <v>63</v>
-      </c>
+      <c r="J50" s="8"/>
       <c r="K50" s="2" t="s">
         <v>363</v>
       </c>
@@ -7004,7 +7086,7 @@
         <v>200</v>
       </c>
       <c r="B51" s="146" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="C51" s="23">
         <v>2</v>
@@ -7116,10 +7198,10 @@
         <v>211</v>
       </c>
       <c r="F54" s="147" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="G54" s="148" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="H54" s="30" t="s">
         <v>63</v>
@@ -7288,20 +7370,20 @@
         <v>232</v>
       </c>
       <c r="B60" s="149" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="C60" s="29">
         <v>9</v>
       </c>
       <c r="D60" s="27"/>
       <c r="E60" s="145" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="F60" s="147" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
       <c r="G60" s="148" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="H60" s="30" t="s">
         <v>63</v>
@@ -7360,10 +7442,10 @@
         <v>238</v>
       </c>
       <c r="F62" s="147" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="G62" s="148" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="H62" s="30" t="s">
         <v>63</v>
@@ -7415,13 +7497,13 @@
       </c>
       <c r="D64" s="27"/>
       <c r="E64" s="145" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="F64" s="147" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="G64" s="148" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="H64" s="30" t="s">
         <v>63</v>
@@ -7453,10 +7535,10 @@
         <v>581</v>
       </c>
       <c r="H65" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I65" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="2"/>
@@ -7482,10 +7564,10 @@
         <v>463</v>
       </c>
       <c r="H66" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I66" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="2"/>
@@ -7511,10 +7593,10 @@
         <v>555</v>
       </c>
       <c r="H67" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I67" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="2"/>
@@ -7540,10 +7622,10 @@
         <v>364</v>
       </c>
       <c r="H68" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I68" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="2"/>
@@ -7569,10 +7651,10 @@
         <v>269</v>
       </c>
       <c r="H69" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I69" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="2"/>
@@ -7598,10 +7680,10 @@
         <v>89</v>
       </c>
       <c r="H70" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="I70" s="150" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="2"/>
@@ -7618,13 +7700,13 @@
       </c>
       <c r="D71" s="24"/>
       <c r="E71" s="138" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="F71" s="144" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="G71" s="138" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="H71" s="30" t="s">
         <v>63</v>
@@ -7647,13 +7729,13 @@
       </c>
       <c r="D72" s="27"/>
       <c r="E72" s="145" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="F72" s="147" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="G72" s="148" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="H72" s="30" t="s">
         <v>63</v>
@@ -7676,13 +7758,13 @@
       </c>
       <c r="D73" s="24"/>
       <c r="E73" s="138" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="F73" s="144" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="G73" s="138" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="H73" s="30" t="s">
         <v>63</v>
@@ -7804,13 +7886,13 @@
       </c>
       <c r="D77" s="24"/>
       <c r="E77" s="138" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="F77" s="144" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="G77" s="138" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="H77" s="30" t="s">
         <v>63</v>
@@ -7822,7 +7904,7 @@
         <v>63</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7869,10 +7951,10 @@
         <v>291</v>
       </c>
       <c r="F79" s="144" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="G79" s="138" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="H79" s="30" t="s">
         <v>63</v>
@@ -7895,7 +7977,7 @@
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="145" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>294</v>
@@ -7927,10 +8009,10 @@
         <v>297</v>
       </c>
       <c r="F81" s="144" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="G81" s="138" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="H81" s="30" t="s">
         <v>63</v>
@@ -7946,7 +8028,7 @@
         <v>298</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="C82" s="29">
         <v>8</v>
@@ -7968,7 +8050,7 @@
         <v>22</v>
       </c>
       <c r="J82" s="8" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="K82" s="2"/>
     </row>
@@ -8002,7 +8084,7 @@
         <v>63</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8020,10 +8102,10 @@
         <v>306</v>
       </c>
       <c r="F84" s="147" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="G84" s="148" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="H84" s="30" t="s">
         <v>63</v>
@@ -8061,7 +8143,7 @@
         <v>22</v>
       </c>
       <c r="J85" s="8" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="K85" s="2"/>
     </row>
@@ -8106,7 +8188,7 @@
       </c>
       <c r="D87" s="24"/>
       <c r="E87" s="138" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="F87" s="21" t="s">
         <v>316</v>
@@ -8157,7 +8239,7 @@
         <v>321</v>
       </c>
       <c r="B89" s="22" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="C89" s="23">
         <v>6</v>
@@ -8179,7 +8261,7 @@
         <v>22</v>
       </c>
       <c r="J89" s="8" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="K89" s="2"/>
     </row>
@@ -8195,7 +8277,7 @@
       </c>
       <c r="D90" s="27"/>
       <c r="E90" s="18" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>326</v>
@@ -8217,14 +8299,14 @@
         <v>327</v>
       </c>
       <c r="B91" s="22" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="C91" s="23">
         <v>7</v>
       </c>
       <c r="D91" s="24"/>
       <c r="E91" s="22" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="F91" s="21" t="s">
         <v>328</v>
@@ -8379,7 +8461,7 @@
       </c>
       <c r="D96" s="27"/>
       <c r="E96" s="137" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>347</v>
@@ -8410,7 +8492,7 @@
       </c>
       <c r="D97" s="24"/>
       <c r="E97" s="136" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="F97" s="21" t="s">
         <v>351</v>
@@ -8472,7 +8554,7 @@
       </c>
       <c r="D99" s="24"/>
       <c r="E99" s="135" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="F99" s="21" t="s">
         <v>361</v>
@@ -10349,10 +10431,10 @@
         <v>506</v>
       </c>
       <c r="F211" s="63" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="G211" s="65" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="H211" s="30" t="s">
         <v>63</v>
@@ -10372,20 +10454,20 @@
         <v>386</v>
       </c>
       <c r="B212" s="66" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="C212" s="67">
         <v>2</v>
       </c>
       <c r="D212" s="66"/>
       <c r="E212" s="66" t="s">
+        <v>834</v>
+      </c>
+      <c r="F212" s="66" t="s">
+        <v>841</v>
+      </c>
+      <c r="G212" s="68" t="s">
         <v>840</v>
-      </c>
-      <c r="F212" s="66" t="s">
-        <v>847</v>
-      </c>
-      <c r="G212" s="68" t="s">
-        <v>846</v>
       </c>
       <c r="H212" s="30" t="s">
         <v>63</v>
@@ -10405,20 +10487,20 @@
         <v>387</v>
       </c>
       <c r="B213" s="63" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="C213" s="64">
         <v>2</v>
       </c>
       <c r="D213" s="63"/>
       <c r="E213" s="63" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="F213" s="63" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="G213" s="65" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="H213" s="30" t="s">
         <v>63</v>
@@ -10430,7 +10512,7 @@
         <v>63</v>
       </c>
       <c r="K213" s="2" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
     </row>
     <row r="214" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10438,20 +10520,20 @@
         <v>388</v>
       </c>
       <c r="B214" s="66" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="C214" s="67">
         <v>2</v>
       </c>
       <c r="D214" s="66"/>
       <c r="E214" s="66" t="s">
+        <v>837</v>
+      </c>
+      <c r="F214" s="66" t="s">
         <v>843</v>
       </c>
-      <c r="F214" s="66" t="s">
-        <v>849</v>
-      </c>
       <c r="G214" s="68" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="H214" s="30" t="s">
         <v>63</v>
@@ -10467,20 +10549,20 @@
         <v>389</v>
       </c>
       <c r="B215" s="63" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="C215" s="151">
         <v>2</v>
       </c>
       <c r="D215" s="63"/>
       <c r="E215" s="63" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="F215" s="63" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="G215" s="65" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="H215" s="30" t="s">
         <v>63</v>
@@ -10494,20 +10576,20 @@
         <v>390</v>
       </c>
       <c r="B216" s="66" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="C216" s="67">
         <v>2</v>
       </c>
       <c r="D216" s="66"/>
       <c r="E216" s="66" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="F216" s="66" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="G216" s="68" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="H216" s="30" t="s">
         <v>63</v>
@@ -10521,20 +10603,20 @@
         <v>391</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="C217" s="69">
         <v>2</v>
       </c>
       <c r="D217" s="2"/>
       <c r="E217" s="2" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="F217" s="63" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="G217" s="65" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="H217" s="30" t="s">
         <v>63</v>
@@ -10548,20 +10630,20 @@
         <v>392</v>
       </c>
       <c r="B218" s="66" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="C218" s="67">
         <v>2</v>
       </c>
       <c r="D218" s="66"/>
       <c r="E218" s="66" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="F218" s="66" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="G218" s="68" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="H218" s="30" t="s">
         <v>63</v>
@@ -10575,20 +10657,20 @@
         <v>393</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="C219" s="69">
         <v>2</v>
       </c>
       <c r="D219" s="2"/>
       <c r="E219" s="2" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="F219" s="63" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="G219" s="65" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="H219" s="30" t="s">
         <v>63</v>
@@ -10828,13 +10910,13 @@
       <c r="H240" s="70"/>
       <c r="I240" s="70"/>
     </row>
-    <row r="241" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C241" s="71"/>
       <c r="F241" s="2"/>
       <c r="H241" s="70"/>
       <c r="I241" s="70"/>
     </row>
-    <row r="242" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="73" t="s">
         <v>507</v>
       </c>
@@ -10848,21 +10930,23 @@
       <c r="E242" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="F242" s="2" t="s">
+      <c r="F242" s="188" t="s">
+        <v>885</v>
+      </c>
+      <c r="G242" s="57">
+        <v>506</v>
+      </c>
+      <c r="H242" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I242" s="70"/>
+    </row>
+    <row r="243" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="73" t="s">
         <v>509</v>
       </c>
-      <c r="G242" s="57">
-        <v>327</v>
-      </c>
-      <c r="H242" s="70"/>
-      <c r="I242" s="70"/>
-    </row>
-    <row r="243" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="73" t="s">
+      <c r="B243" s="26" t="s">
         <v>510</v>
-      </c>
-      <c r="B243" s="26" t="s">
-        <v>511</v>
       </c>
       <c r="C243" s="29">
         <v>3</v>
@@ -10871,54 +10955,58 @@
       <c r="E243" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="F243" s="2" t="s">
+      <c r="F243" s="188" t="s">
+        <v>891</v>
+      </c>
+      <c r="G243" s="74">
+        <v>452</v>
+      </c>
+      <c r="H243" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I243" s="70"/>
+    </row>
+    <row r="244" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="73" t="s">
+        <v>511</v>
+      </c>
+      <c r="B244" s="44" t="s">
         <v>512</v>
-      </c>
-      <c r="G243" s="74">
-        <v>514</v>
-      </c>
-      <c r="H243" s="70"/>
-      <c r="I243" s="70"/>
-    </row>
-    <row r="244" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="73" t="s">
-        <v>513</v>
-      </c>
-      <c r="B244" s="44" t="s">
-        <v>514</v>
       </c>
       <c r="C244" s="55">
         <v>9</v>
       </c>
       <c r="D244" s="56"/>
       <c r="E244" s="45" t="s">
-        <v>515</v>
-      </c>
-      <c r="F244" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
+      </c>
+      <c r="F244" s="188" t="s">
+        <v>888</v>
       </c>
       <c r="G244" s="57">
-        <v>124</v>
-      </c>
-      <c r="H244" s="70"/>
+        <v>167</v>
+      </c>
+      <c r="H244" s="75" t="s">
+        <v>22</v>
+      </c>
       <c r="I244" s="70"/>
     </row>
-    <row r="245" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="73" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B245" s="26" t="s">
-        <v>518</v>
+        <v>868</v>
       </c>
       <c r="C245" s="29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D245" s="27"/>
       <c r="E245" s="18" t="s">
-        <v>519</v>
+        <v>871</v>
       </c>
       <c r="F245" s="2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G245" s="74">
         <v>44</v>
@@ -10928,136 +11016,219 @@
       </c>
       <c r="I245" s="70"/>
     </row>
-    <row r="246" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="73" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B246" s="44" t="s">
-        <v>522</v>
-      </c>
-      <c r="C246" s="55">
-        <v>11</v>
+        <v>872</v>
+      </c>
+      <c r="C246" s="55" t="s">
+        <v>870</v>
       </c>
       <c r="D246" s="56"/>
       <c r="E246" s="45" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="F246" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="G246" s="57"/>
+        <v>518</v>
+      </c>
+      <c r="G246" s="57">
+        <v>130</v>
+      </c>
       <c r="H246" s="75" t="s">
         <v>22</v>
       </c>
       <c r="I246" s="70"/>
-    </row>
-    <row r="247" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K246" s="185" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="73" t="s">
+        <v>519</v>
+      </c>
+      <c r="B247" s="26" t="s">
+        <v>873</v>
+      </c>
+      <c r="C247" s="29">
+        <v>10</v>
+      </c>
+      <c r="D247" s="27"/>
+      <c r="E247" s="18" t="s">
+        <v>867</v>
+      </c>
+      <c r="F247" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="G247" s="74">
+        <v>15</v>
+      </c>
+      <c r="H247" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I247" s="70"/>
+    </row>
+    <row r="248" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="73" t="s">
+        <v>520</v>
+      </c>
+      <c r="B248" s="44" t="s">
+        <v>874</v>
+      </c>
+      <c r="C248" s="55">
+        <v>9</v>
+      </c>
+      <c r="D248" s="56"/>
+      <c r="E248" s="45" t="s">
+        <v>875</v>
+      </c>
+      <c r="F248" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="G248" s="57">
+        <v>539</v>
+      </c>
+      <c r="H248" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I248" s="70"/>
+    </row>
+    <row r="249" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="73" t="s">
+        <v>521</v>
+      </c>
+      <c r="B249" s="26" t="s">
+        <v>877</v>
+      </c>
+      <c r="C249" s="29">
+        <v>3</v>
+      </c>
+      <c r="D249" s="27"/>
+      <c r="E249" s="18" t="s">
+        <v>878</v>
+      </c>
+      <c r="F249" s="188" t="s">
+        <v>884</v>
+      </c>
+      <c r="G249" s="74">
+        <v>512</v>
+      </c>
+      <c r="H249" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I249" s="75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="73" t="s">
+        <v>522</v>
+      </c>
+      <c r="B250" s="186" t="s">
+        <v>879</v>
+      </c>
+      <c r="C250" s="55">
+        <v>3</v>
+      </c>
+      <c r="D250" s="56"/>
+      <c r="E250" s="187" t="s">
+        <v>880</v>
+      </c>
+      <c r="F250" s="188" t="s">
+        <v>889</v>
+      </c>
+      <c r="G250" s="57">
+        <v>3</v>
+      </c>
+      <c r="H250" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I250" s="75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="73" t="s">
+        <v>523</v>
+      </c>
+      <c r="B251" s="26" t="s">
+        <v>881</v>
+      </c>
+      <c r="C251" s="29">
+        <v>3</v>
+      </c>
+      <c r="D251" s="27"/>
+      <c r="E251" s="189" t="s">
+        <v>882</v>
+      </c>
+      <c r="F251" s="188" t="s">
+        <v>890</v>
+      </c>
+      <c r="G251" s="74">
+        <v>504</v>
+      </c>
+      <c r="H251" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I251" s="75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="73" t="s">
+        <v>524</v>
+      </c>
+      <c r="B252" s="186" t="s">
+        <v>883</v>
+      </c>
+      <c r="C252" s="55">
+        <v>4</v>
+      </c>
+      <c r="D252" s="56"/>
+      <c r="E252" s="187" t="s">
+        <v>887</v>
+      </c>
+      <c r="F252" s="188" t="s">
+        <v>886</v>
+      </c>
+      <c r="G252" s="57">
+        <v>548</v>
+      </c>
+      <c r="H252" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="I252" s="70"/>
+    </row>
+    <row r="253" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="73" t="s">
         <v>525</v>
-      </c>
-      <c r="B247" s="26"/>
-      <c r="C247" s="29"/>
-      <c r="D247" s="27"/>
-      <c r="E247" s="18"/>
-      <c r="F247" s="2"/>
-      <c r="G247" s="74"/>
-      <c r="H247" s="70"/>
-      <c r="I247" s="70"/>
-    </row>
-    <row r="248" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="73" t="s">
-        <v>526</v>
-      </c>
-      <c r="B248" s="44"/>
-      <c r="C248" s="55"/>
-      <c r="D248" s="56"/>
-      <c r="E248" s="45"/>
-      <c r="F248" s="2"/>
-      <c r="G248" s="57"/>
-      <c r="H248" s="70"/>
-      <c r="I248" s="70"/>
-    </row>
-    <row r="249" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="73" t="s">
-        <v>527</v>
-      </c>
-      <c r="B249" s="26"/>
-      <c r="C249" s="29"/>
-      <c r="D249" s="27"/>
-      <c r="E249" s="18"/>
-      <c r="F249" s="2"/>
-      <c r="G249" s="74"/>
-      <c r="H249" s="70"/>
-      <c r="I249" s="70"/>
-    </row>
-    <row r="250" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="73" t="s">
-        <v>528</v>
-      </c>
-      <c r="B250" s="44"/>
-      <c r="C250" s="55"/>
-      <c r="D250" s="56"/>
-      <c r="E250" s="45"/>
-      <c r="F250" s="2"/>
-      <c r="G250" s="57"/>
-      <c r="H250" s="70"/>
-      <c r="I250" s="70"/>
-    </row>
-    <row r="251" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="73" t="s">
-        <v>529</v>
-      </c>
-      <c r="B251" s="26"/>
-      <c r="C251" s="29"/>
-      <c r="D251" s="27"/>
-      <c r="E251" s="18"/>
-      <c r="F251" s="2"/>
-      <c r="G251" s="74"/>
-      <c r="H251" s="70"/>
-      <c r="I251" s="70"/>
-    </row>
-    <row r="252" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="73" t="s">
-        <v>530</v>
-      </c>
-      <c r="B252" s="44"/>
-      <c r="C252" s="55"/>
-      <c r="D252" s="56"/>
-      <c r="E252" s="45"/>
-      <c r="F252" s="2"/>
-      <c r="G252" s="57"/>
-      <c r="H252" s="70"/>
-      <c r="I252" s="70"/>
-    </row>
-    <row r="253" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="73" t="s">
-        <v>531</v>
       </c>
       <c r="B253" s="26"/>
       <c r="C253" s="29"/>
       <c r="D253" s="27"/>
-      <c r="E253" s="18"/>
+      <c r="E253" s="189"/>
       <c r="F253" s="2"/>
       <c r="G253" s="74"/>
       <c r="H253" s="70"/>
       <c r="I253" s="70"/>
     </row>
-    <row r="254" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="73" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="B254" s="44"/>
       <c r="C254" s="55"/>
       <c r="D254" s="56"/>
       <c r="E254" s="45"/>
-      <c r="F254" s="2"/>
+      <c r="F254" s="45"/>
       <c r="G254" s="57"/>
       <c r="H254" s="70"/>
       <c r="I254" s="70"/>
     </row>
-    <row r="255" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="73" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="B255" s="26"/>
       <c r="C255" s="29"/>
@@ -11068,9 +11239,9 @@
       <c r="H255" s="70"/>
       <c r="I255" s="70"/>
     </row>
-    <row r="256" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="73" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="B256" s="44"/>
       <c r="C256" s="55"/>
@@ -11083,7 +11254,7 @@
     </row>
     <row r="257" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="73" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="B257" s="26"/>
       <c r="C257" s="29"/>
@@ -11096,7 +11267,7 @@
     </row>
     <row r="258" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="73" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="B258" s="44"/>
       <c r="C258" s="55"/>
@@ -11109,7 +11280,7 @@
     </row>
     <row r="259" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="73" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="B259" s="26"/>
       <c r="C259" s="29"/>
@@ -11122,7 +11293,7 @@
     </row>
     <row r="260" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="73" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="B260" s="44"/>
       <c r="C260" s="55"/>
@@ -11135,7 +11306,7 @@
     </row>
     <row r="261" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="73" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="B261" s="26"/>
       <c r="C261" s="29"/>
@@ -11148,7 +11319,7 @@
     </row>
     <row r="262" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="73" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="B262" s="44"/>
       <c r="C262" s="55"/>
@@ -11161,7 +11332,7 @@
     </row>
     <row r="263" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="73" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="B263" s="26"/>
       <c r="C263" s="29"/>
@@ -11174,7 +11345,7 @@
     </row>
     <row r="264" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="73" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="B264" s="44"/>
       <c r="C264" s="55"/>
@@ -11187,7 +11358,7 @@
     </row>
     <row r="265" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="73" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="B265" s="26"/>
       <c r="C265" s="29"/>
@@ -11200,7 +11371,7 @@
     </row>
     <row r="266" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="73" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="B266" s="44"/>
       <c r="C266" s="55"/>
@@ -11213,7 +11384,7 @@
     </row>
     <row r="267" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="73" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="B267" s="26"/>
       <c r="C267" s="29"/>
@@ -11226,7 +11397,7 @@
     </row>
     <row r="268" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="73" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="B268" s="44"/>
       <c r="C268" s="55"/>
@@ -11239,7 +11410,7 @@
     </row>
     <row r="269" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="73" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="B269" s="26"/>
       <c r="C269" s="29"/>
@@ -11252,7 +11423,7 @@
     </row>
     <row r="270" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="73" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="B270" s="44"/>
       <c r="C270" s="55"/>
@@ -11265,7 +11436,7 @@
     </row>
     <row r="271" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="73" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="B271" s="26"/>
       <c r="C271" s="29"/>
@@ -11278,7 +11449,7 @@
     </row>
     <row r="272" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="73" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="B272" s="44"/>
       <c r="C272" s="55"/>
@@ -11291,7 +11462,7 @@
     </row>
     <row r="273" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="73" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="B273" s="26"/>
       <c r="C273" s="29"/>
@@ -11304,7 +11475,7 @@
     </row>
     <row r="274" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="73" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="B274" s="44"/>
       <c r="C274" s="55"/>
@@ -11317,7 +11488,7 @@
     </row>
     <row r="275" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="73" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B275" s="26"/>
       <c r="C275" s="29"/>
@@ -11330,7 +11501,7 @@
     </row>
     <row r="276" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="73" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B276" s="44"/>
       <c r="C276" s="55"/>
@@ -11343,7 +11514,7 @@
     </row>
     <row r="277" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="73" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B277" s="26"/>
       <c r="C277" s="29"/>
@@ -11356,7 +11527,7 @@
     </row>
     <row r="278" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="73" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="B278" s="44"/>
       <c r="C278" s="55"/>
@@ -11369,7 +11540,7 @@
     </row>
     <row r="279" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="73" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="B279" s="26"/>
       <c r="C279" s="29"/>
@@ -11382,7 +11553,7 @@
     </row>
     <row r="280" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="73" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="B280" s="44"/>
       <c r="C280" s="55"/>
@@ -11395,7 +11566,7 @@
     </row>
     <row r="281" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="73" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="B281" s="26"/>
       <c r="C281" s="29"/>
@@ -11408,7 +11579,7 @@
     </row>
     <row r="282" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="73" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="B282" s="44"/>
       <c r="C282" s="55"/>
@@ -11421,7 +11592,7 @@
     </row>
     <row r="283" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="73" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="B283" s="26"/>
       <c r="C283" s="29"/>
@@ -11434,7 +11605,7 @@
     </row>
     <row r="284" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="73" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="B284" s="44"/>
       <c r="C284" s="55"/>
@@ -11447,7 +11618,7 @@
     </row>
     <row r="285" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="73" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="B285" s="26"/>
       <c r="C285" s="29"/>
@@ -11460,7 +11631,7 @@
     </row>
     <row r="286" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="73" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="B286" s="44"/>
       <c r="C286" s="55"/>
@@ -11473,7 +11644,7 @@
     </row>
     <row r="287" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="73" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="B287" s="26"/>
       <c r="C287" s="29"/>
@@ -11486,7 +11657,7 @@
     </row>
     <row r="288" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="73" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="B288" s="44"/>
       <c r="C288" s="55"/>
@@ -11499,7 +11670,7 @@
     </row>
     <row r="289" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="73" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="B289" s="26"/>
       <c r="C289" s="29"/>
@@ -11512,7 +11683,7 @@
     </row>
     <row r="290" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="73" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="B290" s="44"/>
       <c r="C290" s="55"/>
@@ -11525,7 +11696,7 @@
     </row>
     <row r="291" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="73" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="B291" s="26"/>
       <c r="C291" s="29"/>
@@ -11538,7 +11709,7 @@
     </row>
     <row r="292" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="73" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="B292" s="44"/>
       <c r="C292" s="55"/>
@@ -11551,7 +11722,7 @@
     </row>
     <row r="293" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="73" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="B293" s="26"/>
       <c r="C293" s="29"/>
@@ -11564,7 +11735,7 @@
     </row>
     <row r="294" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="73" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="B294" s="44"/>
       <c r="C294" s="55"/>
@@ -11577,7 +11748,7 @@
     </row>
     <row r="295" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="73" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="B295" s="26"/>
       <c r="C295" s="29"/>
@@ -11590,7 +11761,7 @@
     </row>
     <row r="296" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="73" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="B296" s="44"/>
       <c r="C296" s="55"/>
@@ -11603,7 +11774,7 @@
     </row>
     <row r="297" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="73" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="B297" s="26"/>
       <c r="C297" s="29"/>
@@ -11616,7 +11787,7 @@
     </row>
     <row r="298" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="73" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B298" s="44"/>
       <c r="C298" s="55"/>
@@ -11629,7 +11800,7 @@
     </row>
     <row r="299" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="73" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="B299" s="26"/>
       <c r="C299" s="29"/>
@@ -11642,7 +11813,7 @@
     </row>
     <row r="300" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="73" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="B300" s="44"/>
       <c r="C300" s="55"/>
@@ -11655,7 +11826,7 @@
     </row>
     <row r="301" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="73" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="B301" s="26"/>
       <c r="C301" s="29"/>
@@ -11668,7 +11839,7 @@
     </row>
     <row r="302" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="73" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B302" s="44"/>
       <c r="C302" s="55"/>
@@ -11681,7 +11852,7 @@
     </row>
     <row r="303" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="73" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="B303" s="26"/>
       <c r="C303" s="29"/>
@@ -11694,7 +11865,7 @@
     </row>
     <row r="304" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="73" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="B304" s="44"/>
       <c r="C304" s="55"/>
@@ -11707,7 +11878,7 @@
     </row>
     <row r="305" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="73" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B305" s="26"/>
       <c r="C305" s="29"/>
@@ -11720,7 +11891,7 @@
     </row>
     <row r="306" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="73" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="B306" s="44"/>
       <c r="C306" s="55"/>
@@ -11733,7 +11904,7 @@
     </row>
     <row r="307" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="73" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B307" s="26"/>
       <c r="C307" s="29"/>
@@ -11746,7 +11917,7 @@
     </row>
     <row r="308" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="73" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="B308" s="44"/>
       <c r="C308" s="55"/>
@@ -11759,7 +11930,7 @@
     </row>
     <row r="309" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="73" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="B309" s="26"/>
       <c r="C309" s="29"/>
@@ -11772,7 +11943,7 @@
     </row>
     <row r="310" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="73" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B310" s="44"/>
       <c r="C310" s="55"/>
@@ -11785,7 +11956,7 @@
     </row>
     <row r="311" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="73" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="B311" s="26"/>
       <c r="C311" s="29"/>
@@ -11798,7 +11969,7 @@
     </row>
     <row r="312" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="73" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="B312" s="44"/>
       <c r="C312" s="55"/>
@@ -11811,7 +11982,7 @@
     </row>
     <row r="313" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="73" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="B313" s="26"/>
       <c r="C313" s="29"/>
@@ -11824,7 +11995,7 @@
     </row>
     <row r="314" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="73" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="B314" s="44"/>
       <c r="C314" s="55"/>
@@ -11837,7 +12008,7 @@
     </row>
     <row r="315" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="73" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B315" s="26"/>
       <c r="C315" s="29"/>
@@ -11850,7 +12021,7 @@
     </row>
     <row r="316" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="73" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="B316" s="44"/>
       <c r="C316" s="55"/>
@@ -11863,7 +12034,7 @@
     </row>
     <row r="317" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="73" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="B317" s="26"/>
       <c r="C317" s="29"/>
@@ -11876,7 +12047,7 @@
     </row>
     <row r="318" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="73" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B318" s="44"/>
       <c r="C318" s="55"/>
@@ -11889,7 +12060,7 @@
     </row>
     <row r="319" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="73" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="B319" s="26"/>
       <c r="C319" s="29"/>
@@ -11902,7 +12073,7 @@
     </row>
     <row r="320" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="73" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="B320" s="44"/>
       <c r="C320" s="55"/>
@@ -11915,7 +12086,7 @@
     </row>
     <row r="321" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="73" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B321" s="26"/>
       <c r="C321" s="29"/>
@@ -11928,7 +12099,7 @@
     </row>
     <row r="322" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="73" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B322" s="44"/>
       <c r="C322" s="55"/>
@@ -11941,7 +12112,7 @@
     </row>
     <row r="323" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="73" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B323" s="26"/>
       <c r="C323" s="29"/>
@@ -11954,7 +12125,7 @@
     </row>
     <row r="324" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="73" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="B324" s="44"/>
       <c r="C324" s="55"/>
@@ -11967,7 +12138,7 @@
     </row>
     <row r="325" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="73" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B325" s="26"/>
       <c r="C325" s="29"/>
@@ -11980,7 +12151,7 @@
     </row>
     <row r="326" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="73" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="B326" s="44"/>
       <c r="C326" s="55"/>
@@ -11993,7 +12164,7 @@
     </row>
     <row r="327" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="73" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B327" s="26"/>
       <c r="C327" s="29"/>
@@ -12006,7 +12177,7 @@
     </row>
     <row r="328" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="73" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="B328" s="44"/>
       <c r="C328" s="55"/>
@@ -12019,7 +12190,7 @@
     </row>
     <row r="329" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="73" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B329" s="26"/>
       <c r="C329" s="29"/>
@@ -12032,7 +12203,7 @@
     </row>
     <row r="330" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="73" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="B330" s="44"/>
       <c r="C330" s="55"/>
@@ -12045,7 +12216,7 @@
     </row>
     <row r="331" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="73" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="B331" s="26"/>
       <c r="C331" s="29"/>
@@ -12058,7 +12229,7 @@
     </row>
     <row r="332" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="73" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="B332" s="44"/>
       <c r="C332" s="55"/>
@@ -12071,7 +12242,7 @@
     </row>
     <row r="333" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="73" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B333" s="26"/>
       <c r="C333" s="29"/>
@@ -12084,7 +12255,7 @@
     </row>
     <row r="334" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="73" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="B334" s="44"/>
       <c r="C334" s="55"/>
@@ -12097,7 +12268,7 @@
     </row>
     <row r="335" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="73" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B335" s="26"/>
       <c r="C335" s="29"/>
@@ -12110,7 +12281,7 @@
     </row>
     <row r="336" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="73" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="B336" s="44"/>
       <c r="C336" s="55"/>
@@ -12123,7 +12294,7 @@
     </row>
     <row r="337" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="73" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="B337" s="26"/>
       <c r="C337" s="29"/>
@@ -12136,7 +12307,7 @@
     </row>
     <row r="338" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="73" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B338" s="44"/>
       <c r="C338" s="55"/>
@@ -12149,7 +12320,7 @@
     </row>
     <row r="339" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="73" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B339" s="26"/>
       <c r="C339" s="29"/>
@@ -12162,7 +12333,7 @@
     </row>
     <row r="340" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="73" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B340" s="44"/>
       <c r="C340" s="55"/>
@@ -12175,7 +12346,7 @@
     </row>
     <row r="341" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="73" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B341" s="26"/>
       <c r="C341" s="29"/>
@@ -16972,81 +17143,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="172" t="s">
-        <v>620</v>
-      </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
-      <c r="I1" s="174"/>
+      <c r="A1" s="157" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="159"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="175" t="s">
-        <v>621</v>
-      </c>
-      <c r="B2" s="160"/>
+      <c r="A2" s="160" t="s">
+        <v>615</v>
+      </c>
+      <c r="B2" s="161"/>
       <c r="C2" s="80" t="s">
-        <v>622</v>
-      </c>
-      <c r="D2" s="176" t="s">
-        <v>623</v>
+        <v>616</v>
+      </c>
+      <c r="D2" s="162" t="s">
+        <v>617</v>
       </c>
       <c r="E2" s="163"/>
       <c r="F2" s="163"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="177" t="s">
-        <v>624</v>
-      </c>
-      <c r="I2" s="164"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="164" t="s">
+        <v>618</v>
+      </c>
+      <c r="I2" s="165"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
-        <v>625</v>
-      </c>
-      <c r="B4" s="173"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="173"/>
-      <c r="G4" s="173"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="174"/>
+      <c r="A4" s="166" t="s">
+        <v>619</v>
+      </c>
+      <c r="B4" s="158"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
+      <c r="H4" s="158"/>
+      <c r="I4" s="159"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="E5" s="82" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="G5" s="82" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="82" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="I5" s="83" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="K5" s="84" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -17054,104 +17225,104 @@
         <v>1</v>
       </c>
       <c r="B6" s="86" t="s">
+        <v>629</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>630</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>631</v>
+      </c>
+      <c r="E6" s="86" t="s">
+        <v>632</v>
+      </c>
+      <c r="F6" s="86" t="s">
+        <v>633</v>
+      </c>
+      <c r="G6" s="86" t="s">
+        <v>634</v>
+      </c>
+      <c r="H6" s="86" t="s">
         <v>635</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="I6" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="K6" s="167" t="s">
         <v>637</v>
       </c>
-      <c r="E6" s="86" t="s">
-        <v>638</v>
-      </c>
-      <c r="F6" s="86" t="s">
-        <v>639</v>
-      </c>
-      <c r="G6" s="86" t="s">
-        <v>640</v>
-      </c>
-      <c r="H6" s="86" t="s">
-        <v>641</v>
-      </c>
-      <c r="I6" s="87" t="s">
-        <v>642</v>
-      </c>
-      <c r="K6" s="166" t="s">
-        <v>643</v>
-      </c>
-      <c r="L6" s="167"/>
-      <c r="M6" s="167"/>
-      <c r="N6" s="167"/>
-      <c r="O6" s="167"/>
-      <c r="P6" s="167"/>
-      <c r="Q6" s="167"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
         <v>2</v>
       </c>
       <c r="B7" s="86" t="s">
+        <v>638</v>
+      </c>
+      <c r="C7" s="86" t="s">
+        <v>639</v>
+      </c>
+      <c r="D7" s="86" t="s">
+        <v>640</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>641</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>642</v>
+      </c>
+      <c r="G7" s="86" t="s">
+        <v>643</v>
+      </c>
+      <c r="H7" s="86" t="s">
         <v>644</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="I7" s="87" t="s">
         <v>645</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="K7" s="167" t="s">
         <v>646</v>
       </c>
-      <c r="E7" s="86" t="s">
-        <v>647</v>
-      </c>
-      <c r="F7" s="86" t="s">
-        <v>648</v>
-      </c>
-      <c r="G7" s="86" t="s">
-        <v>649</v>
-      </c>
-      <c r="H7" s="86" t="s">
-        <v>650</v>
-      </c>
-      <c r="I7" s="87" t="s">
-        <v>651</v>
-      </c>
-      <c r="K7" s="166" t="s">
-        <v>652</v>
-      </c>
-      <c r="L7" s="167"/>
-      <c r="M7" s="167"/>
-      <c r="N7" s="167"/>
-      <c r="O7" s="167"/>
-      <c r="P7" s="167"/>
-      <c r="Q7" s="167"/>
+      <c r="L7" s="168"/>
+      <c r="M7" s="168"/>
+      <c r="N7" s="168"/>
+      <c r="O7" s="168"/>
+      <c r="P7" s="168"/>
+      <c r="Q7" s="168"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
         <v>3</v>
       </c>
       <c r="B8" s="86" t="s">
+        <v>647</v>
+      </c>
+      <c r="C8" s="86" t="s">
+        <v>648</v>
+      </c>
+      <c r="D8" s="86" t="s">
+        <v>649</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>650</v>
+      </c>
+      <c r="F8" s="86" t="s">
+        <v>651</v>
+      </c>
+      <c r="G8" s="86" t="s">
+        <v>652</v>
+      </c>
+      <c r="H8" s="86" t="s">
         <v>653</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="I8" s="87" t="s">
         <v>654</v>
-      </c>
-      <c r="D8" s="86" t="s">
-        <v>655</v>
-      </c>
-      <c r="E8" s="86" t="s">
-        <v>656</v>
-      </c>
-      <c r="F8" s="86" t="s">
-        <v>657</v>
-      </c>
-      <c r="G8" s="86" t="s">
-        <v>658</v>
-      </c>
-      <c r="H8" s="86" t="s">
-        <v>659</v>
-      </c>
-      <c r="I8" s="87" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -17231,111 +17402,111 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="168" t="s">
-        <v>661</v>
-      </c>
-      <c r="B15" s="169"/>
-      <c r="C15" s="169"/>
-      <c r="D15" s="169"/>
-      <c r="E15" s="169"/>
-      <c r="F15" s="169"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="170"/>
+      <c r="A15" s="169" t="s">
+        <v>655</v>
+      </c>
+      <c r="B15" s="170"/>
+      <c r="C15" s="170"/>
+      <c r="D15" s="170"/>
+      <c r="E15" s="170"/>
+      <c r="F15" s="170"/>
+      <c r="G15" s="170"/>
+      <c r="H15" s="170"/>
+      <c r="I15" s="171"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
+        <v>620</v>
+      </c>
+      <c r="B16" s="82" t="s">
+        <v>623</v>
+      </c>
+      <c r="C16" s="82" t="s">
         <v>626</v>
       </c>
-      <c r="B16" s="82" t="s">
-        <v>629</v>
-      </c>
-      <c r="C16" s="82" t="s">
-        <v>632</v>
-      </c>
       <c r="D16" s="82" t="s">
-        <v>633</v>
-      </c>
-      <c r="E16" s="171" t="s">
-        <v>662</v>
-      </c>
-      <c r="F16" s="158"/>
-      <c r="G16" s="171" t="s">
-        <v>663</v>
-      </c>
-      <c r="H16" s="161"/>
-      <c r="I16" s="162"/>
+        <v>627</v>
+      </c>
+      <c r="E16" s="172" t="s">
+        <v>656</v>
+      </c>
+      <c r="F16" s="173"/>
+      <c r="G16" s="172" t="s">
+        <v>657</v>
+      </c>
+      <c r="H16" s="174"/>
+      <c r="I16" s="175"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
         <v>1</v>
       </c>
       <c r="B17" s="86" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="C17" s="86" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="D17" s="86" t="s">
+        <v>654</v>
+      </c>
+      <c r="E17" s="176" t="s">
+        <v>659</v>
+      </c>
+      <c r="F17" s="173"/>
+      <c r="G17" s="176" t="s">
         <v>660</v>
       </c>
-      <c r="E17" s="165" t="s">
-        <v>665</v>
-      </c>
-      <c r="F17" s="158"/>
-      <c r="G17" s="165" t="s">
-        <v>666</v>
-      </c>
-      <c r="H17" s="161"/>
-      <c r="I17" s="162"/>
+      <c r="H17" s="174"/>
+      <c r="I17" s="175"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
         <v>2</v>
       </c>
       <c r="B18" s="86" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="C18" s="86" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="D18" s="86" t="s">
-        <v>660</v>
-      </c>
-      <c r="E18" s="165" t="s">
-        <v>665</v>
-      </c>
-      <c r="F18" s="158"/>
-      <c r="G18" s="165" t="s">
-        <v>668</v>
-      </c>
-      <c r="H18" s="161"/>
-      <c r="I18" s="162"/>
+        <v>654</v>
+      </c>
+      <c r="E18" s="176" t="s">
+        <v>659</v>
+      </c>
+      <c r="F18" s="173"/>
+      <c r="G18" s="176" t="s">
+        <v>662</v>
+      </c>
+      <c r="H18" s="174"/>
+      <c r="I18" s="175"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
         <v>3</v>
       </c>
       <c r="B19" s="86" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="C19" s="86" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="D19" s="86" t="s">
-        <v>670</v>
-      </c>
-      <c r="E19" s="165" t="s">
-        <v>671</v>
-      </c>
-      <c r="F19" s="158"/>
-      <c r="G19" s="165" t="s">
-        <v>672</v>
-      </c>
-      <c r="H19" s="161"/>
-      <c r="I19" s="162"/>
+        <v>664</v>
+      </c>
+      <c r="E19" s="176" t="s">
+        <v>665</v>
+      </c>
+      <c r="F19" s="173"/>
+      <c r="G19" s="176" t="s">
+        <v>666</v>
+      </c>
+      <c r="H19" s="174"/>
+      <c r="I19" s="175"/>
       <c r="K19" s="84" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -17345,11 +17516,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="158"/>
-      <c r="G20" s="157"/>
-      <c r="H20" s="161"/>
-      <c r="I20" s="162"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="175"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17358,13 +17529,13 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="158"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="162"/>
+      <c r="E21" s="177"/>
+      <c r="F21" s="173"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="174"/>
+      <c r="I21" s="175"/>
       <c r="K21" s="84" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -17374,11 +17545,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="157"/>
-      <c r="F22" s="158"/>
-      <c r="G22" s="157"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="162"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="174"/>
+      <c r="I22" s="175"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17387,11 +17558,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="157"/>
-      <c r="F23" s="158"/>
-      <c r="G23" s="157"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="162"/>
+      <c r="E23" s="177"/>
+      <c r="F23" s="173"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="174"/>
+      <c r="I23" s="175"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17400,11 +17571,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="162"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="174"/>
+      <c r="I24" s="175"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17413,11 +17584,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="162"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="173"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="174"/>
+      <c r="I25" s="175"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17426,11 +17597,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="160"/>
-      <c r="G26" s="159"/>
+      <c r="E26" s="178"/>
+      <c r="F26" s="161"/>
+      <c r="G26" s="178"/>
       <c r="H26" s="163"/>
-      <c r="I26" s="164"/>
+      <c r="I26" s="165"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18408,16 +18579,14 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18430,14 +18599,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -18472,13 +18643,13 @@
       <c r="A1" s="95"/>
       <c r="B1" s="96"/>
       <c r="C1" s="96" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="D1" s="96"/>
       <c r="E1" s="96"/>
       <c r="F1" s="96"/>
       <c r="G1" s="96" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="H1" s="96"/>
       <c r="I1" s="97"/>
@@ -18486,7 +18657,7 @@
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="179" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="B2" s="180"/>
       <c r="C2" s="156"/>
@@ -18503,7 +18674,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="C3" s="106" t="s">
         <v>7</v>
@@ -18515,10 +18686,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="106" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="G3" s="106" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="H3" s="109" t="s">
         <v>12</v>
@@ -18537,7 +18708,7 @@
     <row r="5" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="91"/>
       <c r="B5" s="111" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="D5" s="91"/>
       <c r="K5" s="112"/>
@@ -18547,7 +18718,7 @@
     </row>
     <row r="6" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="113" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="D6" s="91"/>
       <c r="K6" s="112"/>
@@ -18555,7 +18726,7 @@
     </row>
     <row r="7" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="113" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="D7" s="91"/>
       <c r="K7" s="112"/>
@@ -18563,7 +18734,7 @@
     </row>
     <row r="8" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="113" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="D8" s="91"/>
       <c r="K8" s="112"/>
@@ -18575,14 +18746,14 @@
     </row>
     <row r="10" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="111" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="K10" s="112"/>
       <c r="O10" s="98"/>
     </row>
     <row r="11" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="113" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="K11" s="112"/>
       <c r="O11" s="98"/>
@@ -21582,19 +21753,19 @@
     <row r="1" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="181" t="s">
-        <v>685</v>
-      </c>
-      <c r="C2" s="158"/>
+        <v>679</v>
+      </c>
+      <c r="C2" s="173"/>
       <c r="O2" s="84" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="114" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="C3" s="115" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21602,10 +21773,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="D4" s="84" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21613,10 +21784,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="D5" s="84" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21624,10 +21795,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="D6" s="84" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21635,10 +21806,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="D7" s="84" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21646,10 +21817,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="D8" s="84" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21657,10 +21828,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="D9" s="84" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21668,10 +21839,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="D10" s="84" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21679,10 +21850,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="D11" s="84" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21690,10 +21861,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="D12" s="84" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21701,10 +21872,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="D13" s="84" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21712,10 +21883,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="D14" s="84" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21723,10 +21894,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="D15" s="84" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21734,10 +21905,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -21745,10 +21916,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -22794,60 +22965,60 @@
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J2" s="84" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="181" t="s">
-        <v>718</v>
-      </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="158"/>
+        <v>712</v>
+      </c>
+      <c r="B3" s="174"/>
+      <c r="C3" s="173"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B4" s="183" t="s">
-        <v>719</v>
-      </c>
-      <c r="C4" s="158"/>
+        <v>713</v>
+      </c>
+      <c r="C4" s="173"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="B5" s="182" t="s">
-        <v>721</v>
-      </c>
-      <c r="C5" s="158"/>
+        <v>715</v>
+      </c>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="B6" s="182" t="s">
-        <v>723</v>
-      </c>
-      <c r="C6" s="158"/>
+        <v>717</v>
+      </c>
+      <c r="C6" s="173"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="B7" s="182" t="s">
-        <v>725</v>
-      </c>
-      <c r="C7" s="158"/>
+        <v>719</v>
+      </c>
+      <c r="C7" s="173"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B8" s="182" t="s">
-        <v>727</v>
-      </c>
-      <c r="C8" s="158"/>
+        <v>721</v>
+      </c>
+      <c r="C8" s="173"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23876,111 +24047,111 @@
     </row>
     <row r="2" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="184" t="s">
-        <v>728</v>
-      </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
+        <v>722</v>
+      </c>
+      <c r="C2" s="158"/>
+      <c r="D2" s="159"/>
       <c r="J2" s="84" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="119" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="C3" s="115" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="D3" s="120" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="121" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="C4" s="122" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="D4" s="123" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="121" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="C5" s="122" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="D5" s="124" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="121" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="C6" s="122" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="D6" s="124" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="121" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="C7" s="125" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="D7" s="124" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="121" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="C8" s="122" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="D8" s="124" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="121" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="C9" s="122" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="D9" s="126" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="121" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="C10" s="125" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="D10" s="124" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="127" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="C11" s="128" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="D11" s="90" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26977,24 +27148,24 @@
     <row r="2" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="84" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="84" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="D4" s="129" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="84" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="D6" s="129" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28021,7 +28192,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J1" s="84" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28029,67 +28200,67 @@
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="183" t="s">
-        <v>761</v>
-      </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="158"/>
+        <v>755</v>
+      </c>
+      <c r="B5" s="174"/>
+      <c r="C5" s="173"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="B6" s="116" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="C6" s="116" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="130" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="B7" s="93" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="C7" s="122" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="131" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B8" s="132" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="C8" s="122" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="I8" s="84" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="133" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B9" s="125" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="C9" s="122" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="134" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="B10" s="93" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="C10" s="122" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DRK  folder created in CF to keep them separated, few tgt added for the list
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\_I\Dokumentumok\132\_OPAT\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE339416-08C4-4A91-814C-9FF41324D4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F510309B-48B7-4A25-98A3-55E12AE3BB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3924,6 +3924,17 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3992,17 +4003,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5383,10 +5383,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B240" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B237" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E249" sqref="E249"/>
+      <selection pane="bottomRight" activeCell="E245" sqref="E245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5405,15 +5405,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="152" t="s">
+      <c r="A1" s="157" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="G1" s="154"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="159"/>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
@@ -5426,10 +5426,10 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="156"/>
+      <c r="B2" s="161"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
@@ -10930,7 +10930,7 @@
       <c r="E242" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="F242" s="188" t="s">
+      <c r="F242" s="155" t="s">
         <v>885</v>
       </c>
       <c r="G242" s="57">
@@ -10955,7 +10955,7 @@
       <c r="E243" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="F243" s="188" t="s">
+      <c r="F243" s="155" t="s">
         <v>891</v>
       </c>
       <c r="G243" s="74">
@@ -10980,7 +10980,7 @@
       <c r="E244" s="45" t="s">
         <v>513</v>
       </c>
-      <c r="F244" s="188" t="s">
+      <c r="F244" s="155" t="s">
         <v>888</v>
       </c>
       <c r="G244" s="57">
@@ -11040,7 +11040,7 @@
         <v>22</v>
       </c>
       <c r="I246" s="70"/>
-      <c r="K246" s="185" t="s">
+      <c r="K246" s="152" t="s">
         <v>231</v>
       </c>
     </row>
@@ -11108,7 +11108,7 @@
       <c r="E249" s="18" t="s">
         <v>878</v>
       </c>
-      <c r="F249" s="188" t="s">
+      <c r="F249" s="155" t="s">
         <v>884</v>
       </c>
       <c r="G249" s="74">
@@ -11125,17 +11125,17 @@
       <c r="A250" s="73" t="s">
         <v>522</v>
       </c>
-      <c r="B250" s="186" t="s">
+      <c r="B250" s="153" t="s">
         <v>879</v>
       </c>
       <c r="C250" s="55">
         <v>3</v>
       </c>
       <c r="D250" s="56"/>
-      <c r="E250" s="187" t="s">
+      <c r="E250" s="154" t="s">
         <v>880</v>
       </c>
-      <c r="F250" s="188" t="s">
+      <c r="F250" s="155" t="s">
         <v>889</v>
       </c>
       <c r="G250" s="57">
@@ -11159,10 +11159,10 @@
         <v>3</v>
       </c>
       <c r="D251" s="27"/>
-      <c r="E251" s="189" t="s">
+      <c r="E251" s="156" t="s">
         <v>882</v>
       </c>
-      <c r="F251" s="188" t="s">
+      <c r="F251" s="155" t="s">
         <v>890</v>
       </c>
       <c r="G251" s="74">
@@ -11179,17 +11179,17 @@
       <c r="A252" s="73" t="s">
         <v>524</v>
       </c>
-      <c r="B252" s="186" t="s">
+      <c r="B252" s="153" t="s">
         <v>883</v>
       </c>
       <c r="C252" s="55">
         <v>4</v>
       </c>
       <c r="D252" s="56"/>
-      <c r="E252" s="187" t="s">
+      <c r="E252" s="154" t="s">
         <v>887</v>
       </c>
-      <c r="F252" s="188" t="s">
+      <c r="F252" s="155" t="s">
         <v>886</v>
       </c>
       <c r="G252" s="57">
@@ -11207,7 +11207,7 @@
       <c r="B253" s="26"/>
       <c r="C253" s="29"/>
       <c r="D253" s="27"/>
-      <c r="E253" s="189"/>
+      <c r="E253" s="156"/>
       <c r="F253" s="2"/>
       <c r="G253" s="74"/>
       <c r="H253" s="70"/>
@@ -17126,7 +17126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17143,50 +17145,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="162" t="s">
         <v>614</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="159"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="164"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="165" t="s">
         <v>615</v>
       </c>
-      <c r="B2" s="161"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="80" t="s">
         <v>616</v>
       </c>
-      <c r="D2" s="162" t="s">
+      <c r="D2" s="167" t="s">
         <v>617</v>
       </c>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="161"/>
-      <c r="H2" s="164" t="s">
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="169" t="s">
         <v>618</v>
       </c>
-      <c r="I2" s="165"/>
+      <c r="I2" s="170"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="166" t="s">
+      <c r="A4" s="171" t="s">
         <v>619</v>
       </c>
-      <c r="B4" s="158"/>
-      <c r="C4" s="158"/>
-      <c r="D4" s="158"/>
-      <c r="E4" s="158"/>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="158"/>
-      <c r="I4" s="159"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="164"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -17248,15 +17250,15 @@
       <c r="I6" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="K6" s="167" t="s">
+      <c r="K6" s="172" t="s">
         <v>637</v>
       </c>
-      <c r="L6" s="168"/>
-      <c r="M6" s="168"/>
-      <c r="N6" s="168"/>
-      <c r="O6" s="168"/>
-      <c r="P6" s="168"/>
-      <c r="Q6" s="168"/>
+      <c r="L6" s="173"/>
+      <c r="M6" s="173"/>
+      <c r="N6" s="173"/>
+      <c r="O6" s="173"/>
+      <c r="P6" s="173"/>
+      <c r="Q6" s="173"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
@@ -17286,15 +17288,15 @@
       <c r="I7" s="87" t="s">
         <v>645</v>
       </c>
-      <c r="K7" s="167" t="s">
+      <c r="K7" s="172" t="s">
         <v>646</v>
       </c>
-      <c r="L7" s="168"/>
-      <c r="M7" s="168"/>
-      <c r="N7" s="168"/>
-      <c r="O7" s="168"/>
-      <c r="P7" s="168"/>
-      <c r="Q7" s="168"/>
+      <c r="L7" s="173"/>
+      <c r="M7" s="173"/>
+      <c r="N7" s="173"/>
+      <c r="O7" s="173"/>
+      <c r="P7" s="173"/>
+      <c r="Q7" s="173"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
@@ -17402,17 +17404,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="169" t="s">
+      <c r="A15" s="174" t="s">
         <v>655</v>
       </c>
-      <c r="B15" s="170"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="170"/>
-      <c r="E15" s="170"/>
-      <c r="F15" s="170"/>
-      <c r="G15" s="170"/>
-      <c r="H15" s="170"/>
-      <c r="I15" s="171"/>
+      <c r="B15" s="175"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="175"/>
+      <c r="F15" s="175"/>
+      <c r="G15" s="175"/>
+      <c r="H15" s="175"/>
+      <c r="I15" s="176"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
@@ -17427,15 +17429,15 @@
       <c r="D16" s="82" t="s">
         <v>627</v>
       </c>
-      <c r="E16" s="172" t="s">
+      <c r="E16" s="177" t="s">
         <v>656</v>
       </c>
-      <c r="F16" s="173"/>
-      <c r="G16" s="172" t="s">
+      <c r="F16" s="178"/>
+      <c r="G16" s="177" t="s">
         <v>657</v>
       </c>
-      <c r="H16" s="174"/>
-      <c r="I16" s="175"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="180"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -17450,15 +17452,15 @@
       <c r="D17" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="176" t="s">
+      <c r="E17" s="181" t="s">
         <v>659</v>
       </c>
-      <c r="F17" s="173"/>
-      <c r="G17" s="176" t="s">
+      <c r="F17" s="178"/>
+      <c r="G17" s="181" t="s">
         <v>660</v>
       </c>
-      <c r="H17" s="174"/>
-      <c r="I17" s="175"/>
+      <c r="H17" s="179"/>
+      <c r="I17" s="180"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -17473,15 +17475,15 @@
       <c r="D18" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="176" t="s">
+      <c r="E18" s="181" t="s">
         <v>659</v>
       </c>
-      <c r="F18" s="173"/>
-      <c r="G18" s="176" t="s">
+      <c r="F18" s="178"/>
+      <c r="G18" s="181" t="s">
         <v>662</v>
       </c>
-      <c r="H18" s="174"/>
-      <c r="I18" s="175"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="180"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
@@ -17496,15 +17498,15 @@
       <c r="D19" s="86" t="s">
         <v>664</v>
       </c>
-      <c r="E19" s="176" t="s">
+      <c r="E19" s="181" t="s">
         <v>665</v>
       </c>
-      <c r="F19" s="173"/>
-      <c r="G19" s="176" t="s">
+      <c r="F19" s="178"/>
+      <c r="G19" s="181" t="s">
         <v>666</v>
       </c>
-      <c r="H19" s="174"/>
-      <c r="I19" s="175"/>
+      <c r="H19" s="179"/>
+      <c r="I19" s="180"/>
       <c r="K19" s="84" t="s">
         <v>667</v>
       </c>
@@ -17516,11 +17518,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="177"/>
-      <c r="F20" s="173"/>
-      <c r="G20" s="177"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="175"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="179"/>
+      <c r="I20" s="180"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17529,11 +17531,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="177"/>
-      <c r="F21" s="173"/>
-      <c r="G21" s="177"/>
-      <c r="H21" s="174"/>
-      <c r="I21" s="175"/>
+      <c r="E21" s="182"/>
+      <c r="F21" s="178"/>
+      <c r="G21" s="182"/>
+      <c r="H21" s="179"/>
+      <c r="I21" s="180"/>
       <c r="K21" s="84" t="s">
         <v>668</v>
       </c>
@@ -17545,11 +17547,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="177"/>
-      <c r="F22" s="173"/>
-      <c r="G22" s="177"/>
-      <c r="H22" s="174"/>
-      <c r="I22" s="175"/>
+      <c r="E22" s="182"/>
+      <c r="F22" s="178"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="179"/>
+      <c r="I22" s="180"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17558,11 +17560,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="177"/>
-      <c r="F23" s="173"/>
-      <c r="G23" s="177"/>
-      <c r="H23" s="174"/>
-      <c r="I23" s="175"/>
+      <c r="E23" s="182"/>
+      <c r="F23" s="178"/>
+      <c r="G23" s="182"/>
+      <c r="H23" s="179"/>
+      <c r="I23" s="180"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17571,11 +17573,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="177"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="177"/>
-      <c r="H24" s="174"/>
-      <c r="I24" s="175"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="182"/>
+      <c r="H24" s="179"/>
+      <c r="I24" s="180"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17584,11 +17586,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="177"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="177"/>
-      <c r="H25" s="174"/>
-      <c r="I25" s="175"/>
+      <c r="E25" s="182"/>
+      <c r="F25" s="178"/>
+      <c r="G25" s="182"/>
+      <c r="H25" s="179"/>
+      <c r="I25" s="180"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17597,11 +17599,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="178"/>
-      <c r="F26" s="161"/>
-      <c r="G26" s="178"/>
-      <c r="H26" s="163"/>
-      <c r="I26" s="165"/>
+      <c r="E26" s="183"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="183"/>
+      <c r="H26" s="168"/>
+      <c r="I26" s="170"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18620,7 +18622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18656,11 +18660,11 @@
       <c r="O1" s="98"/>
     </row>
     <row r="2" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="179" t="s">
+      <c r="A2" s="184" t="s">
         <v>671</v>
       </c>
-      <c r="B2" s="180"/>
-      <c r="C2" s="156"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="161"/>
       <c r="D2" s="99"/>
       <c r="E2" s="100"/>
       <c r="F2" s="101"/>
@@ -21752,10 +21756,10 @@
   <sheetData>
     <row r="1" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="186" t="s">
         <v>679</v>
       </c>
-      <c r="C2" s="173"/>
+      <c r="C2" s="178"/>
       <c r="O2" s="84" t="s">
         <v>680</v>
       </c>
@@ -22969,56 +22973,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="186" t="s">
         <v>712</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="173"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="178"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
         <v>620</v>
       </c>
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="188" t="s">
         <v>713</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="178"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
         <v>714</v>
       </c>
-      <c r="B5" s="182" t="s">
+      <c r="B5" s="187" t="s">
         <v>715</v>
       </c>
-      <c r="C5" s="173"/>
+      <c r="C5" s="178"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
         <v>716</v>
       </c>
-      <c r="B6" s="182" t="s">
+      <c r="B6" s="187" t="s">
         <v>717</v>
       </c>
-      <c r="C6" s="173"/>
+      <c r="C6" s="178"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
         <v>718</v>
       </c>
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="187" t="s">
         <v>719</v>
       </c>
-      <c r="C7" s="173"/>
+      <c r="C7" s="178"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
         <v>720</v>
       </c>
-      <c r="B8" s="182" t="s">
+      <c r="B8" s="187" t="s">
         <v>721</v>
       </c>
-      <c r="C8" s="173"/>
+      <c r="C8" s="178"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24046,11 +24050,11 @@
       <c r="D1" s="118"/>
     </row>
     <row r="2" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="189" t="s">
         <v>722</v>
       </c>
-      <c r="C2" s="158"/>
-      <c r="D2" s="159"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="164"/>
       <c r="J2" s="84" t="s">
         <v>680</v>
       </c>
@@ -28199,11 +28203,11 @@
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="183" t="s">
+      <c r="A5" s="188" t="s">
         <v>755</v>
       </c>
-      <c r="B5" s="174"/>
-      <c r="C5" s="173"/>
+      <c r="B5" s="179"/>
+      <c r="C5" s="178"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
Initial version of Kambiland as candidate for Air attack (KCAA) , updates target list with DRK targets
KCAA can now be populated with targets
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\_I\Dokumentumok\132\_OPAT\INTEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\OPAT-background\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F510309B-48B7-4A25-98A3-55E12AE3BB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15320682-5C8A-489F-B3FC-1F6C07028515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="37680" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAC Joint Target List" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="892">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -3944,25 +3944,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3976,17 +3971,22 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5383,10 +5383,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B237" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B216" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E245" sqref="E245"/>
+      <selection pane="bottomRight" activeCell="I252" sqref="I242:I252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10939,7 +10939,9 @@
       <c r="H242" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I242" s="70"/>
+      <c r="I242" s="75" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="243" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="73" t="s">
@@ -10964,7 +10966,9 @@
       <c r="H243" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I243" s="70"/>
+      <c r="I243" s="75" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="244" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="73" t="s">
@@ -10989,7 +10993,9 @@
       <c r="H244" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I244" s="70"/>
+      <c r="I244" s="75" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="245" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="73" t="s">
@@ -11014,7 +11020,9 @@
       <c r="H245" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I245" s="70"/>
+      <c r="I245" s="75" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="246" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="73" t="s">
@@ -11039,7 +11047,9 @@
       <c r="H246" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I246" s="70"/>
+      <c r="I246" s="75" t="s">
+        <v>22</v>
+      </c>
       <c r="K246" s="152" t="s">
         <v>231</v>
       </c>
@@ -11067,7 +11077,9 @@
       <c r="H247" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I247" s="70"/>
+      <c r="I247" s="75" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="248" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="73" t="s">
@@ -11092,7 +11104,9 @@
       <c r="H248" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I248" s="70"/>
+      <c r="I248" s="75" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="249" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="73" t="s">
@@ -11198,7 +11212,9 @@
       <c r="H252" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I252" s="70"/>
+      <c r="I252" s="75" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="253" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="73" t="s">
@@ -17145,50 +17161,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="177" t="s">
         <v>614</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="164"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="179"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="180" t="s">
         <v>615</v>
       </c>
-      <c r="B2" s="166"/>
+      <c r="B2" s="165"/>
       <c r="C2" s="80" t="s">
         <v>616</v>
       </c>
-      <c r="D2" s="167" t="s">
+      <c r="D2" s="181" t="s">
         <v>617</v>
       </c>
       <c r="E2" s="168"/>
       <c r="F2" s="168"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="169" t="s">
+      <c r="G2" s="165"/>
+      <c r="H2" s="182" t="s">
         <v>618</v>
       </c>
-      <c r="I2" s="170"/>
+      <c r="I2" s="169"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="183" t="s">
         <v>619</v>
       </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="164"/>
+      <c r="B4" s="178"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="179"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -17250,15 +17266,15 @@
       <c r="I6" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="K6" s="172" t="s">
+      <c r="K6" s="171" t="s">
         <v>637</v>
       </c>
-      <c r="L6" s="173"/>
-      <c r="M6" s="173"/>
-      <c r="N6" s="173"/>
-      <c r="O6" s="173"/>
-      <c r="P6" s="173"/>
-      <c r="Q6" s="173"/>
+      <c r="L6" s="172"/>
+      <c r="M6" s="172"/>
+      <c r="N6" s="172"/>
+      <c r="O6" s="172"/>
+      <c r="P6" s="172"/>
+      <c r="Q6" s="172"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
@@ -17288,15 +17304,15 @@
       <c r="I7" s="87" t="s">
         <v>645</v>
       </c>
-      <c r="K7" s="172" t="s">
+      <c r="K7" s="171" t="s">
         <v>646</v>
       </c>
-      <c r="L7" s="173"/>
-      <c r="M7" s="173"/>
-      <c r="N7" s="173"/>
-      <c r="O7" s="173"/>
-      <c r="P7" s="173"/>
-      <c r="Q7" s="173"/>
+      <c r="L7" s="172"/>
+      <c r="M7" s="172"/>
+      <c r="N7" s="172"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="172"/>
+      <c r="Q7" s="172"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
@@ -17404,17 +17420,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="174" t="s">
+      <c r="A15" s="173" t="s">
         <v>655</v>
       </c>
-      <c r="B15" s="175"/>
-      <c r="C15" s="175"/>
-      <c r="D15" s="175"/>
-      <c r="E15" s="175"/>
-      <c r="F15" s="175"/>
-      <c r="G15" s="175"/>
-      <c r="H15" s="175"/>
-      <c r="I15" s="176"/>
+      <c r="B15" s="174"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="174"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="174"/>
+      <c r="I15" s="175"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
@@ -17429,15 +17445,15 @@
       <c r="D16" s="82" t="s">
         <v>627</v>
       </c>
-      <c r="E16" s="177" t="s">
+      <c r="E16" s="176" t="s">
         <v>656</v>
       </c>
-      <c r="F16" s="178"/>
-      <c r="G16" s="177" t="s">
+      <c r="F16" s="163"/>
+      <c r="G16" s="176" t="s">
         <v>657</v>
       </c>
-      <c r="H16" s="179"/>
-      <c r="I16" s="180"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="167"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -17452,15 +17468,15 @@
       <c r="D17" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="181" t="s">
+      <c r="E17" s="170" t="s">
         <v>659</v>
       </c>
-      <c r="F17" s="178"/>
-      <c r="G17" s="181" t="s">
+      <c r="F17" s="163"/>
+      <c r="G17" s="170" t="s">
         <v>660</v>
       </c>
-      <c r="H17" s="179"/>
-      <c r="I17" s="180"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="167"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -17475,15 +17491,15 @@
       <c r="D18" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="181" t="s">
+      <c r="E18" s="170" t="s">
         <v>659</v>
       </c>
-      <c r="F18" s="178"/>
-      <c r="G18" s="181" t="s">
+      <c r="F18" s="163"/>
+      <c r="G18" s="170" t="s">
         <v>662</v>
       </c>
-      <c r="H18" s="179"/>
-      <c r="I18" s="180"/>
+      <c r="H18" s="166"/>
+      <c r="I18" s="167"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
@@ -17498,15 +17514,15 @@
       <c r="D19" s="86" t="s">
         <v>664</v>
       </c>
-      <c r="E19" s="181" t="s">
+      <c r="E19" s="170" t="s">
         <v>665</v>
       </c>
-      <c r="F19" s="178"/>
-      <c r="G19" s="181" t="s">
+      <c r="F19" s="163"/>
+      <c r="G19" s="170" t="s">
         <v>666</v>
       </c>
-      <c r="H19" s="179"/>
-      <c r="I19" s="180"/>
+      <c r="H19" s="166"/>
+      <c r="I19" s="167"/>
       <c r="K19" s="84" t="s">
         <v>667</v>
       </c>
@@ -17518,11 +17534,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="182"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="182"/>
-      <c r="H20" s="179"/>
-      <c r="I20" s="180"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="166"/>
+      <c r="I20" s="167"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17531,11 +17547,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="182"/>
-      <c r="F21" s="178"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="179"/>
-      <c r="I21" s="180"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="163"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="166"/>
+      <c r="I21" s="167"/>
       <c r="K21" s="84" t="s">
         <v>668</v>
       </c>
@@ -17547,11 +17563,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="182"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="182"/>
-      <c r="H22" s="179"/>
-      <c r="I22" s="180"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="162"/>
+      <c r="H22" s="166"/>
+      <c r="I22" s="167"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17560,11 +17576,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="182"/>
-      <c r="F23" s="178"/>
-      <c r="G23" s="182"/>
-      <c r="H23" s="179"/>
-      <c r="I23" s="180"/>
+      <c r="E23" s="162"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="162"/>
+      <c r="H23" s="166"/>
+      <c r="I23" s="167"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17573,11 +17589,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="182"/>
-      <c r="F24" s="178"/>
-      <c r="G24" s="182"/>
-      <c r="H24" s="179"/>
-      <c r="I24" s="180"/>
+      <c r="E24" s="162"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="162"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="167"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17586,11 +17602,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="182"/>
-      <c r="F25" s="178"/>
-      <c r="G25" s="182"/>
-      <c r="H25" s="179"/>
-      <c r="I25" s="180"/>
+      <c r="E25" s="162"/>
+      <c r="F25" s="163"/>
+      <c r="G25" s="162"/>
+      <c r="H25" s="166"/>
+      <c r="I25" s="167"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17599,11 +17615,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="183"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="183"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="165"/>
+      <c r="G26" s="164"/>
       <c r="H26" s="168"/>
-      <c r="I26" s="170"/>
+      <c r="I26" s="169"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18581,14 +18597,16 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18601,16 +18619,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21759,7 +21775,7 @@
       <c r="B2" s="186" t="s">
         <v>679</v>
       </c>
-      <c r="C2" s="178"/>
+      <c r="C2" s="163"/>
       <c r="O2" s="84" t="s">
         <v>680</v>
       </c>
@@ -22976,8 +22992,8 @@
       <c r="A3" s="186" t="s">
         <v>712</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="178"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="163"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
@@ -22986,7 +23002,7 @@
       <c r="B4" s="188" t="s">
         <v>713</v>
       </c>
-      <c r="C4" s="178"/>
+      <c r="C4" s="163"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
@@ -22995,7 +23011,7 @@
       <c r="B5" s="187" t="s">
         <v>715</v>
       </c>
-      <c r="C5" s="178"/>
+      <c r="C5" s="163"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
@@ -23004,7 +23020,7 @@
       <c r="B6" s="187" t="s">
         <v>717</v>
       </c>
-      <c r="C6" s="178"/>
+      <c r="C6" s="163"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
@@ -23013,7 +23029,7 @@
       <c r="B7" s="187" t="s">
         <v>719</v>
       </c>
-      <c r="C7" s="178"/>
+      <c r="C7" s="163"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
@@ -23022,7 +23038,7 @@
       <c r="B8" s="187" t="s">
         <v>721</v>
       </c>
-      <c r="C8" s="178"/>
+      <c r="C8" s="163"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24053,8 +24069,8 @@
       <c r="B2" s="189" t="s">
         <v>722</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="164"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="179"/>
       <c r="J2" s="84" t="s">
         <v>680</v>
       </c>
@@ -28206,8 +28222,8 @@
       <c r="A5" s="188" t="s">
         <v>755</v>
       </c>
-      <c r="B5" s="179"/>
-      <c r="C5" s="178"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="163"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
put Robin into DRK list
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\OPAT-background\INTEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\_I\Dokumentumok\132\_OPAT\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15320682-5C8A-489F-B3FC-1F6C07028515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AF8522-F4D0-43CE-9136-1636E6E97645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-120" windowWidth="37680" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="893">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -2732,6 +2732,9 @@
   </si>
   <si>
     <t>N 65 49.046 E 031 28.752</t>
+  </si>
+  <si>
+    <t>Robin</t>
   </si>
 </sst>
 </file>
@@ -3944,20 +3947,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3971,22 +3979,17 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5383,10 +5386,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B216" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I252" sqref="I242:I252"/>
+      <selection pane="bottomRight" activeCell="G255" sqref="G255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10942,6 +10945,9 @@
       <c r="I242" s="75" t="s">
         <v>22</v>
       </c>
+      <c r="K242" t="s">
+        <v>892</v>
+      </c>
     </row>
     <row r="243" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="73" t="s">
@@ -11214,6 +11220,9 @@
       </c>
       <c r="I252" s="75" t="s">
         <v>22</v>
+      </c>
+      <c r="K252" s="152" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="253" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17161,50 +17170,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="162" t="s">
         <v>614</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="179"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="164"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="165" t="s">
         <v>615</v>
       </c>
-      <c r="B2" s="165"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="80" t="s">
         <v>616</v>
       </c>
-      <c r="D2" s="181" t="s">
+      <c r="D2" s="167" t="s">
         <v>617</v>
       </c>
       <c r="E2" s="168"/>
       <c r="F2" s="168"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="182" t="s">
+      <c r="G2" s="166"/>
+      <c r="H2" s="169" t="s">
         <v>618</v>
       </c>
-      <c r="I2" s="169"/>
+      <c r="I2" s="170"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="183" t="s">
+      <c r="A4" s="171" t="s">
         <v>619</v>
       </c>
-      <c r="B4" s="178"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
-      <c r="I4" s="179"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
+      <c r="H4" s="163"/>
+      <c r="I4" s="164"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -17266,15 +17275,15 @@
       <c r="I6" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="K6" s="171" t="s">
+      <c r="K6" s="172" t="s">
         <v>637</v>
       </c>
-      <c r="L6" s="172"/>
-      <c r="M6" s="172"/>
-      <c r="N6" s="172"/>
-      <c r="O6" s="172"/>
-      <c r="P6" s="172"/>
-      <c r="Q6" s="172"/>
+      <c r="L6" s="173"/>
+      <c r="M6" s="173"/>
+      <c r="N6" s="173"/>
+      <c r="O6" s="173"/>
+      <c r="P6" s="173"/>
+      <c r="Q6" s="173"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
@@ -17304,15 +17313,15 @@
       <c r="I7" s="87" t="s">
         <v>645</v>
       </c>
-      <c r="K7" s="171" t="s">
+      <c r="K7" s="172" t="s">
         <v>646</v>
       </c>
-      <c r="L7" s="172"/>
-      <c r="M7" s="172"/>
-      <c r="N7" s="172"/>
-      <c r="O7" s="172"/>
-      <c r="P7" s="172"/>
-      <c r="Q7" s="172"/>
+      <c r="L7" s="173"/>
+      <c r="M7" s="173"/>
+      <c r="N7" s="173"/>
+      <c r="O7" s="173"/>
+      <c r="P7" s="173"/>
+      <c r="Q7" s="173"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
@@ -17420,17 +17429,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="173" t="s">
+      <c r="A15" s="174" t="s">
         <v>655</v>
       </c>
-      <c r="B15" s="174"/>
-      <c r="C15" s="174"/>
-      <c r="D15" s="174"/>
-      <c r="E15" s="174"/>
-      <c r="F15" s="174"/>
-      <c r="G15" s="174"/>
-      <c r="H15" s="174"/>
-      <c r="I15" s="175"/>
+      <c r="B15" s="175"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="175"/>
+      <c r="F15" s="175"/>
+      <c r="G15" s="175"/>
+      <c r="H15" s="175"/>
+      <c r="I15" s="176"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
@@ -17445,15 +17454,15 @@
       <c r="D16" s="82" t="s">
         <v>627</v>
       </c>
-      <c r="E16" s="176" t="s">
+      <c r="E16" s="177" t="s">
         <v>656</v>
       </c>
-      <c r="F16" s="163"/>
-      <c r="G16" s="176" t="s">
+      <c r="F16" s="178"/>
+      <c r="G16" s="177" t="s">
         <v>657</v>
       </c>
-      <c r="H16" s="166"/>
-      <c r="I16" s="167"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="180"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -17468,15 +17477,15 @@
       <c r="D17" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="170" t="s">
+      <c r="E17" s="181" t="s">
         <v>659</v>
       </c>
-      <c r="F17" s="163"/>
-      <c r="G17" s="170" t="s">
+      <c r="F17" s="178"/>
+      <c r="G17" s="181" t="s">
         <v>660</v>
       </c>
-      <c r="H17" s="166"/>
-      <c r="I17" s="167"/>
+      <c r="H17" s="179"/>
+      <c r="I17" s="180"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -17491,15 +17500,15 @@
       <c r="D18" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="170" t="s">
+      <c r="E18" s="181" t="s">
         <v>659</v>
       </c>
-      <c r="F18" s="163"/>
-      <c r="G18" s="170" t="s">
+      <c r="F18" s="178"/>
+      <c r="G18" s="181" t="s">
         <v>662</v>
       </c>
-      <c r="H18" s="166"/>
-      <c r="I18" s="167"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="180"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
@@ -17514,15 +17523,15 @@
       <c r="D19" s="86" t="s">
         <v>664</v>
       </c>
-      <c r="E19" s="170" t="s">
+      <c r="E19" s="181" t="s">
         <v>665</v>
       </c>
-      <c r="F19" s="163"/>
-      <c r="G19" s="170" t="s">
+      <c r="F19" s="178"/>
+      <c r="G19" s="181" t="s">
         <v>666</v>
       </c>
-      <c r="H19" s="166"/>
-      <c r="I19" s="167"/>
+      <c r="H19" s="179"/>
+      <c r="I19" s="180"/>
       <c r="K19" s="84" t="s">
         <v>667</v>
       </c>
@@ -17534,11 +17543,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="162"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="162"/>
-      <c r="H20" s="166"/>
-      <c r="I20" s="167"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="179"/>
+      <c r="I20" s="180"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17547,11 +17556,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="162"/>
-      <c r="F21" s="163"/>
-      <c r="G21" s="162"/>
-      <c r="H21" s="166"/>
-      <c r="I21" s="167"/>
+      <c r="E21" s="182"/>
+      <c r="F21" s="178"/>
+      <c r="G21" s="182"/>
+      <c r="H21" s="179"/>
+      <c r="I21" s="180"/>
       <c r="K21" s="84" t="s">
         <v>668</v>
       </c>
@@ -17563,11 +17572,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="162"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="162"/>
-      <c r="H22" s="166"/>
-      <c r="I22" s="167"/>
+      <c r="E22" s="182"/>
+      <c r="F22" s="178"/>
+      <c r="G22" s="182"/>
+      <c r="H22" s="179"/>
+      <c r="I22" s="180"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17576,11 +17585,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="162"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="162"/>
-      <c r="H23" s="166"/>
-      <c r="I23" s="167"/>
+      <c r="E23" s="182"/>
+      <c r="F23" s="178"/>
+      <c r="G23" s="182"/>
+      <c r="H23" s="179"/>
+      <c r="I23" s="180"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17589,11 +17598,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="162"/>
-      <c r="F24" s="163"/>
-      <c r="G24" s="162"/>
-      <c r="H24" s="166"/>
-      <c r="I24" s="167"/>
+      <c r="E24" s="182"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="182"/>
+      <c r="H24" s="179"/>
+      <c r="I24" s="180"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17602,11 +17611,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="162"/>
-      <c r="F25" s="163"/>
-      <c r="G25" s="162"/>
-      <c r="H25" s="166"/>
-      <c r="I25" s="167"/>
+      <c r="E25" s="182"/>
+      <c r="F25" s="178"/>
+      <c r="G25" s="182"/>
+      <c r="H25" s="179"/>
+      <c r="I25" s="180"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17615,11 +17624,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="164"/>
-      <c r="F26" s="165"/>
-      <c r="G26" s="164"/>
+      <c r="E26" s="183"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="183"/>
       <c r="H26" s="168"/>
-      <c r="I26" s="169"/>
+      <c r="I26" s="170"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18597,16 +18606,14 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18619,14 +18626,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21775,7 +21784,7 @@
       <c r="B2" s="186" t="s">
         <v>679</v>
       </c>
-      <c r="C2" s="163"/>
+      <c r="C2" s="178"/>
       <c r="O2" s="84" t="s">
         <v>680</v>
       </c>
@@ -22992,8 +23001,8 @@
       <c r="A3" s="186" t="s">
         <v>712</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="163"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="178"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
@@ -23002,7 +23011,7 @@
       <c r="B4" s="188" t="s">
         <v>713</v>
       </c>
-      <c r="C4" s="163"/>
+      <c r="C4" s="178"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
@@ -23011,7 +23020,7 @@
       <c r="B5" s="187" t="s">
         <v>715</v>
       </c>
-      <c r="C5" s="163"/>
+      <c r="C5" s="178"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
@@ -23020,7 +23029,7 @@
       <c r="B6" s="187" t="s">
         <v>717</v>
       </c>
-      <c r="C6" s="163"/>
+      <c r="C6" s="178"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
@@ -23029,7 +23038,7 @@
       <c r="B7" s="187" t="s">
         <v>719</v>
       </c>
-      <c r="C7" s="163"/>
+      <c r="C7" s="178"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
@@ -23038,7 +23047,7 @@
       <c r="B8" s="187" t="s">
         <v>721</v>
       </c>
-      <c r="C8" s="163"/>
+      <c r="C8" s="178"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24069,8 +24078,8 @@
       <c r="B2" s="189" t="s">
         <v>722</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="179"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="164"/>
       <c r="J2" s="84" t="s">
         <v>680</v>
       </c>
@@ -28222,8 +28231,8 @@
       <c r="A5" s="188" t="s">
         <v>755</v>
       </c>
-      <c r="B5" s="166"/>
-      <c r="C5" s="163"/>
+      <c r="B5" s="179"/>
+      <c r="C5" s="178"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
All VID provided DRK army elements are now in place in the miz
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\_I\Dokumentumok\132\_OPAT\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AF8522-F4D0-43CE-9136-1636E6E97645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0296E7D-7893-47A8-B1DB-AB6656322772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="37680" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="480" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAC Joint Target List" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="900">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -2735,6 +2735,27 @@
   </si>
   <si>
     <t>Robin</t>
+  </si>
+  <si>
+    <t>822nd Rocket artillery regiment</t>
+  </si>
+  <si>
+    <t>823rd Rocket artillery regiment</t>
+  </si>
+  <si>
+    <t>831th Special Forces Brigade</t>
+  </si>
+  <si>
+    <t>DRK Army Independent Unit</t>
+  </si>
+  <si>
+    <t>N 66 04.098 E 032 57.380</t>
+  </si>
+  <si>
+    <t>N 66 48.688 E 032 21.512</t>
+  </si>
+  <si>
+    <t>N 67 01.221 E 030 19.331</t>
   </si>
 </sst>
 </file>
@@ -3947,25 +3968,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3979,17 +3995,22 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5385,11 +5406,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B243" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G255" sqref="G255"/>
+      <selection pane="bottomRight" activeCell="E258" sqref="E258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10927,7 +10948,7 @@
         <v>508</v>
       </c>
       <c r="C242" s="55">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D242" s="56"/>
       <c r="E242" s="44" t="s">
@@ -10957,7 +10978,7 @@
         <v>510</v>
       </c>
       <c r="C243" s="29">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D243" s="27"/>
       <c r="E243" s="18" t="s">
@@ -10984,7 +11005,7 @@
         <v>512</v>
       </c>
       <c r="C244" s="55">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D244" s="56"/>
       <c r="E244" s="45" t="s">
@@ -11229,39 +11250,75 @@
       <c r="A253" s="73" t="s">
         <v>525</v>
       </c>
-      <c r="B253" s="26"/>
-      <c r="C253" s="29"/>
+      <c r="B253" s="26" t="s">
+        <v>893</v>
+      </c>
+      <c r="C253" s="29">
+        <v>6</v>
+      </c>
       <c r="D253" s="27"/>
-      <c r="E253" s="156"/>
-      <c r="F253" s="2"/>
-      <c r="G253" s="74"/>
-      <c r="H253" s="70"/>
+      <c r="E253" s="156" t="s">
+        <v>896</v>
+      </c>
+      <c r="F253" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="G253" s="74">
+        <v>323</v>
+      </c>
+      <c r="H253" s="75" t="s">
+        <v>22</v>
+      </c>
       <c r="I253" s="70"/>
     </row>
     <row r="254" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="73" t="s">
         <v>526</v>
       </c>
-      <c r="B254" s="44"/>
-      <c r="C254" s="55"/>
+      <c r="B254" s="44" t="s">
+        <v>894</v>
+      </c>
+      <c r="C254" s="55">
+        <v>6</v>
+      </c>
       <c r="D254" s="56"/>
-      <c r="E254" s="45"/>
-      <c r="F254" s="45"/>
-      <c r="G254" s="57"/>
-      <c r="H254" s="70"/>
+      <c r="E254" s="156" t="s">
+        <v>896</v>
+      </c>
+      <c r="F254" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="G254" s="57">
+        <v>188</v>
+      </c>
+      <c r="H254" s="75" t="s">
+        <v>22</v>
+      </c>
       <c r="I254" s="70"/>
     </row>
     <row r="255" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="73" t="s">
         <v>527</v>
       </c>
-      <c r="B255" s="26"/>
-      <c r="C255" s="29"/>
+      <c r="B255" s="26" t="s">
+        <v>895</v>
+      </c>
+      <c r="C255" s="29">
+        <v>6</v>
+      </c>
       <c r="D255" s="27"/>
-      <c r="E255" s="18"/>
-      <c r="F255" s="2"/>
-      <c r="G255" s="74"/>
-      <c r="H255" s="70"/>
+      <c r="E255" s="156" t="s">
+        <v>896</v>
+      </c>
+      <c r="F255" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="G255" s="74">
+        <v>553</v>
+      </c>
+      <c r="H255" s="75" t="s">
+        <v>22</v>
+      </c>
       <c r="I255" s="70"/>
     </row>
     <row r="256" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17170,50 +17227,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="177" t="s">
         <v>614</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="164"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="179"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="180" t="s">
         <v>615</v>
       </c>
-      <c r="B2" s="166"/>
+      <c r="B2" s="165"/>
       <c r="C2" s="80" t="s">
         <v>616</v>
       </c>
-      <c r="D2" s="167" t="s">
+      <c r="D2" s="181" t="s">
         <v>617</v>
       </c>
       <c r="E2" s="168"/>
       <c r="F2" s="168"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="169" t="s">
+      <c r="G2" s="165"/>
+      <c r="H2" s="182" t="s">
         <v>618</v>
       </c>
-      <c r="I2" s="170"/>
+      <c r="I2" s="169"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="183" t="s">
         <v>619</v>
       </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="164"/>
+      <c r="B4" s="178"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="179"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -17275,15 +17332,15 @@
       <c r="I6" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="K6" s="172" t="s">
+      <c r="K6" s="171" t="s">
         <v>637</v>
       </c>
-      <c r="L6" s="173"/>
-      <c r="M6" s="173"/>
-      <c r="N6" s="173"/>
-      <c r="O6" s="173"/>
-      <c r="P6" s="173"/>
-      <c r="Q6" s="173"/>
+      <c r="L6" s="172"/>
+      <c r="M6" s="172"/>
+      <c r="N6" s="172"/>
+      <c r="O6" s="172"/>
+      <c r="P6" s="172"/>
+      <c r="Q6" s="172"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
@@ -17313,15 +17370,15 @@
       <c r="I7" s="87" t="s">
         <v>645</v>
       </c>
-      <c r="K7" s="172" t="s">
+      <c r="K7" s="171" t="s">
         <v>646</v>
       </c>
-      <c r="L7" s="173"/>
-      <c r="M7" s="173"/>
-      <c r="N7" s="173"/>
-      <c r="O7" s="173"/>
-      <c r="P7" s="173"/>
-      <c r="Q7" s="173"/>
+      <c r="L7" s="172"/>
+      <c r="M7" s="172"/>
+      <c r="N7" s="172"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="172"/>
+      <c r="Q7" s="172"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
@@ -17429,17 +17486,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="174" t="s">
+      <c r="A15" s="173" t="s">
         <v>655</v>
       </c>
-      <c r="B15" s="175"/>
-      <c r="C15" s="175"/>
-      <c r="D15" s="175"/>
-      <c r="E15" s="175"/>
-      <c r="F15" s="175"/>
-      <c r="G15" s="175"/>
-      <c r="H15" s="175"/>
-      <c r="I15" s="176"/>
+      <c r="B15" s="174"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="174"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="174"/>
+      <c r="I15" s="175"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
@@ -17454,15 +17511,15 @@
       <c r="D16" s="82" t="s">
         <v>627</v>
       </c>
-      <c r="E16" s="177" t="s">
+      <c r="E16" s="176" t="s">
         <v>656</v>
       </c>
-      <c r="F16" s="178"/>
-      <c r="G16" s="177" t="s">
+      <c r="F16" s="163"/>
+      <c r="G16" s="176" t="s">
         <v>657</v>
       </c>
-      <c r="H16" s="179"/>
-      <c r="I16" s="180"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="167"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -17477,15 +17534,15 @@
       <c r="D17" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="181" t="s">
+      <c r="E17" s="170" t="s">
         <v>659</v>
       </c>
-      <c r="F17" s="178"/>
-      <c r="G17" s="181" t="s">
+      <c r="F17" s="163"/>
+      <c r="G17" s="170" t="s">
         <v>660</v>
       </c>
-      <c r="H17" s="179"/>
-      <c r="I17" s="180"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="167"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -17500,15 +17557,15 @@
       <c r="D18" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="181" t="s">
+      <c r="E18" s="170" t="s">
         <v>659</v>
       </c>
-      <c r="F18" s="178"/>
-      <c r="G18" s="181" t="s">
+      <c r="F18" s="163"/>
+      <c r="G18" s="170" t="s">
         <v>662</v>
       </c>
-      <c r="H18" s="179"/>
-      <c r="I18" s="180"/>
+      <c r="H18" s="166"/>
+      <c r="I18" s="167"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
@@ -17523,15 +17580,15 @@
       <c r="D19" s="86" t="s">
         <v>664</v>
       </c>
-      <c r="E19" s="181" t="s">
+      <c r="E19" s="170" t="s">
         <v>665</v>
       </c>
-      <c r="F19" s="178"/>
-      <c r="G19" s="181" t="s">
+      <c r="F19" s="163"/>
+      <c r="G19" s="170" t="s">
         <v>666</v>
       </c>
-      <c r="H19" s="179"/>
-      <c r="I19" s="180"/>
+      <c r="H19" s="166"/>
+      <c r="I19" s="167"/>
       <c r="K19" s="84" t="s">
         <v>667</v>
       </c>
@@ -17543,11 +17600,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="182"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="182"/>
-      <c r="H20" s="179"/>
-      <c r="I20" s="180"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="166"/>
+      <c r="I20" s="167"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17556,11 +17613,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="182"/>
-      <c r="F21" s="178"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="179"/>
-      <c r="I21" s="180"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="163"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="166"/>
+      <c r="I21" s="167"/>
       <c r="K21" s="84" t="s">
         <v>668</v>
       </c>
@@ -17572,11 +17629,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="182"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="182"/>
-      <c r="H22" s="179"/>
-      <c r="I22" s="180"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="162"/>
+      <c r="H22" s="166"/>
+      <c r="I22" s="167"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17585,11 +17642,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="182"/>
-      <c r="F23" s="178"/>
-      <c r="G23" s="182"/>
-      <c r="H23" s="179"/>
-      <c r="I23" s="180"/>
+      <c r="E23" s="162"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="162"/>
+      <c r="H23" s="166"/>
+      <c r="I23" s="167"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17598,11 +17655,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="182"/>
-      <c r="F24" s="178"/>
-      <c r="G24" s="182"/>
-      <c r="H24" s="179"/>
-      <c r="I24" s="180"/>
+      <c r="E24" s="162"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="162"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="167"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17611,11 +17668,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="182"/>
-      <c r="F25" s="178"/>
-      <c r="G25" s="182"/>
-      <c r="H25" s="179"/>
-      <c r="I25" s="180"/>
+      <c r="E25" s="162"/>
+      <c r="F25" s="163"/>
+      <c r="G25" s="162"/>
+      <c r="H25" s="166"/>
+      <c r="I25" s="167"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17624,11 +17681,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="183"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="183"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="165"/>
+      <c r="G26" s="164"/>
       <c r="H26" s="168"/>
-      <c r="I26" s="170"/>
+      <c r="I26" s="169"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18606,14 +18663,16 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18626,16 +18685,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21784,7 +21841,7 @@
       <c r="B2" s="186" t="s">
         <v>679</v>
       </c>
-      <c r="C2" s="178"/>
+      <c r="C2" s="163"/>
       <c r="O2" s="84" t="s">
         <v>680</v>
       </c>
@@ -23001,8 +23058,8 @@
       <c r="A3" s="186" t="s">
         <v>712</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="178"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="163"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
@@ -23011,7 +23068,7 @@
       <c r="B4" s="188" t="s">
         <v>713</v>
       </c>
-      <c r="C4" s="178"/>
+      <c r="C4" s="163"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
@@ -23020,7 +23077,7 @@
       <c r="B5" s="187" t="s">
         <v>715</v>
       </c>
-      <c r="C5" s="178"/>
+      <c r="C5" s="163"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
@@ -23029,7 +23086,7 @@
       <c r="B6" s="187" t="s">
         <v>717</v>
       </c>
-      <c r="C6" s="178"/>
+      <c r="C6" s="163"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
@@ -23038,7 +23095,7 @@
       <c r="B7" s="187" t="s">
         <v>719</v>
       </c>
-      <c r="C7" s="178"/>
+      <c r="C7" s="163"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
@@ -23047,7 +23104,7 @@
       <c r="B8" s="187" t="s">
         <v>721</v>
       </c>
-      <c r="C8" s="178"/>
+      <c r="C8" s="163"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24078,8 +24135,8 @@
       <c r="B2" s="189" t="s">
         <v>722</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="164"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="179"/>
       <c r="J2" s="84" t="s">
         <v>680</v>
       </c>
@@ -28231,8 +28288,8 @@
       <c r="A5" s="188" t="s">
         <v>755</v>
       </c>
-      <c r="B5" s="179"/>
-      <c r="C5" s="178"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="163"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
updated TGT list w DRK targets, KCAA is now 0.2 with the targets in it
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\OPAT-background\INTEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\OPAT-background\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC09D421-3C66-4845-86ED-C318AEE117D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E472B74C-96E9-4AD4-8AFC-79FC66C843B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="37680" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAC Joint Target List" sheetId="1" r:id="rId1"/>
@@ -23,16 +23,11 @@
     <sheet name="Risk levels" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="" roundtripDataChecksum="jqvuzJn8Lf/XHWAhwIuz09YQ2YQAYUhN1DjVsFh9M+Q="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="905">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -2756,6 +2751,21 @@
   </si>
   <si>
     <t>N 67 01.221 E 030 19.331</t>
+  </si>
+  <si>
+    <t>Zelenoborsky Vehicle Depot</t>
+  </si>
+  <si>
+    <t>Kovda Army Ammunition Storage</t>
+  </si>
+  <si>
+    <t>Louhi Rocket Artillery ammo depot</t>
+  </si>
+  <si>
+    <t>Nationalist TV Studio</t>
+  </si>
+  <si>
+    <t>Air Defense Command Center</t>
   </si>
 </sst>
 </file>
@@ -3546,10 +3556,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3968,25 +3979,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4000,17 +4006,22 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4028,9 +4039,17 @@
     <xf numFmtId="0" fontId="24" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál 2" xfId="1" xr:uid="{AD4AA7C0-7717-4E15-8659-E5F2B8E661BE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5407,10 +5426,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B210" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A57" sqref="A57:XFD57"/>
+      <selection pane="bottomRight" activeCell="A256" sqref="A256:B260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11328,10 +11347,12 @@
       <c r="I255" s="70"/>
     </row>
     <row r="256" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="73" t="s">
+      <c r="A256" s="192" t="s">
         <v>528</v>
       </c>
-      <c r="B256" s="44"/>
+      <c r="B256" s="191" t="s">
+        <v>900</v>
+      </c>
       <c r="C256" s="55"/>
       <c r="D256" s="56"/>
       <c r="E256" s="45"/>
@@ -11341,10 +11362,12 @@
       <c r="I256" s="70"/>
     </row>
     <row r="257" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="73" t="s">
+      <c r="A257" s="192" t="s">
         <v>529</v>
       </c>
-      <c r="B257" s="26"/>
+      <c r="B257" s="190" t="s">
+        <v>901</v>
+      </c>
       <c r="C257" s="29"/>
       <c r="D257" s="27"/>
       <c r="E257" s="18"/>
@@ -11354,10 +11377,12 @@
       <c r="I257" s="70"/>
     </row>
     <row r="258" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="73" t="s">
+      <c r="A258" s="192" t="s">
         <v>530</v>
       </c>
-      <c r="B258" s="44"/>
+      <c r="B258" s="191" t="s">
+        <v>902</v>
+      </c>
       <c r="C258" s="55"/>
       <c r="D258" s="56"/>
       <c r="E258" s="45"/>
@@ -11367,10 +11392,12 @@
       <c r="I258" s="70"/>
     </row>
     <row r="259" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="73" t="s">
+      <c r="A259" s="192" t="s">
         <v>531</v>
       </c>
-      <c r="B259" s="26"/>
+      <c r="B259" s="190" t="s">
+        <v>903</v>
+      </c>
       <c r="C259" s="29"/>
       <c r="D259" s="27"/>
       <c r="E259" s="18"/>
@@ -11380,10 +11407,12 @@
       <c r="I259" s="70"/>
     </row>
     <row r="260" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="73" t="s">
+      <c r="A260" s="192" t="s">
         <v>532</v>
       </c>
-      <c r="B260" s="44"/>
+      <c r="B260" s="191" t="s">
+        <v>904</v>
+      </c>
       <c r="C260" s="55"/>
       <c r="D260" s="56"/>
       <c r="E260" s="45"/>
@@ -17233,50 +17262,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="177" t="s">
         <v>614</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="164"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="179"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="180" t="s">
         <v>615</v>
       </c>
-      <c r="B2" s="166"/>
+      <c r="B2" s="165"/>
       <c r="C2" s="80" t="s">
         <v>616</v>
       </c>
-      <c r="D2" s="167" t="s">
+      <c r="D2" s="181" t="s">
         <v>617</v>
       </c>
       <c r="E2" s="168"/>
       <c r="F2" s="168"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="169" t="s">
+      <c r="G2" s="165"/>
+      <c r="H2" s="182" t="s">
         <v>618</v>
       </c>
-      <c r="I2" s="170"/>
+      <c r="I2" s="169"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="183" t="s">
         <v>619</v>
       </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="164"/>
+      <c r="B4" s="178"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="179"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -17338,15 +17367,15 @@
       <c r="I6" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="K6" s="172" t="s">
+      <c r="K6" s="171" t="s">
         <v>637</v>
       </c>
-      <c r="L6" s="173"/>
-      <c r="M6" s="173"/>
-      <c r="N6" s="173"/>
-      <c r="O6" s="173"/>
-      <c r="P6" s="173"/>
-      <c r="Q6" s="173"/>
+      <c r="L6" s="172"/>
+      <c r="M6" s="172"/>
+      <c r="N6" s="172"/>
+      <c r="O6" s="172"/>
+      <c r="P6" s="172"/>
+      <c r="Q6" s="172"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
@@ -17376,15 +17405,15 @@
       <c r="I7" s="87" t="s">
         <v>645</v>
       </c>
-      <c r="K7" s="172" t="s">
+      <c r="K7" s="171" t="s">
         <v>646</v>
       </c>
-      <c r="L7" s="173"/>
-      <c r="M7" s="173"/>
-      <c r="N7" s="173"/>
-      <c r="O7" s="173"/>
-      <c r="P7" s="173"/>
-      <c r="Q7" s="173"/>
+      <c r="L7" s="172"/>
+      <c r="M7" s="172"/>
+      <c r="N7" s="172"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="172"/>
+      <c r="Q7" s="172"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
@@ -17492,17 +17521,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="174" t="s">
+      <c r="A15" s="173" t="s">
         <v>655</v>
       </c>
-      <c r="B15" s="175"/>
-      <c r="C15" s="175"/>
-      <c r="D15" s="175"/>
-      <c r="E15" s="175"/>
-      <c r="F15" s="175"/>
-      <c r="G15" s="175"/>
-      <c r="H15" s="175"/>
-      <c r="I15" s="176"/>
+      <c r="B15" s="174"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="174"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="174"/>
+      <c r="I15" s="175"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
@@ -17517,15 +17546,15 @@
       <c r="D16" s="82" t="s">
         <v>627</v>
       </c>
-      <c r="E16" s="177" t="s">
+      <c r="E16" s="176" t="s">
         <v>656</v>
       </c>
-      <c r="F16" s="178"/>
-      <c r="G16" s="177" t="s">
+      <c r="F16" s="163"/>
+      <c r="G16" s="176" t="s">
         <v>657</v>
       </c>
-      <c r="H16" s="179"/>
-      <c r="I16" s="180"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="167"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -17540,15 +17569,15 @@
       <c r="D17" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="181" t="s">
+      <c r="E17" s="170" t="s">
         <v>659</v>
       </c>
-      <c r="F17" s="178"/>
-      <c r="G17" s="181" t="s">
+      <c r="F17" s="163"/>
+      <c r="G17" s="170" t="s">
         <v>660</v>
       </c>
-      <c r="H17" s="179"/>
-      <c r="I17" s="180"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="167"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -17563,15 +17592,15 @@
       <c r="D18" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="181" t="s">
+      <c r="E18" s="170" t="s">
         <v>659</v>
       </c>
-      <c r="F18" s="178"/>
-      <c r="G18" s="181" t="s">
+      <c r="F18" s="163"/>
+      <c r="G18" s="170" t="s">
         <v>662</v>
       </c>
-      <c r="H18" s="179"/>
-      <c r="I18" s="180"/>
+      <c r="H18" s="166"/>
+      <c r="I18" s="167"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
@@ -17586,15 +17615,15 @@
       <c r="D19" s="86" t="s">
         <v>664</v>
       </c>
-      <c r="E19" s="181" t="s">
+      <c r="E19" s="170" t="s">
         <v>665</v>
       </c>
-      <c r="F19" s="178"/>
-      <c r="G19" s="181" t="s">
+      <c r="F19" s="163"/>
+      <c r="G19" s="170" t="s">
         <v>666</v>
       </c>
-      <c r="H19" s="179"/>
-      <c r="I19" s="180"/>
+      <c r="H19" s="166"/>
+      <c r="I19" s="167"/>
       <c r="K19" s="84" t="s">
         <v>667</v>
       </c>
@@ -17606,11 +17635,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="182"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="182"/>
-      <c r="H20" s="179"/>
-      <c r="I20" s="180"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="166"/>
+      <c r="I20" s="167"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17619,11 +17648,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="182"/>
-      <c r="F21" s="178"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="179"/>
-      <c r="I21" s="180"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="163"/>
+      <c r="G21" s="162"/>
+      <c r="H21" s="166"/>
+      <c r="I21" s="167"/>
       <c r="K21" s="84" t="s">
         <v>668</v>
       </c>
@@ -17635,11 +17664,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="182"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="182"/>
-      <c r="H22" s="179"/>
-      <c r="I22" s="180"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="163"/>
+      <c r="G22" s="162"/>
+      <c r="H22" s="166"/>
+      <c r="I22" s="167"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17648,11 +17677,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="182"/>
-      <c r="F23" s="178"/>
-      <c r="G23" s="182"/>
-      <c r="H23" s="179"/>
-      <c r="I23" s="180"/>
+      <c r="E23" s="162"/>
+      <c r="F23" s="163"/>
+      <c r="G23" s="162"/>
+      <c r="H23" s="166"/>
+      <c r="I23" s="167"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17661,11 +17690,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="182"/>
-      <c r="F24" s="178"/>
-      <c r="G24" s="182"/>
-      <c r="H24" s="179"/>
-      <c r="I24" s="180"/>
+      <c r="E24" s="162"/>
+      <c r="F24" s="163"/>
+      <c r="G24" s="162"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="167"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17674,11 +17703,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="182"/>
-      <c r="F25" s="178"/>
-      <c r="G25" s="182"/>
-      <c r="H25" s="179"/>
-      <c r="I25" s="180"/>
+      <c r="E25" s="162"/>
+      <c r="F25" s="163"/>
+      <c r="G25" s="162"/>
+      <c r="H25" s="166"/>
+      <c r="I25" s="167"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17687,11 +17716,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="183"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="183"/>
+      <c r="E26" s="164"/>
+      <c r="F26" s="165"/>
+      <c r="G26" s="164"/>
       <c r="H26" s="168"/>
-      <c r="I26" s="170"/>
+      <c r="I26" s="169"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18669,14 +18698,16 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18689,16 +18720,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21847,7 +21876,7 @@
       <c r="B2" s="186" t="s">
         <v>679</v>
       </c>
-      <c r="C2" s="178"/>
+      <c r="C2" s="163"/>
       <c r="O2" s="84" t="s">
         <v>680</v>
       </c>
@@ -23064,8 +23093,8 @@
       <c r="A3" s="186" t="s">
         <v>712</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="178"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="163"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
@@ -23074,7 +23103,7 @@
       <c r="B4" s="188" t="s">
         <v>713</v>
       </c>
-      <c r="C4" s="178"/>
+      <c r="C4" s="163"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
@@ -23083,7 +23112,7 @@
       <c r="B5" s="187" t="s">
         <v>715</v>
       </c>
-      <c r="C5" s="178"/>
+      <c r="C5" s="163"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
@@ -23092,7 +23121,7 @@
       <c r="B6" s="187" t="s">
         <v>717</v>
       </c>
-      <c r="C6" s="178"/>
+      <c r="C6" s="163"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
@@ -23101,7 +23130,7 @@
       <c r="B7" s="187" t="s">
         <v>719</v>
       </c>
-      <c r="C7" s="178"/>
+      <c r="C7" s="163"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
@@ -23110,7 +23139,7 @@
       <c r="B8" s="187" t="s">
         <v>721</v>
       </c>
-      <c r="C8" s="178"/>
+      <c r="C8" s="163"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24141,8 +24170,8 @@
       <c r="B2" s="189" t="s">
         <v>722</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="164"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="179"/>
       <c r="J2" s="84" t="s">
         <v>680</v>
       </c>
@@ -28294,8 +28323,8 @@
       <c r="A5" s="188" t="s">
         <v>755</v>
       </c>
-      <c r="B5" s="179"/>
-      <c r="C5" s="178"/>
+      <c r="B5" s="166"/>
+      <c r="C5" s="163"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">

</xml_diff>

<commit_message>
SRNTGT018 Added, 016 update
</commit_message>
<xml_diff>
--- a/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
+++ b/INTEL/OPAC_JOINT_TARGET_LIST_v 0.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\OPAT-background\INTEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F1C465-6F2F-497E-A074-ED1817DA1C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8493DA13-ACD0-47B9-84DE-DAF170120C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="2610" windowWidth="33705" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="33495" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAC Joint Target List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="911">
   <si>
     <t>OPERATION ARCTIC CITADEL JOINT TARGET LIST</t>
   </si>
@@ -4014,25 +4014,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4046,17 +4041,22 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5454,10 +5454,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6121,7 +6121,9 @@
       <c r="I21" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="8"/>
+      <c r="J21" s="143" t="s">
+        <v>63</v>
+      </c>
       <c r="K21" s="2" t="s">
         <v>363</v>
       </c>
@@ -17374,50 +17376,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="184" t="s">
         <v>614</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="171"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="185"/>
+      <c r="I1" s="186"/>
     </row>
     <row r="2" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="172" t="s">
+      <c r="A2" s="187" t="s">
         <v>615</v>
       </c>
-      <c r="B2" s="173"/>
+      <c r="B2" s="172"/>
       <c r="C2" s="80" t="s">
         <v>616</v>
       </c>
-      <c r="D2" s="174" t="s">
+      <c r="D2" s="188" t="s">
         <v>617</v>
       </c>
       <c r="E2" s="175"/>
       <c r="F2" s="175"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="176" t="s">
+      <c r="G2" s="172"/>
+      <c r="H2" s="189" t="s">
         <v>618</v>
       </c>
-      <c r="I2" s="177"/>
+      <c r="I2" s="176"/>
     </row>
     <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="178" t="s">
+      <c r="A4" s="190" t="s">
         <v>619</v>
       </c>
-      <c r="B4" s="170"/>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="171"/>
+      <c r="B4" s="185"/>
+      <c r="C4" s="185"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="185"/>
+      <c r="G4" s="185"/>
+      <c r="H4" s="185"/>
+      <c r="I4" s="186"/>
     </row>
     <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="81" t="s">
@@ -17479,15 +17481,15 @@
       <c r="I6" s="87" t="s">
         <v>636</v>
       </c>
-      <c r="K6" s="179" t="s">
+      <c r="K6" s="178" t="s">
         <v>637</v>
       </c>
-      <c r="L6" s="180"/>
-      <c r="M6" s="180"/>
-      <c r="N6" s="180"/>
-      <c r="O6" s="180"/>
-      <c r="P6" s="180"/>
-      <c r="Q6" s="180"/>
+      <c r="L6" s="179"/>
+      <c r="M6" s="179"/>
+      <c r="N6" s="179"/>
+      <c r="O6" s="179"/>
+      <c r="P6" s="179"/>
+      <c r="Q6" s="179"/>
     </row>
     <row r="7" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="85">
@@ -17517,15 +17519,15 @@
       <c r="I7" s="87" t="s">
         <v>645</v>
       </c>
-      <c r="K7" s="179" t="s">
+      <c r="K7" s="178" t="s">
         <v>646</v>
       </c>
-      <c r="L7" s="180"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="180"/>
-      <c r="O7" s="180"/>
-      <c r="P7" s="180"/>
-      <c r="Q7" s="180"/>
+      <c r="L7" s="179"/>
+      <c r="M7" s="179"/>
+      <c r="N7" s="179"/>
+      <c r="O7" s="179"/>
+      <c r="P7" s="179"/>
+      <c r="Q7" s="179"/>
     </row>
     <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="85">
@@ -17633,17 +17635,17 @@
       <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="181" t="s">
+      <c r="A15" s="180" t="s">
         <v>655</v>
       </c>
-      <c r="B15" s="182"/>
-      <c r="C15" s="182"/>
-      <c r="D15" s="182"/>
-      <c r="E15" s="182"/>
-      <c r="F15" s="182"/>
-      <c r="G15" s="182"/>
-      <c r="H15" s="182"/>
-      <c r="I15" s="183"/>
+      <c r="B15" s="181"/>
+      <c r="C15" s="181"/>
+      <c r="D15" s="181"/>
+      <c r="E15" s="181"/>
+      <c r="F15" s="181"/>
+      <c r="G15" s="181"/>
+      <c r="H15" s="181"/>
+      <c r="I15" s="182"/>
     </row>
     <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="81" t="s">
@@ -17658,15 +17660,15 @@
       <c r="D16" s="82" t="s">
         <v>627</v>
       </c>
-      <c r="E16" s="184" t="s">
+      <c r="E16" s="183" t="s">
         <v>656</v>
       </c>
-      <c r="F16" s="185"/>
-      <c r="G16" s="184" t="s">
+      <c r="F16" s="170"/>
+      <c r="G16" s="183" t="s">
         <v>657</v>
       </c>
-      <c r="H16" s="186"/>
-      <c r="I16" s="187"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="174"/>
     </row>
     <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="92">
@@ -17681,15 +17683,15 @@
       <c r="D17" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="188" t="s">
+      <c r="E17" s="177" t="s">
         <v>659</v>
       </c>
-      <c r="F17" s="185"/>
-      <c r="G17" s="188" t="s">
+      <c r="F17" s="170"/>
+      <c r="G17" s="177" t="s">
         <v>660</v>
       </c>
-      <c r="H17" s="186"/>
-      <c r="I17" s="187"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="174"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -17704,15 +17706,15 @@
       <c r="D18" s="86" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="188" t="s">
+      <c r="E18" s="177" t="s">
         <v>659</v>
       </c>
-      <c r="F18" s="185"/>
-      <c r="G18" s="188" t="s">
+      <c r="F18" s="170"/>
+      <c r="G18" s="177" t="s">
         <v>662</v>
       </c>
-      <c r="H18" s="186"/>
-      <c r="I18" s="187"/>
+      <c r="H18" s="173"/>
+      <c r="I18" s="174"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="92">
@@ -17727,15 +17729,15 @@
       <c r="D19" s="86" t="s">
         <v>664</v>
       </c>
-      <c r="E19" s="188" t="s">
+      <c r="E19" s="177" t="s">
         <v>665</v>
       </c>
-      <c r="F19" s="185"/>
-      <c r="G19" s="188" t="s">
+      <c r="F19" s="170"/>
+      <c r="G19" s="177" t="s">
         <v>666</v>
       </c>
-      <c r="H19" s="186"/>
-      <c r="I19" s="187"/>
+      <c r="H19" s="173"/>
+      <c r="I19" s="174"/>
       <c r="K19" s="84" t="s">
         <v>667</v>
       </c>
@@ -17747,11 +17749,11 @@
       <c r="B20" s="93"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
-      <c r="E20" s="189"/>
-      <c r="F20" s="185"/>
-      <c r="G20" s="189"/>
-      <c r="H20" s="186"/>
-      <c r="I20" s="187"/>
+      <c r="E20" s="169"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="169"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="174"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="92">
@@ -17760,11 +17762,11 @@
       <c r="B21" s="93"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
-      <c r="E21" s="189"/>
-      <c r="F21" s="185"/>
-      <c r="G21" s="189"/>
-      <c r="H21" s="186"/>
-      <c r="I21" s="187"/>
+      <c r="E21" s="169"/>
+      <c r="F21" s="170"/>
+      <c r="G21" s="169"/>
+      <c r="H21" s="173"/>
+      <c r="I21" s="174"/>
       <c r="K21" s="84" t="s">
         <v>668</v>
       </c>
@@ -17776,11 +17778,11 @@
       <c r="B22" s="93"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
-      <c r="E22" s="189"/>
-      <c r="F22" s="185"/>
-      <c r="G22" s="189"/>
-      <c r="H22" s="186"/>
-      <c r="I22" s="187"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="170"/>
+      <c r="G22" s="169"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="174"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="92">
@@ -17789,11 +17791,11 @@
       <c r="B23" s="93"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
-      <c r="E23" s="189"/>
-      <c r="F23" s="185"/>
-      <c r="G23" s="189"/>
-      <c r="H23" s="186"/>
-      <c r="I23" s="187"/>
+      <c r="E23" s="169"/>
+      <c r="F23" s="170"/>
+      <c r="G23" s="169"/>
+      <c r="H23" s="173"/>
+      <c r="I23" s="174"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="92">
@@ -17802,11 +17804,11 @@
       <c r="B24" s="93"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
-      <c r="E24" s="189"/>
-      <c r="F24" s="185"/>
-      <c r="G24" s="189"/>
-      <c r="H24" s="186"/>
-      <c r="I24" s="187"/>
+      <c r="E24" s="169"/>
+      <c r="F24" s="170"/>
+      <c r="G24" s="169"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="174"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="92">
@@ -17815,11 +17817,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="189"/>
-      <c r="F25" s="185"/>
-      <c r="G25" s="189"/>
-      <c r="H25" s="186"/>
-      <c r="I25" s="187"/>
+      <c r="E25" s="169"/>
+      <c r="F25" s="170"/>
+      <c r="G25" s="169"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="174"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="94">
@@ -17828,11 +17830,11 @@
       <c r="B26" s="89"/>
       <c r="C26" s="89"/>
       <c r="D26" s="89"/>
-      <c r="E26" s="190"/>
-      <c r="F26" s="173"/>
-      <c r="G26" s="190"/>
+      <c r="E26" s="171"/>
+      <c r="F26" s="172"/>
+      <c r="G26" s="171"/>
       <c r="H26" s="175"/>
-      <c r="I26" s="177"/>
+      <c r="I26" s="176"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18810,14 +18812,16 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18830,16 +18834,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21988,7 +21990,7 @@
       <c r="B2" s="193" t="s">
         <v>679</v>
       </c>
-      <c r="C2" s="185"/>
+      <c r="C2" s="170"/>
       <c r="O2" s="84" t="s">
         <v>680</v>
       </c>
@@ -23205,8 +23207,8 @@
       <c r="A3" s="193" t="s">
         <v>712</v>
       </c>
-      <c r="B3" s="186"/>
-      <c r="C3" s="185"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="170"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
@@ -23215,7 +23217,7 @@
       <c r="B4" s="195" t="s">
         <v>713</v>
       </c>
-      <c r="C4" s="185"/>
+      <c r="C4" s="170"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
@@ -23224,7 +23226,7 @@
       <c r="B5" s="194" t="s">
         <v>715</v>
       </c>
-      <c r="C5" s="185"/>
+      <c r="C5" s="170"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
@@ -23233,7 +23235,7 @@
       <c r="B6" s="194" t="s">
         <v>717</v>
       </c>
-      <c r="C6" s="185"/>
+      <c r="C6" s="170"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
@@ -23242,7 +23244,7 @@
       <c r="B7" s="194" t="s">
         <v>719</v>
       </c>
-      <c r="C7" s="185"/>
+      <c r="C7" s="170"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
@@ -23251,7 +23253,7 @@
       <c r="B8" s="194" t="s">
         <v>721</v>
       </c>
-      <c r="C8" s="185"/>
+      <c r="C8" s="170"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24282,8 +24284,8 @@
       <c r="B2" s="196" t="s">
         <v>722</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="186"/>
       <c r="J2" s="84" t="s">
         <v>680</v>
       </c>
@@ -28435,8 +28437,8 @@
       <c r="A5" s="195" t="s">
         <v>755</v>
       </c>
-      <c r="B5" s="186"/>
-      <c r="C5" s="185"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="170"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">

</xml_diff>